<commit_message>
round 4 2021 predictions
</commit_message>
<xml_diff>
--- a/django_AFL_ML/Data/Adelaide_stats.xlsx
+++ b/django_AFL_ML/Data/Adelaide_stats.xlsx
@@ -377,7 +377,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:HU102"/>
+  <dimension ref="A1:HV102"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="GZ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="HA23" activeCellId="0" sqref="HA23"/>
@@ -1075,8 +1075,11 @@
       <c r="HT1" s="1" t="n">
         <v>10330</v>
       </c>
-      <c r="HU1" t="n">
+      <c r="HU1" s="1" t="n">
         <v>10338</v>
+      </c>
+      <c r="HV1" t="n">
+        <v>10347</v>
       </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="2">
@@ -1766,7 +1769,10 @@
       <c r="HT2" s="1" t="n">
         <v>2021</v>
       </c>
-      <c r="HU2" t="n">
+      <c r="HU2" s="1" t="n">
+        <v>2021</v>
+      </c>
+      <c r="HV2" t="n">
         <v>2021</v>
       </c>
     </row>
@@ -2457,8 +2463,11 @@
       <c r="HT3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="HU3" t="n">
+      <c r="HU3" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="HV3" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="2">
@@ -3148,8 +3157,11 @@
       <c r="HT4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="HU4" t="n">
+      <c r="HU4" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="HV4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5" ht="13.8" customHeight="1" s="2">
@@ -3839,7 +3851,10 @@
       <c r="HT5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="HU5" t="n">
+      <c r="HU5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="HV5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4530,8 +4545,11 @@
       <c r="HT6" s="1" t="n">
         <v>103</v>
       </c>
-      <c r="HU6" t="n">
+      <c r="HU6" s="1" t="n">
         <v>88</v>
+      </c>
+      <c r="HV6" t="n">
+        <v>95</v>
       </c>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="2">
@@ -5221,8 +5239,11 @@
       <c r="HT7" s="1" t="n">
         <v>91</v>
       </c>
-      <c r="HU7" t="n">
+      <c r="HU7" s="1" t="n">
         <v>121</v>
+      </c>
+      <c r="HV7" t="n">
+        <v>85</v>
       </c>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="2">
@@ -5912,8 +5933,11 @@
       <c r="HT8" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="HU8" t="n">
+      <c r="HU8" s="1" t="n">
         <v>-33</v>
+      </c>
+      <c r="HV8" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="2">
@@ -6603,8 +6627,11 @@
       <c r="HT9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="HU9" t="n">
+      <c r="HU9" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="HV9" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10" ht="13.8" customHeight="1" s="2">
@@ -7294,8 +7321,11 @@
       <c r="HT10" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="HU10" t="n">
+      <c r="HU10" s="1" t="n">
         <v>16</v>
+      </c>
+      <c r="HV10" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="11" ht="13.8" customHeight="1" s="2">
@@ -7985,8 +8015,11 @@
       <c r="HT11" s="1" t="n">
         <v>199</v>
       </c>
-      <c r="HU11" t="n">
+      <c r="HU11" s="1" t="n">
         <v>184</v>
+      </c>
+      <c r="HV11" t="n">
+        <v>209</v>
       </c>
     </row>
     <row r="12" ht="13.8" customHeight="1" s="2">
@@ -8676,8 +8709,11 @@
       <c r="HT12" s="1" t="n">
         <v>118</v>
       </c>
-      <c r="HU12" t="n">
+      <c r="HU12" s="1" t="n">
         <v>131</v>
+      </c>
+      <c r="HV12" t="n">
+        <v>160</v>
       </c>
     </row>
     <row r="13" ht="13.8" customHeight="1" s="2">
@@ -9367,8 +9403,11 @@
       <c r="HT13" s="1" t="n">
         <v>317</v>
       </c>
-      <c r="HU13" t="n">
+      <c r="HU13" s="1" t="n">
         <v>315</v>
+      </c>
+      <c r="HV13" t="n">
+        <v>369</v>
       </c>
     </row>
     <row r="14" ht="13.8" customHeight="1" s="2">
@@ -10058,8 +10097,11 @@
       <c r="HT14" s="1" t="n">
         <v>1.69</v>
       </c>
-      <c r="HU14" t="n">
+      <c r="HU14" s="1" t="n">
         <v>1.4</v>
+      </c>
+      <c r="HV14" t="n">
+        <v>1.31</v>
       </c>
     </row>
     <row r="15" ht="13.8" customHeight="1" s="2">
@@ -10749,8 +10791,11 @@
       <c r="HT15" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="HU15" t="n">
+      <c r="HU15" s="1" t="n">
         <v>59</v>
+      </c>
+      <c r="HV15" t="n">
+        <v>81</v>
       </c>
     </row>
     <row r="16" ht="13.8" customHeight="1" s="2">
@@ -11440,8 +11485,11 @@
       <c r="HT16" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="HU16" t="n">
+      <c r="HU16" s="1" t="n">
         <v>50</v>
+      </c>
+      <c r="HV16" t="n">
+        <v>58</v>
       </c>
     </row>
     <row r="17" ht="13.8" customHeight="1" s="2">
@@ -12131,8 +12179,11 @@
       <c r="HT17" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="HU17" t="n">
+      <c r="HU17" s="1" t="n">
         <v>32</v>
+      </c>
+      <c r="HV17" t="n">
+        <v>36</v>
       </c>
     </row>
     <row r="18" ht="13.8" customHeight="1" s="2">
@@ -12822,8 +12873,11 @@
       <c r="HT18" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="HU18" t="n">
+      <c r="HU18" s="1" t="n">
         <v>28</v>
+      </c>
+      <c r="HV18" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="19" ht="13.8" customHeight="1" s="2">
@@ -13513,8 +13567,11 @@
       <c r="HT19" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="HU19" t="n">
+      <c r="HU19" s="1" t="n">
         <v>14</v>
+      </c>
+      <c r="HV19" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="20" ht="13.8" customHeight="1" s="2">
@@ -14204,8 +14261,11 @@
       <c r="HT20" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="HU20" t="n">
+      <c r="HU20" s="1" t="n">
         <v>11</v>
+      </c>
+      <c r="HV20" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="21" ht="13.8" customHeight="1" s="2">
@@ -14895,8 +14955,11 @@
       <c r="HT21" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="HU21" t="n">
+      <c r="HU21" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="HV21" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="22" ht="13.8" customHeight="1" s="2">
@@ -15586,8 +15649,11 @@
       <c r="HT22" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="HU22" t="n">
+      <c r="HU22" s="1" t="n">
         <v>19</v>
+      </c>
+      <c r="HV22" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="23" ht="13.8" customHeight="1" s="2">
@@ -16277,8 +16343,11 @@
       <c r="HT23" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="HU23" t="n">
+      <c r="HU23" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="HV23" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="24" ht="13.8" customHeight="1" s="2">
@@ -16968,8 +17037,11 @@
       <c r="HT24" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="HU24" t="n">
+      <c r="HU24" s="1" t="n">
         <v>33</v>
+      </c>
+      <c r="HV24" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="25" ht="13.8" customHeight="1" s="2">
@@ -17659,8 +17731,11 @@
       <c r="HT25" s="1" t="n">
         <v>53.6</v>
       </c>
-      <c r="HU25" t="n">
+      <c r="HU25" s="1" t="n">
         <v>33.3</v>
+      </c>
+      <c r="HV25" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="26" ht="13.8" customHeight="1" s="2">
@@ -18350,8 +18425,11 @@
       <c r="HT26" s="1" t="n">
         <v>21.13</v>
       </c>
-      <c r="HU26" t="n">
+      <c r="HU26" s="1" t="n">
         <v>28.64</v>
+      </c>
+      <c r="HV26" t="n">
+        <v>26.36</v>
       </c>
     </row>
     <row r="27" ht="13.8" customHeight="1" s="2">
@@ -19041,8 +19119,11 @@
       <c r="HT27" s="1" t="n">
         <v>11.32</v>
       </c>
-      <c r="HU27" t="n">
+      <c r="HU27" s="1" t="n">
         <v>9.550000000000001</v>
+      </c>
+      <c r="HV27" t="n">
+        <v>14.76</v>
       </c>
     </row>
     <row r="28" ht="13.8" customHeight="1" s="2">
@@ -19732,8 +19813,11 @@
       <c r="HT28" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="HU28" t="n">
+      <c r="HU28" s="1" t="n">
         <v>41</v>
+      </c>
+      <c r="HV28" t="n">
+        <v>34</v>
       </c>
     </row>
     <row r="29" ht="13.8" customHeight="1" s="2">
@@ -20423,8 +20507,11 @@
       <c r="HT29" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="HU29" t="n">
+      <c r="HU29" s="1" t="n">
         <v>42</v>
+      </c>
+      <c r="HV29" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="30" ht="13.8" customHeight="1" s="2">
@@ -21114,8 +21201,11 @@
       <c r="HT30" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="HU30" t="n">
+      <c r="HU30" s="1" t="n">
         <v>43</v>
+      </c>
+      <c r="HV30" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="31" ht="13.8" customHeight="1" s="2">
@@ -21805,8 +21895,11 @@
       <c r="HT31" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="HU31" t="n">
+      <c r="HU31" s="1" t="n">
         <v>55</v>
+      </c>
+      <c r="HV31" t="n">
+        <v>57</v>
       </c>
     </row>
     <row r="32" ht="13.8" customHeight="1" s="2">
@@ -22496,8 +22589,11 @@
       <c r="HT32" s="1" t="n">
         <v>1.82</v>
       </c>
-      <c r="HU32" t="n">
+      <c r="HU32" s="1" t="n">
         <v>1.67</v>
+      </c>
+      <c r="HV32" t="n">
+        <v>2.28</v>
       </c>
     </row>
     <row r="33" ht="13.8" customHeight="1" s="2">
@@ -23187,8 +23283,11 @@
       <c r="HT33" s="1" t="n">
         <v>3.4</v>
       </c>
-      <c r="HU33" t="n">
+      <c r="HU33" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="HV33" t="n">
+        <v>4.07</v>
       </c>
     </row>
     <row r="34" ht="13.8" customHeight="1" s="2">
@@ -23878,8 +23977,11 @@
       <c r="HT34" s="1" t="n">
         <v>54.9</v>
       </c>
-      <c r="HU34" t="n">
+      <c r="HU34" s="1" t="n">
         <v>54.5</v>
+      </c>
+      <c r="HV34" t="n">
+        <v>42.1</v>
       </c>
     </row>
     <row r="35" ht="13.8" customHeight="1" s="2">
@@ -24569,8 +24671,11 @@
       <c r="HT35" s="1" t="n">
         <v>29.4</v>
       </c>
-      <c r="HU35" t="n">
+      <c r="HU35" s="1" t="n">
         <v>20</v>
+      </c>
+      <c r="HV35" t="n">
+        <v>24.6</v>
       </c>
     </row>
     <row r="36" ht="13.8" customHeight="1" s="2">
@@ -25260,8 +25365,11 @@
       <c r="HT36" s="1" t="n">
         <v>186.3</v>
       </c>
-      <c r="HU36" t="n">
+      <c r="HU36" s="1" t="n">
         <v>186.3</v>
+      </c>
+      <c r="HV36" t="n">
+        <v>186.1</v>
       </c>
     </row>
     <row r="37" ht="13.8" customHeight="1" s="2">
@@ -25951,7 +26059,10 @@
       <c r="HT37" s="1" t="n">
         <v>83.3</v>
       </c>
-      <c r="HU37" t="n">
+      <c r="HU37" s="1" t="n">
+        <v>83.3</v>
+      </c>
+      <c r="HV37" t="n">
         <v>83.3</v>
       </c>
     </row>
@@ -26642,8 +26753,11 @@
       <c r="HT38" s="1" t="n">
         <v>24.66</v>
       </c>
-      <c r="HU38" t="n">
+      <c r="HU38" s="1" t="n">
         <v>24.66</v>
+      </c>
+      <c r="HV38" t="n">
+        <v>24.74</v>
       </c>
     </row>
     <row r="39" ht="13.8" customHeight="1" s="2">
@@ -27333,8 +27447,11 @@
       <c r="HT39" s="1" t="n">
         <v>66.2</v>
       </c>
-      <c r="HU39" t="n">
+      <c r="HU39" s="1" t="n">
         <v>68.7</v>
+      </c>
+      <c r="HV39" t="n">
+        <v>71</v>
       </c>
     </row>
     <row r="40" ht="13.8" customHeight="1" s="2">
@@ -28024,8 +28141,11 @@
       <c r="HT40" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="HU40" t="n">
+      <c r="HU40" s="1" t="n">
         <v>15</v>
+      </c>
+      <c r="HV40" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="41" ht="13.8" customHeight="1" s="2">
@@ -28715,8 +28835,11 @@
       <c r="HT41" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="HU41" t="n">
+      <c r="HU41" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="HV41" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="42" ht="13.8" customHeight="1" s="2">
@@ -29406,7 +29529,10 @@
       <c r="HT42" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="HU42" t="n">
+      <c r="HU42" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="HV42" t="n">
         <v>1</v>
       </c>
     </row>
@@ -30097,7 +30223,10 @@
       <c r="HT43" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="HU43" t="n">
+      <c r="HU43" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="HV43" t="n">
         <v>6</v>
       </c>
     </row>
@@ -30788,8 +30917,11 @@
       <c r="HT44" s="1" t="n">
         <v>139</v>
       </c>
-      <c r="HU44" t="n">
+      <c r="HU44" s="1" t="n">
         <v>124</v>
+      </c>
+      <c r="HV44" t="n">
+        <v>148</v>
       </c>
     </row>
     <row r="45" ht="13.8" customHeight="1" s="2">
@@ -31479,8 +31611,11 @@
       <c r="HT45" s="1" t="n">
         <v>174</v>
       </c>
-      <c r="HU45" t="n">
+      <c r="HU45" s="1" t="n">
         <v>179</v>
+      </c>
+      <c r="HV45" t="n">
+        <v>218</v>
       </c>
     </row>
     <row r="46" ht="13.8" customHeight="1" s="2">
@@ -32170,8 +32305,11 @@
       <c r="HT46" s="1" t="n">
         <v>225</v>
       </c>
-      <c r="HU46" t="n">
+      <c r="HU46" s="1" t="n">
         <v>230</v>
+      </c>
+      <c r="HV46" t="n">
+        <v>276</v>
       </c>
     </row>
     <row r="47" ht="13.8" customHeight="1" s="2">
@@ -32861,8 +32999,11 @@
       <c r="HT47" s="1" t="n">
         <v>71</v>
       </c>
-      <c r="HU47" t="n">
+      <c r="HU47" s="1" t="n">
         <v>73</v>
+      </c>
+      <c r="HV47" t="n">
+        <v>74.8</v>
       </c>
     </row>
     <row r="48" ht="13.8" customHeight="1" s="2">
@@ -33552,8 +33693,11 @@
       <c r="HT48" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="HU48" t="n">
+      <c r="HU48" s="1" t="n">
         <v>42</v>
+      </c>
+      <c r="HV48" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="49" ht="13.8" customHeight="1" s="2">
@@ -34243,8 +34387,11 @@
       <c r="HT49" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="HU49" t="n">
+      <c r="HU49" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="HV49" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="50" ht="13.8" customHeight="1" s="2">
@@ -34934,8 +35081,11 @@
       <c r="HT50" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="HU50" t="n">
+      <c r="HU50" s="1" t="n">
         <v>12</v>
+      </c>
+      <c r="HV50" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="51" ht="13.8" customHeight="1" s="2">
@@ -35625,8 +35775,11 @@
       <c r="HT51" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="HU51" t="n">
+      <c r="HU51" s="1" t="n">
         <v>41</v>
+      </c>
+      <c r="HV51" t="n">
+        <v>34</v>
       </c>
     </row>
     <row r="52" ht="13.8" customHeight="1" s="2">
@@ -36316,8 +36469,11 @@
       <c r="HT52" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="HU52" t="n">
+      <c r="HU52" s="1" t="n">
         <v>43</v>
+      </c>
+      <c r="HV52" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="53" ht="13.8" customHeight="1" s="2">
@@ -37007,8 +37163,11 @@
       <c r="HT53" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="HU53" t="n">
+      <c r="HU53" s="1" t="n">
         <v>33</v>
+      </c>
+      <c r="HV53" t="n">
+        <v>57</v>
       </c>
     </row>
     <row r="54" ht="13.8" customHeight="1" s="2">
@@ -37698,8 +37857,11 @@
       <c r="HT54" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="HU54" t="n">
+      <c r="HU54" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="HV54" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="55" ht="13.8" customHeight="1" s="2">
@@ -38389,8 +38551,11 @@
       <c r="HT55" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="HU55" t="n">
+      <c r="HU55" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="HV55" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="56" ht="13.8" customHeight="1" s="2">
@@ -39080,8 +39245,11 @@
       <c r="HT56" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="HU56" t="n">
+      <c r="HU56" s="1" t="n">
         <v>54.5</v>
+      </c>
+      <c r="HV56" t="n">
+        <v>64.3</v>
       </c>
     </row>
     <row r="57" ht="13.8" customHeight="1" s="2">
@@ -39771,8 +39939,11 @@
       <c r="HT57" s="1" t="n">
         <v>195</v>
       </c>
-      <c r="HU57" t="n">
+      <c r="HU57" s="1" t="n">
         <v>239</v>
+      </c>
+      <c r="HV57" t="n">
+        <v>230</v>
       </c>
     </row>
     <row r="58" ht="13.8" customHeight="1" s="2">
@@ -40462,8 +40633,11 @@
       <c r="HT58" s="1" t="n">
         <v>154</v>
       </c>
-      <c r="HU58" t="n">
+      <c r="HU58" s="1" t="n">
         <v>137</v>
+      </c>
+      <c r="HV58" t="n">
+        <v>99</v>
       </c>
     </row>
     <row r="59" ht="13.8" customHeight="1" s="2">
@@ -41153,8 +41327,11 @@
       <c r="HT59" s="1" t="n">
         <v>349</v>
       </c>
-      <c r="HU59" t="n">
+      <c r="HU59" s="1" t="n">
         <v>376</v>
+      </c>
+      <c r="HV59" t="n">
+        <v>329</v>
       </c>
     </row>
     <row r="60" ht="13.8" customHeight="1" s="2">
@@ -41844,8 +42021,11 @@
       <c r="HT60" s="1" t="n">
         <v>1.27</v>
       </c>
-      <c r="HU60" t="n">
+      <c r="HU60" s="1" t="n">
         <v>1.74</v>
+      </c>
+      <c r="HV60" t="n">
+        <v>2.32</v>
       </c>
     </row>
     <row r="61" ht="13.8" customHeight="1" s="2">
@@ -42535,7 +42715,10 @@
       <c r="HT61" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="HU61" t="n">
+      <c r="HU61" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="HV61" t="n">
         <v>104</v>
       </c>
     </row>
@@ -43226,8 +43409,11 @@
       <c r="HT62" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="HU62" t="n">
+      <c r="HU62" s="1" t="n">
         <v>55</v>
+      </c>
+      <c r="HV62" t="n">
+        <v>71</v>
       </c>
     </row>
     <row r="63" ht="13.8" customHeight="1" s="2">
@@ -43917,7 +44103,10 @@
       <c r="HT63" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="HU63" t="n">
+      <c r="HU63" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="HV63" t="n">
         <v>34</v>
       </c>
     </row>
@@ -44608,8 +44797,11 @@
       <c r="HT64" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="HU64" t="n">
+      <c r="HU64" s="1" t="n">
         <v>14</v>
+      </c>
+      <c r="HV64" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="65" ht="13.8" customHeight="1" s="2">
@@ -45299,8 +45491,11 @@
       <c r="HT65" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="HU65" t="n">
+      <c r="HU65" s="1" t="n">
         <v>28</v>
+      </c>
+      <c r="HV65" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="66" ht="13.8" customHeight="1" s="2">
@@ -45990,8 +46185,11 @@
       <c r="HT66" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="HU66" t="n">
+      <c r="HU66" s="1" t="n">
         <v>18</v>
+      </c>
+      <c r="HV66" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="67" ht="13.8" customHeight="1" s="2">
@@ -46681,8 +46879,11 @@
       <c r="HT67" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="HU67" t="n">
+      <c r="HU67" s="1" t="n">
         <v>14</v>
+      </c>
+      <c r="HV67" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="68" ht="13.8" customHeight="1" s="2">
@@ -47372,7 +47573,10 @@
       <c r="HT68" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="HU68" t="n">
+      <c r="HU68" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="HV68" t="n">
         <v>11</v>
       </c>
     </row>
@@ -48063,7 +48267,10 @@
       <c r="HT69" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="HU69" t="n">
+      <c r="HU69" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="HV69" t="n">
         <v>2</v>
       </c>
     </row>
@@ -48754,8 +48961,11 @@
       <c r="HT70" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="HU70" t="n">
+      <c r="HU70" s="1" t="n">
         <v>31</v>
+      </c>
+      <c r="HV70" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="71" ht="13.8" customHeight="1" s="2">
@@ -49445,8 +49655,11 @@
       <c r="HT71" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="HU71" t="n">
+      <c r="HU71" s="1" t="n">
         <v>58.1</v>
+      </c>
+      <c r="HV71" t="n">
+        <v>48</v>
       </c>
     </row>
     <row r="72" ht="13.8" customHeight="1" s="2">
@@ -50136,8 +50349,11 @@
       <c r="HT72" s="1" t="n">
         <v>26.85</v>
       </c>
-      <c r="HU72" t="n">
+      <c r="HU72" s="1" t="n">
         <v>20.89</v>
+      </c>
+      <c r="HV72" t="n">
+        <v>27.42</v>
       </c>
     </row>
     <row r="73" ht="13.8" customHeight="1" s="2">
@@ -50827,8 +51043,11 @@
       <c r="HT73" s="1" t="n">
         <v>13.42</v>
       </c>
-      <c r="HU73" t="n">
+      <c r="HU73" s="1" t="n">
         <v>12.13</v>
+      </c>
+      <c r="HV73" t="n">
+        <v>13.16</v>
       </c>
     </row>
     <row r="74" ht="13.8" customHeight="1" s="2">
@@ -51518,8 +51737,11 @@
       <c r="HT74" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="HU74" t="n">
+      <c r="HU74" s="1" t="n">
         <v>28</v>
+      </c>
+      <c r="HV74" t="n">
+        <v>41</v>
       </c>
     </row>
     <row r="75" ht="13.8" customHeight="1" s="2">
@@ -52209,8 +52431,11 @@
       <c r="HT75" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="HU75" t="n">
+      <c r="HU75" s="1" t="n">
         <v>47</v>
+      </c>
+      <c r="HV75" t="n">
+        <v>55</v>
       </c>
     </row>
     <row r="76" ht="13.8" customHeight="1" s="2">
@@ -52900,8 +53125,11 @@
       <c r="HT76" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="HU76" t="n">
+      <c r="HU76" s="1" t="n">
         <v>44</v>
+      </c>
+      <c r="HV76" t="n">
+        <v>41</v>
       </c>
     </row>
     <row r="77" ht="13.8" customHeight="1" s="2">
@@ -53591,8 +53819,11 @@
       <c r="HT77" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="HU77" t="n">
+      <c r="HU77" s="1" t="n">
         <v>61</v>
+      </c>
+      <c r="HV77" t="n">
+        <v>58</v>
       </c>
     </row>
     <row r="78" ht="13.8" customHeight="1" s="2">
@@ -54282,8 +54513,11 @@
       <c r="HT78" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="HU78" t="n">
+      <c r="HU78" s="1" t="n">
         <v>1.97</v>
+      </c>
+      <c r="HV78" t="n">
+        <v>2.32</v>
       </c>
     </row>
     <row r="79" ht="13.8" customHeight="1" s="2">
@@ -54973,8 +55207,11 @@
       <c r="HT79" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="HU79" t="n">
+      <c r="HU79" s="1" t="n">
         <v>3.39</v>
+      </c>
+      <c r="HV79" t="n">
+        <v>4.83</v>
       </c>
     </row>
     <row r="80" ht="13.8" customHeight="1" s="2">
@@ -55664,8 +55901,11 @@
       <c r="HT80" s="1" t="n">
         <v>46.2</v>
       </c>
-      <c r="HU80" t="n">
+      <c r="HU80" s="1" t="n">
         <v>47.5</v>
+      </c>
+      <c r="HV80" t="n">
+        <v>39.7</v>
       </c>
     </row>
     <row r="81" ht="13.8" customHeight="1" s="2">
@@ -56355,8 +56595,11 @@
       <c r="HT81" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="HU81" t="n">
+      <c r="HU81" s="1" t="n">
         <v>29.5</v>
+      </c>
+      <c r="HV81" t="n">
+        <v>20.7</v>
       </c>
     </row>
     <row r="82" ht="13.8" customHeight="1" s="2">
@@ -57046,8 +57289,11 @@
       <c r="HT82" s="1" t="n">
         <v>188.7</v>
       </c>
-      <c r="HU82" t="n">
+      <c r="HU82" s="1" t="n">
         <v>187.4</v>
+      </c>
+      <c r="HV82" t="n">
+        <v>187.3</v>
       </c>
     </row>
     <row r="83" ht="13.8" customHeight="1" s="2">
@@ -57737,8 +57983,11 @@
       <c r="HT83" s="1" t="n">
         <v>88.8</v>
       </c>
-      <c r="HU83" t="n">
+      <c r="HU83" s="1" t="n">
         <v>84.2</v>
+      </c>
+      <c r="HV83" t="n">
+        <v>84.90000000000001</v>
       </c>
     </row>
     <row r="84" ht="13.8" customHeight="1" s="2">
@@ -58428,7 +58677,10 @@
       <c r="HT84" s="1" t="n">
         <v>27.91</v>
       </c>
-      <c r="HU84" t="n">
+      <c r="HU84" s="1" t="n">
+        <v>24.8</v>
+      </c>
+      <c r="HV84" t="n">
         <v>24.8</v>
       </c>
     </row>
@@ -59119,8 +59371,11 @@
       <c r="HT85" s="1" t="n">
         <v>136.6</v>
       </c>
-      <c r="HU85" t="n">
+      <c r="HU85" s="1" t="n">
         <v>97</v>
+      </c>
+      <c r="HV85" t="n">
+        <v>78.3</v>
       </c>
     </row>
     <row r="86" ht="13.8" customHeight="1" s="2">
@@ -59810,8 +60065,11 @@
       <c r="HT86" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="HU86" t="n">
+      <c r="HU86" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="HV86" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="87" ht="13.8" customHeight="1" s="2">
@@ -60501,8 +60759,11 @@
       <c r="HT87" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="HU87" t="n">
+      <c r="HU87" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="HV87" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="88" ht="13.8" customHeight="1" s="2">
@@ -61192,8 +61453,11 @@
       <c r="HT88" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="HU88" t="n">
+      <c r="HU88" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="HV88" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="89" ht="13.8" customHeight="1" s="2">
@@ -61883,8 +62147,11 @@
       <c r="HT89" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="HU89" t="n">
+      <c r="HU89" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="HV89" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="90" ht="13.8" customHeight="1" s="2">
@@ -62574,8 +62841,11 @@
       <c r="HT90" s="1" t="n">
         <v>127</v>
       </c>
-      <c r="HU90" t="n">
+      <c r="HU90" s="1" t="n">
         <v>128</v>
+      </c>
+      <c r="HV90" t="n">
+        <v>150</v>
       </c>
     </row>
     <row r="91" ht="13.8" customHeight="1" s="2">
@@ -63265,8 +63535,11 @@
       <c r="HT91" s="1" t="n">
         <v>218</v>
       </c>
-      <c r="HU91" t="n">
+      <c r="HU91" s="1" t="n">
         <v>232</v>
+      </c>
+      <c r="HV91" t="n">
+        <v>169</v>
       </c>
     </row>
     <row r="92" ht="13.8" customHeight="1" s="2">
@@ -63956,8 +64229,11 @@
       <c r="HT92" s="1" t="n">
         <v>266</v>
       </c>
-      <c r="HU92" t="n">
+      <c r="HU92" s="1" t="n">
         <v>280</v>
+      </c>
+      <c r="HV92" t="n">
+        <v>227</v>
       </c>
     </row>
     <row r="93" ht="13.8" customHeight="1" s="2">
@@ -64647,8 +64923,11 @@
       <c r="HT93" s="1" t="n">
         <v>76.2</v>
       </c>
-      <c r="HU93" t="n">
+      <c r="HU93" s="1" t="n">
         <v>74.5</v>
+      </c>
+      <c r="HV93" t="n">
+        <v>69</v>
       </c>
     </row>
     <row r="94" ht="13.8" customHeight="1" s="2">
@@ -65338,8 +65617,11 @@
       <c r="HT94" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="HU94" t="n">
+      <c r="HU94" s="1" t="n">
         <v>47</v>
+      </c>
+      <c r="HV94" t="n">
+        <v>55</v>
       </c>
     </row>
     <row r="95" ht="13.8" customHeight="1" s="2">
@@ -66029,8 +66311,11 @@
       <c r="HT95" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="HU95" t="n">
+      <c r="HU95" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="HV95" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="96" ht="13.8" customHeight="1" s="2">
@@ -66720,8 +67005,11 @@
       <c r="HT96" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="HU96" t="n">
+      <c r="HU96" s="1" t="n">
         <v>15</v>
+      </c>
+      <c r="HV96" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="97" ht="13.8" customHeight="1" s="2">
@@ -67411,8 +67699,11 @@
       <c r="HT97" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="HU97" t="n">
+      <c r="HU97" s="1" t="n">
         <v>28</v>
+      </c>
+      <c r="HV97" t="n">
+        <v>41</v>
       </c>
     </row>
     <row r="98" ht="13.8" customHeight="1" s="2">
@@ -68102,8 +68393,11 @@
       <c r="HT98" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="HU98" t="n">
+      <c r="HU98" s="1" t="n">
         <v>44</v>
+      </c>
+      <c r="HV98" t="n">
+        <v>41</v>
       </c>
     </row>
     <row r="99" ht="13.8" customHeight="1" s="2">
@@ -68793,8 +69087,11 @@
       <c r="HT99" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="HU99" t="n">
+      <c r="HU99" s="1" t="n">
         <v>53</v>
+      </c>
+      <c r="HV99" t="n">
+        <v>43</v>
       </c>
     </row>
     <row r="100" ht="13.8" customHeight="1" s="2">
@@ -69484,7 +69781,10 @@
       <c r="HT100" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="HU100" t="n">
+      <c r="HU100" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="HV100" t="n">
         <v>6</v>
       </c>
     </row>
@@ -70175,8 +70475,11 @@
       <c r="HT101" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="HU101" t="n">
+      <c r="HU101" s="1" t="n">
         <v>14</v>
+      </c>
+      <c r="HV101" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="102" ht="13.8" customHeight="1" s="2">
@@ -70866,8 +71169,11 @@
       <c r="HT102" s="1" t="n">
         <v>76.90000000000001</v>
       </c>
-      <c r="HU102" t="n">
+      <c r="HU102" s="1" t="n">
         <v>77.8</v>
+      </c>
+      <c r="HV102" t="n">
+        <v>83.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
round 5 predictions 2021
</commit_message>
<xml_diff>
--- a/django_AFL_ML/Data/Adelaide_stats.xlsx
+++ b/django_AFL_ML/Data/Adelaide_stats.xlsx
@@ -377,7 +377,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:HV102"/>
+  <dimension ref="A1:HW102"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="GZ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="HA23" activeCellId="0" sqref="HA23"/>
@@ -1078,8 +1078,11 @@
       <c r="HU1" s="1" t="n">
         <v>10338</v>
       </c>
-      <c r="HV1" t="n">
+      <c r="HV1" s="1" t="n">
         <v>10347</v>
+      </c>
+      <c r="HW1" t="n">
+        <v>10360</v>
       </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="2">
@@ -1772,7 +1775,10 @@
       <c r="HU2" s="1" t="n">
         <v>2021</v>
       </c>
-      <c r="HV2" t="n">
+      <c r="HV2" s="1" t="n">
+        <v>2021</v>
+      </c>
+      <c r="HW2" t="n">
         <v>2021</v>
       </c>
     </row>
@@ -2466,8 +2472,11 @@
       <c r="HU3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="HV3" t="n">
+      <c r="HV3" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="HW3" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="2">
@@ -3160,8 +3169,11 @@
       <c r="HU4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="HV4" t="n">
+      <c r="HV4" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="HW4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5" ht="13.8" customHeight="1" s="2">
@@ -3854,8 +3866,11 @@
       <c r="HU5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="HV5" t="n">
+      <c r="HV5" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="HW5" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6" ht="13.8" customHeight="1" s="2">
@@ -4548,8 +4563,11 @@
       <c r="HU6" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="HV6" t="n">
+      <c r="HV6" s="1" t="n">
         <v>95</v>
+      </c>
+      <c r="HW6" t="n">
+        <v>109</v>
       </c>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="2">
@@ -5242,8 +5260,11 @@
       <c r="HU7" s="1" t="n">
         <v>121</v>
       </c>
-      <c r="HV7" t="n">
+      <c r="HV7" s="1" t="n">
         <v>85</v>
+      </c>
+      <c r="HW7" t="n">
+        <v>68</v>
       </c>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="2">
@@ -5936,8 +5957,11 @@
       <c r="HU8" s="1" t="n">
         <v>-33</v>
       </c>
-      <c r="HV8" t="n">
+      <c r="HV8" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="HW8" t="n">
+        <v>41</v>
       </c>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="2">
@@ -6630,7 +6654,10 @@
       <c r="HU9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="HV9" t="n">
+      <c r="HV9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="HW9" t="n">
         <v>1</v>
       </c>
     </row>
@@ -7324,8 +7351,11 @@
       <c r="HU10" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="HV10" t="n">
+      <c r="HV10" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="HW10" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="11" ht="13.8" customHeight="1" s="2">
@@ -8018,8 +8048,11 @@
       <c r="HU11" s="1" t="n">
         <v>184</v>
       </c>
-      <c r="HV11" t="n">
+      <c r="HV11" s="1" t="n">
         <v>209</v>
+      </c>
+      <c r="HW11" t="n">
+        <v>221</v>
       </c>
     </row>
     <row r="12" ht="13.8" customHeight="1" s="2">
@@ -8712,8 +8745,11 @@
       <c r="HU12" s="1" t="n">
         <v>131</v>
       </c>
-      <c r="HV12" t="n">
+      <c r="HV12" s="1" t="n">
         <v>160</v>
+      </c>
+      <c r="HW12" t="n">
+        <v>149</v>
       </c>
     </row>
     <row r="13" ht="13.8" customHeight="1" s="2">
@@ -9406,8 +9442,11 @@
       <c r="HU13" s="1" t="n">
         <v>315</v>
       </c>
-      <c r="HV13" t="n">
+      <c r="HV13" s="1" t="n">
         <v>369</v>
+      </c>
+      <c r="HW13" t="n">
+        <v>370</v>
       </c>
     </row>
     <row r="14" ht="13.8" customHeight="1" s="2">
@@ -10100,8 +10139,11 @@
       <c r="HU14" s="1" t="n">
         <v>1.4</v>
       </c>
-      <c r="HV14" t="n">
+      <c r="HV14" s="1" t="n">
         <v>1.31</v>
+      </c>
+      <c r="HW14" t="n">
+        <v>1.48</v>
       </c>
     </row>
     <row r="15" ht="13.8" customHeight="1" s="2">
@@ -10794,8 +10836,11 @@
       <c r="HU15" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="HV15" t="n">
+      <c r="HV15" s="1" t="n">
         <v>81</v>
+      </c>
+      <c r="HW15" t="n">
+        <v>105</v>
       </c>
     </row>
     <row r="16" ht="13.8" customHeight="1" s="2">
@@ -11488,8 +11533,11 @@
       <c r="HU16" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="HV16" t="n">
+      <c r="HV16" s="1" t="n">
         <v>58</v>
+      </c>
+      <c r="HW16" t="n">
+        <v>68</v>
       </c>
     </row>
     <row r="17" ht="13.8" customHeight="1" s="2">
@@ -12182,8 +12230,11 @@
       <c r="HU17" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="HV17" t="n">
+      <c r="HV17" s="1" t="n">
         <v>36</v>
+      </c>
+      <c r="HW17" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="18" ht="13.8" customHeight="1" s="2">
@@ -12876,8 +12927,11 @@
       <c r="HU18" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="HV18" t="n">
+      <c r="HV18" s="1" t="n">
         <v>17</v>
+      </c>
+      <c r="HW18" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="19" ht="13.8" customHeight="1" s="2">
@@ -13570,8 +13624,11 @@
       <c r="HU19" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="HV19" t="n">
+      <c r="HV19" s="1" t="n">
         <v>20</v>
+      </c>
+      <c r="HW19" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="20" ht="13.8" customHeight="1" s="2">
@@ -14264,8 +14321,11 @@
       <c r="HU20" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="HV20" t="n">
+      <c r="HV20" s="1" t="n">
         <v>14</v>
+      </c>
+      <c r="HW20" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="21" ht="13.8" customHeight="1" s="2">
@@ -14958,8 +15018,11 @@
       <c r="HU21" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="HV21" t="n">
+      <c r="HV21" s="1" t="n">
         <v>9</v>
+      </c>
+      <c r="HW21" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="22" ht="13.8" customHeight="1" s="2">
@@ -15652,8 +15715,11 @@
       <c r="HU22" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="HV22" t="n">
+      <c r="HV22" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="HW22" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="23" ht="13.8" customHeight="1" s="2">
@@ -16346,8 +16412,11 @@
       <c r="HU23" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="HV23" t="n">
+      <c r="HV23" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="HW23" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="24" ht="13.8" customHeight="1" s="2">
@@ -17040,8 +17109,11 @@
       <c r="HU24" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="HV24" t="n">
+      <c r="HV24" s="1" t="n">
         <v>25</v>
+      </c>
+      <c r="HW24" t="n">
+        <v>29</v>
       </c>
     </row>
     <row r="25" ht="13.8" customHeight="1" s="2">
@@ -17734,8 +17806,11 @@
       <c r="HU25" s="1" t="n">
         <v>33.3</v>
       </c>
-      <c r="HV25" t="n">
+      <c r="HV25" s="1" t="n">
         <v>56</v>
+      </c>
+      <c r="HW25" t="n">
+        <v>55.2</v>
       </c>
     </row>
     <row r="26" ht="13.8" customHeight="1" s="2">
@@ -18428,8 +18503,11 @@
       <c r="HU26" s="1" t="n">
         <v>28.64</v>
       </c>
-      <c r="HV26" t="n">
+      <c r="HV26" s="1" t="n">
         <v>26.36</v>
+      </c>
+      <c r="HW26" t="n">
+        <v>23.12</v>
       </c>
     </row>
     <row r="27" ht="13.8" customHeight="1" s="2">
@@ -19122,8 +19200,11 @@
       <c r="HU27" s="1" t="n">
         <v>9.550000000000001</v>
       </c>
-      <c r="HV27" t="n">
+      <c r="HV27" s="1" t="n">
         <v>14.76</v>
+      </c>
+      <c r="HW27" t="n">
+        <v>12.76</v>
       </c>
     </row>
     <row r="28" ht="13.8" customHeight="1" s="2">
@@ -19816,8 +19897,11 @@
       <c r="HU28" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="HV28" t="n">
+      <c r="HV28" s="1" t="n">
         <v>34</v>
+      </c>
+      <c r="HW28" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="29" ht="13.8" customHeight="1" s="2">
@@ -20510,8 +20594,11 @@
       <c r="HU29" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="HV29" t="n">
+      <c r="HV29" s="1" t="n">
         <v>60</v>
+      </c>
+      <c r="HW29" t="n">
+        <v>55</v>
       </c>
     </row>
     <row r="30" ht="13.8" customHeight="1" s="2">
@@ -21204,8 +21291,11 @@
       <c r="HU30" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="HV30" t="n">
+      <c r="HV30" s="1" t="n">
         <v>45</v>
+      </c>
+      <c r="HW30" t="n">
+        <v>42</v>
       </c>
     </row>
     <row r="31" ht="13.8" customHeight="1" s="2">
@@ -21898,8 +21988,11 @@
       <c r="HU31" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="HV31" t="n">
+      <c r="HV31" s="1" t="n">
         <v>57</v>
+      </c>
+      <c r="HW31" t="n">
+        <v>59</v>
       </c>
     </row>
     <row r="32" ht="13.8" customHeight="1" s="2">
@@ -22592,8 +22685,11 @@
       <c r="HU32" s="1" t="n">
         <v>1.67</v>
       </c>
-      <c r="HV32" t="n">
+      <c r="HV32" s="1" t="n">
         <v>2.28</v>
+      </c>
+      <c r="HW32" t="n">
+        <v>2.03</v>
       </c>
     </row>
     <row r="33" ht="13.8" customHeight="1" s="2">
@@ -23286,8 +23382,11 @@
       <c r="HU33" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="HV33" t="n">
+      <c r="HV33" s="1" t="n">
         <v>4.07</v>
+      </c>
+      <c r="HW33" t="n">
+        <v>3.69</v>
       </c>
     </row>
     <row r="34" ht="13.8" customHeight="1" s="2">
@@ -23980,8 +24079,11 @@
       <c r="HU34" s="1" t="n">
         <v>54.5</v>
       </c>
-      <c r="HV34" t="n">
+      <c r="HV34" s="1" t="n">
         <v>42.1</v>
+      </c>
+      <c r="HW34" t="n">
+        <v>45.8</v>
       </c>
     </row>
     <row r="35" ht="13.8" customHeight="1" s="2">
@@ -24674,8 +24776,11 @@
       <c r="HU35" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="HV35" t="n">
+      <c r="HV35" s="1" t="n">
         <v>24.6</v>
+      </c>
+      <c r="HW35" t="n">
+        <v>27.1</v>
       </c>
     </row>
     <row r="36" ht="13.8" customHeight="1" s="2">
@@ -25368,8 +25473,11 @@
       <c r="HU36" s="1" t="n">
         <v>186.3</v>
       </c>
-      <c r="HV36" t="n">
+      <c r="HV36" s="1" t="n">
         <v>186.1</v>
+      </c>
+      <c r="HW36" t="n">
+        <v>186.6</v>
       </c>
     </row>
     <row r="37" ht="13.8" customHeight="1" s="2">
@@ -26062,8 +26170,11 @@
       <c r="HU37" s="1" t="n">
         <v>83.3</v>
       </c>
-      <c r="HV37" t="n">
+      <c r="HV37" s="1" t="n">
         <v>83.3</v>
+      </c>
+      <c r="HW37" t="n">
+        <v>83.8</v>
       </c>
     </row>
     <row r="38" ht="13.8" customHeight="1" s="2">
@@ -26756,8 +26867,11 @@
       <c r="HU38" s="1" t="n">
         <v>24.66</v>
       </c>
-      <c r="HV38" t="n">
+      <c r="HV38" s="1" t="n">
         <v>24.74</v>
+      </c>
+      <c r="HW38" t="n">
+        <v>24.41</v>
       </c>
     </row>
     <row r="39" ht="13.8" customHeight="1" s="2">
@@ -27450,8 +27564,11 @@
       <c r="HU39" s="1" t="n">
         <v>68.7</v>
       </c>
-      <c r="HV39" t="n">
+      <c r="HV39" s="1" t="n">
         <v>71</v>
+      </c>
+      <c r="HW39" t="n">
+        <v>63.3</v>
       </c>
     </row>
     <row r="40" ht="13.8" customHeight="1" s="2">
@@ -28144,7 +28261,10 @@
       <c r="HU40" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="HV40" t="n">
+      <c r="HV40" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="HW40" t="n">
         <v>14</v>
       </c>
     </row>
@@ -28838,8 +28958,11 @@
       <c r="HU41" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="HV41" t="n">
+      <c r="HV41" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="HW41" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="42" ht="13.8" customHeight="1" s="2">
@@ -29532,7 +29655,10 @@
       <c r="HU42" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="HV42" t="n">
+      <c r="HV42" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="HW42" t="n">
         <v>1</v>
       </c>
     </row>
@@ -30226,8 +30352,11 @@
       <c r="HU43" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="HV43" t="n">
+      <c r="HV43" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="HW43" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="44" ht="13.8" customHeight="1" s="2">
@@ -30920,8 +31049,11 @@
       <c r="HU44" s="1" t="n">
         <v>124</v>
       </c>
-      <c r="HV44" t="n">
+      <c r="HV44" s="1" t="n">
         <v>148</v>
+      </c>
+      <c r="HW44" t="n">
+        <v>141</v>
       </c>
     </row>
     <row r="45" ht="13.8" customHeight="1" s="2">
@@ -31614,8 +31746,11 @@
       <c r="HU45" s="1" t="n">
         <v>179</v>
       </c>
-      <c r="HV45" t="n">
+      <c r="HV45" s="1" t="n">
         <v>218</v>
+      </c>
+      <c r="HW45" t="n">
+        <v>227</v>
       </c>
     </row>
     <row r="46" ht="13.8" customHeight="1" s="2">
@@ -32308,8 +32443,11 @@
       <c r="HU46" s="1" t="n">
         <v>230</v>
       </c>
-      <c r="HV46" t="n">
+      <c r="HV46" s="1" t="n">
         <v>276</v>
+      </c>
+      <c r="HW46" t="n">
+        <v>288</v>
       </c>
     </row>
     <row r="47" ht="13.8" customHeight="1" s="2">
@@ -33002,8 +33140,11 @@
       <c r="HU47" s="1" t="n">
         <v>73</v>
       </c>
-      <c r="HV47" t="n">
+      <c r="HV47" s="1" t="n">
         <v>74.8</v>
+      </c>
+      <c r="HW47" t="n">
+        <v>77.8</v>
       </c>
     </row>
     <row r="48" ht="13.8" customHeight="1" s="2">
@@ -33696,8 +33837,11 @@
       <c r="HU48" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="HV48" t="n">
+      <c r="HV48" s="1" t="n">
         <v>60</v>
+      </c>
+      <c r="HW48" t="n">
+        <v>55</v>
       </c>
     </row>
     <row r="49" ht="13.8" customHeight="1" s="2">
@@ -34390,8 +34534,11 @@
       <c r="HU49" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="HV49" t="n">
+      <c r="HV49" s="1" t="n">
         <v>12</v>
+      </c>
+      <c r="HW49" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="50" ht="13.8" customHeight="1" s="2">
@@ -35084,8 +35231,11 @@
       <c r="HU50" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="HV50" t="n">
+      <c r="HV50" s="1" t="n">
         <v>11</v>
+      </c>
+      <c r="HW50" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="51" ht="13.8" customHeight="1" s="2">
@@ -35778,8 +35928,11 @@
       <c r="HU51" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="HV51" t="n">
+      <c r="HV51" s="1" t="n">
         <v>34</v>
+      </c>
+      <c r="HW51" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="52" ht="13.8" customHeight="1" s="2">
@@ -36472,8 +36625,11 @@
       <c r="HU52" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="HV52" t="n">
+      <c r="HV52" s="1" t="n">
         <v>45</v>
+      </c>
+      <c r="HW52" t="n">
+        <v>42</v>
       </c>
     </row>
     <row r="53" ht="13.8" customHeight="1" s="2">
@@ -37166,8 +37322,11 @@
       <c r="HU53" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="HV53" t="n">
+      <c r="HV53" s="1" t="n">
         <v>57</v>
+      </c>
+      <c r="HW53" t="n">
+        <v>46</v>
       </c>
     </row>
     <row r="54" ht="13.8" customHeight="1" s="2">
@@ -37860,8 +38019,11 @@
       <c r="HU54" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="HV54" t="n">
+      <c r="HV54" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="HW54" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="55" ht="13.8" customHeight="1" s="2">
@@ -38554,8 +38716,11 @@
       <c r="HU55" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="HV55" t="n">
+      <c r="HV55" s="1" t="n">
         <v>9</v>
+      </c>
+      <c r="HW55" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="56" ht="13.8" customHeight="1" s="2">
@@ -39248,8 +39413,11 @@
       <c r="HU56" s="1" t="n">
         <v>54.5</v>
       </c>
-      <c r="HV56" t="n">
+      <c r="HV56" s="1" t="n">
         <v>64.3</v>
+      </c>
+      <c r="HW56" t="n">
+        <v>81.2</v>
       </c>
     </row>
     <row r="57" ht="13.8" customHeight="1" s="2">
@@ -39942,8 +40110,11 @@
       <c r="HU57" s="1" t="n">
         <v>239</v>
       </c>
-      <c r="HV57" t="n">
+      <c r="HV57" s="1" t="n">
         <v>230</v>
+      </c>
+      <c r="HW57" t="n">
+        <v>190</v>
       </c>
     </row>
     <row r="58" ht="13.8" customHeight="1" s="2">
@@ -40636,8 +40807,11 @@
       <c r="HU58" s="1" t="n">
         <v>137</v>
       </c>
-      <c r="HV58" t="n">
+      <c r="HV58" s="1" t="n">
         <v>99</v>
+      </c>
+      <c r="HW58" t="n">
+        <v>138</v>
       </c>
     </row>
     <row r="59" ht="13.8" customHeight="1" s="2">
@@ -41330,8 +41504,11 @@
       <c r="HU59" s="1" t="n">
         <v>376</v>
       </c>
-      <c r="HV59" t="n">
+      <c r="HV59" s="1" t="n">
         <v>329</v>
+      </c>
+      <c r="HW59" t="n">
+        <v>328</v>
       </c>
     </row>
     <row r="60" ht="13.8" customHeight="1" s="2">
@@ -42024,8 +42201,11 @@
       <c r="HU60" s="1" t="n">
         <v>1.74</v>
       </c>
-      <c r="HV60" t="n">
+      <c r="HV60" s="1" t="n">
         <v>2.32</v>
+      </c>
+      <c r="HW60" t="n">
+        <v>1.38</v>
       </c>
     </row>
     <row r="61" ht="13.8" customHeight="1" s="2">
@@ -42718,8 +42898,11 @@
       <c r="HU61" s="1" t="n">
         <v>104</v>
       </c>
-      <c r="HV61" t="n">
+      <c r="HV61" s="1" t="n">
         <v>104</v>
+      </c>
+      <c r="HW61" t="n">
+        <v>76</v>
       </c>
     </row>
     <row r="62" ht="13.8" customHeight="1" s="2">
@@ -43412,8 +43595,11 @@
       <c r="HU62" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="HV62" t="n">
+      <c r="HV62" s="1" t="n">
         <v>71</v>
+      </c>
+      <c r="HW62" t="n">
+        <v>66</v>
       </c>
     </row>
     <row r="63" ht="13.8" customHeight="1" s="2">
@@ -44106,8 +44292,11 @@
       <c r="HU63" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="HV63" t="n">
+      <c r="HV63" s="1" t="n">
         <v>34</v>
+      </c>
+      <c r="HW63" t="n">
+        <v>38</v>
       </c>
     </row>
     <row r="64" ht="13.8" customHeight="1" s="2">
@@ -44800,8 +44989,11 @@
       <c r="HU64" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="HV64" t="n">
+      <c r="HV64" s="1" t="n">
         <v>20</v>
+      </c>
+      <c r="HW64" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="65" ht="13.8" customHeight="1" s="2">
@@ -45494,8 +45686,11 @@
       <c r="HU65" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="HV65" t="n">
+      <c r="HV65" s="1" t="n">
         <v>17</v>
+      </c>
+      <c r="HW65" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="66" ht="13.8" customHeight="1" s="2">
@@ -46188,8 +46383,11 @@
       <c r="HU66" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="HV66" t="n">
+      <c r="HV66" s="1" t="n">
         <v>12</v>
+      </c>
+      <c r="HW66" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="67" ht="13.8" customHeight="1" s="2">
@@ -46882,8 +47080,11 @@
       <c r="HU67" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="HV67" t="n">
+      <c r="HV67" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="HW67" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="68" ht="13.8" customHeight="1" s="2">
@@ -47576,8 +47777,11 @@
       <c r="HU68" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="HV68" t="n">
+      <c r="HV68" s="1" t="n">
         <v>11</v>
+      </c>
+      <c r="HW68" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="69" ht="13.8" customHeight="1" s="2">
@@ -48270,7 +48474,10 @@
       <c r="HU69" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="HV69" t="n">
+      <c r="HV69" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="HW69" t="n">
         <v>2</v>
       </c>
     </row>
@@ -48964,8 +49171,11 @@
       <c r="HU70" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="HV70" t="n">
+      <c r="HV70" s="1" t="n">
         <v>25</v>
+      </c>
+      <c r="HW70" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="71" ht="13.8" customHeight="1" s="2">
@@ -49658,8 +49868,11 @@
       <c r="HU71" s="1" t="n">
         <v>58.1</v>
       </c>
-      <c r="HV71" t="n">
+      <c r="HV71" s="1" t="n">
         <v>48</v>
+      </c>
+      <c r="HW71" t="n">
+        <v>55.6</v>
       </c>
     </row>
     <row r="72" ht="13.8" customHeight="1" s="2">
@@ -50352,8 +50565,11 @@
       <c r="HU72" s="1" t="n">
         <v>20.89</v>
       </c>
-      <c r="HV72" t="n">
+      <c r="HV72" s="1" t="n">
         <v>27.42</v>
+      </c>
+      <c r="HW72" t="n">
+        <v>32.8</v>
       </c>
     </row>
     <row r="73" ht="13.8" customHeight="1" s="2">
@@ -51046,8 +51262,11 @@
       <c r="HU73" s="1" t="n">
         <v>12.13</v>
       </c>
-      <c r="HV73" t="n">
+      <c r="HV73" s="1" t="n">
         <v>13.16</v>
+      </c>
+      <c r="HW73" t="n">
+        <v>18.22</v>
       </c>
     </row>
     <row r="74" ht="13.8" customHeight="1" s="2">
@@ -51740,8 +51959,11 @@
       <c r="HU74" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="HV74" t="n">
+      <c r="HV74" s="1" t="n">
         <v>41</v>
+      </c>
+      <c r="HW74" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="75" ht="13.8" customHeight="1" s="2">
@@ -52434,8 +52656,11 @@
       <c r="HU75" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="HV75" t="n">
+      <c r="HV75" s="1" t="n">
         <v>55</v>
+      </c>
+      <c r="HW75" t="n">
+        <v>68</v>
       </c>
     </row>
     <row r="76" ht="13.8" customHeight="1" s="2">
@@ -53128,8 +53353,11 @@
       <c r="HU76" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="HV76" t="n">
+      <c r="HV76" s="1" t="n">
         <v>41</v>
+      </c>
+      <c r="HW76" t="n">
+        <v>42</v>
       </c>
     </row>
     <row r="77" ht="13.8" customHeight="1" s="2">
@@ -53822,8 +54050,11 @@
       <c r="HU77" s="1" t="n">
         <v>61</v>
       </c>
-      <c r="HV77" t="n">
+      <c r="HV77" s="1" t="n">
         <v>58</v>
+      </c>
+      <c r="HW77" t="n">
+        <v>53</v>
       </c>
     </row>
     <row r="78" ht="13.8" customHeight="1" s="2">
@@ -54516,8 +54747,11 @@
       <c r="HU78" s="1" t="n">
         <v>1.97</v>
       </c>
-      <c r="HV78" t="n">
+      <c r="HV78" s="1" t="n">
         <v>2.32</v>
+      </c>
+      <c r="HW78" t="n">
+        <v>2.94</v>
       </c>
     </row>
     <row r="79" ht="13.8" customHeight="1" s="2">
@@ -55210,8 +55444,11 @@
       <c r="HU79" s="1" t="n">
         <v>3.39</v>
       </c>
-      <c r="HV79" t="n">
+      <c r="HV79" s="1" t="n">
         <v>4.83</v>
+      </c>
+      <c r="HW79" t="n">
+        <v>5.3</v>
       </c>
     </row>
     <row r="80" ht="13.8" customHeight="1" s="2">
@@ -55904,8 +56141,11 @@
       <c r="HU80" s="1" t="n">
         <v>47.5</v>
       </c>
-      <c r="HV80" t="n">
+      <c r="HV80" s="1" t="n">
         <v>39.7</v>
+      </c>
+      <c r="HW80" t="n">
+        <v>30.2</v>
       </c>
     </row>
     <row r="81" ht="13.8" customHeight="1" s="2">
@@ -56598,8 +56838,11 @@
       <c r="HU81" s="1" t="n">
         <v>29.5</v>
       </c>
-      <c r="HV81" t="n">
+      <c r="HV81" s="1" t="n">
         <v>20.7</v>
+      </c>
+      <c r="HW81" t="n">
+        <v>18.9</v>
       </c>
     </row>
     <row r="82" ht="13.8" customHeight="1" s="2">
@@ -57292,8 +57535,11 @@
       <c r="HU82" s="1" t="n">
         <v>187.4</v>
       </c>
-      <c r="HV82" t="n">
+      <c r="HV82" s="1" t="n">
         <v>187.3</v>
+      </c>
+      <c r="HW82" t="n">
+        <v>187.8</v>
       </c>
     </row>
     <row r="83" ht="13.8" customHeight="1" s="2">
@@ -57986,8 +58232,11 @@
       <c r="HU83" s="1" t="n">
         <v>84.2</v>
       </c>
-      <c r="HV83" t="n">
+      <c r="HV83" s="1" t="n">
         <v>84.90000000000001</v>
+      </c>
+      <c r="HW83" t="n">
+        <v>84.09999999999999</v>
       </c>
     </row>
     <row r="84" ht="13.8" customHeight="1" s="2">
@@ -58680,7 +58929,10 @@
       <c r="HU84" s="1" t="n">
         <v>24.8</v>
       </c>
-      <c r="HV84" t="n">
+      <c r="HV84" s="1" t="n">
+        <v>24.8</v>
+      </c>
+      <c r="HW84" t="n">
         <v>24.8</v>
       </c>
     </row>
@@ -59374,8 +59626,11 @@
       <c r="HU85" s="1" t="n">
         <v>97</v>
       </c>
-      <c r="HV85" t="n">
+      <c r="HV85" s="1" t="n">
         <v>78.3</v>
+      </c>
+      <c r="HW85" t="n">
+        <v>72.8</v>
       </c>
     </row>
     <row r="86" ht="13.8" customHeight="1" s="2">
@@ -60068,8 +60323,11 @@
       <c r="HU86" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="HV86" t="n">
+      <c r="HV86" s="1" t="n">
         <v>9</v>
+      </c>
+      <c r="HW86" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="87" ht="13.8" customHeight="1" s="2">
@@ -60762,8 +61020,11 @@
       <c r="HU87" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="HV87" t="n">
+      <c r="HV87" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="HW87" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="88" ht="13.8" customHeight="1" s="2">
@@ -61456,8 +61717,11 @@
       <c r="HU88" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="HV88" t="n">
+      <c r="HV88" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="HW88" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="89" ht="13.8" customHeight="1" s="2">
@@ -62150,8 +62414,11 @@
       <c r="HU89" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="HV89" t="n">
+      <c r="HV89" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="HW89" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="90" ht="13.8" customHeight="1" s="2">
@@ -62844,8 +63111,11 @@
       <c r="HU90" s="1" t="n">
         <v>128</v>
       </c>
-      <c r="HV90" t="n">
+      <c r="HV90" s="1" t="n">
         <v>150</v>
+      </c>
+      <c r="HW90" t="n">
+        <v>132</v>
       </c>
     </row>
     <row r="91" ht="13.8" customHeight="1" s="2">
@@ -63538,8 +63808,11 @@
       <c r="HU91" s="1" t="n">
         <v>232</v>
       </c>
-      <c r="HV91" t="n">
+      <c r="HV91" s="1" t="n">
         <v>169</v>
+      </c>
+      <c r="HW91" t="n">
+        <v>188</v>
       </c>
     </row>
     <row r="92" ht="13.8" customHeight="1" s="2">
@@ -64232,8 +64505,11 @@
       <c r="HU92" s="1" t="n">
         <v>280</v>
       </c>
-      <c r="HV92" t="n">
+      <c r="HV92" s="1" t="n">
         <v>227</v>
+      </c>
+      <c r="HW92" t="n">
+        <v>230</v>
       </c>
     </row>
     <row r="93" ht="13.8" customHeight="1" s="2">
@@ -64926,8 +65202,11 @@
       <c r="HU93" s="1" t="n">
         <v>74.5</v>
       </c>
-      <c r="HV93" t="n">
+      <c r="HV93" s="1" t="n">
         <v>69</v>
+      </c>
+      <c r="HW93" t="n">
+        <v>70.09999999999999</v>
       </c>
     </row>
     <row r="94" ht="13.8" customHeight="1" s="2">
@@ -65620,8 +65899,11 @@
       <c r="HU94" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="HV94" t="n">
+      <c r="HV94" s="1" t="n">
         <v>55</v>
+      </c>
+      <c r="HW94" t="n">
+        <v>68</v>
       </c>
     </row>
     <row r="95" ht="13.8" customHeight="1" s="2">
@@ -66314,8 +66596,11 @@
       <c r="HU95" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="HV95" t="n">
+      <c r="HV95" s="1" t="n">
         <v>14</v>
+      </c>
+      <c r="HW95" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="96" ht="13.8" customHeight="1" s="2">
@@ -67008,8 +67293,11 @@
       <c r="HU96" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="HV96" t="n">
+      <c r="HV96" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="HW96" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="97" ht="13.8" customHeight="1" s="2">
@@ -67702,8 +67990,11 @@
       <c r="HU97" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="HV97" t="n">
+      <c r="HV97" s="1" t="n">
         <v>41</v>
+      </c>
+      <c r="HW97" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="98" ht="13.8" customHeight="1" s="2">
@@ -68396,8 +68687,11 @@
       <c r="HU98" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="HV98" t="n">
+      <c r="HV98" s="1" t="n">
         <v>41</v>
+      </c>
+      <c r="HW98" t="n">
+        <v>42</v>
       </c>
     </row>
     <row r="99" ht="13.8" customHeight="1" s="2">
@@ -69090,8 +69384,11 @@
       <c r="HU99" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="HV99" t="n">
+      <c r="HV99" s="1" t="n">
         <v>43</v>
+      </c>
+      <c r="HW99" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="100" ht="13.8" customHeight="1" s="2">
@@ -69784,8 +70081,11 @@
       <c r="HU100" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="HV100" t="n">
+      <c r="HV100" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="HW100" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="101" ht="13.8" customHeight="1" s="2">
@@ -70478,8 +70778,11 @@
       <c r="HU101" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="HV101" t="n">
+      <c r="HV101" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="HW101" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="102" ht="13.8" customHeight="1" s="2">
@@ -71172,8 +71475,11 @@
       <c r="HU102" s="1" t="n">
         <v>77.8</v>
       </c>
-      <c r="HV102" t="n">
+      <c r="HV102" s="1" t="n">
         <v>83.3</v>
+      </c>
+      <c r="HW102" t="n">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
round 6 predictions 2021
</commit_message>
<xml_diff>
--- a/django_AFL_ML/Data/Adelaide_stats.xlsx
+++ b/django_AFL_ML/Data/Adelaide_stats.xlsx
@@ -377,7 +377,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:HW102"/>
+  <dimension ref="A1:HX102"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="GZ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="HA23" activeCellId="0" sqref="HA23"/>
@@ -1081,8 +1081,11 @@
       <c r="HV1" s="1" t="n">
         <v>10347</v>
       </c>
-      <c r="HW1" t="n">
+      <c r="HW1" s="1" t="n">
         <v>10360</v>
+      </c>
+      <c r="HX1" t="n">
+        <v>10369</v>
       </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="2">
@@ -1778,7 +1781,10 @@
       <c r="HV2" s="1" t="n">
         <v>2021</v>
       </c>
-      <c r="HW2" t="n">
+      <c r="HW2" s="1" t="n">
+        <v>2021</v>
+      </c>
+      <c r="HX2" t="n">
         <v>2021</v>
       </c>
     </row>
@@ -2475,8 +2481,11 @@
       <c r="HV3" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="HW3" t="n">
+      <c r="HW3" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="HX3" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="2">
@@ -3172,8 +3181,11 @@
       <c r="HV4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="HW4" t="n">
+      <c r="HW4" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="HX4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5" ht="13.8" customHeight="1" s="2">
@@ -3869,7 +3881,10 @@
       <c r="HV5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="HW5" t="n">
+      <c r="HW5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="HX5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4566,8 +4581,11 @@
       <c r="HV6" s="1" t="n">
         <v>95</v>
       </c>
-      <c r="HW6" t="n">
+      <c r="HW6" s="1" t="n">
         <v>109</v>
+      </c>
+      <c r="HX6" t="n">
+        <v>72</v>
       </c>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="2">
@@ -5263,8 +5281,11 @@
       <c r="HV7" s="1" t="n">
         <v>85</v>
       </c>
-      <c r="HW7" t="n">
+      <c r="HW7" s="1" t="n">
         <v>68</v>
+      </c>
+      <c r="HX7" t="n">
+        <v>84</v>
       </c>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="2">
@@ -5960,8 +5981,11 @@
       <c r="HV8" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="HW8" t="n">
+      <c r="HW8" s="1" t="n">
         <v>41</v>
+      </c>
+      <c r="HX8" t="n">
+        <v>-12</v>
       </c>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="2">
@@ -6657,8 +6681,11 @@
       <c r="HV9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="HW9" t="n">
+      <c r="HW9" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="HX9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10" ht="13.8" customHeight="1" s="2">
@@ -7354,8 +7381,11 @@
       <c r="HV10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="HW10" t="n">
+      <c r="HW10" s="1" t="n">
         <v>12</v>
+      </c>
+      <c r="HX10" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="11" ht="13.8" customHeight="1" s="2">
@@ -8051,8 +8081,11 @@
       <c r="HV11" s="1" t="n">
         <v>209</v>
       </c>
-      <c r="HW11" t="n">
+      <c r="HW11" s="1" t="n">
         <v>221</v>
+      </c>
+      <c r="HX11" t="n">
+        <v>213</v>
       </c>
     </row>
     <row r="12" ht="13.8" customHeight="1" s="2">
@@ -8748,8 +8781,11 @@
       <c r="HV12" s="1" t="n">
         <v>160</v>
       </c>
-      <c r="HW12" t="n">
+      <c r="HW12" s="1" t="n">
         <v>149</v>
+      </c>
+      <c r="HX12" t="n">
+        <v>161</v>
       </c>
     </row>
     <row r="13" ht="13.8" customHeight="1" s="2">
@@ -9445,8 +9481,11 @@
       <c r="HV13" s="1" t="n">
         <v>369</v>
       </c>
-      <c r="HW13" t="n">
+      <c r="HW13" s="1" t="n">
         <v>370</v>
+      </c>
+      <c r="HX13" t="n">
+        <v>374</v>
       </c>
     </row>
     <row r="14" ht="13.8" customHeight="1" s="2">
@@ -10142,8 +10181,11 @@
       <c r="HV14" s="1" t="n">
         <v>1.31</v>
       </c>
-      <c r="HW14" t="n">
+      <c r="HW14" s="1" t="n">
         <v>1.48</v>
+      </c>
+      <c r="HX14" t="n">
+        <v>1.32</v>
       </c>
     </row>
     <row r="15" ht="13.8" customHeight="1" s="2">
@@ -10839,8 +10881,11 @@
       <c r="HV15" s="1" t="n">
         <v>81</v>
       </c>
-      <c r="HW15" t="n">
+      <c r="HW15" s="1" t="n">
         <v>105</v>
+      </c>
+      <c r="HX15" t="n">
+        <v>94</v>
       </c>
     </row>
     <row r="16" ht="13.8" customHeight="1" s="2">
@@ -11536,8 +11581,11 @@
       <c r="HV16" s="1" t="n">
         <v>58</v>
       </c>
-      <c r="HW16" t="n">
+      <c r="HW16" s="1" t="n">
         <v>68</v>
+      </c>
+      <c r="HX16" t="n">
+        <v>51</v>
       </c>
     </row>
     <row r="17" ht="13.8" customHeight="1" s="2">
@@ -12233,8 +12281,11 @@
       <c r="HV17" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="HW17" t="n">
+      <c r="HW17" s="1" t="n">
         <v>32</v>
+      </c>
+      <c r="HX17" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="18" ht="13.8" customHeight="1" s="2">
@@ -12930,8 +12981,11 @@
       <c r="HV18" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="HW18" t="n">
+      <c r="HW18" s="1" t="n">
         <v>26</v>
+      </c>
+      <c r="HX18" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="19" ht="13.8" customHeight="1" s="2">
@@ -13627,8 +13681,11 @@
       <c r="HV19" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="HW19" t="n">
+      <c r="HW19" s="1" t="n">
         <v>28</v>
+      </c>
+      <c r="HX19" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="20" ht="13.8" customHeight="1" s="2">
@@ -14324,8 +14381,11 @@
       <c r="HV20" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="HW20" t="n">
+      <c r="HW20" s="1" t="n">
         <v>16</v>
+      </c>
+      <c r="HX20" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="21" ht="13.8" customHeight="1" s="2">
@@ -15021,8 +15081,11 @@
       <c r="HV21" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="HW21" t="n">
+      <c r="HW21" s="1" t="n">
         <v>13</v>
+      </c>
+      <c r="HX21" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="22" ht="13.8" customHeight="1" s="2">
@@ -15718,8 +15781,11 @@
       <c r="HV22" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="HW22" t="n">
+      <c r="HW22" s="1" t="n">
         <v>11</v>
+      </c>
+      <c r="HX22" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="23" ht="13.8" customHeight="1" s="2">
@@ -16415,8 +16481,11 @@
       <c r="HV23" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="HW23" t="n">
+      <c r="HW23" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="HX23" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="24" ht="13.8" customHeight="1" s="2">
@@ -17112,8 +17181,11 @@
       <c r="HV24" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="HW24" t="n">
+      <c r="HW24" s="1" t="n">
         <v>29</v>
+      </c>
+      <c r="HX24" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="25" ht="13.8" customHeight="1" s="2">
@@ -17809,8 +17881,11 @@
       <c r="HV25" s="1" t="n">
         <v>56</v>
       </c>
-      <c r="HW25" t="n">
+      <c r="HW25" s="1" t="n">
         <v>55.2</v>
+      </c>
+      <c r="HX25" t="n">
+        <v>64.7</v>
       </c>
     </row>
     <row r="26" ht="13.8" customHeight="1" s="2">
@@ -18506,8 +18581,11 @@
       <c r="HV26" s="1" t="n">
         <v>26.36</v>
       </c>
-      <c r="HW26" t="n">
+      <c r="HW26" s="1" t="n">
         <v>23.12</v>
+      </c>
+      <c r="HX26" t="n">
+        <v>34</v>
       </c>
     </row>
     <row r="27" ht="13.8" customHeight="1" s="2">
@@ -19203,8 +19281,11 @@
       <c r="HV27" s="1" t="n">
         <v>14.76</v>
       </c>
-      <c r="HW27" t="n">
+      <c r="HW27" s="1" t="n">
         <v>12.76</v>
+      </c>
+      <c r="HX27" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="28" ht="13.8" customHeight="1" s="2">
@@ -19900,8 +19981,11 @@
       <c r="HV28" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="HW28" t="n">
+      <c r="HW28" s="1" t="n">
         <v>32</v>
+      </c>
+      <c r="HX28" t="n">
+        <v>35</v>
       </c>
     </row>
     <row r="29" ht="13.8" customHeight="1" s="2">
@@ -20597,8 +20681,11 @@
       <c r="HV29" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="HW29" t="n">
+      <c r="HW29" s="1" t="n">
         <v>55</v>
+      </c>
+      <c r="HX29" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="30" ht="13.8" customHeight="1" s="2">
@@ -21294,7 +21381,10 @@
       <c r="HV30" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="HW30" t="n">
+      <c r="HW30" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="HX30" t="n">
         <v>42</v>
       </c>
     </row>
@@ -21991,8 +22081,11 @@
       <c r="HV31" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="HW31" t="n">
+      <c r="HW31" s="1" t="n">
         <v>59</v>
+      </c>
+      <c r="HX31" t="n">
+        <v>55</v>
       </c>
     </row>
     <row r="32" ht="13.8" customHeight="1" s="2">
@@ -22688,8 +22781,11 @@
       <c r="HV32" s="1" t="n">
         <v>2.28</v>
       </c>
-      <c r="HW32" t="n">
+      <c r="HW32" s="1" t="n">
         <v>2.03</v>
+      </c>
+      <c r="HX32" t="n">
+        <v>3.24</v>
       </c>
     </row>
     <row r="33" ht="13.8" customHeight="1" s="2">
@@ -23385,8 +23481,11 @@
       <c r="HV33" s="1" t="n">
         <v>4.07</v>
       </c>
-      <c r="HW33" t="n">
+      <c r="HW33" s="1" t="n">
         <v>3.69</v>
+      </c>
+      <c r="HX33" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="34" ht="13.8" customHeight="1" s="2">
@@ -24082,8 +24181,11 @@
       <c r="HV34" s="1" t="n">
         <v>42.1</v>
       </c>
-      <c r="HW34" t="n">
+      <c r="HW34" s="1" t="n">
         <v>45.8</v>
+      </c>
+      <c r="HX34" t="n">
+        <v>30.9</v>
       </c>
     </row>
     <row r="35" ht="13.8" customHeight="1" s="2">
@@ -24779,8 +24881,11 @@
       <c r="HV35" s="1" t="n">
         <v>24.6</v>
       </c>
-      <c r="HW35" t="n">
+      <c r="HW35" s="1" t="n">
         <v>27.1</v>
+      </c>
+      <c r="HX35" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="36" ht="13.8" customHeight="1" s="2">
@@ -25476,7 +25581,10 @@
       <c r="HV36" s="1" t="n">
         <v>186.1</v>
       </c>
-      <c r="HW36" t="n">
+      <c r="HW36" s="1" t="n">
+        <v>186.6</v>
+      </c>
+      <c r="HX36" t="n">
         <v>186.6</v>
       </c>
     </row>
@@ -26173,7 +26281,10 @@
       <c r="HV37" s="1" t="n">
         <v>83.3</v>
       </c>
-      <c r="HW37" t="n">
+      <c r="HW37" s="1" t="n">
+        <v>83.8</v>
+      </c>
+      <c r="HX37" t="n">
         <v>83.8</v>
       </c>
     </row>
@@ -26870,7 +26981,10 @@
       <c r="HV38" s="1" t="n">
         <v>24.74</v>
       </c>
-      <c r="HW38" t="n">
+      <c r="HW38" s="1" t="n">
+        <v>24.41</v>
+      </c>
+      <c r="HX38" t="n">
         <v>24.41</v>
       </c>
     </row>
@@ -27567,8 +27681,11 @@
       <c r="HV39" s="1" t="n">
         <v>71</v>
       </c>
-      <c r="HW39" t="n">
+      <c r="HW39" s="1" t="n">
         <v>63.3</v>
+      </c>
+      <c r="HX39" t="n">
+        <v>64.3</v>
       </c>
     </row>
     <row r="40" ht="13.8" customHeight="1" s="2">
@@ -28264,7 +28381,10 @@
       <c r="HV40" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="HW40" t="n">
+      <c r="HW40" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="HX40" t="n">
         <v>14</v>
       </c>
     </row>
@@ -28961,7 +29081,10 @@
       <c r="HV41" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="HW41" t="n">
+      <c r="HW41" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="HX41" t="n">
         <v>2</v>
       </c>
     </row>
@@ -29658,7 +29781,10 @@
       <c r="HV42" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="HW42" t="n">
+      <c r="HW42" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="HX42" t="n">
         <v>1</v>
       </c>
     </row>
@@ -30355,7 +30481,10 @@
       <c r="HV43" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="HW43" t="n">
+      <c r="HW43" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="HX43" t="n">
         <v>5</v>
       </c>
     </row>
@@ -31052,8 +31181,11 @@
       <c r="HV44" s="1" t="n">
         <v>148</v>
       </c>
-      <c r="HW44" t="n">
+      <c r="HW44" s="1" t="n">
         <v>141</v>
+      </c>
+      <c r="HX44" t="n">
+        <v>139</v>
       </c>
     </row>
     <row r="45" ht="13.8" customHeight="1" s="2">
@@ -31749,8 +31881,11 @@
       <c r="HV45" s="1" t="n">
         <v>218</v>
       </c>
-      <c r="HW45" t="n">
+      <c r="HW45" s="1" t="n">
         <v>227</v>
+      </c>
+      <c r="HX45" t="n">
+        <v>229</v>
       </c>
     </row>
     <row r="46" ht="13.8" customHeight="1" s="2">
@@ -32446,8 +32581,11 @@
       <c r="HV46" s="1" t="n">
         <v>276</v>
       </c>
-      <c r="HW46" t="n">
+      <c r="HW46" s="1" t="n">
         <v>288</v>
+      </c>
+      <c r="HX46" t="n">
+        <v>275</v>
       </c>
     </row>
     <row r="47" ht="13.8" customHeight="1" s="2">
@@ -33143,8 +33281,11 @@
       <c r="HV47" s="1" t="n">
         <v>74.8</v>
       </c>
-      <c r="HW47" t="n">
+      <c r="HW47" s="1" t="n">
         <v>77.8</v>
+      </c>
+      <c r="HX47" t="n">
+        <v>73.5</v>
       </c>
     </row>
     <row r="48" ht="13.8" customHeight="1" s="2">
@@ -33840,8 +33981,11 @@
       <c r="HV48" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="HW48" t="n">
+      <c r="HW48" s="1" t="n">
         <v>55</v>
+      </c>
+      <c r="HX48" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="49" ht="13.8" customHeight="1" s="2">
@@ -34537,8 +34681,11 @@
       <c r="HV49" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="HW49" t="n">
+      <c r="HW49" s="1" t="n">
         <v>19</v>
+      </c>
+      <c r="HX49" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="50" ht="13.8" customHeight="1" s="2">
@@ -35234,8 +35381,11 @@
       <c r="HV50" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="HW50" t="n">
+      <c r="HW50" s="1" t="n">
         <v>15</v>
+      </c>
+      <c r="HX50" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="51" ht="13.8" customHeight="1" s="2">
@@ -35931,8 +36081,11 @@
       <c r="HV51" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="HW51" t="n">
+      <c r="HW51" s="1" t="n">
         <v>32</v>
+      </c>
+      <c r="HX51" t="n">
+        <v>35</v>
       </c>
     </row>
     <row r="52" ht="13.8" customHeight="1" s="2">
@@ -36628,7 +36781,10 @@
       <c r="HV52" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="HW52" t="n">
+      <c r="HW52" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="HX52" t="n">
         <v>42</v>
       </c>
     </row>
@@ -37325,8 +37481,11 @@
       <c r="HV53" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="HW53" t="n">
+      <c r="HW53" s="1" t="n">
         <v>46</v>
+      </c>
+      <c r="HX53" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="54" ht="13.8" customHeight="1" s="2">
@@ -38022,8 +38181,11 @@
       <c r="HV54" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="HW54" t="n">
+      <c r="HW54" s="1" t="n">
         <v>9</v>
+      </c>
+      <c r="HX54" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="55" ht="13.8" customHeight="1" s="2">
@@ -38719,8 +38881,11 @@
       <c r="HV55" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="HW55" t="n">
+      <c r="HW55" s="1" t="n">
         <v>13</v>
+      </c>
+      <c r="HX55" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="56" ht="13.8" customHeight="1" s="2">
@@ -39416,8 +39581,11 @@
       <c r="HV56" s="1" t="n">
         <v>64.3</v>
       </c>
-      <c r="HW56" t="n">
+      <c r="HW56" s="1" t="n">
         <v>81.2</v>
+      </c>
+      <c r="HX56" t="n">
+        <v>63.6</v>
       </c>
     </row>
     <row r="57" ht="13.8" customHeight="1" s="2">
@@ -40113,8 +40281,11 @@
       <c r="HV57" s="1" t="n">
         <v>230</v>
       </c>
-      <c r="HW57" t="n">
+      <c r="HW57" s="1" t="n">
         <v>190</v>
+      </c>
+      <c r="HX57" t="n">
+        <v>218</v>
       </c>
     </row>
     <row r="58" ht="13.8" customHeight="1" s="2">
@@ -40810,8 +40981,11 @@
       <c r="HV58" s="1" t="n">
         <v>99</v>
       </c>
-      <c r="HW58" t="n">
+      <c r="HW58" s="1" t="n">
         <v>138</v>
+      </c>
+      <c r="HX58" t="n">
+        <v>141</v>
       </c>
     </row>
     <row r="59" ht="13.8" customHeight="1" s="2">
@@ -41507,8 +41681,11 @@
       <c r="HV59" s="1" t="n">
         <v>329</v>
       </c>
-      <c r="HW59" t="n">
+      <c r="HW59" s="1" t="n">
         <v>328</v>
+      </c>
+      <c r="HX59" t="n">
+        <v>359</v>
       </c>
     </row>
     <row r="60" ht="13.8" customHeight="1" s="2">
@@ -42204,8 +42381,11 @@
       <c r="HV60" s="1" t="n">
         <v>2.32</v>
       </c>
-      <c r="HW60" t="n">
+      <c r="HW60" s="1" t="n">
         <v>1.38</v>
+      </c>
+      <c r="HX60" t="n">
+        <v>1.55</v>
       </c>
     </row>
     <row r="61" ht="13.8" customHeight="1" s="2">
@@ -42901,8 +43081,11 @@
       <c r="HV61" s="1" t="n">
         <v>104</v>
       </c>
-      <c r="HW61" t="n">
+      <c r="HW61" s="1" t="n">
         <v>76</v>
+      </c>
+      <c r="HX61" t="n">
+        <v>102</v>
       </c>
     </row>
     <row r="62" ht="13.8" customHeight="1" s="2">
@@ -43598,8 +43781,11 @@
       <c r="HV62" s="1" t="n">
         <v>71</v>
       </c>
-      <c r="HW62" t="n">
+      <c r="HW62" s="1" t="n">
         <v>66</v>
+      </c>
+      <c r="HX62" t="n">
+        <v>57</v>
       </c>
     </row>
     <row r="63" ht="13.8" customHeight="1" s="2">
@@ -44295,8 +44481,11 @@
       <c r="HV63" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="HW63" t="n">
+      <c r="HW63" s="1" t="n">
         <v>38</v>
+      </c>
+      <c r="HX63" t="n">
+        <v>39</v>
       </c>
     </row>
     <row r="64" ht="13.8" customHeight="1" s="2">
@@ -44992,8 +45181,11 @@
       <c r="HV64" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="HW64" t="n">
+      <c r="HW64" s="1" t="n">
         <v>28</v>
+      </c>
+      <c r="HX64" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="65" ht="13.8" customHeight="1" s="2">
@@ -45689,8 +45881,11 @@
       <c r="HV65" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="HW65" t="n">
+      <c r="HW65" s="1" t="n">
         <v>25</v>
+      </c>
+      <c r="HX65" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="66" ht="13.8" customHeight="1" s="2">
@@ -46386,8 +46581,11 @@
       <c r="HV66" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="HW66" t="n">
+      <c r="HW66" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="HX66" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="67" ht="13.8" customHeight="1" s="2">
@@ -47083,8 +47281,11 @@
       <c r="HV67" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="HW67" t="n">
+      <c r="HW67" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="HX67" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="68" ht="13.8" customHeight="1" s="2">
@@ -47780,8 +47981,11 @@
       <c r="HV68" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="HW68" t="n">
+      <c r="HW68" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="HX68" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="69" ht="13.8" customHeight="1" s="2">
@@ -48477,8 +48681,11 @@
       <c r="HV69" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="HW69" t="n">
+      <c r="HW69" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="HX69" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="70" ht="13.8" customHeight="1" s="2">
@@ -49174,8 +49381,11 @@
       <c r="HV70" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="HW70" t="n">
+      <c r="HW70" s="1" t="n">
         <v>18</v>
+      </c>
+      <c r="HX70" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="71" ht="13.8" customHeight="1" s="2">
@@ -49871,8 +50081,11 @@
       <c r="HV71" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="HW71" t="n">
+      <c r="HW71" s="1" t="n">
         <v>55.6</v>
+      </c>
+      <c r="HX71" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="72" ht="13.8" customHeight="1" s="2">
@@ -50568,8 +50781,11 @@
       <c r="HV72" s="1" t="n">
         <v>27.42</v>
       </c>
-      <c r="HW72" t="n">
+      <c r="HW72" s="1" t="n">
         <v>32.8</v>
+      </c>
+      <c r="HX72" t="n">
+        <v>29.92</v>
       </c>
     </row>
     <row r="73" ht="13.8" customHeight="1" s="2">
@@ -51265,8 +51481,11 @@
       <c r="HV73" s="1" t="n">
         <v>13.16</v>
       </c>
-      <c r="HW73" t="n">
+      <c r="HW73" s="1" t="n">
         <v>18.22</v>
+      </c>
+      <c r="HX73" t="n">
+        <v>14.96</v>
       </c>
     </row>
     <row r="74" ht="13.8" customHeight="1" s="2">
@@ -51962,8 +52181,11 @@
       <c r="HV74" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="HW74" t="n">
+      <c r="HW74" s="1" t="n">
         <v>30</v>
+      </c>
+      <c r="HX74" t="n">
+        <v>42</v>
       </c>
     </row>
     <row r="75" ht="13.8" customHeight="1" s="2">
@@ -52659,8 +52881,11 @@
       <c r="HV75" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="HW75" t="n">
+      <c r="HW75" s="1" t="n">
         <v>68</v>
+      </c>
+      <c r="HX75" t="n">
+        <v>53</v>
       </c>
     </row>
     <row r="76" ht="13.8" customHeight="1" s="2">
@@ -53356,7 +53581,10 @@
       <c r="HV76" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="HW76" t="n">
+      <c r="HW76" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="HX76" t="n">
         <v>42</v>
       </c>
     </row>
@@ -54053,8 +54281,11 @@
       <c r="HV77" s="1" t="n">
         <v>58</v>
       </c>
-      <c r="HW77" t="n">
+      <c r="HW77" s="1" t="n">
         <v>53</v>
+      </c>
+      <c r="HX77" t="n">
+        <v>54</v>
       </c>
     </row>
     <row r="78" ht="13.8" customHeight="1" s="2">
@@ -54750,8 +54981,11 @@
       <c r="HV78" s="1" t="n">
         <v>2.32</v>
       </c>
-      <c r="HW78" t="n">
+      <c r="HW78" s="1" t="n">
         <v>2.94</v>
+      </c>
+      <c r="HX78" t="n">
+        <v>2.25</v>
       </c>
     </row>
     <row r="79" ht="13.8" customHeight="1" s="2">
@@ -55447,8 +55681,11 @@
       <c r="HV79" s="1" t="n">
         <v>4.83</v>
       </c>
-      <c r="HW79" t="n">
+      <c r="HW79" s="1" t="n">
         <v>5.3</v>
+      </c>
+      <c r="HX79" t="n">
+        <v>4.5</v>
       </c>
     </row>
     <row r="80" ht="13.8" customHeight="1" s="2">
@@ -56144,8 +56381,11 @@
       <c r="HV80" s="1" t="n">
         <v>39.7</v>
       </c>
-      <c r="HW80" t="n">
+      <c r="HW80" s="1" t="n">
         <v>30.2</v>
+      </c>
+      <c r="HX80" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="81" ht="13.8" customHeight="1" s="2">
@@ -56841,8 +57081,11 @@
       <c r="HV81" s="1" t="n">
         <v>20.7</v>
       </c>
-      <c r="HW81" t="n">
+      <c r="HW81" s="1" t="n">
         <v>18.9</v>
+      </c>
+      <c r="HX81" t="n">
+        <v>22.2</v>
       </c>
     </row>
     <row r="82" ht="13.8" customHeight="1" s="2">
@@ -57538,8 +57781,11 @@
       <c r="HV82" s="1" t="n">
         <v>187.3</v>
       </c>
-      <c r="HW82" t="n">
+      <c r="HW82" s="1" t="n">
         <v>187.8</v>
+      </c>
+      <c r="HX82" t="n">
+        <v>187.9</v>
       </c>
     </row>
     <row r="83" ht="13.8" customHeight="1" s="2">
@@ -58235,8 +58481,11 @@
       <c r="HV83" s="1" t="n">
         <v>84.90000000000001</v>
       </c>
-      <c r="HW83" t="n">
+      <c r="HW83" s="1" t="n">
         <v>84.09999999999999</v>
+      </c>
+      <c r="HX83" t="n">
+        <v>88.59999999999999</v>
       </c>
     </row>
     <row r="84" ht="13.8" customHeight="1" s="2">
@@ -58932,8 +59181,11 @@
       <c r="HV84" s="1" t="n">
         <v>24.8</v>
       </c>
-      <c r="HW84" t="n">
+      <c r="HW84" s="1" t="n">
         <v>24.8</v>
+      </c>
+      <c r="HX84" t="n">
+        <v>25.8</v>
       </c>
     </row>
     <row r="85" ht="13.8" customHeight="1" s="2">
@@ -59629,8 +59881,11 @@
       <c r="HV85" s="1" t="n">
         <v>78.3</v>
       </c>
-      <c r="HW85" t="n">
+      <c r="HW85" s="1" t="n">
         <v>72.8</v>
+      </c>
+      <c r="HX85" t="n">
+        <v>85.3</v>
       </c>
     </row>
     <row r="86" ht="13.8" customHeight="1" s="2">
@@ -60326,8 +60581,11 @@
       <c r="HV86" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="HW86" t="n">
+      <c r="HW86" s="1" t="n">
         <v>14</v>
+      </c>
+      <c r="HX86" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="87" ht="13.8" customHeight="1" s="2">
@@ -61023,8 +61281,11 @@
       <c r="HV87" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="HW87" t="n">
+      <c r="HW87" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="HX87" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="88" ht="13.8" customHeight="1" s="2">
@@ -61720,8 +61981,11 @@
       <c r="HV88" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="HW88" t="n">
+      <c r="HW88" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="HX88" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="89" ht="13.8" customHeight="1" s="2">
@@ -62417,8 +62681,11 @@
       <c r="HV89" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="HW89" t="n">
+      <c r="HW89" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="HX89" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="90" ht="13.8" customHeight="1" s="2">
@@ -63114,8 +63381,11 @@
       <c r="HV90" s="1" t="n">
         <v>150</v>
       </c>
-      <c r="HW90" t="n">
+      <c r="HW90" s="1" t="n">
         <v>132</v>
+      </c>
+      <c r="HX90" t="n">
+        <v>152</v>
       </c>
     </row>
     <row r="91" ht="13.8" customHeight="1" s="2">
@@ -63811,8 +64081,11 @@
       <c r="HV91" s="1" t="n">
         <v>169</v>
       </c>
-      <c r="HW91" t="n">
+      <c r="HW91" s="1" t="n">
         <v>188</v>
+      </c>
+      <c r="HX91" t="n">
+        <v>210</v>
       </c>
     </row>
     <row r="92" ht="13.8" customHeight="1" s="2">
@@ -64508,8 +64781,11 @@
       <c r="HV92" s="1" t="n">
         <v>227</v>
       </c>
-      <c r="HW92" t="n">
+      <c r="HW92" s="1" t="n">
         <v>230</v>
+      </c>
+      <c r="HX92" t="n">
+        <v>266</v>
       </c>
     </row>
     <row r="93" ht="13.8" customHeight="1" s="2">
@@ -65205,8 +65481,11 @@
       <c r="HV93" s="1" t="n">
         <v>69</v>
       </c>
-      <c r="HW93" t="n">
+      <c r="HW93" s="1" t="n">
         <v>70.09999999999999</v>
+      </c>
+      <c r="HX93" t="n">
+        <v>74.09999999999999</v>
       </c>
     </row>
     <row r="94" ht="13.8" customHeight="1" s="2">
@@ -65902,8 +66181,11 @@
       <c r="HV94" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="HW94" t="n">
+      <c r="HW94" s="1" t="n">
         <v>68</v>
+      </c>
+      <c r="HX94" t="n">
+        <v>53</v>
       </c>
     </row>
     <row r="95" ht="13.8" customHeight="1" s="2">
@@ -66599,8 +66881,11 @@
       <c r="HV95" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="HW95" t="n">
+      <c r="HW95" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="HX95" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="96" ht="13.8" customHeight="1" s="2">
@@ -67296,8 +67581,11 @@
       <c r="HV96" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="HW96" t="n">
+      <c r="HW96" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="HX96" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="97" ht="13.8" customHeight="1" s="2">
@@ -67993,8 +68281,11 @@
       <c r="HV97" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="HW97" t="n">
+      <c r="HW97" s="1" t="n">
         <v>30</v>
+      </c>
+      <c r="HX97" t="n">
+        <v>42</v>
       </c>
     </row>
     <row r="98" ht="13.8" customHeight="1" s="2">
@@ -68690,7 +68981,10 @@
       <c r="HV98" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="HW98" t="n">
+      <c r="HW98" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="HX98" t="n">
         <v>42</v>
       </c>
     </row>
@@ -69387,8 +69681,11 @@
       <c r="HV99" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="HW99" t="n">
+      <c r="HW99" s="1" t="n">
         <v>44</v>
+      </c>
+      <c r="HX99" t="n">
+        <v>52</v>
       </c>
     </row>
     <row r="100" ht="13.8" customHeight="1" s="2">
@@ -70084,7 +70381,10 @@
       <c r="HV100" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="HW100" t="n">
+      <c r="HW100" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="HX100" t="n">
         <v>12</v>
       </c>
     </row>
@@ -70781,8 +71081,11 @@
       <c r="HV101" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="HW101" t="n">
+      <c r="HW101" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="HX101" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="102" ht="13.8" customHeight="1" s="2">
@@ -71478,8 +71781,11 @@
       <c r="HV102" s="1" t="n">
         <v>83.3</v>
       </c>
-      <c r="HW102" t="n">
+      <c r="HW102" s="1" t="n">
         <v>50</v>
+      </c>
+      <c r="HX102" t="n">
+        <v>91.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
round 7 2021 predictions
</commit_message>
<xml_diff>
--- a/django_AFL_ML/Data/Adelaide_stats.xlsx
+++ b/django_AFL_ML/Data/Adelaide_stats.xlsx
@@ -85,6 +85,74 @@
     <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
     <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -377,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:HX102"/>
+  <dimension ref="A1:HY102"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="GZ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="HA23" activeCellId="0" sqref="HA23"/>
@@ -1084,8 +1152,11 @@
       <c r="HW1" s="1" t="n">
         <v>10360</v>
       </c>
-      <c r="HX1" t="n">
+      <c r="HX1" s="1" t="n">
         <v>10369</v>
+      </c>
+      <c r="HY1" t="n">
+        <v>10378</v>
       </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="2">
@@ -1784,7 +1855,10 @@
       <c r="HW2" s="1" t="n">
         <v>2021</v>
       </c>
-      <c r="HX2" t="n">
+      <c r="HX2" s="1" t="n">
+        <v>2021</v>
+      </c>
+      <c r="HY2" t="n">
         <v>2021</v>
       </c>
     </row>
@@ -2484,8 +2558,11 @@
       <c r="HW3" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="HX3" t="n">
+      <c r="HX3" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="HY3" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="2">
@@ -3184,8 +3261,11 @@
       <c r="HW4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="HX4" t="n">
+      <c r="HX4" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="HY4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5" ht="13.8" customHeight="1" s="2">
@@ -3884,8 +3964,11 @@
       <c r="HW5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="HX5" t="n">
+      <c r="HX5" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="HY5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6" ht="13.8" customHeight="1" s="2">
@@ -4584,8 +4667,11 @@
       <c r="HW6" s="1" t="n">
         <v>109</v>
       </c>
-      <c r="HX6" t="n">
+      <c r="HX6" s="1" t="n">
         <v>72</v>
+      </c>
+      <c r="HY6" t="n">
+        <v>99</v>
       </c>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="2">
@@ -5284,8 +5370,11 @@
       <c r="HW7" s="1" t="n">
         <v>68</v>
       </c>
-      <c r="HX7" t="n">
+      <c r="HX7" s="1" t="n">
         <v>84</v>
+      </c>
+      <c r="HY7" t="n">
+        <v>102</v>
       </c>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="2">
@@ -5984,8 +6073,11 @@
       <c r="HW8" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="HX8" t="n">
+      <c r="HX8" s="1" t="n">
         <v>-12</v>
+      </c>
+      <c r="HY8" t="n">
+        <v>-3</v>
       </c>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="2">
@@ -6684,7 +6776,10 @@
       <c r="HW9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="HX9" t="n">
+      <c r="HX9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="HY9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7384,8 +7479,11 @@
       <c r="HW10" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="HX10" t="n">
+      <c r="HX10" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="HY10" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="11" ht="13.8" customHeight="1" s="2">
@@ -8084,8 +8182,11 @@
       <c r="HW11" s="1" t="n">
         <v>221</v>
       </c>
-      <c r="HX11" t="n">
+      <c r="HX11" s="1" t="n">
         <v>213</v>
+      </c>
+      <c r="HY11" t="n">
+        <v>197</v>
       </c>
     </row>
     <row r="12" ht="13.8" customHeight="1" s="2">
@@ -8784,8 +8885,11 @@
       <c r="HW12" s="1" t="n">
         <v>149</v>
       </c>
-      <c r="HX12" t="n">
+      <c r="HX12" s="1" t="n">
         <v>161</v>
+      </c>
+      <c r="HY12" t="n">
+        <v>141</v>
       </c>
     </row>
     <row r="13" ht="13.8" customHeight="1" s="2">
@@ -9484,8 +9588,11 @@
       <c r="HW13" s="1" t="n">
         <v>370</v>
       </c>
-      <c r="HX13" t="n">
+      <c r="HX13" s="1" t="n">
         <v>374</v>
+      </c>
+      <c r="HY13" t="n">
+        <v>338</v>
       </c>
     </row>
     <row r="14" ht="13.8" customHeight="1" s="2">
@@ -10184,8 +10291,11 @@
       <c r="HW14" s="1" t="n">
         <v>1.48</v>
       </c>
-      <c r="HX14" t="n">
+      <c r="HX14" s="1" t="n">
         <v>1.32</v>
+      </c>
+      <c r="HY14" t="n">
+        <v>1.4</v>
       </c>
     </row>
     <row r="15" ht="13.8" customHeight="1" s="2">
@@ -10884,8 +10994,11 @@
       <c r="HW15" s="1" t="n">
         <v>105</v>
       </c>
-      <c r="HX15" t="n">
+      <c r="HX15" s="1" t="n">
         <v>94</v>
+      </c>
+      <c r="HY15" t="n">
+        <v>80</v>
       </c>
     </row>
     <row r="16" ht="13.8" customHeight="1" s="2">
@@ -11584,8 +11697,11 @@
       <c r="HW16" s="1" t="n">
         <v>68</v>
       </c>
-      <c r="HX16" t="n">
+      <c r="HX16" s="1" t="n">
         <v>51</v>
+      </c>
+      <c r="HY16" t="n">
+        <v>58</v>
       </c>
     </row>
     <row r="17" ht="13.8" customHeight="1" s="2">
@@ -12284,8 +12400,11 @@
       <c r="HW17" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="HX17" t="n">
+      <c r="HX17" s="1" t="n">
         <v>37</v>
+      </c>
+      <c r="HY17" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="18" ht="13.8" customHeight="1" s="2">
@@ -12984,8 +13103,11 @@
       <c r="HW18" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="HX18" t="n">
+      <c r="HX18" s="1" t="n">
         <v>18</v>
+      </c>
+      <c r="HY18" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="19" ht="13.8" customHeight="1" s="2">
@@ -13684,8 +13806,11 @@
       <c r="HW19" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="HX19" t="n">
+      <c r="HX19" s="1" t="n">
         <v>20</v>
+      </c>
+      <c r="HY19" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="20" ht="13.8" customHeight="1" s="2">
@@ -14384,8 +14509,11 @@
       <c r="HW20" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="HX20" t="n">
+      <c r="HX20" s="1" t="n">
         <v>11</v>
+      </c>
+      <c r="HY20" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="21" ht="13.8" customHeight="1" s="2">
@@ -15084,8 +15212,11 @@
       <c r="HW21" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="HX21" t="n">
+      <c r="HX21" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="HY21" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="22" ht="13.8" customHeight="1" s="2">
@@ -15784,8 +15915,11 @@
       <c r="HW22" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="HX22" t="n">
+      <c r="HX22" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="HY22" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="23" ht="13.8" customHeight="1" s="2">
@@ -16484,7 +16618,10 @@
       <c r="HW23" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="HX23" t="n">
+      <c r="HX23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="HY23" t="n">
         <v>0</v>
       </c>
     </row>
@@ -17184,8 +17321,11 @@
       <c r="HW24" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="HX24" t="n">
+      <c r="HX24" s="1" t="n">
         <v>17</v>
+      </c>
+      <c r="HY24" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="25" ht="13.8" customHeight="1" s="2">
@@ -17884,8 +18024,11 @@
       <c r="HW25" s="1" t="n">
         <v>55.2</v>
       </c>
-      <c r="HX25" t="n">
+      <c r="HX25" s="1" t="n">
         <v>64.7</v>
+      </c>
+      <c r="HY25" t="n">
+        <v>84.2</v>
       </c>
     </row>
     <row r="26" ht="13.8" customHeight="1" s="2">
@@ -18584,8 +18727,11 @@
       <c r="HW26" s="1" t="n">
         <v>23.12</v>
       </c>
-      <c r="HX26" t="n">
+      <c r="HX26" s="1" t="n">
         <v>34</v>
+      </c>
+      <c r="HY26" t="n">
+        <v>21.12</v>
       </c>
     </row>
     <row r="27" ht="13.8" customHeight="1" s="2">
@@ -19284,8 +19430,11 @@
       <c r="HW27" s="1" t="n">
         <v>12.76</v>
       </c>
-      <c r="HX27" t="n">
+      <c r="HX27" s="1" t="n">
         <v>22</v>
+      </c>
+      <c r="HY27" t="n">
+        <v>17.79</v>
       </c>
     </row>
     <row r="28" ht="13.8" customHeight="1" s="2">
@@ -19984,8 +20133,11 @@
       <c r="HW28" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="HX28" t="n">
+      <c r="HX28" s="1" t="n">
         <v>35</v>
+      </c>
+      <c r="HY28" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="29" ht="13.8" customHeight="1" s="2">
@@ -20684,8 +20836,11 @@
       <c r="HW29" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="HX29" t="n">
+      <c r="HX29" s="1" t="n">
         <v>60</v>
+      </c>
+      <c r="HY29" t="n">
+        <v>69</v>
       </c>
     </row>
     <row r="30" ht="13.8" customHeight="1" s="2">
@@ -21384,8 +21539,11 @@
       <c r="HW30" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="HX30" t="n">
+      <c r="HX30" s="1" t="n">
         <v>42</v>
+      </c>
+      <c r="HY30" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="31" ht="13.8" customHeight="1" s="2">
@@ -22084,8 +22242,11 @@
       <c r="HW31" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="HX31" t="n">
+      <c r="HX31" s="1" t="n">
         <v>55</v>
+      </c>
+      <c r="HY31" t="n">
+        <v>51</v>
       </c>
     </row>
     <row r="32" ht="13.8" customHeight="1" s="2">
@@ -22784,8 +22945,11 @@
       <c r="HW32" s="1" t="n">
         <v>2.03</v>
       </c>
-      <c r="HX32" t="n">
+      <c r="HX32" s="1" t="n">
         <v>3.24</v>
+      </c>
+      <c r="HY32" t="n">
+        <v>2.68</v>
       </c>
     </row>
     <row r="33" ht="13.8" customHeight="1" s="2">
@@ -23484,8 +23648,11 @@
       <c r="HW33" s="1" t="n">
         <v>3.69</v>
       </c>
-      <c r="HX33" t="n">
+      <c r="HX33" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="HY33" t="n">
+        <v>3.19</v>
       </c>
     </row>
     <row r="34" ht="13.8" customHeight="1" s="2">
@@ -24184,8 +24351,11 @@
       <c r="HW34" s="1" t="n">
         <v>45.8</v>
       </c>
-      <c r="HX34" t="n">
+      <c r="HX34" s="1" t="n">
         <v>30.9</v>
+      </c>
+      <c r="HY34" t="n">
+        <v>37.3</v>
       </c>
     </row>
     <row r="35" ht="13.8" customHeight="1" s="2">
@@ -24884,8 +25054,11 @@
       <c r="HW35" s="1" t="n">
         <v>27.1</v>
       </c>
-      <c r="HX35" t="n">
+      <c r="HX35" s="1" t="n">
         <v>20</v>
+      </c>
+      <c r="HY35" t="n">
+        <v>31.4</v>
       </c>
     </row>
     <row r="36" ht="13.8" customHeight="1" s="2">
@@ -25584,8 +25757,11 @@
       <c r="HW36" s="1" t="n">
         <v>186.6</v>
       </c>
-      <c r="HX36" t="n">
+      <c r="HX36" s="1" t="n">
         <v>186.6</v>
+      </c>
+      <c r="HY36" t="n">
+        <v>187.6</v>
       </c>
     </row>
     <row r="37" ht="13.8" customHeight="1" s="2">
@@ -26284,8 +26460,11 @@
       <c r="HW37" s="1" t="n">
         <v>83.8</v>
       </c>
-      <c r="HX37" t="n">
+      <c r="HX37" s="1" t="n">
         <v>83.8</v>
+      </c>
+      <c r="HY37" t="n">
+        <v>84.90000000000001</v>
       </c>
     </row>
     <row r="38" ht="13.8" customHeight="1" s="2">
@@ -26984,8 +27163,11 @@
       <c r="HW38" s="1" t="n">
         <v>24.41</v>
       </c>
-      <c r="HX38" t="n">
+      <c r="HX38" s="1" t="n">
         <v>24.41</v>
+      </c>
+      <c r="HY38" t="n">
+        <v>24.16</v>
       </c>
     </row>
     <row r="39" ht="13.8" customHeight="1" s="2">
@@ -27684,8 +27866,11 @@
       <c r="HW39" s="1" t="n">
         <v>63.3</v>
       </c>
-      <c r="HX39" t="n">
+      <c r="HX39" s="1" t="n">
         <v>64.3</v>
+      </c>
+      <c r="HY39" t="n">
+        <v>63.1</v>
       </c>
     </row>
     <row r="40" ht="13.8" customHeight="1" s="2">
@@ -28384,7 +28569,10 @@
       <c r="HW40" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="HX40" t="n">
+      <c r="HX40" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="HY40" t="n">
         <v>14</v>
       </c>
     </row>
@@ -29084,8 +29272,11 @@
       <c r="HW41" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="HX41" t="n">
+      <c r="HX41" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="HY41" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="42" ht="13.8" customHeight="1" s="2">
@@ -29784,7 +29975,10 @@
       <c r="HW42" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="HX42" t="n">
+      <c r="HX42" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="HY42" t="n">
         <v>1</v>
       </c>
     </row>
@@ -30484,7 +30678,10 @@
       <c r="HW43" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="HX43" t="n">
+      <c r="HX43" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="HY43" t="n">
         <v>5</v>
       </c>
     </row>
@@ -31184,8 +31381,11 @@
       <c r="HW44" s="1" t="n">
         <v>141</v>
       </c>
-      <c r="HX44" t="n">
+      <c r="HX44" s="1" t="n">
         <v>139</v>
+      </c>
+      <c r="HY44" t="n">
+        <v>144</v>
       </c>
     </row>
     <row r="45" ht="13.8" customHeight="1" s="2">
@@ -31884,8 +32084,11 @@
       <c r="HW45" s="1" t="n">
         <v>227</v>
       </c>
-      <c r="HX45" t="n">
+      <c r="HX45" s="1" t="n">
         <v>229</v>
+      </c>
+      <c r="HY45" t="n">
+        <v>195</v>
       </c>
     </row>
     <row r="46" ht="13.8" customHeight="1" s="2">
@@ -32584,8 +32787,11 @@
       <c r="HW46" s="1" t="n">
         <v>288</v>
       </c>
-      <c r="HX46" t="n">
+      <c r="HX46" s="1" t="n">
         <v>275</v>
+      </c>
+      <c r="HY46" t="n">
+        <v>252</v>
       </c>
     </row>
     <row r="47" ht="13.8" customHeight="1" s="2">
@@ -33284,8 +33490,11 @@
       <c r="HW47" s="1" t="n">
         <v>77.8</v>
       </c>
-      <c r="HX47" t="n">
+      <c r="HX47" s="1" t="n">
         <v>73.5</v>
+      </c>
+      <c r="HY47" t="n">
+        <v>74.59999999999999</v>
       </c>
     </row>
     <row r="48" ht="13.8" customHeight="1" s="2">
@@ -33984,8 +34193,11 @@
       <c r="HW48" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="HX48" t="n">
+      <c r="HX48" s="1" t="n">
         <v>60</v>
+      </c>
+      <c r="HY48" t="n">
+        <v>69</v>
       </c>
     </row>
     <row r="49" ht="13.8" customHeight="1" s="2">
@@ -34684,8 +34896,11 @@
       <c r="HW49" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="HX49" t="n">
+      <c r="HX49" s="1" t="n">
         <v>13</v>
+      </c>
+      <c r="HY49" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="50" ht="13.8" customHeight="1" s="2">
@@ -35384,8 +35599,11 @@
       <c r="HW50" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="HX50" t="n">
+      <c r="HX50" s="1" t="n">
         <v>9</v>
+      </c>
+      <c r="HY50" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="51" ht="13.8" customHeight="1" s="2">
@@ -36084,8 +36302,11 @@
       <c r="HW51" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="HX51" t="n">
+      <c r="HX51" s="1" t="n">
         <v>35</v>
+      </c>
+      <c r="HY51" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="52" ht="13.8" customHeight="1" s="2">
@@ -36784,8 +37005,11 @@
       <c r="HW52" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="HX52" t="n">
+      <c r="HX52" s="1" t="n">
         <v>42</v>
+      </c>
+      <c r="HY52" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="53" ht="13.8" customHeight="1" s="2">
@@ -37484,8 +37708,11 @@
       <c r="HW53" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="HX53" t="n">
+      <c r="HX53" s="1" t="n">
         <v>56</v>
+      </c>
+      <c r="HY53" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="54" ht="13.8" customHeight="1" s="2">
@@ -38184,8 +38411,11 @@
       <c r="HW54" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="HX54" t="n">
+      <c r="HX54" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="HY54" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="55" ht="13.8" customHeight="1" s="2">
@@ -38884,8 +39114,11 @@
       <c r="HW55" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="HX55" t="n">
+      <c r="HX55" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="HY55" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="56" ht="13.8" customHeight="1" s="2">
@@ -39584,8 +39817,11 @@
       <c r="HW56" s="1" t="n">
         <v>81.2</v>
       </c>
-      <c r="HX56" t="n">
+      <c r="HX56" s="1" t="n">
         <v>63.6</v>
+      </c>
+      <c r="HY56" t="n">
+        <v>62.5</v>
       </c>
     </row>
     <row r="57" ht="13.8" customHeight="1" s="2">
@@ -40284,8 +40520,11 @@
       <c r="HW57" s="1" t="n">
         <v>190</v>
       </c>
-      <c r="HX57" t="n">
+      <c r="HX57" s="1" t="n">
         <v>218</v>
+      </c>
+      <c r="HY57" t="n">
+        <v>206</v>
       </c>
     </row>
     <row r="58" ht="13.8" customHeight="1" s="2">
@@ -40984,8 +41223,11 @@
       <c r="HW58" s="1" t="n">
         <v>138</v>
       </c>
-      <c r="HX58" t="n">
+      <c r="HX58" s="1" t="n">
         <v>141</v>
+      </c>
+      <c r="HY58" t="n">
+        <v>162</v>
       </c>
     </row>
     <row r="59" ht="13.8" customHeight="1" s="2">
@@ -41684,8 +41926,11 @@
       <c r="HW59" s="1" t="n">
         <v>328</v>
       </c>
-      <c r="HX59" t="n">
+      <c r="HX59" s="1" t="n">
         <v>359</v>
+      </c>
+      <c r="HY59" t="n">
+        <v>368</v>
       </c>
     </row>
     <row r="60" ht="13.8" customHeight="1" s="2">
@@ -42384,8 +42629,11 @@
       <c r="HW60" s="1" t="n">
         <v>1.38</v>
       </c>
-      <c r="HX60" t="n">
+      <c r="HX60" s="1" t="n">
         <v>1.55</v>
+      </c>
+      <c r="HY60" t="n">
+        <v>1.27</v>
       </c>
     </row>
     <row r="61" ht="13.8" customHeight="1" s="2">
@@ -43084,8 +43332,11 @@
       <c r="HW61" s="1" t="n">
         <v>76</v>
       </c>
-      <c r="HX61" t="n">
+      <c r="HX61" s="1" t="n">
         <v>102</v>
+      </c>
+      <c r="HY61" t="n">
+        <v>86</v>
       </c>
     </row>
     <row r="62" ht="13.8" customHeight="1" s="2">
@@ -43784,8 +44035,11 @@
       <c r="HW62" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="HX62" t="n">
+      <c r="HX62" s="1" t="n">
         <v>57</v>
+      </c>
+      <c r="HY62" t="n">
+        <v>51</v>
       </c>
     </row>
     <row r="63" ht="13.8" customHeight="1" s="2">
@@ -44484,8 +44738,11 @@
       <c r="HW63" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="HX63" t="n">
+      <c r="HX63" s="1" t="n">
         <v>39</v>
+      </c>
+      <c r="HY63" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="64" ht="13.8" customHeight="1" s="2">
@@ -45184,8 +45441,11 @@
       <c r="HW64" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="HX64" t="n">
+      <c r="HX64" s="1" t="n">
         <v>20</v>
+      </c>
+      <c r="HY64" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="65" ht="13.8" customHeight="1" s="2">
@@ -45884,8 +46144,11 @@
       <c r="HW65" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="HX65" t="n">
+      <c r="HX65" s="1" t="n">
         <v>18</v>
+      </c>
+      <c r="HY65" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="66" ht="13.8" customHeight="1" s="2">
@@ -46584,8 +46847,11 @@
       <c r="HW66" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="HX66" t="n">
+      <c r="HX66" s="1" t="n">
         <v>12</v>
+      </c>
+      <c r="HY66" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="67" ht="13.8" customHeight="1" s="2">
@@ -47284,7 +47550,10 @@
       <c r="HW67" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="HX67" t="n">
+      <c r="HX67" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="HY67" t="n">
         <v>11</v>
       </c>
     </row>
@@ -47984,8 +48253,11 @@
       <c r="HW68" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="HX68" t="n">
+      <c r="HX68" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="HY68" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="69" ht="13.8" customHeight="1" s="2">
@@ -48684,8 +48956,11 @@
       <c r="HW69" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="HX69" t="n">
+      <c r="HX69" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="HY69" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="70" ht="13.8" customHeight="1" s="2">
@@ -49384,8 +49659,11 @@
       <c r="HW70" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="HX70" t="n">
+      <c r="HX70" s="1" t="n">
         <v>24</v>
+      </c>
+      <c r="HY70" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="71" ht="13.8" customHeight="1" s="2">
@@ -50084,8 +50362,11 @@
       <c r="HW71" s="1" t="n">
         <v>55.6</v>
       </c>
-      <c r="HX71" t="n">
+      <c r="HX71" s="1" t="n">
         <v>50</v>
+      </c>
+      <c r="HY71" t="n">
+        <v>55.6</v>
       </c>
     </row>
     <row r="72" ht="13.8" customHeight="1" s="2">
@@ -50784,8 +51065,11 @@
       <c r="HW72" s="1" t="n">
         <v>32.8</v>
       </c>
-      <c r="HX72" t="n">
+      <c r="HX72" s="1" t="n">
         <v>29.92</v>
+      </c>
+      <c r="HY72" t="n">
+        <v>24.53</v>
       </c>
     </row>
     <row r="73" ht="13.8" customHeight="1" s="2">
@@ -51484,8 +51768,11 @@
       <c r="HW73" s="1" t="n">
         <v>18.22</v>
       </c>
-      <c r="HX73" t="n">
+      <c r="HX73" s="1" t="n">
         <v>14.96</v>
+      </c>
+      <c r="HY73" t="n">
+        <v>13.63</v>
       </c>
     </row>
     <row r="74" ht="13.8" customHeight="1" s="2">
@@ -52184,8 +52471,11 @@
       <c r="HW74" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="HX74" t="n">
+      <c r="HX74" s="1" t="n">
         <v>42</v>
+      </c>
+      <c r="HY74" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="75" ht="13.8" customHeight="1" s="2">
@@ -52884,8 +53174,11 @@
       <c r="HW75" s="1" t="n">
         <v>68</v>
       </c>
-      <c r="HX75" t="n">
+      <c r="HX75" s="1" t="n">
         <v>53</v>
+      </c>
+      <c r="HY75" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="76" ht="13.8" customHeight="1" s="2">
@@ -53584,8 +53877,11 @@
       <c r="HW76" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="HX76" t="n">
+      <c r="HX76" s="1" t="n">
         <v>42</v>
+      </c>
+      <c r="HY76" t="n">
+        <v>35</v>
       </c>
     </row>
     <row r="77" ht="13.8" customHeight="1" s="2">
@@ -54284,8 +54580,11 @@
       <c r="HW77" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="HX77" t="n">
+      <c r="HX77" s="1" t="n">
         <v>54</v>
+      </c>
+      <c r="HY77" t="n">
+        <v>61</v>
       </c>
     </row>
     <row r="78" ht="13.8" customHeight="1" s="2">
@@ -54984,8 +55283,11 @@
       <c r="HW78" s="1" t="n">
         <v>2.94</v>
       </c>
-      <c r="HX78" t="n">
+      <c r="HX78" s="1" t="n">
         <v>2.25</v>
+      </c>
+      <c r="HY78" t="n">
+        <v>2.26</v>
       </c>
     </row>
     <row r="79" ht="13.8" customHeight="1" s="2">
@@ -55684,8 +55986,11 @@
       <c r="HW79" s="1" t="n">
         <v>5.3</v>
       </c>
-      <c r="HX79" t="n">
+      <c r="HX79" s="1" t="n">
         <v>4.5</v>
+      </c>
+      <c r="HY79" t="n">
+        <v>4.07</v>
       </c>
     </row>
     <row r="80" ht="13.8" customHeight="1" s="2">
@@ -56384,8 +56689,11 @@
       <c r="HW80" s="1" t="n">
         <v>30.2</v>
       </c>
-      <c r="HX80" t="n">
+      <c r="HX80" s="1" t="n">
         <v>37</v>
+      </c>
+      <c r="HY80" t="n">
+        <v>39.3</v>
       </c>
     </row>
     <row r="81" ht="13.8" customHeight="1" s="2">
@@ -57084,8 +57392,11 @@
       <c r="HW81" s="1" t="n">
         <v>18.9</v>
       </c>
-      <c r="HX81" t="n">
+      <c r="HX81" s="1" t="n">
         <v>22.2</v>
+      </c>
+      <c r="HY81" t="n">
+        <v>24.6</v>
       </c>
     </row>
     <row r="82" ht="13.8" customHeight="1" s="2">
@@ -57784,8 +58095,11 @@
       <c r="HW82" s="1" t="n">
         <v>187.8</v>
       </c>
-      <c r="HX82" t="n">
+      <c r="HX82" s="1" t="n">
         <v>187.9</v>
+      </c>
+      <c r="HY82" t="n">
+        <v>186.7</v>
       </c>
     </row>
     <row r="83" ht="13.8" customHeight="1" s="2">
@@ -58484,8 +58798,11 @@
       <c r="HW83" s="1" t="n">
         <v>84.09999999999999</v>
       </c>
-      <c r="HX83" t="n">
+      <c r="HX83" s="1" t="n">
         <v>88.59999999999999</v>
+      </c>
+      <c r="HY83" t="n">
+        <v>85</v>
       </c>
     </row>
     <row r="84" ht="13.8" customHeight="1" s="2">
@@ -59184,8 +59501,11 @@
       <c r="HW84" s="1" t="n">
         <v>24.8</v>
       </c>
-      <c r="HX84" t="n">
+      <c r="HX84" s="1" t="n">
         <v>25.8</v>
+      </c>
+      <c r="HY84" t="n">
+        <v>25.74</v>
       </c>
     </row>
     <row r="85" ht="13.8" customHeight="1" s="2">
@@ -59884,8 +60204,11 @@
       <c r="HW85" s="1" t="n">
         <v>72.8</v>
       </c>
-      <c r="HX85" t="n">
+      <c r="HX85" s="1" t="n">
         <v>85.3</v>
+      </c>
+      <c r="HY85" t="n">
+        <v>102.9</v>
       </c>
     </row>
     <row r="86" ht="13.8" customHeight="1" s="2">
@@ -60584,8 +60907,11 @@
       <c r="HW86" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="HX86" t="n">
+      <c r="HX86" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="HY86" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="87" ht="13.8" customHeight="1" s="2">
@@ -61284,8 +61610,11 @@
       <c r="HW87" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="HX87" t="n">
+      <c r="HX87" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="HY87" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="88" ht="13.8" customHeight="1" s="2">
@@ -61984,7 +62313,10 @@
       <c r="HW88" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="HX88" t="n">
+      <c r="HX88" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="HY88" t="n">
         <v>5</v>
       </c>
     </row>
@@ -62684,8 +63016,11 @@
       <c r="HW89" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="HX89" t="n">
+      <c r="HX89" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="HY89" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="90" ht="13.8" customHeight="1" s="2">
@@ -63384,8 +63719,11 @@
       <c r="HW90" s="1" t="n">
         <v>132</v>
       </c>
-      <c r="HX90" t="n">
+      <c r="HX90" s="1" t="n">
         <v>152</v>
+      </c>
+      <c r="HY90" t="n">
+        <v>146</v>
       </c>
     </row>
     <row r="91" ht="13.8" customHeight="1" s="2">
@@ -64084,8 +64422,11 @@
       <c r="HW91" s="1" t="n">
         <v>188</v>
       </c>
-      <c r="HX91" t="n">
+      <c r="HX91" s="1" t="n">
         <v>210</v>
+      </c>
+      <c r="HY91" t="n">
+        <v>214</v>
       </c>
     </row>
     <row r="92" ht="13.8" customHeight="1" s="2">
@@ -64784,8 +65125,11 @@
       <c r="HW92" s="1" t="n">
         <v>230</v>
       </c>
-      <c r="HX92" t="n">
+      <c r="HX92" s="1" t="n">
         <v>266</v>
+      </c>
+      <c r="HY92" t="n">
+        <v>260</v>
       </c>
     </row>
     <row r="93" ht="13.8" customHeight="1" s="2">
@@ -65484,8 +65828,11 @@
       <c r="HW93" s="1" t="n">
         <v>70.09999999999999</v>
       </c>
-      <c r="HX93" t="n">
+      <c r="HX93" s="1" t="n">
         <v>74.09999999999999</v>
+      </c>
+      <c r="HY93" t="n">
+        <v>70.7</v>
       </c>
     </row>
     <row r="94" ht="13.8" customHeight="1" s="2">
@@ -66184,8 +66531,11 @@
       <c r="HW94" s="1" t="n">
         <v>68</v>
       </c>
-      <c r="HX94" t="n">
+      <c r="HX94" s="1" t="n">
         <v>53</v>
+      </c>
+      <c r="HY94" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="95" ht="13.8" customHeight="1" s="2">
@@ -66884,8 +67234,11 @@
       <c r="HW95" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="HX95" t="n">
+      <c r="HX95" s="1" t="n">
         <v>18</v>
+      </c>
+      <c r="HY95" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="96" ht="13.8" customHeight="1" s="2">
@@ -67584,8 +67937,11 @@
       <c r="HW96" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="HX96" t="n">
+      <c r="HX96" s="1" t="n">
         <v>14</v>
+      </c>
+      <c r="HY96" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="97" ht="13.8" customHeight="1" s="2">
@@ -68284,8 +68640,11 @@
       <c r="HW97" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="HX97" t="n">
+      <c r="HX97" s="1" t="n">
         <v>42</v>
+      </c>
+      <c r="HY97" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="98" ht="13.8" customHeight="1" s="2">
@@ -68984,8 +69343,11 @@
       <c r="HW98" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="HX98" t="n">
+      <c r="HX98" s="1" t="n">
         <v>42</v>
+      </c>
+      <c r="HY98" t="n">
+        <v>35</v>
       </c>
     </row>
     <row r="99" ht="13.8" customHeight="1" s="2">
@@ -69684,8 +70046,11 @@
       <c r="HW99" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="HX99" t="n">
+      <c r="HX99" s="1" t="n">
         <v>52</v>
+      </c>
+      <c r="HY99" t="n">
+        <v>39</v>
       </c>
     </row>
     <row r="100" ht="13.8" customHeight="1" s="2">
@@ -70384,8 +70749,11 @@
       <c r="HW100" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="HX100" t="n">
+      <c r="HX100" s="1" t="n">
         <v>12</v>
+      </c>
+      <c r="HY100" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="101" ht="13.8" customHeight="1" s="2">
@@ -71084,7 +71452,10 @@
       <c r="HW101" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="HX101" t="n">
+      <c r="HX101" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="HY101" t="n">
         <v>11</v>
       </c>
     </row>
@@ -71784,8 +72155,11 @@
       <c r="HW102" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="HX102" t="n">
+      <c r="HX102" s="1" t="n">
         <v>91.7</v>
+      </c>
+      <c r="HY102" t="n">
+        <v>73.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
round 8 2021 predictions done
</commit_message>
<xml_diff>
--- a/django_AFL_ML/Data/Adelaide_stats.xlsx
+++ b/django_AFL_ML/Data/Adelaide_stats.xlsx
@@ -85,74 +85,6 @@
     <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
     <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -445,7 +377,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:HY102"/>
+  <dimension ref="A1:HZ102"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="GZ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="HA23" activeCellId="0" sqref="HA23"/>
@@ -1155,8 +1087,11 @@
       <c r="HX1" s="1" t="n">
         <v>10369</v>
       </c>
-      <c r="HY1" t="n">
+      <c r="HY1" s="1" t="n">
         <v>10378</v>
+      </c>
+      <c r="HZ1" t="n">
+        <v>10388</v>
       </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="2">
@@ -1858,7 +1793,10 @@
       <c r="HX2" s="1" t="n">
         <v>2021</v>
       </c>
-      <c r="HY2" t="n">
+      <c r="HY2" s="1" t="n">
+        <v>2021</v>
+      </c>
+      <c r="HZ2" t="n">
         <v>2021</v>
       </c>
     </row>
@@ -2561,8 +2499,11 @@
       <c r="HX3" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="HY3" t="n">
+      <c r="HY3" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="HZ3" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="2">
@@ -3264,8 +3205,11 @@
       <c r="HX4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="HY4" t="n">
+      <c r="HY4" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="HZ4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5" ht="13.8" customHeight="1" s="2">
@@ -3967,8 +3911,11 @@
       <c r="HX5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="HY5" t="n">
+      <c r="HY5" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="HZ5" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6" ht="13.8" customHeight="1" s="2">
@@ -4670,8 +4617,11 @@
       <c r="HX6" s="1" t="n">
         <v>72</v>
       </c>
-      <c r="HY6" t="n">
+      <c r="HY6" s="1" t="n">
         <v>99</v>
+      </c>
+      <c r="HZ6" t="n">
+        <v>39</v>
       </c>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="2">
@@ -5373,8 +5323,11 @@
       <c r="HX7" s="1" t="n">
         <v>84</v>
       </c>
-      <c r="HY7" t="n">
+      <c r="HY7" s="1" t="n">
         <v>102</v>
+      </c>
+      <c r="HZ7" t="n">
+        <v>106</v>
       </c>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="2">
@@ -6076,8 +6029,11 @@
       <c r="HX8" s="1" t="n">
         <v>-12</v>
       </c>
-      <c r="HY8" t="n">
+      <c r="HY8" s="1" t="n">
         <v>-3</v>
+      </c>
+      <c r="HZ8" t="n">
+        <v>-67</v>
       </c>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="2">
@@ -6779,7 +6735,10 @@
       <c r="HX9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="HY9" t="n">
+      <c r="HY9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="HZ9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7482,8 +7441,11 @@
       <c r="HX10" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="HY10" t="n">
+      <c r="HY10" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="HZ10" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="11" ht="13.8" customHeight="1" s="2">
@@ -8185,7 +8147,10 @@
       <c r="HX11" s="1" t="n">
         <v>213</v>
       </c>
-      <c r="HY11" t="n">
+      <c r="HY11" s="1" t="n">
+        <v>197</v>
+      </c>
+      <c r="HZ11" t="n">
         <v>197</v>
       </c>
     </row>
@@ -8888,8 +8853,11 @@
       <c r="HX12" s="1" t="n">
         <v>161</v>
       </c>
-      <c r="HY12" t="n">
+      <c r="HY12" s="1" t="n">
         <v>141</v>
+      </c>
+      <c r="HZ12" t="n">
+        <v>152</v>
       </c>
     </row>
     <row r="13" ht="13.8" customHeight="1" s="2">
@@ -9591,8 +9559,11 @@
       <c r="HX13" s="1" t="n">
         <v>374</v>
       </c>
-      <c r="HY13" t="n">
+      <c r="HY13" s="1" t="n">
         <v>338</v>
+      </c>
+      <c r="HZ13" t="n">
+        <v>349</v>
       </c>
     </row>
     <row r="14" ht="13.8" customHeight="1" s="2">
@@ -10294,8 +10265,11 @@
       <c r="HX14" s="1" t="n">
         <v>1.32</v>
       </c>
-      <c r="HY14" t="n">
+      <c r="HY14" s="1" t="n">
         <v>1.4</v>
+      </c>
+      <c r="HZ14" t="n">
+        <v>1.3</v>
       </c>
     </row>
     <row r="15" ht="13.8" customHeight="1" s="2">
@@ -10997,8 +10971,11 @@
       <c r="HX15" s="1" t="n">
         <v>94</v>
       </c>
-      <c r="HY15" t="n">
+      <c r="HY15" s="1" t="n">
         <v>80</v>
+      </c>
+      <c r="HZ15" t="n">
+        <v>86</v>
       </c>
     </row>
     <row r="16" ht="13.8" customHeight="1" s="2">
@@ -11700,8 +11677,11 @@
       <c r="HX16" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="HY16" t="n">
+      <c r="HY16" s="1" t="n">
         <v>58</v>
+      </c>
+      <c r="HZ16" t="n">
+        <v>43</v>
       </c>
     </row>
     <row r="17" ht="13.8" customHeight="1" s="2">
@@ -12403,8 +12383,11 @@
       <c r="HX17" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="HY17" t="n">
+      <c r="HY17" s="1" t="n">
         <v>44</v>
+      </c>
+      <c r="HZ17" t="n">
+        <v>29</v>
       </c>
     </row>
     <row r="18" ht="13.8" customHeight="1" s="2">
@@ -13106,8 +13089,11 @@
       <c r="HX18" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="HY18" t="n">
+      <c r="HY18" s="1" t="n">
         <v>25</v>
+      </c>
+      <c r="HZ18" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="19" ht="13.8" customHeight="1" s="2">
@@ -13809,8 +13795,11 @@
       <c r="HX19" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="HY19" t="n">
+      <c r="HY19" s="1" t="n">
         <v>30</v>
+      </c>
+      <c r="HZ19" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="20" ht="13.8" customHeight="1" s="2">
@@ -14512,8 +14501,11 @@
       <c r="HX20" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="HY20" t="n">
+      <c r="HY20" s="1" t="n">
         <v>16</v>
+      </c>
+      <c r="HZ20" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="21" ht="13.8" customHeight="1" s="2">
@@ -15215,8 +15207,11 @@
       <c r="HX21" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="HY21" t="n">
+      <c r="HY21" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="HZ21" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="22" ht="13.8" customHeight="1" s="2">
@@ -15918,8 +15913,11 @@
       <c r="HX22" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="HY22" t="n">
+      <c r="HY22" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="HZ22" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="23" ht="13.8" customHeight="1" s="2">
@@ -16621,8 +16619,11 @@
       <c r="HX23" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="HY23" t="n">
+      <c r="HY23" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="HZ23" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="24" ht="13.8" customHeight="1" s="2">
@@ -17324,7 +17325,10 @@
       <c r="HX24" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="HY24" t="n">
+      <c r="HY24" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="HZ24" t="n">
         <v>19</v>
       </c>
     </row>
@@ -18027,8 +18031,11 @@
       <c r="HX25" s="1" t="n">
         <v>64.7</v>
       </c>
-      <c r="HY25" t="n">
+      <c r="HY25" s="1" t="n">
         <v>84.2</v>
+      </c>
+      <c r="HZ25" t="n">
+        <v>21.1</v>
       </c>
     </row>
     <row r="26" ht="13.8" customHeight="1" s="2">
@@ -18730,8 +18737,11 @@
       <c r="HX26" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="HY26" t="n">
+      <c r="HY26" s="1" t="n">
         <v>21.12</v>
+      </c>
+      <c r="HZ26" t="n">
+        <v>87.25</v>
       </c>
     </row>
     <row r="27" ht="13.8" customHeight="1" s="2">
@@ -19433,8 +19443,11 @@
       <c r="HX27" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="HY27" t="n">
+      <c r="HY27" s="1" t="n">
         <v>17.79</v>
+      </c>
+      <c r="HZ27" t="n">
+        <v>18.37</v>
       </c>
     </row>
     <row r="28" ht="13.8" customHeight="1" s="2">
@@ -20136,8 +20149,11 @@
       <c r="HX28" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="HY28" t="n">
+      <c r="HY28" s="1" t="n">
         <v>40</v>
+      </c>
+      <c r="HZ28" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="29" ht="13.8" customHeight="1" s="2">
@@ -20839,8 +20855,11 @@
       <c r="HX29" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="HY29" t="n">
+      <c r="HY29" s="1" t="n">
         <v>69</v>
+      </c>
+      <c r="HZ29" t="n">
+        <v>54</v>
       </c>
     </row>
     <row r="30" ht="13.8" customHeight="1" s="2">
@@ -21542,8 +21561,11 @@
       <c r="HX30" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="HY30" t="n">
+      <c r="HY30" s="1" t="n">
         <v>44</v>
+      </c>
+      <c r="HZ30" t="n">
+        <v>42</v>
       </c>
     </row>
     <row r="31" ht="13.8" customHeight="1" s="2">
@@ -22245,8 +22267,11 @@
       <c r="HX31" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="HY31" t="n">
+      <c r="HY31" s="1" t="n">
         <v>51</v>
+      </c>
+      <c r="HZ31" t="n">
+        <v>52</v>
       </c>
     </row>
     <row r="32" ht="13.8" customHeight="1" s="2">
@@ -22948,8 +22973,11 @@
       <c r="HX32" s="1" t="n">
         <v>3.24</v>
       </c>
-      <c r="HY32" t="n">
+      <c r="HY32" s="1" t="n">
         <v>2.68</v>
+      </c>
+      <c r="HZ32" t="n">
+        <v>2.74</v>
       </c>
     </row>
     <row r="33" ht="13.8" customHeight="1" s="2">
@@ -23651,8 +23679,11 @@
       <c r="HX33" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="HY33" t="n">
+      <c r="HY33" s="1" t="n">
         <v>3.19</v>
+      </c>
+      <c r="HZ33" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="34" ht="13.8" customHeight="1" s="2">
@@ -24354,8 +24385,11 @@
       <c r="HX34" s="1" t="n">
         <v>30.9</v>
       </c>
-      <c r="HY34" t="n">
+      <c r="HY34" s="1" t="n">
         <v>37.3</v>
+      </c>
+      <c r="HZ34" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="35" ht="13.8" customHeight="1" s="2">
@@ -25057,8 +25091,11 @@
       <c r="HX35" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="HY35" t="n">
+      <c r="HY35" s="1" t="n">
         <v>31.4</v>
+      </c>
+      <c r="HZ35" t="n">
+        <v>7.7</v>
       </c>
     </row>
     <row r="36" ht="13.8" customHeight="1" s="2">
@@ -25760,8 +25797,11 @@
       <c r="HX36" s="1" t="n">
         <v>186.6</v>
       </c>
-      <c r="HY36" t="n">
+      <c r="HY36" s="1" t="n">
         <v>187.6</v>
+      </c>
+      <c r="HZ36" t="n">
+        <v>187.1</v>
       </c>
     </row>
     <row r="37" ht="13.8" customHeight="1" s="2">
@@ -26463,8 +26503,11 @@
       <c r="HX37" s="1" t="n">
         <v>83.8</v>
       </c>
-      <c r="HY37" t="n">
+      <c r="HY37" s="1" t="n">
         <v>84.90000000000001</v>
+      </c>
+      <c r="HZ37" t="n">
+        <v>85</v>
       </c>
     </row>
     <row r="38" ht="13.8" customHeight="1" s="2">
@@ -27166,8 +27209,11 @@
       <c r="HX38" s="1" t="n">
         <v>24.41</v>
       </c>
-      <c r="HY38" t="n">
+      <c r="HY38" s="1" t="n">
         <v>24.16</v>
+      </c>
+      <c r="HZ38" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="39" ht="13.8" customHeight="1" s="2">
@@ -27869,8 +27915,11 @@
       <c r="HX39" s="1" t="n">
         <v>64.3</v>
       </c>
-      <c r="HY39" t="n">
+      <c r="HY39" s="1" t="n">
         <v>63.1</v>
+      </c>
+      <c r="HZ39" t="n">
+        <v>60.9</v>
       </c>
     </row>
     <row r="40" ht="13.8" customHeight="1" s="2">
@@ -28572,7 +28621,10 @@
       <c r="HX40" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="HY40" t="n">
+      <c r="HY40" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="HZ40" t="n">
         <v>14</v>
       </c>
     </row>
@@ -29275,7 +29327,10 @@
       <c r="HX41" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="HY41" t="n">
+      <c r="HY41" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="HZ41" t="n">
         <v>3</v>
       </c>
     </row>
@@ -29978,7 +30033,10 @@
       <c r="HX42" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="HY42" t="n">
+      <c r="HY42" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="HZ42" t="n">
         <v>1</v>
       </c>
     </row>
@@ -30681,8 +30739,11 @@
       <c r="HX43" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="HY43" t="n">
+      <c r="HY43" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="HZ43" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="44" ht="13.8" customHeight="1" s="2">
@@ -31384,8 +31445,11 @@
       <c r="HX44" s="1" t="n">
         <v>139</v>
       </c>
-      <c r="HY44" t="n">
+      <c r="HY44" s="1" t="n">
         <v>144</v>
+      </c>
+      <c r="HZ44" t="n">
+        <v>114</v>
       </c>
     </row>
     <row r="45" ht="13.8" customHeight="1" s="2">
@@ -32087,8 +32151,11 @@
       <c r="HX45" s="1" t="n">
         <v>229</v>
       </c>
-      <c r="HY45" t="n">
+      <c r="HY45" s="1" t="n">
         <v>195</v>
+      </c>
+      <c r="HZ45" t="n">
+        <v>230</v>
       </c>
     </row>
     <row r="46" ht="13.8" customHeight="1" s="2">
@@ -32790,8 +32857,11 @@
       <c r="HX46" s="1" t="n">
         <v>275</v>
       </c>
-      <c r="HY46" t="n">
+      <c r="HY46" s="1" t="n">
         <v>252</v>
+      </c>
+      <c r="HZ46" t="n">
+        <v>266</v>
       </c>
     </row>
     <row r="47" ht="13.8" customHeight="1" s="2">
@@ -33493,8 +33563,11 @@
       <c r="HX47" s="1" t="n">
         <v>73.5</v>
       </c>
-      <c r="HY47" t="n">
+      <c r="HY47" s="1" t="n">
         <v>74.59999999999999</v>
+      </c>
+      <c r="HZ47" t="n">
+        <v>76.2</v>
       </c>
     </row>
     <row r="48" ht="13.8" customHeight="1" s="2">
@@ -34196,8 +34269,11 @@
       <c r="HX48" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="HY48" t="n">
+      <c r="HY48" s="1" t="n">
         <v>69</v>
+      </c>
+      <c r="HZ48" t="n">
+        <v>54</v>
       </c>
     </row>
     <row r="49" ht="13.8" customHeight="1" s="2">
@@ -34899,8 +34975,11 @@
       <c r="HX49" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="HY49" t="n">
+      <c r="HY49" s="1" t="n">
         <v>19</v>
+      </c>
+      <c r="HZ49" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="50" ht="13.8" customHeight="1" s="2">
@@ -35602,8 +35681,11 @@
       <c r="HX50" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="HY50" t="n">
+      <c r="HY50" s="1" t="n">
         <v>14</v>
+      </c>
+      <c r="HZ50" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="51" ht="13.8" customHeight="1" s="2">
@@ -36305,8 +36387,11 @@
       <c r="HX51" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="HY51" t="n">
+      <c r="HY51" s="1" t="n">
         <v>40</v>
+      </c>
+      <c r="HZ51" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="52" ht="13.8" customHeight="1" s="2">
@@ -37008,8 +37093,11 @@
       <c r="HX52" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="HY52" t="n">
+      <c r="HY52" s="1" t="n">
         <v>44</v>
+      </c>
+      <c r="HZ52" t="n">
+        <v>42</v>
       </c>
     </row>
     <row r="53" ht="13.8" customHeight="1" s="2">
@@ -37711,8 +37799,11 @@
       <c r="HX53" s="1" t="n">
         <v>56</v>
       </c>
-      <c r="HY53" t="n">
+      <c r="HY53" s="1" t="n">
         <v>32</v>
+      </c>
+      <c r="HZ53" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="54" ht="13.8" customHeight="1" s="2">
@@ -38414,8 +38505,11 @@
       <c r="HX54" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="HY54" t="n">
+      <c r="HY54" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="HZ54" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="55" ht="13.8" customHeight="1" s="2">
@@ -39117,8 +39211,11 @@
       <c r="HX55" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="HY55" t="n">
+      <c r="HY55" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="HZ55" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="56" ht="13.8" customHeight="1" s="2">
@@ -39820,8 +39917,11 @@
       <c r="HX56" s="1" t="n">
         <v>63.6</v>
       </c>
-      <c r="HY56" t="n">
+      <c r="HY56" s="1" t="n">
         <v>62.5</v>
+      </c>
+      <c r="HZ56" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="57" ht="13.8" customHeight="1" s="2">
@@ -40523,8 +40623,11 @@
       <c r="HX57" s="1" t="n">
         <v>218</v>
       </c>
-      <c r="HY57" t="n">
+      <c r="HY57" s="1" t="n">
         <v>206</v>
+      </c>
+      <c r="HZ57" t="n">
+        <v>246</v>
       </c>
     </row>
     <row r="58" ht="13.8" customHeight="1" s="2">
@@ -41226,8 +41329,11 @@
       <c r="HX58" s="1" t="n">
         <v>141</v>
       </c>
-      <c r="HY58" t="n">
+      <c r="HY58" s="1" t="n">
         <v>162</v>
+      </c>
+      <c r="HZ58" t="n">
+        <v>163</v>
       </c>
     </row>
     <row r="59" ht="13.8" customHeight="1" s="2">
@@ -41929,8 +42035,11 @@
       <c r="HX59" s="1" t="n">
         <v>359</v>
       </c>
-      <c r="HY59" t="n">
+      <c r="HY59" s="1" t="n">
         <v>368</v>
+      </c>
+      <c r="HZ59" t="n">
+        <v>409</v>
       </c>
     </row>
     <row r="60" ht="13.8" customHeight="1" s="2">
@@ -42632,8 +42741,11 @@
       <c r="HX60" s="1" t="n">
         <v>1.55</v>
       </c>
-      <c r="HY60" t="n">
+      <c r="HY60" s="1" t="n">
         <v>1.27</v>
+      </c>
+      <c r="HZ60" t="n">
+        <v>1.51</v>
       </c>
     </row>
     <row r="61" ht="13.8" customHeight="1" s="2">
@@ -43335,8 +43447,11 @@
       <c r="HX61" s="1" t="n">
         <v>102</v>
       </c>
-      <c r="HY61" t="n">
+      <c r="HY61" s="1" t="n">
         <v>86</v>
+      </c>
+      <c r="HZ61" t="n">
+        <v>112</v>
       </c>
     </row>
     <row r="62" ht="13.8" customHeight="1" s="2">
@@ -44038,8 +44153,11 @@
       <c r="HX62" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="HY62" t="n">
+      <c r="HY62" s="1" t="n">
         <v>51</v>
+      </c>
+      <c r="HZ62" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="63" ht="13.8" customHeight="1" s="2">
@@ -44741,8 +44859,11 @@
       <c r="HX63" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="HY63" t="n">
+      <c r="HY63" s="1" t="n">
         <v>27</v>
+      </c>
+      <c r="HZ63" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="64" ht="13.8" customHeight="1" s="2">
@@ -45444,8 +45565,11 @@
       <c r="HX64" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="HY64" t="n">
+      <c r="HY64" s="1" t="n">
         <v>30</v>
+      </c>
+      <c r="HZ64" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="65" ht="13.8" customHeight="1" s="2">
@@ -46147,8 +46271,11 @@
       <c r="HX65" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="HY65" t="n">
+      <c r="HY65" s="1" t="n">
         <v>25</v>
+      </c>
+      <c r="HZ65" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="66" ht="13.8" customHeight="1" s="2">
@@ -46850,7 +46977,10 @@
       <c r="HX66" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="HY66" t="n">
+      <c r="HY66" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="HZ66" t="n">
         <v>15</v>
       </c>
     </row>
@@ -47553,8 +47683,11 @@
       <c r="HX67" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="HY67" t="n">
+      <c r="HY67" s="1" t="n">
         <v>11</v>
+      </c>
+      <c r="HZ67" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="68" ht="13.8" customHeight="1" s="2">
@@ -48256,8 +48389,11 @@
       <c r="HX68" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="HY68" t="n">
+      <c r="HY68" s="1" t="n">
         <v>9</v>
+      </c>
+      <c r="HZ68" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="69" ht="13.8" customHeight="1" s="2">
@@ -48959,8 +49095,11 @@
       <c r="HX69" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="HY69" t="n">
+      <c r="HY69" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="HZ69" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="70" ht="13.8" customHeight="1" s="2">
@@ -49662,8 +49801,11 @@
       <c r="HX70" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="HY70" t="n">
+      <c r="HY70" s="1" t="n">
         <v>27</v>
+      </c>
+      <c r="HZ70" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="71" ht="13.8" customHeight="1" s="2">
@@ -50365,8 +50507,11 @@
       <c r="HX71" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="HY71" t="n">
+      <c r="HY71" s="1" t="n">
         <v>55.6</v>
+      </c>
+      <c r="HZ71" t="n">
+        <v>48.4</v>
       </c>
     </row>
     <row r="72" ht="13.8" customHeight="1" s="2">
@@ -51068,8 +51213,11 @@
       <c r="HX72" s="1" t="n">
         <v>29.92</v>
       </c>
-      <c r="HY72" t="n">
+      <c r="HY72" s="1" t="n">
         <v>24.53</v>
+      </c>
+      <c r="HZ72" t="n">
+        <v>27.27</v>
       </c>
     </row>
     <row r="73" ht="13.8" customHeight="1" s="2">
@@ -51771,8 +51919,11 @@
       <c r="HX73" s="1" t="n">
         <v>14.96</v>
       </c>
-      <c r="HY73" t="n">
+      <c r="HY73" s="1" t="n">
         <v>13.63</v>
+      </c>
+      <c r="HZ73" t="n">
+        <v>13.19</v>
       </c>
     </row>
     <row r="74" ht="13.8" customHeight="1" s="2">
@@ -52474,8 +52625,11 @@
       <c r="HX74" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="HY74" t="n">
+      <c r="HY74" s="1" t="n">
         <v>30</v>
+      </c>
+      <c r="HZ74" t="n">
+        <v>41</v>
       </c>
     </row>
     <row r="75" ht="13.8" customHeight="1" s="2">
@@ -53177,8 +53331,11 @@
       <c r="HX75" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="HY75" t="n">
+      <c r="HY75" s="1" t="n">
         <v>70</v>
+      </c>
+      <c r="HZ75" t="n">
+        <v>52</v>
       </c>
     </row>
     <row r="76" ht="13.8" customHeight="1" s="2">
@@ -53880,8 +54037,11 @@
       <c r="HX76" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="HY76" t="n">
+      <c r="HY76" s="1" t="n">
         <v>35</v>
+      </c>
+      <c r="HZ76" t="n">
+        <v>48</v>
       </c>
     </row>
     <row r="77" ht="13.8" customHeight="1" s="2">
@@ -54583,8 +54743,11 @@
       <c r="HX77" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="HY77" t="n">
+      <c r="HY77" s="1" t="n">
         <v>61</v>
+      </c>
+      <c r="HZ77" t="n">
+        <v>58</v>
       </c>
     </row>
     <row r="78" ht="13.8" customHeight="1" s="2">
@@ -55286,8 +55449,11 @@
       <c r="HX78" s="1" t="n">
         <v>2.25</v>
       </c>
-      <c r="HY78" t="n">
+      <c r="HY78" s="1" t="n">
         <v>2.26</v>
+      </c>
+      <c r="HZ78" t="n">
+        <v>1.87</v>
       </c>
     </row>
     <row r="79" ht="13.8" customHeight="1" s="2">
@@ -55989,8 +56155,11 @@
       <c r="HX79" s="1" t="n">
         <v>4.5</v>
       </c>
-      <c r="HY79" t="n">
+      <c r="HY79" s="1" t="n">
         <v>4.07</v>
+      </c>
+      <c r="HZ79" t="n">
+        <v>3.87</v>
       </c>
     </row>
     <row r="80" ht="13.8" customHeight="1" s="2">
@@ -56692,8 +56861,11 @@
       <c r="HX80" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="HY80" t="n">
+      <c r="HY80" s="1" t="n">
         <v>39.3</v>
+      </c>
+      <c r="HZ80" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="81" ht="13.8" customHeight="1" s="2">
@@ -57395,8 +57567,11 @@
       <c r="HX81" s="1" t="n">
         <v>22.2</v>
       </c>
-      <c r="HY81" t="n">
+      <c r="HY81" s="1" t="n">
         <v>24.6</v>
+      </c>
+      <c r="HZ81" t="n">
+        <v>25.9</v>
       </c>
     </row>
     <row r="82" ht="13.8" customHeight="1" s="2">
@@ -58098,8 +58273,11 @@
       <c r="HX82" s="1" t="n">
         <v>187.9</v>
       </c>
-      <c r="HY82" t="n">
+      <c r="HY82" s="1" t="n">
         <v>186.7</v>
+      </c>
+      <c r="HZ82" t="n">
+        <v>188.3</v>
       </c>
     </row>
     <row r="83" ht="13.8" customHeight="1" s="2">
@@ -58801,8 +58979,11 @@
       <c r="HX83" s="1" t="n">
         <v>88.59999999999999</v>
       </c>
-      <c r="HY83" t="n">
+      <c r="HY83" s="1" t="n">
         <v>85</v>
+      </c>
+      <c r="HZ83" t="n">
+        <v>86.40000000000001</v>
       </c>
     </row>
     <row r="84" ht="13.8" customHeight="1" s="2">
@@ -59504,8 +59685,11 @@
       <c r="HX84" s="1" t="n">
         <v>25.8</v>
       </c>
-      <c r="HY84" t="n">
+      <c r="HY84" s="1" t="n">
         <v>25.74</v>
+      </c>
+      <c r="HZ84" t="n">
+        <v>25.8</v>
       </c>
     </row>
     <row r="85" ht="13.8" customHeight="1" s="2">
@@ -60207,8 +60391,11 @@
       <c r="HX85" s="1" t="n">
         <v>85.3</v>
       </c>
-      <c r="HY85" t="n">
+      <c r="HY85" s="1" t="n">
         <v>102.9</v>
+      </c>
+      <c r="HZ85" t="n">
+        <v>77.5</v>
       </c>
     </row>
     <row r="86" ht="13.8" customHeight="1" s="2">
@@ -60910,8 +61097,11 @@
       <c r="HX86" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="HY86" t="n">
+      <c r="HY86" s="1" t="n">
         <v>9</v>
+      </c>
+      <c r="HZ86" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="87" ht="13.8" customHeight="1" s="2">
@@ -61613,8 +61803,11 @@
       <c r="HX87" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="HY87" t="n">
+      <c r="HY87" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="HZ87" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="88" ht="13.8" customHeight="1" s="2">
@@ -62316,8 +62509,11 @@
       <c r="HX88" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="HY88" t="n">
+      <c r="HY88" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="HZ88" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="89" ht="13.8" customHeight="1" s="2">
@@ -63019,8 +63215,11 @@
       <c r="HX89" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="HY89" t="n">
+      <c r="HY89" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="HZ89" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="90" ht="13.8" customHeight="1" s="2">
@@ -63722,8 +63921,11 @@
       <c r="HX90" s="1" t="n">
         <v>152</v>
       </c>
-      <c r="HY90" t="n">
+      <c r="HY90" s="1" t="n">
         <v>146</v>
+      </c>
+      <c r="HZ90" t="n">
+        <v>135</v>
       </c>
     </row>
     <row r="91" ht="13.8" customHeight="1" s="2">
@@ -64425,8 +64627,11 @@
       <c r="HX91" s="1" t="n">
         <v>210</v>
       </c>
-      <c r="HY91" t="n">
+      <c r="HY91" s="1" t="n">
         <v>214</v>
+      </c>
+      <c r="HZ91" t="n">
+        <v>262</v>
       </c>
     </row>
     <row r="92" ht="13.8" customHeight="1" s="2">
@@ -65128,8 +65333,11 @@
       <c r="HX92" s="1" t="n">
         <v>266</v>
       </c>
-      <c r="HY92" t="n">
+      <c r="HY92" s="1" t="n">
         <v>260</v>
+      </c>
+      <c r="HZ92" t="n">
+        <v>309</v>
       </c>
     </row>
     <row r="93" ht="13.8" customHeight="1" s="2">
@@ -65831,8 +66039,11 @@
       <c r="HX93" s="1" t="n">
         <v>74.09999999999999</v>
       </c>
-      <c r="HY93" t="n">
+      <c r="HY93" s="1" t="n">
         <v>70.7</v>
+      </c>
+      <c r="HZ93" t="n">
+        <v>75.59999999999999</v>
       </c>
     </row>
     <row r="94" ht="13.8" customHeight="1" s="2">
@@ -66534,8 +66745,11 @@
       <c r="HX94" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="HY94" t="n">
+      <c r="HY94" s="1" t="n">
         <v>70</v>
+      </c>
+      <c r="HZ94" t="n">
+        <v>52</v>
       </c>
     </row>
     <row r="95" ht="13.8" customHeight="1" s="2">
@@ -67237,8 +67451,11 @@
       <c r="HX95" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="HY95" t="n">
+      <c r="HY95" s="1" t="n">
         <v>16</v>
+      </c>
+      <c r="HZ95" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="96" ht="13.8" customHeight="1" s="2">
@@ -67940,8 +68157,11 @@
       <c r="HX96" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="HY96" t="n">
+      <c r="HY96" s="1" t="n">
         <v>18</v>
+      </c>
+      <c r="HZ96" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="97" ht="13.8" customHeight="1" s="2">
@@ -68643,8 +68863,11 @@
       <c r="HX97" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="HY97" t="n">
+      <c r="HY97" s="1" t="n">
         <v>30</v>
+      </c>
+      <c r="HZ97" t="n">
+        <v>41</v>
       </c>
     </row>
     <row r="98" ht="13.8" customHeight="1" s="2">
@@ -69346,8 +69569,11 @@
       <c r="HX98" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="HY98" t="n">
+      <c r="HY98" s="1" t="n">
         <v>35</v>
+      </c>
+      <c r="HZ98" t="n">
+        <v>48</v>
       </c>
     </row>
     <row r="99" ht="13.8" customHeight="1" s="2">
@@ -70049,8 +70275,11 @@
       <c r="HX99" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="HY99" t="n">
+      <c r="HY99" s="1" t="n">
         <v>39</v>
+      </c>
+      <c r="HZ99" t="n">
+        <v>57</v>
       </c>
     </row>
     <row r="100" ht="13.8" customHeight="1" s="2">
@@ -70752,8 +70981,11 @@
       <c r="HX100" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="HY100" t="n">
+      <c r="HY100" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="HZ100" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="101" ht="13.8" customHeight="1" s="2">
@@ -71455,8 +71687,11 @@
       <c r="HX101" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="HY101" t="n">
+      <c r="HY101" s="1" t="n">
         <v>11</v>
+      </c>
+      <c r="HZ101" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="102" ht="13.8" customHeight="1" s="2">
@@ -72158,8 +72393,11 @@
       <c r="HX102" s="1" t="n">
         <v>91.7</v>
       </c>
-      <c r="HY102" t="n">
+      <c r="HY102" s="1" t="n">
         <v>73.3</v>
+      </c>
+      <c r="HZ102" t="n">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
round 9 2021 predictions
</commit_message>
<xml_diff>
--- a/django_AFL_ML/Data/Adelaide_stats.xlsx
+++ b/django_AFL_ML/Data/Adelaide_stats.xlsx
@@ -377,7 +377,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:HZ102"/>
+  <dimension ref="A1:IA102"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="GZ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="HA23" activeCellId="0" sqref="HA23"/>
@@ -1090,8 +1090,11 @@
       <c r="HY1" s="1" t="n">
         <v>10378</v>
       </c>
-      <c r="HZ1" t="n">
+      <c r="HZ1" s="1" t="n">
         <v>10388</v>
+      </c>
+      <c r="IA1" t="n">
+        <v>10397</v>
       </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="2">
@@ -1796,7 +1799,10 @@
       <c r="HY2" s="1" t="n">
         <v>2021</v>
       </c>
-      <c r="HZ2" t="n">
+      <c r="HZ2" s="1" t="n">
+        <v>2021</v>
+      </c>
+      <c r="IA2" t="n">
         <v>2021</v>
       </c>
     </row>
@@ -2502,8 +2508,11 @@
       <c r="HY3" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="HZ3" t="n">
+      <c r="HZ3" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="IA3" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="2">
@@ -3208,8 +3217,11 @@
       <c r="HY4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="HZ4" t="n">
+      <c r="HZ4" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="IA4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5" ht="13.8" customHeight="1" s="2">
@@ -3914,8 +3926,11 @@
       <c r="HY5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="HZ5" t="n">
+      <c r="HZ5" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="IA5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6" ht="13.8" customHeight="1" s="2">
@@ -4620,8 +4635,11 @@
       <c r="HY6" s="1" t="n">
         <v>99</v>
       </c>
-      <c r="HZ6" t="n">
+      <c r="HZ6" s="1" t="n">
         <v>39</v>
+      </c>
+      <c r="IA6" t="n">
+        <v>38</v>
       </c>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="2">
@@ -5326,8 +5344,11 @@
       <c r="HY7" s="1" t="n">
         <v>102</v>
       </c>
-      <c r="HZ7" t="n">
+      <c r="HZ7" s="1" t="n">
         <v>106</v>
+      </c>
+      <c r="IA7" t="n">
+        <v>87</v>
       </c>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="2">
@@ -6032,8 +6053,11 @@
       <c r="HY8" s="1" t="n">
         <v>-3</v>
       </c>
-      <c r="HZ8" t="n">
+      <c r="HZ8" s="1" t="n">
         <v>-67</v>
+      </c>
+      <c r="IA8" t="n">
+        <v>-49</v>
       </c>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="2">
@@ -6738,7 +6762,10 @@
       <c r="HY9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="HZ9" t="n">
+      <c r="HZ9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="IA9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7444,8 +7471,11 @@
       <c r="HY10" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="HZ10" t="n">
+      <c r="HZ10" s="1" t="n">
         <v>9</v>
+      </c>
+      <c r="IA10" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="11" ht="13.8" customHeight="1" s="2">
@@ -8150,7 +8180,10 @@
       <c r="HY11" s="1" t="n">
         <v>197</v>
       </c>
-      <c r="HZ11" t="n">
+      <c r="HZ11" s="1" t="n">
+        <v>197</v>
+      </c>
+      <c r="IA11" t="n">
         <v>197</v>
       </c>
     </row>
@@ -8856,8 +8889,11 @@
       <c r="HY12" s="1" t="n">
         <v>141</v>
       </c>
-      <c r="HZ12" t="n">
+      <c r="HZ12" s="1" t="n">
         <v>152</v>
+      </c>
+      <c r="IA12" t="n">
+        <v>125</v>
       </c>
     </row>
     <row r="13" ht="13.8" customHeight="1" s="2">
@@ -9562,8 +9598,11 @@
       <c r="HY13" s="1" t="n">
         <v>338</v>
       </c>
-      <c r="HZ13" t="n">
+      <c r="HZ13" s="1" t="n">
         <v>349</v>
+      </c>
+      <c r="IA13" t="n">
+        <v>322</v>
       </c>
     </row>
     <row r="14" ht="13.8" customHeight="1" s="2">
@@ -10268,8 +10307,11 @@
       <c r="HY14" s="1" t="n">
         <v>1.4</v>
       </c>
-      <c r="HZ14" t="n">
+      <c r="HZ14" s="1" t="n">
         <v>1.3</v>
+      </c>
+      <c r="IA14" t="n">
+        <v>1.58</v>
       </c>
     </row>
     <row r="15" ht="13.8" customHeight="1" s="2">
@@ -10974,8 +11016,11 @@
       <c r="HY15" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="HZ15" t="n">
+      <c r="HZ15" s="1" t="n">
         <v>86</v>
+      </c>
+      <c r="IA15" t="n">
+        <v>46</v>
       </c>
     </row>
     <row r="16" ht="13.8" customHeight="1" s="2">
@@ -11680,8 +11725,11 @@
       <c r="HY16" s="1" t="n">
         <v>58</v>
       </c>
-      <c r="HZ16" t="n">
+      <c r="HZ16" s="1" t="n">
         <v>43</v>
+      </c>
+      <c r="IA16" t="n">
+        <v>76</v>
       </c>
     </row>
     <row r="17" ht="13.8" customHeight="1" s="2">
@@ -12386,8 +12434,11 @@
       <c r="HY17" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="HZ17" t="n">
+      <c r="HZ17" s="1" t="n">
         <v>29</v>
+      </c>
+      <c r="IA17" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="18" ht="13.8" customHeight="1" s="2">
@@ -13092,8 +13143,11 @@
       <c r="HY18" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="HZ18" t="n">
+      <c r="HZ18" s="1" t="n">
         <v>17</v>
+      </c>
+      <c r="IA18" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="19" ht="13.8" customHeight="1" s="2">
@@ -13798,7 +13852,10 @@
       <c r="HY19" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="HZ19" t="n">
+      <c r="HZ19" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="IA19" t="n">
         <v>18</v>
       </c>
     </row>
@@ -14504,8 +14561,11 @@
       <c r="HY20" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="HZ20" t="n">
+      <c r="HZ20" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="IA20" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="21" ht="13.8" customHeight="1" s="2">
@@ -15210,8 +15270,11 @@
       <c r="HY21" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="HZ21" t="n">
+      <c r="HZ21" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="IA21" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="22" ht="13.8" customHeight="1" s="2">
@@ -15916,8 +15979,11 @@
       <c r="HY22" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="HZ22" t="n">
+      <c r="HZ22" s="1" t="n">
         <v>9</v>
+      </c>
+      <c r="IA22" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="23" ht="13.8" customHeight="1" s="2">
@@ -16622,8 +16688,11 @@
       <c r="HY23" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="HZ23" t="n">
+      <c r="HZ23" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="IA23" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="24" ht="13.8" customHeight="1" s="2">
@@ -17328,8 +17397,11 @@
       <c r="HY24" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="HZ24" t="n">
+      <c r="HZ24" s="1" t="n">
         <v>19</v>
+      </c>
+      <c r="IA24" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="25" ht="13.8" customHeight="1" s="2">
@@ -18034,8 +18106,11 @@
       <c r="HY25" s="1" t="n">
         <v>84.2</v>
       </c>
-      <c r="HZ25" t="n">
+      <c r="HZ25" s="1" t="n">
         <v>21.1</v>
+      </c>
+      <c r="IA25" t="n">
+        <v>38.5</v>
       </c>
     </row>
     <row r="26" ht="13.8" customHeight="1" s="2">
@@ -18740,8 +18815,11 @@
       <c r="HY26" s="1" t="n">
         <v>21.12</v>
       </c>
-      <c r="HZ26" t="n">
+      <c r="HZ26" s="1" t="n">
         <v>87.25</v>
+      </c>
+      <c r="IA26" t="n">
+        <v>64.40000000000001</v>
       </c>
     </row>
     <row r="27" ht="13.8" customHeight="1" s="2">
@@ -19446,8 +19524,11 @@
       <c r="HY27" s="1" t="n">
         <v>17.79</v>
       </c>
-      <c r="HZ27" t="n">
+      <c r="HZ27" s="1" t="n">
         <v>18.37</v>
+      </c>
+      <c r="IA27" t="n">
+        <v>24.77</v>
       </c>
     </row>
     <row r="28" ht="13.8" customHeight="1" s="2">
@@ -20152,8 +20233,11 @@
       <c r="HY28" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="HZ28" t="n">
+      <c r="HZ28" s="1" t="n">
         <v>17</v>
+      </c>
+      <c r="IA28" t="n">
+        <v>38</v>
       </c>
     </row>
     <row r="29" ht="13.8" customHeight="1" s="2">
@@ -20858,8 +20942,11 @@
       <c r="HY29" s="1" t="n">
         <v>69</v>
       </c>
-      <c r="HZ29" t="n">
+      <c r="HZ29" s="1" t="n">
         <v>54</v>
+      </c>
+      <c r="IA29" t="n">
+        <v>59</v>
       </c>
     </row>
     <row r="30" ht="13.8" customHeight="1" s="2">
@@ -21564,8 +21651,11 @@
       <c r="HY30" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="HZ30" t="n">
+      <c r="HZ30" s="1" t="n">
         <v>42</v>
+      </c>
+      <c r="IA30" t="n">
+        <v>48</v>
       </c>
     </row>
     <row r="31" ht="13.8" customHeight="1" s="2">
@@ -22270,8 +22360,11 @@
       <c r="HY31" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="HZ31" t="n">
+      <c r="HZ31" s="1" t="n">
         <v>52</v>
+      </c>
+      <c r="IA31" t="n">
+        <v>48</v>
       </c>
     </row>
     <row r="32" ht="13.8" customHeight="1" s="2">
@@ -22976,8 +23069,11 @@
       <c r="HY32" s="1" t="n">
         <v>2.68</v>
       </c>
-      <c r="HZ32" t="n">
+      <c r="HZ32" s="1" t="n">
         <v>2.74</v>
+      </c>
+      <c r="IA32" t="n">
+        <v>3.69</v>
       </c>
     </row>
     <row r="33" ht="13.8" customHeight="1" s="2">
@@ -23682,8 +23778,11 @@
       <c r="HY33" s="1" t="n">
         <v>3.19</v>
       </c>
-      <c r="HZ33" t="n">
+      <c r="HZ33" s="1" t="n">
         <v>13</v>
+      </c>
+      <c r="IA33" t="n">
+        <v>9.6</v>
       </c>
     </row>
     <row r="34" ht="13.8" customHeight="1" s="2">
@@ -24388,8 +24487,11 @@
       <c r="HY34" s="1" t="n">
         <v>37.3</v>
       </c>
-      <c r="HZ34" t="n">
+      <c r="HZ34" s="1" t="n">
         <v>25</v>
+      </c>
+      <c r="IA34" t="n">
+        <v>27.1</v>
       </c>
     </row>
     <row r="35" ht="13.8" customHeight="1" s="2">
@@ -25094,8 +25196,11 @@
       <c r="HY35" s="1" t="n">
         <v>31.4</v>
       </c>
-      <c r="HZ35" t="n">
+      <c r="HZ35" s="1" t="n">
         <v>7.7</v>
+      </c>
+      <c r="IA35" t="n">
+        <v>10.4</v>
       </c>
     </row>
     <row r="36" ht="13.8" customHeight="1" s="2">
@@ -25800,8 +25905,11 @@
       <c r="HY36" s="1" t="n">
         <v>187.6</v>
       </c>
-      <c r="HZ36" t="n">
+      <c r="HZ36" s="1" t="n">
         <v>187.1</v>
+      </c>
+      <c r="IA36" t="n">
+        <v>186.7</v>
       </c>
     </row>
     <row r="37" ht="13.8" customHeight="1" s="2">
@@ -26506,8 +26614,11 @@
       <c r="HY37" s="1" t="n">
         <v>84.90000000000001</v>
       </c>
-      <c r="HZ37" t="n">
+      <c r="HZ37" s="1" t="n">
         <v>85</v>
+      </c>
+      <c r="IA37" t="n">
+        <v>84.59999999999999</v>
       </c>
     </row>
     <row r="38" ht="13.8" customHeight="1" s="2">
@@ -27212,8 +27323,11 @@
       <c r="HY38" s="1" t="n">
         <v>24.16</v>
       </c>
-      <c r="HZ38" t="n">
+      <c r="HZ38" s="1" t="n">
         <v>24</v>
+      </c>
+      <c r="IA38" t="n">
+        <v>24.49</v>
       </c>
     </row>
     <row r="39" ht="13.8" customHeight="1" s="2">
@@ -27918,8 +28032,11 @@
       <c r="HY39" s="1" t="n">
         <v>63.1</v>
       </c>
-      <c r="HZ39" t="n">
+      <c r="HZ39" s="1" t="n">
         <v>60.9</v>
+      </c>
+      <c r="IA39" t="n">
+        <v>76.2</v>
       </c>
     </row>
     <row r="40" ht="13.8" customHeight="1" s="2">
@@ -28624,8 +28741,11 @@
       <c r="HY40" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="HZ40" t="n">
+      <c r="HZ40" s="1" t="n">
         <v>14</v>
+      </c>
+      <c r="IA40" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="41" ht="13.8" customHeight="1" s="2">
@@ -29330,7 +29450,10 @@
       <c r="HY41" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="HZ41" t="n">
+      <c r="HZ41" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="IA41" t="n">
         <v>3</v>
       </c>
     </row>
@@ -30036,7 +30159,10 @@
       <c r="HY42" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="HZ42" t="n">
+      <c r="HZ42" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="IA42" t="n">
         <v>1</v>
       </c>
     </row>
@@ -30742,8 +30868,11 @@
       <c r="HY43" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="HZ43" t="n">
+      <c r="HZ43" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="IA43" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="44" ht="13.8" customHeight="1" s="2">
@@ -31448,8 +31577,11 @@
       <c r="HY44" s="1" t="n">
         <v>144</v>
       </c>
-      <c r="HZ44" t="n">
+      <c r="HZ44" s="1" t="n">
         <v>114</v>
+      </c>
+      <c r="IA44" t="n">
+        <v>159</v>
       </c>
     </row>
     <row r="45" ht="13.8" customHeight="1" s="2">
@@ -32154,8 +32286,11 @@
       <c r="HY45" s="1" t="n">
         <v>195</v>
       </c>
-      <c r="HZ45" t="n">
+      <c r="HZ45" s="1" t="n">
         <v>230</v>
+      </c>
+      <c r="IA45" t="n">
+        <v>145</v>
       </c>
     </row>
     <row r="46" ht="13.8" customHeight="1" s="2">
@@ -32860,8 +32995,11 @@
       <c r="HY46" s="1" t="n">
         <v>252</v>
       </c>
-      <c r="HZ46" t="n">
+      <c r="HZ46" s="1" t="n">
         <v>266</v>
+      </c>
+      <c r="IA46" t="n">
+        <v>199</v>
       </c>
     </row>
     <row r="47" ht="13.8" customHeight="1" s="2">
@@ -33566,8 +33704,11 @@
       <c r="HY47" s="1" t="n">
         <v>74.59999999999999</v>
       </c>
-      <c r="HZ47" t="n">
+      <c r="HZ47" s="1" t="n">
         <v>76.2</v>
+      </c>
+      <c r="IA47" t="n">
+        <v>61.8</v>
       </c>
     </row>
     <row r="48" ht="13.8" customHeight="1" s="2">
@@ -34272,8 +34413,11 @@
       <c r="HY48" s="1" t="n">
         <v>69</v>
       </c>
-      <c r="HZ48" t="n">
+      <c r="HZ48" s="1" t="n">
         <v>54</v>
+      </c>
+      <c r="IA48" t="n">
+        <v>59</v>
       </c>
     </row>
     <row r="49" ht="13.8" customHeight="1" s="2">
@@ -34978,8 +35122,11 @@
       <c r="HY49" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="HZ49" t="n">
+      <c r="HZ49" s="1" t="n">
         <v>9</v>
+      </c>
+      <c r="IA49" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="50" ht="13.8" customHeight="1" s="2">
@@ -35684,8 +35831,11 @@
       <c r="HY50" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="HZ50" t="n">
+      <c r="HZ50" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="IA50" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="51" ht="13.8" customHeight="1" s="2">
@@ -36390,8 +36540,11 @@
       <c r="HY51" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="HZ51" t="n">
+      <c r="HZ51" s="1" t="n">
         <v>17</v>
+      </c>
+      <c r="IA51" t="n">
+        <v>38</v>
       </c>
     </row>
     <row r="52" ht="13.8" customHeight="1" s="2">
@@ -37096,8 +37249,11 @@
       <c r="HY52" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="HZ52" t="n">
+      <c r="HZ52" s="1" t="n">
         <v>42</v>
+      </c>
+      <c r="IA52" t="n">
+        <v>48</v>
       </c>
     </row>
     <row r="53" ht="13.8" customHeight="1" s="2">
@@ -37802,8 +37958,11 @@
       <c r="HY53" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="HZ53" t="n">
+      <c r="HZ53" s="1" t="n">
         <v>44</v>
+      </c>
+      <c r="IA53" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="54" ht="13.8" customHeight="1" s="2">
@@ -38508,8 +38667,11 @@
       <c r="HY54" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="HZ54" t="n">
+      <c r="HZ54" s="1" t="n">
         <v>9</v>
+      </c>
+      <c r="IA54" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="55" ht="13.8" customHeight="1" s="2">
@@ -39214,8 +39376,11 @@
       <c r="HY55" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="HZ55" t="n">
+      <c r="HZ55" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="IA55" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="56" ht="13.8" customHeight="1" s="2">
@@ -39920,8 +40085,11 @@
       <c r="HY56" s="1" t="n">
         <v>62.5</v>
       </c>
-      <c r="HZ56" t="n">
+      <c r="HZ56" s="1" t="n">
         <v>50</v>
+      </c>
+      <c r="IA56" t="n">
+        <v>80</v>
       </c>
     </row>
     <row r="57" ht="13.8" customHeight="1" s="2">
@@ -40626,8 +40794,11 @@
       <c r="HY57" s="1" t="n">
         <v>206</v>
       </c>
-      <c r="HZ57" t="n">
+      <c r="HZ57" s="1" t="n">
         <v>246</v>
+      </c>
+      <c r="IA57" t="n">
+        <v>257</v>
       </c>
     </row>
     <row r="58" ht="13.8" customHeight="1" s="2">
@@ -41332,8 +41503,11 @@
       <c r="HY58" s="1" t="n">
         <v>162</v>
       </c>
-      <c r="HZ58" t="n">
+      <c r="HZ58" s="1" t="n">
         <v>163</v>
+      </c>
+      <c r="IA58" t="n">
+        <v>161</v>
       </c>
     </row>
     <row r="59" ht="13.8" customHeight="1" s="2">
@@ -42038,8 +42212,11 @@
       <c r="HY59" s="1" t="n">
         <v>368</v>
       </c>
-      <c r="HZ59" t="n">
+      <c r="HZ59" s="1" t="n">
         <v>409</v>
+      </c>
+      <c r="IA59" t="n">
+        <v>418</v>
       </c>
     </row>
     <row r="60" ht="13.8" customHeight="1" s="2">
@@ -42744,8 +42921,11 @@
       <c r="HY60" s="1" t="n">
         <v>1.27</v>
       </c>
-      <c r="HZ60" t="n">
+      <c r="HZ60" s="1" t="n">
         <v>1.51</v>
+      </c>
+      <c r="IA60" t="n">
+        <v>1.6</v>
       </c>
     </row>
     <row r="61" ht="13.8" customHeight="1" s="2">
@@ -43450,8 +43630,11 @@
       <c r="HY61" s="1" t="n">
         <v>86</v>
       </c>
-      <c r="HZ61" t="n">
+      <c r="HZ61" s="1" t="n">
         <v>112</v>
+      </c>
+      <c r="IA61" t="n">
+        <v>84</v>
       </c>
     </row>
     <row r="62" ht="13.8" customHeight="1" s="2">
@@ -44156,8 +44339,11 @@
       <c r="HY62" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="HZ62" t="n">
+      <c r="HZ62" s="1" t="n">
         <v>60</v>
+      </c>
+      <c r="IA62" t="n">
+        <v>85</v>
       </c>
     </row>
     <row r="63" ht="13.8" customHeight="1" s="2">
@@ -44862,8 +45048,11 @@
       <c r="HY63" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="HZ63" t="n">
+      <c r="HZ63" s="1" t="n">
         <v>24</v>
+      </c>
+      <c r="IA63" t="n">
+        <v>42</v>
       </c>
     </row>
     <row r="64" ht="13.8" customHeight="1" s="2">
@@ -45568,7 +45757,10 @@
       <c r="HY64" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="HZ64" t="n">
+      <c r="HZ64" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="IA64" t="n">
         <v>18</v>
       </c>
     </row>
@@ -46274,8 +46466,11 @@
       <c r="HY65" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="HZ65" t="n">
+      <c r="HZ65" s="1" t="n">
         <v>17</v>
+      </c>
+      <c r="IA65" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="66" ht="13.8" customHeight="1" s="2">
@@ -46980,8 +47175,11 @@
       <c r="HY66" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="HZ66" t="n">
+      <c r="HZ66" s="1" t="n">
         <v>15</v>
+      </c>
+      <c r="IA66" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="67" ht="13.8" customHeight="1" s="2">
@@ -47686,8 +47884,11 @@
       <c r="HY67" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="HZ67" t="n">
+      <c r="HZ67" s="1" t="n">
         <v>12</v>
+      </c>
+      <c r="IA67" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="68" ht="13.8" customHeight="1" s="2">
@@ -48392,8 +48593,11 @@
       <c r="HY68" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="HZ68" t="n">
+      <c r="HZ68" s="1" t="n">
         <v>14</v>
+      </c>
+      <c r="IA68" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="69" ht="13.8" customHeight="1" s="2">
@@ -49098,8 +49302,11 @@
       <c r="HY69" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="HZ69" t="n">
+      <c r="HZ69" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="IA69" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="70" ht="13.8" customHeight="1" s="2">
@@ -49804,8 +50011,11 @@
       <c r="HY70" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="HZ70" t="n">
+      <c r="HZ70" s="1" t="n">
         <v>31</v>
+      </c>
+      <c r="IA70" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="71" ht="13.8" customHeight="1" s="2">
@@ -50510,8 +50720,11 @@
       <c r="HY71" s="1" t="n">
         <v>55.6</v>
       </c>
-      <c r="HZ71" t="n">
+      <c r="HZ71" s="1" t="n">
         <v>48.4</v>
+      </c>
+      <c r="IA71" t="n">
+        <v>44.4</v>
       </c>
     </row>
     <row r="72" ht="13.8" customHeight="1" s="2">
@@ -51216,8 +51429,11 @@
       <c r="HY72" s="1" t="n">
         <v>24.53</v>
       </c>
-      <c r="HZ72" t="n">
+      <c r="HZ72" s="1" t="n">
         <v>27.27</v>
+      </c>
+      <c r="IA72" t="n">
+        <v>34.83</v>
       </c>
     </row>
     <row r="73" ht="13.8" customHeight="1" s="2">
@@ -51922,8 +52138,11 @@
       <c r="HY73" s="1" t="n">
         <v>13.63</v>
       </c>
-      <c r="HZ73" t="n">
+      <c r="HZ73" s="1" t="n">
         <v>13.19</v>
+      </c>
+      <c r="IA73" t="n">
+        <v>15.48</v>
       </c>
     </row>
     <row r="74" ht="13.8" customHeight="1" s="2">
@@ -52628,8 +52847,11 @@
       <c r="HY74" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="HZ74" t="n">
+      <c r="HZ74" s="1" t="n">
         <v>41</v>
+      </c>
+      <c r="IA74" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="75" ht="13.8" customHeight="1" s="2">
@@ -53334,8 +53556,11 @@
       <c r="HY75" s="1" t="n">
         <v>70</v>
       </c>
-      <c r="HZ75" t="n">
+      <c r="HZ75" s="1" t="n">
         <v>52</v>
+      </c>
+      <c r="IA75" t="n">
+        <v>65</v>
       </c>
     </row>
     <row r="76" ht="13.8" customHeight="1" s="2">
@@ -54040,8 +54265,11 @@
       <c r="HY76" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="HZ76" t="n">
+      <c r="HZ76" s="1" t="n">
         <v>48</v>
+      </c>
+      <c r="IA76" t="n">
+        <v>43</v>
       </c>
     </row>
     <row r="77" ht="13.8" customHeight="1" s="2">
@@ -54746,8 +54974,11 @@
       <c r="HY77" s="1" t="n">
         <v>61</v>
       </c>
-      <c r="HZ77" t="n">
+      <c r="HZ77" s="1" t="n">
         <v>58</v>
+      </c>
+      <c r="IA77" t="n">
+        <v>63</v>
       </c>
     </row>
     <row r="78" ht="13.8" customHeight="1" s="2">
@@ -55452,8 +55683,11 @@
       <c r="HY78" s="1" t="n">
         <v>2.26</v>
       </c>
-      <c r="HZ78" t="n">
+      <c r="HZ78" s="1" t="n">
         <v>1.87</v>
+      </c>
+      <c r="IA78" t="n">
+        <v>2.33</v>
       </c>
     </row>
     <row r="79" ht="13.8" customHeight="1" s="2">
@@ -56158,8 +56392,11 @@
       <c r="HY79" s="1" t="n">
         <v>4.07</v>
       </c>
-      <c r="HZ79" t="n">
+      <c r="HZ79" s="1" t="n">
         <v>3.87</v>
+      </c>
+      <c r="IA79" t="n">
+        <v>5.25</v>
       </c>
     </row>
     <row r="80" ht="13.8" customHeight="1" s="2">
@@ -56864,8 +57101,11 @@
       <c r="HY80" s="1" t="n">
         <v>39.3</v>
       </c>
-      <c r="HZ80" t="n">
+      <c r="HZ80" s="1" t="n">
         <v>50</v>
+      </c>
+      <c r="IA80" t="n">
+        <v>38.1</v>
       </c>
     </row>
     <row r="81" ht="13.8" customHeight="1" s="2">
@@ -57570,8 +57810,11 @@
       <c r="HY81" s="1" t="n">
         <v>24.6</v>
       </c>
-      <c r="HZ81" t="n">
+      <c r="HZ81" s="1" t="n">
         <v>25.9</v>
+      </c>
+      <c r="IA81" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="82" ht="13.8" customHeight="1" s="2">
@@ -58276,8 +58519,11 @@
       <c r="HY82" s="1" t="n">
         <v>186.7</v>
       </c>
-      <c r="HZ82" t="n">
+      <c r="HZ82" s="1" t="n">
         <v>188.3</v>
+      </c>
+      <c r="IA82" t="n">
+        <v>187.5</v>
       </c>
     </row>
     <row r="83" ht="13.8" customHeight="1" s="2">
@@ -58982,8 +59228,11 @@
       <c r="HY83" s="1" t="n">
         <v>85</v>
       </c>
-      <c r="HZ83" t="n">
+      <c r="HZ83" s="1" t="n">
         <v>86.40000000000001</v>
+      </c>
+      <c r="IA83" t="n">
+        <v>83.5</v>
       </c>
     </row>
     <row r="84" ht="13.8" customHeight="1" s="2">
@@ -59688,7 +59937,10 @@
       <c r="HY84" s="1" t="n">
         <v>25.74</v>
       </c>
-      <c r="HZ84" t="n">
+      <c r="HZ84" s="1" t="n">
+        <v>25.8</v>
+      </c>
+      <c r="IA84" t="n">
         <v>25.8</v>
       </c>
     </row>
@@ -60394,8 +60646,11 @@
       <c r="HY85" s="1" t="n">
         <v>102.9</v>
       </c>
-      <c r="HZ85" t="n">
+      <c r="HZ85" s="1" t="n">
         <v>77.5</v>
+      </c>
+      <c r="IA85" t="n">
+        <v>103.7</v>
       </c>
     </row>
     <row r="86" ht="13.8" customHeight="1" s="2">
@@ -61100,8 +61355,11 @@
       <c r="HY86" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="HZ86" t="n">
+      <c r="HZ86" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="IA86" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="87" ht="13.8" customHeight="1" s="2">
@@ -61806,8 +62064,11 @@
       <c r="HY87" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="HZ87" t="n">
+      <c r="HZ87" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="IA87" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="88" ht="13.8" customHeight="1" s="2">
@@ -62512,8 +62773,11 @@
       <c r="HY88" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="HZ88" t="n">
+      <c r="HZ88" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="IA88" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="89" ht="13.8" customHeight="1" s="2">
@@ -63218,8 +63482,11 @@
       <c r="HY89" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="HZ89" t="n">
+      <c r="HZ89" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="IA89" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="90" ht="13.8" customHeight="1" s="2">
@@ -63924,8 +64191,11 @@
       <c r="HY90" s="1" t="n">
         <v>146</v>
       </c>
-      <c r="HZ90" t="n">
+      <c r="HZ90" s="1" t="n">
         <v>135</v>
+      </c>
+      <c r="IA90" t="n">
+        <v>170</v>
       </c>
     </row>
     <row r="91" ht="13.8" customHeight="1" s="2">
@@ -64630,8 +64900,11 @@
       <c r="HY91" s="1" t="n">
         <v>214</v>
       </c>
-      <c r="HZ91" t="n">
+      <c r="HZ91" s="1" t="n">
         <v>262</v>
+      </c>
+      <c r="IA91" t="n">
+        <v>235</v>
       </c>
     </row>
     <row r="92" ht="13.8" customHeight="1" s="2">
@@ -65336,8 +65609,11 @@
       <c r="HY92" s="1" t="n">
         <v>260</v>
       </c>
-      <c r="HZ92" t="n">
+      <c r="HZ92" s="1" t="n">
         <v>309</v>
+      </c>
+      <c r="IA92" t="n">
+        <v>290</v>
       </c>
     </row>
     <row r="93" ht="13.8" customHeight="1" s="2">
@@ -66042,8 +66318,11 @@
       <c r="HY93" s="1" t="n">
         <v>70.7</v>
       </c>
-      <c r="HZ93" t="n">
+      <c r="HZ93" s="1" t="n">
         <v>75.59999999999999</v>
+      </c>
+      <c r="IA93" t="n">
+        <v>69.40000000000001</v>
       </c>
     </row>
     <row r="94" ht="13.8" customHeight="1" s="2">
@@ -66748,8 +67027,11 @@
       <c r="HY94" s="1" t="n">
         <v>70</v>
       </c>
-      <c r="HZ94" t="n">
+      <c r="HZ94" s="1" t="n">
         <v>52</v>
+      </c>
+      <c r="IA94" t="n">
+        <v>65</v>
       </c>
     </row>
     <row r="95" ht="13.8" customHeight="1" s="2">
@@ -67454,8 +67736,11 @@
       <c r="HY95" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="HZ95" t="n">
+      <c r="HZ95" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="IA95" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="96" ht="13.8" customHeight="1" s="2">
@@ -68160,8 +68445,11 @@
       <c r="HY96" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="HZ96" t="n">
+      <c r="HZ96" s="1" t="n">
         <v>14</v>
+      </c>
+      <c r="IA96" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="97" ht="13.8" customHeight="1" s="2">
@@ -68866,8 +69154,11 @@
       <c r="HY97" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="HZ97" t="n">
+      <c r="HZ97" s="1" t="n">
         <v>41</v>
+      </c>
+      <c r="IA97" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="98" ht="13.8" customHeight="1" s="2">
@@ -69572,8 +69863,11 @@
       <c r="HY98" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="HZ98" t="n">
+      <c r="HZ98" s="1" t="n">
         <v>48</v>
+      </c>
+      <c r="IA98" t="n">
+        <v>43</v>
       </c>
     </row>
     <row r="99" ht="13.8" customHeight="1" s="2">
@@ -70278,7 +70572,10 @@
       <c r="HY99" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="HZ99" t="n">
+      <c r="HZ99" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="IA99" t="n">
         <v>57</v>
       </c>
     </row>
@@ -70984,8 +71281,11 @@
       <c r="HY100" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="HZ100" t="n">
+      <c r="HZ100" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="IA100" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="101" ht="13.8" customHeight="1" s="2">
@@ -71690,8 +71990,11 @@
       <c r="HY101" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="HZ101" t="n">
+      <c r="HZ101" s="1" t="n">
         <v>12</v>
+      </c>
+      <c r="IA101" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="102" ht="13.8" customHeight="1" s="2">
@@ -72396,8 +72699,11 @@
       <c r="HY102" s="1" t="n">
         <v>73.3</v>
       </c>
-      <c r="HZ102" t="n">
+      <c r="HZ102" s="1" t="n">
         <v>80</v>
+      </c>
+      <c r="IA102" t="n">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
round 12 2021, gather data bug fix
</commit_message>
<xml_diff>
--- a/django_AFL_ML/Data/Adelaide_stats.xlsx
+++ b/django_AFL_ML/Data/Adelaide_stats.xlsx
@@ -377,7 +377,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:IC102"/>
+  <dimension ref="A1:ID102"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="GZ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="HA23" activeCellId="0" sqref="HA23"/>
@@ -1099,8 +1099,11 @@
       <c r="IB1" s="1" t="n">
         <v>10407</v>
       </c>
-      <c r="IC1" t="n">
+      <c r="IC1" s="1" t="n">
         <v>10415</v>
+      </c>
+      <c r="ID1" t="n">
+        <v>10419</v>
       </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="2">
@@ -1814,7 +1817,10 @@
       <c r="IB2" s="1" t="n">
         <v>2021</v>
       </c>
-      <c r="IC2" t="n">
+      <c r="IC2" s="1" t="n">
+        <v>2021</v>
+      </c>
+      <c r="ID2" t="n">
         <v>2021</v>
       </c>
     </row>
@@ -2529,8 +2535,11 @@
       <c r="IB3" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="IC3" t="n">
+      <c r="IC3" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="ID3" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="2">
@@ -3244,8 +3253,11 @@
       <c r="IB4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="IC4" t="n">
+      <c r="IC4" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="ID4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5" ht="13.8" customHeight="1" s="2">
@@ -3959,7 +3971,10 @@
       <c r="IB5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="IC5" t="n">
+      <c r="IC5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="ID5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4674,8 +4689,11 @@
       <c r="IB6" s="1" t="n">
         <v>76</v>
       </c>
-      <c r="IC6" t="n">
+      <c r="IC6" s="1" t="n">
         <v>96</v>
+      </c>
+      <c r="ID6" t="n">
+        <v>83</v>
       </c>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="2">
@@ -5389,8 +5407,11 @@
       <c r="IB7" s="1" t="n">
         <v>106</v>
       </c>
-      <c r="IC7" t="n">
+      <c r="IC7" s="1" t="n">
         <v>95</v>
+      </c>
+      <c r="ID7" t="n">
+        <v>111</v>
       </c>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="2">
@@ -6104,8 +6125,11 @@
       <c r="IB8" s="1" t="n">
         <v>-30</v>
       </c>
-      <c r="IC8" t="n">
+      <c r="IC8" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="ID8" t="n">
+        <v>-28</v>
       </c>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="2">
@@ -6819,8 +6843,11 @@
       <c r="IB9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="IC9" t="n">
+      <c r="IC9" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="ID9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10" ht="13.8" customHeight="1" s="2">
@@ -7534,8 +7561,11 @@
       <c r="IB10" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="IC10" t="n">
+      <c r="IC10" s="1" t="n">
         <v>11</v>
+      </c>
+      <c r="ID10" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="11" ht="13.8" customHeight="1" s="2">
@@ -8249,8 +8279,11 @@
       <c r="IB11" s="1" t="n">
         <v>201</v>
       </c>
-      <c r="IC11" t="n">
+      <c r="IC11" s="1" t="n">
         <v>207</v>
+      </c>
+      <c r="ID11" t="n">
+        <v>181</v>
       </c>
     </row>
     <row r="12" ht="13.8" customHeight="1" s="2">
@@ -8964,8 +8997,11 @@
       <c r="IB12" s="1" t="n">
         <v>171</v>
       </c>
-      <c r="IC12" t="n">
+      <c r="IC12" s="1" t="n">
         <v>163</v>
+      </c>
+      <c r="ID12" t="n">
+        <v>136</v>
       </c>
     </row>
     <row r="13" ht="13.8" customHeight="1" s="2">
@@ -9679,8 +9715,11 @@
       <c r="IB13" s="1" t="n">
         <v>372</v>
       </c>
-      <c r="IC13" t="n">
+      <c r="IC13" s="1" t="n">
         <v>370</v>
+      </c>
+      <c r="ID13" t="n">
+        <v>317</v>
       </c>
     </row>
     <row r="14" ht="13.8" customHeight="1" s="2">
@@ -10394,8 +10433,11 @@
       <c r="IB14" s="1" t="n">
         <v>1.18</v>
       </c>
-      <c r="IC14" t="n">
+      <c r="IC14" s="1" t="n">
         <v>1.27</v>
+      </c>
+      <c r="ID14" t="n">
+        <v>1.33</v>
       </c>
     </row>
     <row r="15" ht="13.8" customHeight="1" s="2">
@@ -11109,8 +11151,11 @@
       <c r="IB15" s="1" t="n">
         <v>82</v>
       </c>
-      <c r="IC15" t="n">
+      <c r="IC15" s="1" t="n">
         <v>88</v>
+      </c>
+      <c r="ID15" t="n">
+        <v>55</v>
       </c>
     </row>
     <row r="16" ht="13.8" customHeight="1" s="2">
@@ -11824,8 +11869,11 @@
       <c r="IB16" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="IC16" t="n">
+      <c r="IC16" s="1" t="n">
         <v>65</v>
+      </c>
+      <c r="ID16" t="n">
+        <v>53</v>
       </c>
     </row>
     <row r="17" ht="13.8" customHeight="1" s="2">
@@ -12539,8 +12587,11 @@
       <c r="IB17" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="IC17" t="n">
+      <c r="IC17" s="1" t="n">
         <v>27</v>
+      </c>
+      <c r="ID17" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="18" ht="13.8" customHeight="1" s="2">
@@ -13254,8 +13305,11 @@
       <c r="IB18" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="IC18" t="n">
+      <c r="IC18" s="1" t="n">
         <v>24</v>
+      </c>
+      <c r="ID18" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="19" ht="13.8" customHeight="1" s="2">
@@ -13969,8 +14023,11 @@
       <c r="IB19" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="IC19" t="n">
+      <c r="IC19" s="1" t="n">
         <v>24</v>
+      </c>
+      <c r="ID19" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="20" ht="13.8" customHeight="1" s="2">
@@ -14684,8 +14741,11 @@
       <c r="IB20" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="IC20" t="n">
+      <c r="IC20" s="1" t="n">
         <v>15</v>
+      </c>
+      <c r="ID20" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="21" ht="13.8" customHeight="1" s="2">
@@ -15399,8 +15459,11 @@
       <c r="IB21" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="IC21" t="n">
+      <c r="IC21" s="1" t="n">
         <v>11</v>
+      </c>
+      <c r="ID21" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="22" ht="13.8" customHeight="1" s="2">
@@ -16114,8 +16177,11 @@
       <c r="IB22" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="IC22" t="n">
+      <c r="IC22" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="ID22" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="23" ht="13.8" customHeight="1" s="2">
@@ -16829,8 +16895,11 @@
       <c r="IB23" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="IC23" t="n">
+      <c r="IC23" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="ID23" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="24" ht="13.8" customHeight="1" s="2">
@@ -17544,8 +17613,11 @@
       <c r="IB24" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="IC24" t="n">
+      <c r="IC24" s="1" t="n">
         <v>21</v>
+      </c>
+      <c r="ID24" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="25" ht="13.8" customHeight="1" s="2">
@@ -18259,8 +18331,11 @@
       <c r="IB25" s="1" t="n">
         <v>52.4</v>
       </c>
-      <c r="IC25" t="n">
+      <c r="IC25" s="1" t="n">
         <v>71.40000000000001</v>
+      </c>
+      <c r="ID25" t="n">
+        <v>52.2</v>
       </c>
     </row>
     <row r="26" ht="13.8" customHeight="1" s="2">
@@ -18974,8 +19049,11 @@
       <c r="IB26" s="1" t="n">
         <v>33.82</v>
       </c>
-      <c r="IC26" t="n">
+      <c r="IC26" s="1" t="n">
         <v>24.67</v>
+      </c>
+      <c r="ID26" t="n">
+        <v>26.42</v>
       </c>
     </row>
     <row r="27" ht="13.8" customHeight="1" s="2">
@@ -19689,8 +19767,11 @@
       <c r="IB27" s="1" t="n">
         <v>17.71</v>
       </c>
-      <c r="IC27" t="n">
+      <c r="IC27" s="1" t="n">
         <v>17.62</v>
+      </c>
+      <c r="ID27" t="n">
+        <v>13.78</v>
       </c>
     </row>
     <row r="28" ht="13.8" customHeight="1" s="2">
@@ -20404,8 +20485,11 @@
       <c r="IB28" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="IC28" t="n">
+      <c r="IC28" s="1" t="n">
         <v>23</v>
+      </c>
+      <c r="ID28" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="29" ht="13.8" customHeight="1" s="2">
@@ -21119,7 +21203,10 @@
       <c r="IB29" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="IC29" t="n">
+      <c r="IC29" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="ID29" t="n">
         <v>59</v>
       </c>
     </row>
@@ -21834,8 +21921,11 @@
       <c r="IB30" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="IC30" t="n">
+      <c r="IC30" s="1" t="n">
         <v>37</v>
+      </c>
+      <c r="ID30" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="31" ht="13.8" customHeight="1" s="2">
@@ -22549,8 +22639,11 @@
       <c r="IB31" s="1" t="n">
         <v>56</v>
       </c>
-      <c r="IC31" t="n">
+      <c r="IC31" s="1" t="n">
         <v>47</v>
+      </c>
+      <c r="ID31" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="32" ht="13.8" customHeight="1" s="2">
@@ -23264,8 +23357,11 @@
       <c r="IB32" s="1" t="n">
         <v>2.67</v>
       </c>
-      <c r="IC32" t="n">
+      <c r="IC32" s="1" t="n">
         <v>2.24</v>
+      </c>
+      <c r="ID32" t="n">
+        <v>2.17</v>
       </c>
     </row>
     <row r="33" ht="13.8" customHeight="1" s="2">
@@ -23979,8 +24075,11 @@
       <c r="IB33" s="1" t="n">
         <v>5.09</v>
       </c>
-      <c r="IC33" t="n">
+      <c r="IC33" s="1" t="n">
         <v>3.13</v>
+      </c>
+      <c r="ID33" t="n">
+        <v>4.17</v>
       </c>
     </row>
     <row r="34" ht="13.8" customHeight="1" s="2">
@@ -24694,8 +24793,11 @@
       <c r="IB34" s="1" t="n">
         <v>37.5</v>
       </c>
-      <c r="IC34" t="n">
+      <c r="IC34" s="1" t="n">
         <v>42.6</v>
+      </c>
+      <c r="ID34" t="n">
+        <v>42</v>
       </c>
     </row>
     <row r="35" ht="13.8" customHeight="1" s="2">
@@ -25409,8 +25511,11 @@
       <c r="IB35" s="1" t="n">
         <v>19.6</v>
       </c>
-      <c r="IC35" t="n">
+      <c r="IC35" s="1" t="n">
         <v>31.9</v>
+      </c>
+      <c r="ID35" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="36" ht="13.8" customHeight="1" s="2">
@@ -26124,8 +26229,11 @@
       <c r="IB36" s="1" t="n">
         <v>187</v>
       </c>
-      <c r="IC36" t="n">
+      <c r="IC36" s="1" t="n">
         <v>186.5</v>
+      </c>
+      <c r="ID36" t="n">
+        <v>186.4</v>
       </c>
     </row>
     <row r="37" ht="13.8" customHeight="1" s="2">
@@ -26839,8 +26947,11 @@
       <c r="IB37" s="1" t="n">
         <v>84.3</v>
       </c>
-      <c r="IC37" t="n">
+      <c r="IC37" s="1" t="n">
         <v>85</v>
+      </c>
+      <c r="ID37" t="n">
+        <v>84.40000000000001</v>
       </c>
     </row>
     <row r="38" ht="13.8" customHeight="1" s="2">
@@ -27554,8 +27665,11 @@
       <c r="IB38" s="1" t="n">
         <v>24.33</v>
       </c>
-      <c r="IC38" t="n">
+      <c r="IC38" s="1" t="n">
         <v>24.66</v>
+      </c>
+      <c r="ID38" t="n">
+        <v>24.49</v>
       </c>
     </row>
     <row r="39" ht="13.8" customHeight="1" s="2">
@@ -28269,8 +28383,11 @@
       <c r="IB39" s="1" t="n">
         <v>68.8</v>
       </c>
-      <c r="IC39" t="n">
+      <c r="IC39" s="1" t="n">
         <v>78.8</v>
+      </c>
+      <c r="ID39" t="n">
+        <v>77</v>
       </c>
     </row>
     <row r="40" ht="13.8" customHeight="1" s="2">
@@ -28984,8 +29101,11 @@
       <c r="IB40" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="IC40" t="n">
+      <c r="IC40" s="1" t="n">
         <v>13</v>
+      </c>
+      <c r="ID40" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="41" ht="13.8" customHeight="1" s="2">
@@ -29699,8 +29819,11 @@
       <c r="IB41" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="IC41" t="n">
+      <c r="IC41" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="ID41" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="42" ht="13.8" customHeight="1" s="2">
@@ -30414,8 +30537,11 @@
       <c r="IB42" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="IC42" t="n">
+      <c r="IC42" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="ID42" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="43" ht="13.8" customHeight="1" s="2">
@@ -31129,7 +31255,10 @@
       <c r="IB43" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="IC43" t="n">
+      <c r="IC43" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="ID43" t="n">
         <v>6</v>
       </c>
     </row>
@@ -31844,8 +31973,11 @@
       <c r="IB44" s="1" t="n">
         <v>143</v>
       </c>
-      <c r="IC44" t="n">
+      <c r="IC44" s="1" t="n">
         <v>142</v>
+      </c>
+      <c r="ID44" t="n">
+        <v>134</v>
       </c>
     </row>
     <row r="45" ht="13.8" customHeight="1" s="2">
@@ -32559,8 +32691,11 @@
       <c r="IB45" s="1" t="n">
         <v>229</v>
       </c>
-      <c r="IC45" t="n">
+      <c r="IC45" s="1" t="n">
         <v>220</v>
+      </c>
+      <c r="ID45" t="n">
+        <v>167</v>
       </c>
     </row>
     <row r="46" ht="13.8" customHeight="1" s="2">
@@ -33274,8 +33409,11 @@
       <c r="IB46" s="1" t="n">
         <v>272</v>
       </c>
-      <c r="IC46" t="n">
+      <c r="IC46" s="1" t="n">
         <v>277</v>
+      </c>
+      <c r="ID46" t="n">
+        <v>224</v>
       </c>
     </row>
     <row r="47" ht="13.8" customHeight="1" s="2">
@@ -33989,8 +34127,11 @@
       <c r="IB47" s="1" t="n">
         <v>73.09999999999999</v>
       </c>
-      <c r="IC47" t="n">
+      <c r="IC47" s="1" t="n">
         <v>74.90000000000001</v>
+      </c>
+      <c r="ID47" t="n">
+        <v>70.7</v>
       </c>
     </row>
     <row r="48" ht="13.8" customHeight="1" s="2">
@@ -34704,7 +34845,10 @@
       <c r="IB48" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="IC48" t="n">
+      <c r="IC48" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="ID48" t="n">
         <v>59</v>
       </c>
     </row>
@@ -35419,8 +35563,11 @@
       <c r="IB49" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="IC49" t="n">
+      <c r="IC49" s="1" t="n">
         <v>17</v>
+      </c>
+      <c r="ID49" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="50" ht="13.8" customHeight="1" s="2">
@@ -36134,7 +36281,10 @@
       <c r="IB50" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="IC50" t="n">
+      <c r="IC50" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="ID50" t="n">
         <v>8</v>
       </c>
     </row>
@@ -36849,8 +36999,11 @@
       <c r="IB51" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="IC51" t="n">
+      <c r="IC51" s="1" t="n">
         <v>23</v>
+      </c>
+      <c r="ID51" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="52" ht="13.8" customHeight="1" s="2">
@@ -37564,8 +37717,11 @@
       <c r="IB52" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="IC52" t="n">
+      <c r="IC52" s="1" t="n">
         <v>37</v>
+      </c>
+      <c r="ID52" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="53" ht="13.8" customHeight="1" s="2">
@@ -38279,8 +38435,11 @@
       <c r="IB53" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="IC53" t="n">
+      <c r="IC53" s="1" t="n">
         <v>50</v>
+      </c>
+      <c r="ID53" t="n">
+        <v>42</v>
       </c>
     </row>
     <row r="54" ht="13.8" customHeight="1" s="2">
@@ -38994,8 +39153,11 @@
       <c r="IB54" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="IC54" t="n">
+      <c r="IC54" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="ID54" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="55" ht="13.8" customHeight="1" s="2">
@@ -39709,8 +39871,11 @@
       <c r="IB55" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="IC55" t="n">
+      <c r="IC55" s="1" t="n">
         <v>11</v>
+      </c>
+      <c r="ID55" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="56" ht="13.8" customHeight="1" s="2">
@@ -40424,8 +40589,11 @@
       <c r="IB56" s="1" t="n">
         <v>63.6</v>
       </c>
-      <c r="IC56" t="n">
+      <c r="IC56" s="1" t="n">
         <v>73.3</v>
+      </c>
+      <c r="ID56" t="n">
+        <v>58.3</v>
       </c>
     </row>
     <row r="57" ht="13.8" customHeight="1" s="2">
@@ -41139,8 +41307,11 @@
       <c r="IB57" s="1" t="n">
         <v>241</v>
       </c>
-      <c r="IC57" t="n">
+      <c r="IC57" s="1" t="n">
         <v>207</v>
+      </c>
+      <c r="ID57" t="n">
+        <v>247</v>
       </c>
     </row>
     <row r="58" ht="13.8" customHeight="1" s="2">
@@ -41854,8 +42025,11 @@
       <c r="IB58" s="1" t="n">
         <v>148</v>
       </c>
-      <c r="IC58" t="n">
+      <c r="IC58" s="1" t="n">
         <v>126</v>
+      </c>
+      <c r="ID58" t="n">
+        <v>143</v>
       </c>
     </row>
     <row r="59" ht="13.8" customHeight="1" s="2">
@@ -42569,8 +42743,11 @@
       <c r="IB59" s="1" t="n">
         <v>389</v>
       </c>
-      <c r="IC59" t="n">
+      <c r="IC59" s="1" t="n">
         <v>333</v>
+      </c>
+      <c r="ID59" t="n">
+        <v>390</v>
       </c>
     </row>
     <row r="60" ht="13.8" customHeight="1" s="2">
@@ -43284,8 +43461,11 @@
       <c r="IB60" s="1" t="n">
         <v>1.63</v>
       </c>
-      <c r="IC60" t="n">
+      <c r="IC60" s="1" t="n">
         <v>1.64</v>
+      </c>
+      <c r="ID60" t="n">
+        <v>1.73</v>
       </c>
     </row>
     <row r="61" ht="13.8" customHeight="1" s="2">
@@ -43999,8 +44179,11 @@
       <c r="IB61" s="1" t="n">
         <v>127</v>
       </c>
-      <c r="IC61" t="n">
+      <c r="IC61" s="1" t="n">
         <v>74</v>
+      </c>
+      <c r="ID61" t="n">
+        <v>146</v>
       </c>
     </row>
     <row r="62" ht="13.8" customHeight="1" s="2">
@@ -44714,8 +44897,11 @@
       <c r="IB62" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="IC62" t="n">
+      <c r="IC62" s="1" t="n">
         <v>78</v>
+      </c>
+      <c r="ID62" t="n">
+        <v>68</v>
       </c>
     </row>
     <row r="63" ht="13.8" customHeight="1" s="2">
@@ -45429,8 +45615,11 @@
       <c r="IB63" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="IC63" t="n">
+      <c r="IC63" s="1" t="n">
         <v>49</v>
+      </c>
+      <c r="ID63" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="64" ht="13.8" customHeight="1" s="2">
@@ -46144,8 +46333,11 @@
       <c r="IB64" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="IC64" t="n">
+      <c r="IC64" s="1" t="n">
         <v>24</v>
+      </c>
+      <c r="ID64" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="65" ht="13.8" customHeight="1" s="2">
@@ -46859,8 +47051,11 @@
       <c r="IB65" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="IC65" t="n">
+      <c r="IC65" s="1" t="n">
         <v>24</v>
+      </c>
+      <c r="ID65" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="66" ht="13.8" customHeight="1" s="2">
@@ -47574,8 +47769,11 @@
       <c r="IB66" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="IC66" t="n">
+      <c r="IC66" s="1" t="n">
         <v>14</v>
+      </c>
+      <c r="ID66" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="67" ht="13.8" customHeight="1" s="2">
@@ -48289,8 +48487,11 @@
       <c r="IB67" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="IC67" t="n">
+      <c r="IC67" s="1" t="n">
         <v>9</v>
+      </c>
+      <c r="ID67" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="68" ht="13.8" customHeight="1" s="2">
@@ -49004,8 +49205,11 @@
       <c r="IB68" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="IC68" t="n">
+      <c r="IC68" s="1" t="n">
         <v>9</v>
+      </c>
+      <c r="ID68" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="69" ht="13.8" customHeight="1" s="2">
@@ -49719,8 +49923,11 @@
       <c r="IB69" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="IC69" t="n">
+      <c r="IC69" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="ID69" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="70" ht="13.8" customHeight="1" s="2">
@@ -50434,8 +50641,11 @@
       <c r="IB70" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="IC70" t="n">
+      <c r="IC70" s="1" t="n">
         <v>25</v>
+      </c>
+      <c r="ID70" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="71" ht="13.8" customHeight="1" s="2">
@@ -51149,8 +51359,11 @@
       <c r="IB71" s="1" t="n">
         <v>61.5</v>
       </c>
-      <c r="IC71" t="n">
+      <c r="IC71" s="1" t="n">
         <v>56</v>
+      </c>
+      <c r="ID71" t="n">
+        <v>65.40000000000001</v>
       </c>
     </row>
     <row r="72" ht="13.8" customHeight="1" s="2">
@@ -51864,8 +52077,11 @@
       <c r="IB72" s="1" t="n">
         <v>24.31</v>
       </c>
-      <c r="IC72" t="n">
+      <c r="IC72" s="1" t="n">
         <v>23.79</v>
+      </c>
+      <c r="ID72" t="n">
+        <v>22.94</v>
       </c>
     </row>
     <row r="73" ht="13.8" customHeight="1" s="2">
@@ -52579,8 +52795,11 @@
       <c r="IB73" s="1" t="n">
         <v>14.96</v>
       </c>
-      <c r="IC73" t="n">
+      <c r="IC73" s="1" t="n">
         <v>13.32</v>
+      </c>
+      <c r="ID73" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="74" ht="13.8" customHeight="1" s="2">
@@ -53294,8 +53513,11 @@
       <c r="IB74" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="IC74" t="n">
+      <c r="IC74" s="1" t="n">
         <v>44</v>
+      </c>
+      <c r="ID74" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="75" ht="13.8" customHeight="1" s="2">
@@ -54009,8 +54231,11 @@
       <c r="IB75" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="IC75" t="n">
+      <c r="IC75" s="1" t="n">
         <v>59</v>
+      </c>
+      <c r="ID75" t="n">
+        <v>51</v>
       </c>
     </row>
     <row r="76" ht="13.8" customHeight="1" s="2">
@@ -54724,8 +54949,11 @@
       <c r="IB76" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="IC76" t="n">
+      <c r="IC76" s="1" t="n">
         <v>30</v>
+      </c>
+      <c r="ID76" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="77" ht="13.8" customHeight="1" s="2">
@@ -55439,8 +55667,11 @@
       <c r="IB77" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="IC77" t="n">
+      <c r="IC77" s="1" t="n">
         <v>54</v>
+      </c>
+      <c r="ID77" t="n">
+        <v>48</v>
       </c>
     </row>
     <row r="78" ht="13.8" customHeight="1" s="2">
@@ -56154,8 +56385,11 @@
       <c r="IB78" s="1" t="n">
         <v>1.85</v>
       </c>
-      <c r="IC78" t="n">
+      <c r="IC78" s="1" t="n">
         <v>2.16</v>
+      </c>
+      <c r="ID78" t="n">
+        <v>1.85</v>
       </c>
     </row>
     <row r="79" ht="13.8" customHeight="1" s="2">
@@ -56869,8 +57103,11 @@
       <c r="IB79" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="IC79" t="n">
+      <c r="IC79" s="1" t="n">
         <v>3.86</v>
+      </c>
+      <c r="ID79" t="n">
+        <v>2.82</v>
       </c>
     </row>
     <row r="80" ht="13.8" customHeight="1" s="2">
@@ -57584,8 +57821,11 @@
       <c r="IB80" s="1" t="n">
         <v>52.1</v>
       </c>
-      <c r="IC80" t="n">
+      <c r="IC80" s="1" t="n">
         <v>42.6</v>
+      </c>
+      <c r="ID80" t="n">
+        <v>52.1</v>
       </c>
     </row>
     <row r="81" ht="13.8" customHeight="1" s="2">
@@ -58299,8 +58539,11 @@
       <c r="IB81" s="1" t="n">
         <v>33.3</v>
       </c>
-      <c r="IC81" t="n">
+      <c r="IC81" s="1" t="n">
         <v>25.9</v>
+      </c>
+      <c r="ID81" t="n">
+        <v>35.4</v>
       </c>
     </row>
     <row r="82" ht="13.8" customHeight="1" s="2">
@@ -59014,8 +59257,11 @@
       <c r="IB82" s="1" t="n">
         <v>189.8</v>
       </c>
-      <c r="IC82" t="n">
+      <c r="IC82" s="1" t="n">
         <v>187.9</v>
+      </c>
+      <c r="ID82" t="n">
+        <v>186.5</v>
       </c>
     </row>
     <row r="83" ht="13.8" customHeight="1" s="2">
@@ -59729,8 +59975,11 @@
       <c r="IB83" s="1" t="n">
         <v>89.09999999999999</v>
       </c>
-      <c r="IC83" t="n">
+      <c r="IC83" s="1" t="n">
         <v>86.40000000000001</v>
+      </c>
+      <c r="ID83" t="n">
+        <v>86.3</v>
       </c>
     </row>
     <row r="84" ht="13.8" customHeight="1" s="2">
@@ -60444,8 +60693,11 @@
       <c r="IB84" s="1" t="n">
         <v>26.16</v>
       </c>
-      <c r="IC84" t="n">
+      <c r="IC84" s="1" t="n">
         <v>25.16</v>
+      </c>
+      <c r="ID84" t="n">
+        <v>26.24</v>
       </c>
     </row>
     <row r="85" ht="13.8" customHeight="1" s="2">
@@ -61159,8 +61411,11 @@
       <c r="IB85" s="1" t="n">
         <v>110</v>
       </c>
-      <c r="IC85" t="n">
+      <c r="IC85" s="1" t="n">
         <v>92.7</v>
+      </c>
+      <c r="ID85" t="n">
+        <v>113.4</v>
       </c>
     </row>
     <row r="86" ht="13.8" customHeight="1" s="2">
@@ -61874,8 +62129,11 @@
       <c r="IB86" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="IC86" t="n">
+      <c r="IC86" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="ID86" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="87" ht="13.8" customHeight="1" s="2">
@@ -62589,8 +62847,11 @@
       <c r="IB87" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="IC87" t="n">
+      <c r="IC87" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="ID87" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="88" ht="13.8" customHeight="1" s="2">
@@ -63304,8 +63565,11 @@
       <c r="IB88" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="IC88" t="n">
+      <c r="IC88" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="ID88" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="89" ht="13.8" customHeight="1" s="2">
@@ -64019,8 +64283,11 @@
       <c r="IB89" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="IC89" t="n">
+      <c r="IC89" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="ID89" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="90" ht="13.8" customHeight="1" s="2">
@@ -64734,8 +65001,11 @@
       <c r="IB90" s="1" t="n">
         <v>132</v>
       </c>
-      <c r="IC90" t="n">
+      <c r="IC90" s="1" t="n">
         <v>153</v>
+      </c>
+      <c r="ID90" t="n">
+        <v>132</v>
       </c>
     </row>
     <row r="91" ht="13.8" customHeight="1" s="2">
@@ -65449,8 +65719,11 @@
       <c r="IB91" s="1" t="n">
         <v>256</v>
       </c>
-      <c r="IC91" t="n">
+      <c r="IC91" s="1" t="n">
         <v>175</v>
+      </c>
+      <c r="ID91" t="n">
+        <v>260</v>
       </c>
     </row>
     <row r="92" ht="13.8" customHeight="1" s="2">
@@ -66164,8 +66437,11 @@
       <c r="IB92" s="1" t="n">
         <v>306</v>
       </c>
-      <c r="IC92" t="n">
+      <c r="IC92" s="1" t="n">
         <v>235</v>
+      </c>
+      <c r="ID92" t="n">
+        <v>303</v>
       </c>
     </row>
     <row r="93" ht="13.8" customHeight="1" s="2">
@@ -66879,8 +67155,11 @@
       <c r="IB93" s="1" t="n">
         <v>78.7</v>
       </c>
-      <c r="IC93" t="n">
+      <c r="IC93" s="1" t="n">
         <v>70.59999999999999</v>
+      </c>
+      <c r="ID93" t="n">
+        <v>77.7</v>
       </c>
     </row>
     <row r="94" ht="13.8" customHeight="1" s="2">
@@ -67594,8 +67873,11 @@
       <c r="IB94" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="IC94" t="n">
+      <c r="IC94" s="1" t="n">
         <v>59</v>
+      </c>
+      <c r="ID94" t="n">
+        <v>51</v>
       </c>
     </row>
     <row r="95" ht="13.8" customHeight="1" s="2">
@@ -68309,8 +68591,11 @@
       <c r="IB95" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="IC95" t="n">
+      <c r="IC95" s="1" t="n">
         <v>18</v>
+      </c>
+      <c r="ID95" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="96" ht="13.8" customHeight="1" s="2">
@@ -69024,8 +69309,11 @@
       <c r="IB96" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="IC96" t="n">
+      <c r="IC96" s="1" t="n">
         <v>11</v>
+      </c>
+      <c r="ID96" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="97" ht="13.8" customHeight="1" s="2">
@@ -69739,8 +70027,11 @@
       <c r="IB97" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="IC97" t="n">
+      <c r="IC97" s="1" t="n">
         <v>44</v>
+      </c>
+      <c r="ID97" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="98" ht="13.8" customHeight="1" s="2">
@@ -70454,8 +70745,11 @@
       <c r="IB98" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="IC98" t="n">
+      <c r="IC98" s="1" t="n">
         <v>30</v>
+      </c>
+      <c r="ID98" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="99" ht="13.8" customHeight="1" s="2">
@@ -71169,8 +71463,11 @@
       <c r="IB99" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="IC99" t="n">
+      <c r="IC99" s="1" t="n">
         <v>44</v>
+      </c>
+      <c r="ID99" t="n">
+        <v>38</v>
       </c>
     </row>
     <row r="100" ht="13.8" customHeight="1" s="2">
@@ -71884,8 +72181,11 @@
       <c r="IB100" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="IC100" t="n">
+      <c r="IC100" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="ID100" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="101" ht="13.8" customHeight="1" s="2">
@@ -72599,8 +72899,11 @@
       <c r="IB101" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="IC101" t="n">
+      <c r="IC101" s="1" t="n">
         <v>9</v>
+      </c>
+      <c r="ID101" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="102" ht="13.8" customHeight="1" s="2">
@@ -73314,8 +73617,11 @@
       <c r="IB102" s="1" t="n">
         <v>81.2</v>
       </c>
-      <c r="IC102" t="n">
+      <c r="IC102" s="1" t="n">
         <v>64.3</v>
+      </c>
+      <c r="ID102" t="n">
+        <v>70.59999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
round 17 2021 predictions
</commit_message>
<xml_diff>
--- a/django_AFL_ML/Data/Adelaide_stats.xlsx
+++ b/django_AFL_ML/Data/Adelaide_stats.xlsx
@@ -4,13 +4,13 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1" iterate="0" iterateCount="100" iterateDelta="0.0001" refMode="A1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
@@ -59,31 +59,31 @@
     </border>
   </borders>
   <cellStyleXfs count="6">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" name="Comma" xfId="1"/>
-    <cellStyle builtinId="6" name="Comma [0]" xfId="2"/>
-    <cellStyle builtinId="4" name="Currency" xfId="3"/>
-    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
-    <cellStyle builtinId="5" name="Percent" xfId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -377,18 +377,18 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:IG102"/>
+  <dimension ref="A1:IH102"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="GZ1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="HA23" activeCellId="0" pane="topLeft" sqref="HA23"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="GZ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="HA23" activeCellId="0" sqref="HA23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col customWidth="1" max="1025" min="1" style="1" width="8.529999999999999"/>
+    <col width="8.529999999999999" customWidth="1" style="1" min="1" max="1025"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="13.8" r="1" s="2">
+    <row r="1" ht="13.8" customHeight="1" s="2">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Match_ID</t>
@@ -1111,11 +1111,14 @@
       <c r="IF1" s="1" t="n">
         <v>10434</v>
       </c>
-      <c r="IG1" t="n">
+      <c r="IG1" s="1" t="n">
         <v>10445</v>
       </c>
+      <c r="IH1" t="n">
+        <v>10460</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="2" s="2">
+    <row r="2" ht="13.8" customHeight="1" s="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
           <t>Year</t>
@@ -1838,11 +1841,14 @@
       <c r="IF2" s="1" t="n">
         <v>2021</v>
       </c>
-      <c r="IG2" t="n">
+      <c r="IG2" s="1" t="n">
         <v>2021</v>
       </c>
+      <c r="IH2" t="n">
+        <v>2021</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="3" s="2">
+    <row r="3" ht="13.8" customHeight="1" s="2">
       <c r="A3" s="1" t="inlineStr">
         <is>
           <t>Round</t>
@@ -2565,11 +2571,14 @@
       <c r="IF3" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="IG3" t="n">
+      <c r="IG3" s="1" t="n">
         <v>15</v>
       </c>
+      <c r="IH3" t="n">
+        <v>16</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="4" s="2">
+    <row r="4" ht="13.8" customHeight="1" s="2">
       <c r="A4" s="1" t="inlineStr">
         <is>
           <t>H/A?</t>
@@ -3292,11 +3301,14 @@
       <c r="IF4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="IG4" t="n">
+      <c r="IG4" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="IH4" t="n">
+        <v>0</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="5" s="2">
+    <row r="5" ht="13.8" customHeight="1" s="2">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>H/A Win?</t>
@@ -4019,11 +4031,14 @@
       <c r="IF5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="IG5" t="n">
+      <c r="IG5" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="IH5" t="n">
+        <v>1</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="6" s="2">
+    <row r="6" ht="13.8" customHeight="1" s="2">
       <c r="A6" s="1" t="inlineStr">
         <is>
           <t>Points For</t>
@@ -4746,11 +4761,14 @@
       <c r="IF6" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="IG6" t="n">
+      <c r="IG6" s="1" t="n">
         <v>73</v>
       </c>
+      <c r="IH6" t="n">
+        <v>59</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="7" s="2">
+    <row r="7" ht="13.8" customHeight="1" s="2">
       <c r="A7" s="1" t="inlineStr">
         <is>
           <t>Points Against</t>
@@ -5473,11 +5491,14 @@
       <c r="IF7" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="IG7" t="n">
+      <c r="IG7" s="1" t="n">
         <v>83</v>
       </c>
+      <c r="IH7" t="n">
+        <v>111</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="8" s="2">
+    <row r="8" ht="13.8" customHeight="1" s="2">
       <c r="A8" s="1" t="inlineStr">
         <is>
           <t>Margin</t>
@@ -6200,11 +6221,14 @@
       <c r="IF8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="IG8" t="n">
+      <c r="IG8" s="1" t="n">
         <v>-10</v>
       </c>
+      <c r="IH8" t="n">
+        <v>-52</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="9" s="2">
+    <row r="9" ht="13.8" customHeight="1" s="2">
       <c r="A9" s="1" t="inlineStr">
         <is>
           <t>Team Won? (1=W, 0=L)</t>
@@ -6927,11 +6951,14 @@
       <c r="IF9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="IG9" t="n">
+      <c r="IG9" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="IH9" t="n">
+        <v>0</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="10" s="2">
+    <row r="10" ht="13.8" customHeight="1" s="2">
       <c r="A10" s="1" t="inlineStr">
         <is>
           <t>Team_against_ID</t>
@@ -7654,11 +7681,14 @@
       <c r="IF10" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="IG10" t="n">
+      <c r="IG10" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="IH10" t="n">
+        <v>2</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="11" s="2">
+    <row r="11" ht="13.8" customHeight="1" s="2">
       <c r="A11" s="1" t="inlineStr">
         <is>
           <t>Kicks</t>
@@ -8381,11 +8411,14 @@
       <c r="IF11" s="1" t="n">
         <v>223</v>
       </c>
-      <c r="IG11" t="n">
+      <c r="IG11" s="1" t="n">
         <v>199</v>
       </c>
+      <c r="IH11" t="n">
+        <v>212</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="12" s="2">
+    <row r="12" ht="13.8" customHeight="1" s="2">
       <c r="A12" s="1" t="inlineStr">
         <is>
           <t>Handballs</t>
@@ -9108,11 +9141,14 @@
       <c r="IF12" s="1" t="n">
         <v>134</v>
       </c>
-      <c r="IG12" t="n">
+      <c r="IG12" s="1" t="n">
         <v>127</v>
       </c>
+      <c r="IH12" t="n">
+        <v>144</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="13" s="2">
+    <row r="13" ht="13.8" customHeight="1" s="2">
       <c r="A13" s="1" t="inlineStr">
         <is>
           <t>Disposals</t>
@@ -9835,11 +9871,14 @@
       <c r="IF13" s="1" t="n">
         <v>357</v>
       </c>
-      <c r="IG13" t="n">
+      <c r="IG13" s="1" t="n">
         <v>326</v>
       </c>
+      <c r="IH13" t="n">
+        <v>356</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="14" s="2">
+    <row r="14" ht="13.8" customHeight="1" s="2">
       <c r="A14" s="1" t="inlineStr">
         <is>
           <t>Kick to HB Ratio</t>
@@ -10562,11 +10601,14 @@
       <c r="IF14" s="1" t="n">
         <v>1.66</v>
       </c>
-      <c r="IG14" t="n">
+      <c r="IG14" s="1" t="n">
         <v>1.57</v>
       </c>
+      <c r="IH14" t="n">
+        <v>1.47</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="15" s="2">
+    <row r="15" ht="13.8" customHeight="1" s="2">
       <c r="A15" s="1" t="inlineStr">
         <is>
           <t>Marks</t>
@@ -11289,11 +11331,14 @@
       <c r="IF15" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="IG15" t="n">
+      <c r="IG15" s="1" t="n">
         <v>83</v>
       </c>
+      <c r="IH15" t="n">
+        <v>54</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="16" s="2">
+    <row r="16" ht="13.8" customHeight="1" s="2">
       <c r="A16" s="1" t="inlineStr">
         <is>
           <t>Tackles</t>
@@ -12016,11 +12061,14 @@
       <c r="IF16" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="IG16" t="n">
+      <c r="IG16" s="1" t="n">
         <v>52</v>
       </c>
+      <c r="IH16" t="n">
+        <v>61</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="17" s="2">
+    <row r="17" ht="13.8" customHeight="1" s="2">
       <c r="A17" s="1" t="inlineStr">
         <is>
           <t>Hitouts</t>
@@ -12743,11 +12791,14 @@
       <c r="IF17" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="IG17" t="n">
+      <c r="IG17" s="1" t="n">
         <v>34</v>
       </c>
+      <c r="IH17" t="n">
+        <v>45</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="18" s="2">
+    <row r="18" ht="13.8" customHeight="1" s="2">
       <c r="A18" s="1" t="inlineStr">
         <is>
           <t>Frees For</t>
@@ -13470,11 +13521,14 @@
       <c r="IF18" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="IG18" t="n">
+      <c r="IG18" s="1" t="n">
         <v>22</v>
       </c>
+      <c r="IH18" t="n">
+        <v>18</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="19" s="2">
+    <row r="19" ht="13.8" customHeight="1" s="2">
       <c r="A19" s="1" t="inlineStr">
         <is>
           <t>Frees Against</t>
@@ -14197,11 +14251,14 @@
       <c r="IF19" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="IG19" t="n">
+      <c r="IG19" s="1" t="n">
         <v>14</v>
       </c>
+      <c r="IH19" t="n">
+        <v>20</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="20" s="2">
+    <row r="20" ht="13.8" customHeight="1" s="2">
       <c r="A20" s="1" t="inlineStr">
         <is>
           <t>Goals Kicked</t>
@@ -14924,11 +14981,14 @@
       <c r="IF20" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="IG20" t="n">
+      <c r="IG20" s="1" t="n">
         <v>10</v>
       </c>
+      <c r="IH20" t="n">
+        <v>8</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="21" s="2">
+    <row r="21" ht="13.8" customHeight="1" s="2">
       <c r="A21" s="1" t="inlineStr">
         <is>
           <t>Goal Assists1</t>
@@ -15651,11 +15711,14 @@
       <c r="IF21" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="IG21" t="n">
+      <c r="IG21" s="1" t="n">
         <v>8</v>
       </c>
+      <c r="IH21" t="n">
+        <v>7</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="22" s="2">
+    <row r="22" ht="13.8" customHeight="1" s="2">
       <c r="A22" s="1" t="inlineStr">
         <is>
           <t>Behinds Kicked</t>
@@ -16378,11 +16441,14 @@
       <c r="IF22" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="IG22" t="n">
+      <c r="IG22" s="1" t="n">
         <v>9</v>
       </c>
+      <c r="IH22" t="n">
+        <v>10</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="23" s="2">
+    <row r="23" ht="13.8" customHeight="1" s="2">
       <c r="A23" s="1" t="inlineStr">
         <is>
           <t>Rushed Behinds</t>
@@ -17105,11 +17171,14 @@
       <c r="IF23" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="IG23" t="n">
+      <c r="IG23" s="1" t="n">
         <v>4</v>
       </c>
+      <c r="IH23" t="n">
+        <v>1</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="24" s="2">
+    <row r="24" ht="13.8" customHeight="1" s="2">
       <c r="A24" s="1" t="inlineStr">
         <is>
           <t>Scoring Shots</t>
@@ -17832,11 +17901,14 @@
       <c r="IF24" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="IG24" t="n">
+      <c r="IG24" s="1" t="n">
         <v>23</v>
       </c>
+      <c r="IH24" t="n">
+        <v>19</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="25" s="2">
+    <row r="25" ht="13.8" customHeight="1" s="2">
       <c r="A25" s="1" t="inlineStr">
         <is>
           <t>Conversion %</t>
@@ -18559,11 +18631,14 @@
       <c r="IF25" s="1" t="n">
         <v>42.9</v>
       </c>
-      <c r="IG25" t="n">
+      <c r="IG25" s="1" t="n">
         <v>43.5</v>
       </c>
+      <c r="IH25" t="n">
+        <v>42.1</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="26" s="2">
+    <row r="26" ht="13.8" customHeight="1" s="2">
       <c r="A26" s="1" t="inlineStr">
         <is>
           <t>Disposals Per Goal</t>
@@ -19286,11 +19361,14 @@
       <c r="IF26" s="1" t="n">
         <v>39.67</v>
       </c>
-      <c r="IG26" t="n">
+      <c r="IG26" s="1" t="n">
         <v>32.6</v>
       </c>
+      <c r="IH26" t="n">
+        <v>44.5</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="27" s="2">
+    <row r="27" ht="13.8" customHeight="1" s="2">
       <c r="A27" s="1" t="inlineStr">
         <is>
           <t>Disposals Per Scoring Shot</t>
@@ -20013,11 +20091,14 @@
       <c r="IF27" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="IG27" t="n">
+      <c r="IG27" s="1" t="n">
         <v>14.17</v>
       </c>
+      <c r="IH27" t="n">
+        <v>18.74</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="28" s="2">
+    <row r="28" ht="13.8" customHeight="1" s="2">
       <c r="A28" s="1" t="inlineStr">
         <is>
           <t>Clearances1</t>
@@ -20740,11 +20821,14 @@
       <c r="IF28" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="IG28" t="n">
+      <c r="IG28" s="1" t="n">
         <v>38</v>
       </c>
+      <c r="IH28" t="n">
+        <v>41</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="29" s="2">
+    <row r="29" ht="13.8" customHeight="1" s="2">
       <c r="A29" s="1" t="inlineStr">
         <is>
           <t>Clangers1</t>
@@ -21467,11 +21551,14 @@
       <c r="IF29" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="IG29" t="n">
+      <c r="IG29" s="1" t="n">
         <v>47</v>
       </c>
+      <c r="IH29" t="n">
+        <v>60</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="30" s="2">
+    <row r="30" ht="13.8" customHeight="1" s="2">
       <c r="A30" s="1" t="inlineStr">
         <is>
           <t>Rebound 50s1</t>
@@ -22194,11 +22281,14 @@
       <c r="IF30" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="IG30" t="n">
+      <c r="IG30" s="1" t="n">
         <v>42</v>
       </c>
+      <c r="IH30" t="n">
+        <v>43</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="31" s="2">
+    <row r="31" ht="13.8" customHeight="1" s="2">
       <c r="A31" s="1" t="inlineStr">
         <is>
           <t>Inside 50s</t>
@@ -22921,11 +23011,14 @@
       <c r="IF31" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="IG31" t="n">
+      <c r="IG31" s="1" t="n">
         <v>50</v>
       </c>
+      <c r="IH31" t="n">
+        <v>45</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="32" s="2">
+    <row r="32" ht="13.8" customHeight="1" s="2">
       <c r="A32" s="1" t="inlineStr">
         <is>
           <t>In50s Per Scoring Shot</t>
@@ -23648,11 +23741,14 @@
       <c r="IF32" s="1" t="n">
         <v>2.57</v>
       </c>
-      <c r="IG32" t="n">
+      <c r="IG32" s="1" t="n">
         <v>2.17</v>
       </c>
+      <c r="IH32" t="n">
+        <v>2.37</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="33" s="2">
+    <row r="33" ht="13.8" customHeight="1" s="2">
       <c r="A33" s="1" t="inlineStr">
         <is>
           <t>In50s Per Goal</t>
@@ -24375,11 +24471,14 @@
       <c r="IF33" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="IG33" t="n">
+      <c r="IG33" s="1" t="n">
         <v>5</v>
       </c>
+      <c r="IH33" t="n">
+        <v>5.62</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="34" s="2">
+    <row r="34" ht="13.8" customHeight="1" s="2">
       <c r="A34" s="1" t="inlineStr">
         <is>
           <t>% In50s Score</t>
@@ -25102,11 +25201,14 @@
       <c r="IF34" s="1" t="n">
         <v>33.3</v>
       </c>
-      <c r="IG34" t="n">
+      <c r="IG34" s="1" t="n">
         <v>38</v>
       </c>
+      <c r="IH34" t="n">
+        <v>40</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="35" s="2">
+    <row r="35" ht="13.8" customHeight="1" s="2">
       <c r="A35" s="1" t="inlineStr">
         <is>
           <t>% In50s Goal</t>
@@ -25829,11 +25931,14 @@
       <c r="IF35" s="1" t="n">
         <v>16.7</v>
       </c>
-      <c r="IG35" t="n">
+      <c r="IG35" s="1" t="n">
         <v>20</v>
       </c>
+      <c r="IH35" t="n">
+        <v>17.8</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="36" s="2">
+    <row r="36" ht="13.8" customHeight="1" s="2">
       <c r="A36" s="1" t="inlineStr">
         <is>
           <t>Height</t>
@@ -26556,11 +26661,14 @@
       <c r="IF36" s="1" t="n">
         <v>186.8</v>
       </c>
-      <c r="IG36" t="n">
+      <c r="IG36" s="1" t="n">
         <v>186.1</v>
       </c>
+      <c r="IH36" t="n">
+        <v>187</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="37" s="2">
+    <row r="37" ht="13.8" customHeight="1" s="2">
       <c r="A37" s="1" t="inlineStr">
         <is>
           <t>Weight</t>
@@ -27283,11 +27391,14 @@
       <c r="IF37" s="1" t="n">
         <v>83.8</v>
       </c>
-      <c r="IG37" t="n">
+      <c r="IG37" s="1" t="n">
         <v>84</v>
       </c>
+      <c r="IH37" t="n">
+        <v>84.8</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="38" s="2">
+    <row r="38" ht="13.8" customHeight="1" s="2">
       <c r="A38" s="1" t="inlineStr">
         <is>
           <t>Age</t>
@@ -28010,11 +28121,14 @@
       <c r="IF38" s="1" t="n">
         <v>24.41</v>
       </c>
-      <c r="IG38" t="n">
+      <c r="IG38" s="1" t="n">
         <v>24.8</v>
       </c>
+      <c r="IH38" t="n">
+        <v>24.41</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="39" s="2">
+    <row r="39" ht="13.8" customHeight="1" s="2">
       <c r="A39" s="1" t="inlineStr">
         <is>
           <t>Av Games</t>
@@ -28737,11 +28851,14 @@
       <c r="IF39" s="1" t="n">
         <v>74.2</v>
       </c>
-      <c r="IG39" t="n">
+      <c r="IG39" s="1" t="n">
         <v>83.2</v>
       </c>
+      <c r="IH39" t="n">
+        <v>78.5</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="40" s="2">
+    <row r="40" ht="13.8" customHeight="1" s="2">
       <c r="A40" s="1" t="inlineStr">
         <is>
           <t>&lt;50 Games</t>
@@ -29464,11 +29581,14 @@
       <c r="IF40" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="IG40" t="n">
+      <c r="IG40" s="1" t="n">
         <v>12</v>
       </c>
+      <c r="IH40" t="n">
+        <v>13</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="41" s="2">
+    <row r="41" ht="13.8" customHeight="1" s="2">
       <c r="A41" s="1" t="inlineStr">
         <is>
           <t>50-99 Games</t>
@@ -30191,11 +30311,14 @@
       <c r="IF41" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="IG41" t="n">
+      <c r="IG41" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="IH41" t="n">
+        <v>2</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="42" s="2">
+    <row r="42" ht="13.8" customHeight="1" s="2">
       <c r="A42" s="1" t="inlineStr">
         <is>
           <t>100-149 Games</t>
@@ -30918,11 +31041,14 @@
       <c r="IF42" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="IG42" t="n">
+      <c r="IG42" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="IH42" t="n">
+        <v>2</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="43" s="2">
+    <row r="43" ht="13.8" customHeight="1" s="2">
       <c r="A43" s="1" t="inlineStr">
         <is>
           <t>&gt;150 Games</t>
@@ -31645,11 +31771,14 @@
       <c r="IF43" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="IG43" t="n">
+      <c r="IG43" s="1" t="n">
         <v>6</v>
       </c>
+      <c r="IH43" t="n">
+        <v>6</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="44" s="2">
+    <row r="44" ht="13.8" customHeight="1" s="2">
       <c r="A44" s="1" t="inlineStr">
         <is>
           <t>Contested Poss</t>
@@ -32372,11 +32501,14 @@
       <c r="IF44" s="1" t="n">
         <v>164</v>
       </c>
-      <c r="IG44" t="n">
+      <c r="IG44" s="1" t="n">
         <v>117</v>
       </c>
+      <c r="IH44" t="n">
+        <v>167</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="45" s="2">
+    <row r="45" ht="13.8" customHeight="1" s="2">
       <c r="A45" s="1" t="inlineStr">
         <is>
           <t>Uncontested Poss</t>
@@ -33099,11 +33231,14 @@
       <c r="IF45" s="1" t="n">
         <v>168</v>
       </c>
-      <c r="IG45" t="n">
+      <c r="IG45" s="1" t="n">
         <v>202</v>
       </c>
+      <c r="IH45" t="n">
+        <v>181</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="46" s="2">
+    <row r="46" ht="13.8" customHeight="1" s="2">
       <c r="A46" s="1" t="inlineStr">
         <is>
           <t>Effective Disposals</t>
@@ -33826,11 +33961,14 @@
       <c r="IF46" s="1" t="n">
         <v>227</v>
       </c>
-      <c r="IG46" t="n">
+      <c r="IG46" s="1" t="n">
         <v>246</v>
       </c>
+      <c r="IH46" t="n">
+        <v>224</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="47" s="2">
+    <row r="47" ht="13.8" customHeight="1" s="2">
       <c r="A47" s="1" t="inlineStr">
         <is>
           <t>Disposal Efficiency</t>
@@ -34553,11 +34691,14 @@
       <c r="IF47" s="1" t="n">
         <v>63.6</v>
       </c>
-      <c r="IG47" t="n">
+      <c r="IG47" s="1" t="n">
         <v>75.5</v>
       </c>
+      <c r="IH47" t="n">
+        <v>62.9</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="48" s="2">
+    <row r="48" ht="13.8" customHeight="1" s="2">
       <c r="A48" s="1" t="inlineStr">
         <is>
           <t>Clangers2</t>
@@ -35280,11 +35421,14 @@
       <c r="IF48" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="IG48" t="n">
+      <c r="IG48" s="1" t="n">
         <v>47</v>
       </c>
+      <c r="IH48" t="n">
+        <v>60</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="49" s="2">
+    <row r="49" ht="13.8" customHeight="1" s="2">
       <c r="A49" s="1" t="inlineStr">
         <is>
           <t>Contested Marks</t>
@@ -36007,11 +36151,14 @@
       <c r="IF49" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="IG49" t="n">
+      <c r="IG49" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="IH49" t="n">
+        <v>11</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="50" s="2">
+    <row r="50" ht="13.8" customHeight="1" s="2">
       <c r="A50" s="1" t="inlineStr">
         <is>
           <t>Marks Inside 50</t>
@@ -36734,11 +36881,14 @@
       <c r="IF50" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="IG50" t="n">
+      <c r="IG50" s="1" t="n">
         <v>10</v>
       </c>
+      <c r="IH50" t="n">
+        <v>6</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="51" s="2">
+    <row r="51" ht="13.8" customHeight="1" s="2">
       <c r="A51" s="1" t="inlineStr">
         <is>
           <t>Clearances2</t>
@@ -37461,11 +37611,14 @@
       <c r="IF51" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="IG51" t="n">
+      <c r="IG51" s="1" t="n">
         <v>38</v>
       </c>
+      <c r="IH51" t="n">
+        <v>41</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="52" s="2">
+    <row r="52" ht="13.8" customHeight="1" s="2">
       <c r="A52" s="1" t="inlineStr">
         <is>
           <t>Rebound 50s2</t>
@@ -38188,11 +38341,14 @@
       <c r="IF52" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="IG52" t="n">
+      <c r="IG52" s="1" t="n">
         <v>42</v>
       </c>
+      <c r="IH52" t="n">
+        <v>43</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="53" s="2">
+    <row r="53" ht="13.8" customHeight="1" s="2">
       <c r="A53" s="1" t="inlineStr">
         <is>
           <t>1%ers</t>
@@ -38915,11 +39071,14 @@
       <c r="IF53" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="IG53" t="n">
+      <c r="IG53" s="1" t="n">
         <v>38</v>
       </c>
+      <c r="IH53" t="n">
+        <v>63</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="54" s="2">
+    <row r="54" ht="13.8" customHeight="1" s="2">
       <c r="A54" s="1" t="inlineStr">
         <is>
           <t>Bounces</t>
@@ -39642,11 +39801,14 @@
       <c r="IF54" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="IG54" t="n">
+      <c r="IG54" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="IH54" t="n">
+        <v>6</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="55" s="2">
+    <row r="55" ht="13.8" customHeight="1" s="2">
       <c r="A55" s="1" t="inlineStr">
         <is>
           <t>Goals Assists2</t>
@@ -40369,11 +40531,14 @@
       <c r="IF55" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="IG55" t="n">
+      <c r="IG55" s="1" t="n">
         <v>8</v>
       </c>
+      <c r="IH55" t="n">
+        <v>7</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="56" s="2">
+    <row r="56" ht="13.8" customHeight="1" s="2">
       <c r="A56" s="1" t="inlineStr">
         <is>
           <t>Goal Assist %</t>
@@ -41096,11 +41261,14 @@
       <c r="IF56" s="1" t="n">
         <v>44.4</v>
       </c>
-      <c r="IG56" t="n">
+      <c r="IG56" s="1" t="n">
         <v>80</v>
       </c>
+      <c r="IH56" t="n">
+        <v>87.5</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="57" s="2">
+    <row r="57" ht="13.8" customHeight="1" s="2">
       <c r="A57" s="1" t="inlineStr">
         <is>
           <t>Kicks (O)</t>
@@ -41823,11 +41991,14 @@
       <c r="IF57" s="1" t="n">
         <v>236</v>
       </c>
-      <c r="IG57" t="n">
+      <c r="IG57" s="1" t="n">
         <v>244</v>
       </c>
+      <c r="IH57" t="n">
+        <v>217</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="58" s="2">
+    <row r="58" ht="13.8" customHeight="1" s="2">
       <c r="A58" s="1" t="inlineStr">
         <is>
           <t>Handballs (O)</t>
@@ -42550,11 +42721,14 @@
       <c r="IF58" s="1" t="n">
         <v>145</v>
       </c>
-      <c r="IG58" t="n">
+      <c r="IG58" s="1" t="n">
         <v>136</v>
       </c>
+      <c r="IH58" t="n">
+        <v>133</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="59" s="2">
+    <row r="59" ht="13.8" customHeight="1" s="2">
       <c r="A59" s="1" t="inlineStr">
         <is>
           <t>Disposals (O)</t>
@@ -43277,11 +43451,14 @@
       <c r="IF59" s="1" t="n">
         <v>381</v>
       </c>
-      <c r="IG59" t="n">
+      <c r="IG59" s="1" t="n">
         <v>380</v>
       </c>
+      <c r="IH59" t="n">
+        <v>350</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="60" s="2">
+    <row r="60" ht="13.8" customHeight="1" s="2">
       <c r="A60" s="1" t="inlineStr">
         <is>
           <t>Kick to HB Ratio (O)</t>
@@ -44004,11 +44181,14 @@
       <c r="IF60" s="1" t="n">
         <v>1.63</v>
       </c>
-      <c r="IG60" t="n">
+      <c r="IG60" s="1" t="n">
         <v>1.79</v>
       </c>
+      <c r="IH60" t="n">
+        <v>1.63</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="61" s="2">
+    <row r="61" ht="13.8" customHeight="1" s="2">
       <c r="A61" s="1" t="inlineStr">
         <is>
           <t>Marks (O)</t>
@@ -44731,11 +44911,14 @@
       <c r="IF61" s="1" t="n">
         <v>70</v>
       </c>
-      <c r="IG61" t="n">
+      <c r="IG61" s="1" t="n">
         <v>128</v>
       </c>
+      <c r="IH61" t="n">
+        <v>69</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="62" s="2">
+    <row r="62" ht="13.8" customHeight="1" s="2">
       <c r="A62" s="1" t="inlineStr">
         <is>
           <t>Tackles(O)</t>
@@ -45458,11 +45641,14 @@
       <c r="IF62" s="1" t="n">
         <v>102</v>
       </c>
-      <c r="IG62" t="n">
+      <c r="IG62" s="1" t="n">
         <v>45</v>
       </c>
+      <c r="IH62" t="n">
+        <v>77</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="63" s="2">
+    <row r="63" ht="13.8" customHeight="1" s="2">
       <c r="A63" s="1" t="inlineStr">
         <is>
           <t>Hitouts(O)</t>
@@ -46185,11 +46371,14 @@
       <c r="IF63" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="IG63" t="n">
+      <c r="IG63" s="1" t="n">
         <v>30</v>
       </c>
+      <c r="IH63" t="n">
+        <v>31</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="64" s="2">
+    <row r="64" ht="13.8" customHeight="1" s="2">
       <c r="A64" s="1" t="inlineStr">
         <is>
           <t>Frees For(O)</t>
@@ -46912,11 +47101,14 @@
       <c r="IF64" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="IG64" t="n">
+      <c r="IG64" s="1" t="n">
         <v>14</v>
       </c>
+      <c r="IH64" t="n">
+        <v>20</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="65" s="2">
+    <row r="65" ht="13.8" customHeight="1" s="2">
       <c r="A65" s="1" t="inlineStr">
         <is>
           <t>Frees Against(O)</t>
@@ -47639,11 +47831,14 @@
       <c r="IF65" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="IG65" t="n">
+      <c r="IG65" s="1" t="n">
         <v>22</v>
       </c>
+      <c r="IH65" t="n">
+        <v>18</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="66" s="2">
+    <row r="66" ht="13.8" customHeight="1" s="2">
       <c r="A66" s="1" t="inlineStr">
         <is>
           <t>Goals Kicked(O)</t>
@@ -48366,11 +48561,14 @@
       <c r="IF66" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="IG66" t="n">
+      <c r="IG66" s="1" t="n">
         <v>12</v>
       </c>
+      <c r="IH66" t="n">
+        <v>17</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="67" s="2">
+    <row r="67" ht="13.8" customHeight="1" s="2">
       <c r="A67" s="1" t="inlineStr">
         <is>
           <t>Goal Assists1(O)</t>
@@ -49093,11 +49291,14 @@
       <c r="IF67" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="IG67" t="n">
+      <c r="IG67" s="1" t="n">
         <v>9</v>
       </c>
+      <c r="IH67" t="n">
+        <v>10</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="68" s="2">
+    <row r="68" ht="13.8" customHeight="1" s="2">
       <c r="A68" s="1" t="inlineStr">
         <is>
           <t>Behinds Kicked(O)</t>
@@ -49820,11 +50021,14 @@
       <c r="IF68" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="IG68" t="n">
+      <c r="IG68" s="1" t="n">
         <v>11</v>
       </c>
+      <c r="IH68" t="n">
+        <v>7</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="69" s="2">
+    <row r="69" ht="13.8" customHeight="1" s="2">
       <c r="A69" s="1" t="inlineStr">
         <is>
           <t>Rushed Behinds(O)</t>
@@ -50547,11 +50751,14 @@
       <c r="IF69" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="IG69" t="n">
+      <c r="IG69" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="IH69" t="n">
+        <v>2</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="70" s="2">
+    <row r="70" ht="13.8" customHeight="1" s="2">
       <c r="A70" s="1" t="inlineStr">
         <is>
           <t>Scoring Shots(O)</t>
@@ -51274,11 +51481,14 @@
       <c r="IF70" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="IG70" t="n">
+      <c r="IG70" s="1" t="n">
         <v>23</v>
       </c>
+      <c r="IH70" t="n">
+        <v>26</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="71" s="2">
+    <row r="71" ht="13.8" customHeight="1" s="2">
       <c r="A71" s="1" t="inlineStr">
         <is>
           <t>Conversion %(O)</t>
@@ -52001,11 +52211,14 @@
       <c r="IF71" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="IG71" t="n">
+      <c r="IG71" s="1" t="n">
         <v>52.2</v>
       </c>
+      <c r="IH71" t="n">
+        <v>65.40000000000001</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="72" s="2">
+    <row r="72" ht="13.8" customHeight="1" s="2">
       <c r="A72" s="1" t="inlineStr">
         <is>
           <t>Disposals Per Goal(O)</t>
@@ -52728,11 +52941,14 @@
       <c r="IF72" s="1" t="n">
         <v>47.62</v>
       </c>
-      <c r="IG72" t="n">
+      <c r="IG72" s="1" t="n">
         <v>31.67</v>
       </c>
+      <c r="IH72" t="n">
+        <v>20.59</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="73" s="2">
+    <row r="73" ht="13.8" customHeight="1" s="2">
       <c r="A73" s="1" t="inlineStr">
         <is>
           <t>Disposals Per Scoring Shot(O)</t>
@@ -53455,11 +53671,14 @@
       <c r="IF73" s="1" t="n">
         <v>19.05</v>
       </c>
-      <c r="IG73" t="n">
+      <c r="IG73" s="1" t="n">
         <v>16.52</v>
       </c>
+      <c r="IH73" t="n">
+        <v>13.46</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="74" s="2">
+    <row r="74" ht="13.8" customHeight="1" s="2">
       <c r="A74" s="1" t="inlineStr">
         <is>
           <t>Clearances1(O)</t>
@@ -54182,11 +54401,14 @@
       <c r="IF74" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="IG74" t="n">
+      <c r="IG74" s="1" t="n">
         <v>22</v>
       </c>
+      <c r="IH74" t="n">
+        <v>53</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="75" s="2">
+    <row r="75" ht="13.8" customHeight="1" s="2">
       <c r="A75" s="1" t="inlineStr">
         <is>
           <t>Clangers1(O)</t>
@@ -54909,11 +55131,14 @@
       <c r="IF75" s="1" t="n">
         <v>74</v>
       </c>
-      <c r="IG75" t="n">
+      <c r="IG75" s="1" t="n">
         <v>54</v>
       </c>
+      <c r="IH75" t="n">
+        <v>47</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="76" s="2">
+    <row r="76" ht="13.8" customHeight="1" s="2">
       <c r="A76" s="1" t="inlineStr">
         <is>
           <t>Rebound 50s1(O)</t>
@@ -55636,11 +55861,14 @@
       <c r="IF76" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="IG76" t="n">
+      <c r="IG76" s="1" t="n">
         <v>41</v>
       </c>
+      <c r="IH76" t="n">
+        <v>35</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="77" s="2">
+    <row r="77" ht="13.8" customHeight="1" s="2">
       <c r="A77" s="1" t="inlineStr">
         <is>
           <t>Inside 50s(O)</t>
@@ -56363,11 +56591,14 @@
       <c r="IF77" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="IG77" t="n">
+      <c r="IG77" s="1" t="n">
         <v>54</v>
       </c>
+      <c r="IH77" t="n">
+        <v>62</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="78" s="2">
+    <row r="78" ht="13.8" customHeight="1" s="2">
       <c r="A78" s="1" t="inlineStr">
         <is>
           <t>In50s Per Scoring Shot(O)</t>
@@ -57090,11 +57321,14 @@
       <c r="IF78" s="1" t="n">
         <v>2.85</v>
       </c>
-      <c r="IG78" t="n">
+      <c r="IG78" s="1" t="n">
         <v>2.35</v>
       </c>
+      <c r="IH78" t="n">
+        <v>2.38</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="79" s="2">
+    <row r="79" ht="13.8" customHeight="1" s="2">
       <c r="A79" s="1" t="inlineStr">
         <is>
           <t>In50s Per Goal(O)</t>
@@ -57817,11 +58051,14 @@
       <c r="IF79" s="1" t="n">
         <v>7.12</v>
       </c>
-      <c r="IG79" t="n">
+      <c r="IG79" s="1" t="n">
         <v>4.5</v>
       </c>
+      <c r="IH79" t="n">
+        <v>3.65</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="80" s="2">
+    <row r="80" ht="13.8" customHeight="1" s="2">
       <c r="A80" s="1" t="inlineStr">
         <is>
           <t>% In50s Score(O)</t>
@@ -58544,11 +58781,14 @@
       <c r="IF80" s="1" t="n">
         <v>29.8</v>
       </c>
-      <c r="IG80" t="n">
+      <c r="IG80" s="1" t="n">
         <v>42.6</v>
       </c>
+      <c r="IH80" t="n">
+        <v>38.7</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="81" s="2">
+    <row r="81" ht="13.8" customHeight="1" s="2">
       <c r="A81" s="1" t="inlineStr">
         <is>
           <t>% In50s Goal(O)</t>
@@ -59271,11 +59511,14 @@
       <c r="IF81" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="IG81" t="n">
+      <c r="IG81" s="1" t="n">
         <v>22.2</v>
       </c>
+      <c r="IH81" t="n">
+        <v>27.4</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="82" s="2">
+    <row r="82" ht="13.8" customHeight="1" s="2">
       <c r="A82" s="1" t="inlineStr">
         <is>
           <t>Height(O)</t>
@@ -59998,11 +60241,14 @@
       <c r="IF82" s="1" t="n">
         <v>187.9</v>
       </c>
-      <c r="IG82" t="n">
+      <c r="IG82" s="1" t="n">
         <v>187.5</v>
       </c>
+      <c r="IH82" t="n">
+        <v>188.9</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="83" s="2">
+    <row r="83" ht="13.8" customHeight="1" s="2">
       <c r="A83" s="1" t="inlineStr">
         <is>
           <t>Weight(O)</t>
@@ -60725,11 +60971,14 @@
       <c r="IF83" s="1" t="n">
         <v>84.7</v>
       </c>
-      <c r="IG83" t="n">
+      <c r="IG83" s="1" t="n">
         <v>85.7</v>
       </c>
+      <c r="IH83" t="n">
+        <v>88.2</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="84" s="2">
+    <row r="84" ht="13.8" customHeight="1" s="2">
       <c r="A84" s="1" t="inlineStr">
         <is>
           <t>Age(O)</t>
@@ -61452,11 +61701,14 @@
       <c r="IF84" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="IG84" t="n">
+      <c r="IG84" s="1" t="n">
         <v>26</v>
       </c>
+      <c r="IH84" t="n">
+        <v>25.91</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="85" s="2">
+    <row r="85" ht="13.8" customHeight="1" s="2">
       <c r="A85" s="1" t="inlineStr">
         <is>
           <t>Av Games(O)</t>
@@ -62179,11 +62431,14 @@
       <c r="IF85" s="1" t="n">
         <v>78.90000000000001</v>
       </c>
-      <c r="IG85" t="n">
+      <c r="IG85" s="1" t="n">
         <v>110</v>
       </c>
+      <c r="IH85" t="n">
+        <v>107.8</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="86" s="2">
+    <row r="86" ht="13.8" customHeight="1" s="2">
       <c r="A86" s="1" t="inlineStr">
         <is>
           <t>&lt;50 Games(O)</t>
@@ -62906,11 +63161,14 @@
       <c r="IF86" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="IG86" t="n">
+      <c r="IG86" s="1" t="n">
         <v>4</v>
       </c>
+      <c r="IH86" t="n">
+        <v>4</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="87" s="2">
+    <row r="87" ht="13.8" customHeight="1" s="2">
       <c r="A87" s="1" t="inlineStr">
         <is>
           <t>50-99 Games(O)</t>
@@ -63633,11 +63891,14 @@
       <c r="IF87" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="IG87" t="n">
+      <c r="IG87" s="1" t="n">
         <v>7</v>
       </c>
+      <c r="IH87" t="n">
+        <v>8</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="88" s="2">
+    <row r="88" ht="13.8" customHeight="1" s="2">
       <c r="A88" s="1" t="inlineStr">
         <is>
           <t>100-149 Games(O)</t>
@@ -64360,11 +64621,14 @@
       <c r="IF88" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="IG88" t="n">
+      <c r="IG88" s="1" t="n">
         <v>7</v>
       </c>
+      <c r="IH88" t="n">
+        <v>5</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="89" s="2">
+    <row r="89" ht="13.8" customHeight="1" s="2">
       <c r="A89" s="1" t="inlineStr">
         <is>
           <t>&gt;150 Games(O)</t>
@@ -65087,11 +65351,14 @@
       <c r="IF89" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="IG89" t="n">
+      <c r="IG89" s="1" t="n">
         <v>5</v>
       </c>
+      <c r="IH89" t="n">
+        <v>5</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="90" s="2">
+    <row r="90" ht="13.8" customHeight="1" s="2">
       <c r="A90" s="1" t="inlineStr">
         <is>
           <t>Contested Poss(O)</t>
@@ -65814,11 +66081,14 @@
       <c r="IF90" s="1" t="n">
         <v>161</v>
       </c>
-      <c r="IG90" t="n">
+      <c r="IG90" s="1" t="n">
         <v>130</v>
       </c>
+      <c r="IH90" t="n">
+        <v>166</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="91" s="2">
+    <row r="91" ht="13.8" customHeight="1" s="2">
       <c r="A91" s="1" t="inlineStr">
         <is>
           <t>Uncontested Poss(O)</t>
@@ -66541,11 +66811,14 @@
       <c r="IF91" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="IG91" t="n">
+      <c r="IG91" s="1" t="n">
         <v>251</v>
       </c>
+      <c r="IH91" t="n">
+        <v>179</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="92" s="2">
+    <row r="92" ht="13.8" customHeight="1" s="2">
       <c r="A92" s="1" t="inlineStr">
         <is>
           <t>Effective Disposals(O)</t>
@@ -67268,11 +67541,14 @@
       <c r="IF92" s="1" t="n">
         <v>241</v>
       </c>
-      <c r="IG92" t="n">
+      <c r="IG92" s="1" t="n">
         <v>275</v>
       </c>
+      <c r="IH92" t="n">
+        <v>240</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="93" s="2">
+    <row r="93" ht="13.8" customHeight="1" s="2">
       <c r="A93" s="1" t="inlineStr">
         <is>
           <t>Disposal Efficiency(O)</t>
@@ -67995,11 +68271,14 @@
       <c r="IF93" s="1" t="n">
         <v>63.3</v>
       </c>
-      <c r="IG93" t="n">
+      <c r="IG93" s="1" t="n">
         <v>72.40000000000001</v>
       </c>
+      <c r="IH93" t="n">
+        <v>68.59999999999999</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="94" s="2">
+    <row r="94" ht="13.8" customHeight="1" s="2">
       <c r="A94" s="1" t="inlineStr">
         <is>
           <t>Clangers2(O)</t>
@@ -68722,11 +69001,14 @@
       <c r="IF94" s="1" t="n">
         <v>74</v>
       </c>
-      <c r="IG94" t="n">
+      <c r="IG94" s="1" t="n">
         <v>54</v>
       </c>
+      <c r="IH94" t="n">
+        <v>47</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="95" s="2">
+    <row r="95" ht="13.8" customHeight="1" s="2">
       <c r="A95" s="1" t="inlineStr">
         <is>
           <t>Contested Marks(O)</t>
@@ -69449,11 +69731,14 @@
       <c r="IF95" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="IG95" t="n">
+      <c r="IG95" s="1" t="n">
         <v>11</v>
       </c>
+      <c r="IH95" t="n">
+        <v>12</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="96" s="2">
+    <row r="96" ht="13.8" customHeight="1" s="2">
       <c r="A96" s="1" t="inlineStr">
         <is>
           <t>Marks Inside 50(O)</t>
@@ -70176,11 +70461,14 @@
       <c r="IF96" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="IG96" t="n">
+      <c r="IG96" s="1" t="n">
         <v>19</v>
       </c>
+      <c r="IH96" t="n">
+        <v>9</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="97" s="2">
+    <row r="97" ht="13.8" customHeight="1" s="2">
       <c r="A97" s="1" t="inlineStr">
         <is>
           <t>Clearances2(O)</t>
@@ -70903,11 +71191,14 @@
       <c r="IF97" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="IG97" t="n">
+      <c r="IG97" s="1" t="n">
         <v>22</v>
       </c>
+      <c r="IH97" t="n">
+        <v>53</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="98" s="2">
+    <row r="98" ht="13.8" customHeight="1" s="2">
       <c r="A98" s="1" t="inlineStr">
         <is>
           <t>Rebound 50s2(O)</t>
@@ -71630,11 +71921,14 @@
       <c r="IF98" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="IG98" t="n">
+      <c r="IG98" s="1" t="n">
         <v>41</v>
       </c>
+      <c r="IH98" t="n">
+        <v>35</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="99" s="2">
+    <row r="99" ht="13.8" customHeight="1" s="2">
       <c r="A99" s="1" t="inlineStr">
         <is>
           <t>1%ers(O)</t>
@@ -72357,11 +72651,14 @@
       <c r="IF99" s="1" t="n">
         <v>73</v>
       </c>
-      <c r="IG99" t="n">
+      <c r="IG99" s="1" t="n">
         <v>54</v>
       </c>
+      <c r="IH99" t="n">
+        <v>55</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="100" s="2">
+    <row r="100" ht="13.8" customHeight="1" s="2">
       <c r="A100" s="1" t="inlineStr">
         <is>
           <t>Bounces(O)</t>
@@ -73084,11 +73381,14 @@
       <c r="IF100" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="IG100" t="n">
+      <c r="IG100" s="1" t="n">
         <v>12</v>
       </c>
+      <c r="IH100" t="n">
+        <v>2</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="101" s="2">
+    <row r="101" ht="13.8" customHeight="1" s="2">
       <c r="A101" s="1" t="inlineStr">
         <is>
           <t>Goals Assists2(O)</t>
@@ -73811,11 +74111,14 @@
       <c r="IF101" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="IG101" t="n">
+      <c r="IG101" s="1" t="n">
         <v>9</v>
       </c>
+      <c r="IH101" t="n">
+        <v>10</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="102" s="2">
+    <row r="102" ht="13.8" customHeight="1" s="2">
       <c r="A102" s="1" t="inlineStr">
         <is>
           <t>Goal Assist %(O)</t>
@@ -74538,13 +74841,16 @@
       <c r="IF102" s="1" t="n">
         <v>37.5</v>
       </c>
-      <c r="IG102" t="n">
+      <c r="IG102" s="1" t="n">
         <v>75</v>
+      </c>
+      <c r="IH102" t="n">
+        <v>58.8</v>
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
-  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="0" useFirstPageNumber="0" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update functions for each main script compiled in a bash script.
</commit_message>
<xml_diff>
--- a/django_AFL_ML/Data/Adelaide_stats.xlsx
+++ b/django_AFL_ML/Data/Adelaide_stats.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:IO102"/>
+  <dimension ref="A1:IP102"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="GZ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="HA23" activeCellId="0" sqref="HA23"/>
@@ -1203,8 +1203,11 @@
       <c r="IN1" s="1" t="n">
         <v>10512</v>
       </c>
-      <c r="IO1" t="n">
+      <c r="IO1" s="1" t="n">
         <v>10524</v>
+      </c>
+      <c r="IP1" t="n">
+        <v>10551</v>
       </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="2">
@@ -1954,8 +1957,11 @@
       <c r="IN2" s="1" t="n">
         <v>2021</v>
       </c>
-      <c r="IO2" t="n">
+      <c r="IO2" s="1" t="n">
         <v>2021</v>
+      </c>
+      <c r="IP2" t="n">
+        <v>2022</v>
       </c>
     </row>
     <row r="3" ht="13.8" customHeight="1" s="2">
@@ -2705,8 +2711,11 @@
       <c r="IN3" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="IO3" t="n">
+      <c r="IO3" s="1" t="n">
         <v>23</v>
+      </c>
+      <c r="IP3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="2">
@@ -3456,7 +3465,10 @@
       <c r="IN4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="IO4" t="n">
+      <c r="IO4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="IP4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4207,8 +4219,11 @@
       <c r="IN5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="IO5" t="n">
+      <c r="IO5" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="IP5" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6" ht="13.8" customHeight="1" s="2">
@@ -4958,8 +4973,11 @@
       <c r="IN6" s="1" t="n">
         <v>63</v>
       </c>
-      <c r="IO6" t="n">
+      <c r="IO6" s="1" t="n">
         <v>98</v>
+      </c>
+      <c r="IP6" t="n">
+        <v>82</v>
       </c>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="2">
@@ -5709,8 +5727,11 @@
       <c r="IN7" s="1" t="n">
         <v>104</v>
       </c>
-      <c r="IO7" t="n">
+      <c r="IO7" s="1" t="n">
         <v>54</v>
+      </c>
+      <c r="IP7" t="n">
+        <v>83</v>
       </c>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="2">
@@ -6460,8 +6481,11 @@
       <c r="IN8" s="1" t="n">
         <v>-41</v>
       </c>
-      <c r="IO8" t="n">
+      <c r="IO8" s="1" t="n">
         <v>44</v>
+      </c>
+      <c r="IP8" t="n">
+        <v>-1</v>
       </c>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="2">
@@ -7211,8 +7235,11 @@
       <c r="IN9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="IO9" t="n">
+      <c r="IO9" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="IP9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10" ht="13.8" customHeight="1" s="2">
@@ -7962,8 +7989,11 @@
       <c r="IN10" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="IO10" t="n">
+      <c r="IO10" s="1" t="n">
         <v>12</v>
+      </c>
+      <c r="IP10" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="11" ht="13.8" customHeight="1" s="2">
@@ -8713,8 +8743,11 @@
       <c r="IN11" s="1" t="n">
         <v>220</v>
       </c>
-      <c r="IO11" t="n">
+      <c r="IO11" s="1" t="n">
         <v>222</v>
+      </c>
+      <c r="IP11" t="n">
+        <v>215</v>
       </c>
     </row>
     <row r="12" ht="13.8" customHeight="1" s="2">
@@ -9464,8 +9497,11 @@
       <c r="IN12" s="1" t="n">
         <v>166</v>
       </c>
-      <c r="IO12" t="n">
+      <c r="IO12" s="1" t="n">
         <v>196</v>
+      </c>
+      <c r="IP12" t="n">
+        <v>144</v>
       </c>
     </row>
     <row r="13" ht="13.8" customHeight="1" s="2">
@@ -10215,8 +10251,11 @@
       <c r="IN13" s="1" t="n">
         <v>386</v>
       </c>
-      <c r="IO13" t="n">
+      <c r="IO13" s="1" t="n">
         <v>418</v>
+      </c>
+      <c r="IP13" t="n">
+        <v>359</v>
       </c>
     </row>
     <row r="14" ht="13.8" customHeight="1" s="2">
@@ -10966,8 +11005,11 @@
       <c r="IN14" s="1" t="n">
         <v>1.33</v>
       </c>
-      <c r="IO14" t="n">
+      <c r="IO14" s="1" t="n">
         <v>1.13</v>
+      </c>
+      <c r="IP14" t="n">
+        <v>1.49</v>
       </c>
     </row>
     <row r="15" ht="13.8" customHeight="1" s="2">
@@ -11717,8 +11759,11 @@
       <c r="IN15" s="1" t="n">
         <v>97</v>
       </c>
-      <c r="IO15" t="n">
+      <c r="IO15" s="1" t="n">
         <v>90</v>
+      </c>
+      <c r="IP15" t="n">
+        <v>92</v>
       </c>
     </row>
     <row r="16" ht="13.8" customHeight="1" s="2">
@@ -12468,8 +12513,11 @@
       <c r="IN16" s="1" t="n">
         <v>63</v>
       </c>
-      <c r="IO16" t="n">
+      <c r="IO16" s="1" t="n">
         <v>57</v>
+      </c>
+      <c r="IP16" t="n">
+        <v>51</v>
       </c>
     </row>
     <row r="17" ht="13.8" customHeight="1" s="2">
@@ -13219,8 +13267,11 @@
       <c r="IN17" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="IO17" t="n">
+      <c r="IO17" s="1" t="n">
         <v>37</v>
+      </c>
+      <c r="IP17" t="n">
+        <v>29</v>
       </c>
     </row>
     <row r="18" ht="13.8" customHeight="1" s="2">
@@ -13970,8 +14021,11 @@
       <c r="IN18" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="IO18" t="n">
+      <c r="IO18" s="1" t="n">
         <v>14</v>
+      </c>
+      <c r="IP18" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="19" ht="13.8" customHeight="1" s="2">
@@ -14721,8 +14775,11 @@
       <c r="IN19" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="IO19" t="n">
+      <c r="IO19" s="1" t="n">
         <v>19</v>
+      </c>
+      <c r="IP19" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="20" ht="13.8" customHeight="1" s="2">
@@ -15472,8 +15529,11 @@
       <c r="IN20" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="IO20" t="n">
+      <c r="IO20" s="1" t="n">
         <v>13</v>
+      </c>
+      <c r="IP20" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="21" ht="13.8" customHeight="1" s="2">
@@ -16223,8 +16283,11 @@
       <c r="IN21" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="IO21" t="n">
+      <c r="IO21" s="1" t="n">
         <v>9</v>
+      </c>
+      <c r="IP21" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="22" ht="13.8" customHeight="1" s="2">
@@ -16974,8 +17037,11 @@
       <c r="IN22" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="IO22" t="n">
+      <c r="IO22" s="1" t="n">
         <v>17</v>
+      </c>
+      <c r="IP22" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="23" ht="13.8" customHeight="1" s="2">
@@ -17725,8 +17791,11 @@
       <c r="IN23" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="IO23" t="n">
+      <c r="IO23" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="IP23" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="24" ht="13.8" customHeight="1" s="2">
@@ -18476,8 +18545,11 @@
       <c r="IN24" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="IO24" t="n">
+      <c r="IO24" s="1" t="n">
         <v>33</v>
+      </c>
+      <c r="IP24" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="25" ht="13.8" customHeight="1" s="2">
@@ -19227,8 +19299,11 @@
       <c r="IN25" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="IO25" t="n">
+      <c r="IO25" s="1" t="n">
         <v>39.4</v>
+      </c>
+      <c r="IP25" t="n">
+        <v>54.5</v>
       </c>
     </row>
     <row r="26" ht="13.8" customHeight="1" s="2">
@@ -19978,8 +20053,11 @@
       <c r="IN26" s="1" t="n">
         <v>42.89</v>
       </c>
-      <c r="IO26" t="n">
+      <c r="IO26" s="1" t="n">
         <v>32.15</v>
+      </c>
+      <c r="IP26" t="n">
+        <v>29.92</v>
       </c>
     </row>
     <row r="27" ht="13.8" customHeight="1" s="2">
@@ -20729,8 +20807,11 @@
       <c r="IN27" s="1" t="n">
         <v>21.44</v>
       </c>
-      <c r="IO27" t="n">
+      <c r="IO27" s="1" t="n">
         <v>12.67</v>
+      </c>
+      <c r="IP27" t="n">
+        <v>16.32</v>
       </c>
     </row>
     <row r="28" ht="13.8" customHeight="1" s="2">
@@ -21480,8 +21561,11 @@
       <c r="IN28" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="IO28" t="n">
+      <c r="IO28" s="1" t="n">
         <v>42</v>
+      </c>
+      <c r="IP28" t="n">
+        <v>35</v>
       </c>
     </row>
     <row r="29" ht="13.8" customHeight="1" s="2">
@@ -22231,7 +22315,10 @@
       <c r="IN29" s="1" t="n">
         <v>64</v>
       </c>
-      <c r="IO29" t="n">
+      <c r="IO29" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="IP29" t="n">
         <v>55</v>
       </c>
     </row>
@@ -22982,8 +23069,11 @@
       <c r="IN30" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="IO30" t="n">
+      <c r="IO30" s="1" t="n">
         <v>28</v>
+      </c>
+      <c r="IP30" t="n">
+        <v>43</v>
       </c>
     </row>
     <row r="31" ht="13.8" customHeight="1" s="2">
@@ -23733,8 +23823,11 @@
       <c r="IN31" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="IO31" t="n">
+      <c r="IO31" s="1" t="n">
         <v>57</v>
+      </c>
+      <c r="IP31" t="n">
+        <v>48</v>
       </c>
     </row>
     <row r="32" ht="13.8" customHeight="1" s="2">
@@ -24484,8 +24577,11 @@
       <c r="IN32" s="1" t="n">
         <v>2.61</v>
       </c>
-      <c r="IO32" t="n">
+      <c r="IO32" s="1" t="n">
         <v>1.73</v>
+      </c>
+      <c r="IP32" t="n">
+        <v>2.18</v>
       </c>
     </row>
     <row r="33" ht="13.8" customHeight="1" s="2">
@@ -25235,8 +25331,11 @@
       <c r="IN33" s="1" t="n">
         <v>5.22</v>
       </c>
-      <c r="IO33" t="n">
+      <c r="IO33" s="1" t="n">
         <v>4.38</v>
+      </c>
+      <c r="IP33" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="34" ht="13.8" customHeight="1" s="2">
@@ -25986,8 +26085,11 @@
       <c r="IN34" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="IO34" t="n">
+      <c r="IO34" s="1" t="n">
         <v>52.6</v>
+      </c>
+      <c r="IP34" t="n">
+        <v>45.8</v>
       </c>
     </row>
     <row r="35" ht="13.8" customHeight="1" s="2">
@@ -26737,8 +26839,11 @@
       <c r="IN35" s="1" t="n">
         <v>19.1</v>
       </c>
-      <c r="IO35" t="n">
+      <c r="IO35" s="1" t="n">
         <v>22.8</v>
+      </c>
+      <c r="IP35" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="36" ht="13.8" customHeight="1" s="2">
@@ -27488,8 +27593,11 @@
       <c r="IN36" s="1" t="n">
         <v>187.7</v>
       </c>
-      <c r="IO36" t="n">
+      <c r="IO36" s="1" t="n">
         <v>187.7</v>
+      </c>
+      <c r="IP36" t="n">
+        <v>187.2</v>
       </c>
     </row>
     <row r="37" ht="13.8" customHeight="1" s="2">
@@ -28239,8 +28347,11 @@
       <c r="IN37" s="1" t="n">
         <v>84.5</v>
       </c>
-      <c r="IO37" t="n">
+      <c r="IO37" s="1" t="n">
         <v>83.7</v>
+      </c>
+      <c r="IP37" t="n">
+        <v>87</v>
       </c>
     </row>
     <row r="38" ht="13.8" customHeight="1" s="2">
@@ -28990,8 +29101,11 @@
       <c r="IN38" s="1" t="n">
         <v>24.33</v>
       </c>
-      <c r="IO38" t="n">
+      <c r="IO38" s="1" t="n">
         <v>24.66</v>
+      </c>
+      <c r="IP38" t="n">
+        <v>23.8</v>
       </c>
     </row>
     <row r="39" ht="13.8" customHeight="1" s="2">
@@ -29741,8 +29855,11 @@
       <c r="IN39" s="1" t="n">
         <v>66.3</v>
       </c>
-      <c r="IO39" t="n">
+      <c r="IO39" s="1" t="n">
         <v>72.5</v>
+      </c>
+      <c r="IP39" t="n">
+        <v>58.5</v>
       </c>
     </row>
     <row r="40" ht="13.8" customHeight="1" s="2">
@@ -30492,8 +30609,11 @@
       <c r="IN40" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="IO40" t="n">
+      <c r="IO40" s="1" t="n">
         <v>13</v>
+      </c>
+      <c r="IP40" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="41" ht="13.8" customHeight="1" s="2">
@@ -31243,8 +31363,11 @@
       <c r="IN41" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="IO41" t="n">
+      <c r="IO41" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="IP41" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="42" ht="13.8" customHeight="1" s="2">
@@ -31994,7 +32117,10 @@
       <c r="IN42" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="IO42" t="n">
+      <c r="IO42" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="IP42" t="n">
         <v>1</v>
       </c>
     </row>
@@ -32745,8 +32871,11 @@
       <c r="IN43" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="IO43" t="n">
+      <c r="IO43" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="IP43" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="44" ht="13.8" customHeight="1" s="2">
@@ -33496,8 +33625,11 @@
       <c r="IN44" s="1" t="n">
         <v>139</v>
       </c>
-      <c r="IO44" t="n">
+      <c r="IO44" s="1" t="n">
         <v>152</v>
+      </c>
+      <c r="IP44" t="n">
+        <v>143</v>
       </c>
     </row>
     <row r="45" ht="13.8" customHeight="1" s="2">
@@ -34247,8 +34379,11 @@
       <c r="IN45" s="1" t="n">
         <v>244</v>
       </c>
-      <c r="IO45" t="n">
+      <c r="IO45" s="1" t="n">
         <v>266</v>
+      </c>
+      <c r="IP45" t="n">
+        <v>219</v>
       </c>
     </row>
     <row r="46" ht="13.8" customHeight="1" s="2">
@@ -34998,8 +35133,11 @@
       <c r="IN46" s="1" t="n">
         <v>289</v>
       </c>
-      <c r="IO46" t="n">
+      <c r="IO46" s="1" t="n">
         <v>317</v>
+      </c>
+      <c r="IP46" t="n">
+        <v>259</v>
       </c>
     </row>
     <row r="47" ht="13.8" customHeight="1" s="2">
@@ -35749,8 +35887,11 @@
       <c r="IN47" s="1" t="n">
         <v>74.90000000000001</v>
       </c>
-      <c r="IO47" t="n">
+      <c r="IO47" s="1" t="n">
         <v>75.8</v>
+      </c>
+      <c r="IP47" t="n">
+        <v>72.09999999999999</v>
       </c>
     </row>
     <row r="48" ht="13.8" customHeight="1" s="2">
@@ -36500,7 +36641,10 @@
       <c r="IN48" s="1" t="n">
         <v>64</v>
       </c>
-      <c r="IO48" t="n">
+      <c r="IO48" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="IP48" t="n">
         <v>55</v>
       </c>
     </row>
@@ -37251,8 +37395,11 @@
       <c r="IN49" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="IO49" t="n">
+      <c r="IO49" s="1" t="n">
         <v>14</v>
+      </c>
+      <c r="IP49" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="50" ht="13.8" customHeight="1" s="2">
@@ -38002,8 +38149,11 @@
       <c r="IN50" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="IO50" t="n">
+      <c r="IO50" s="1" t="n">
         <v>22</v>
+      </c>
+      <c r="IP50" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="51" ht="13.8" customHeight="1" s="2">
@@ -38753,8 +38903,11 @@
       <c r="IN51" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="IO51" t="n">
+      <c r="IO51" s="1" t="n">
         <v>42</v>
+      </c>
+      <c r="IP51" t="n">
+        <v>35</v>
       </c>
     </row>
     <row r="52" ht="13.8" customHeight="1" s="2">
@@ -39504,8 +39657,11 @@
       <c r="IN52" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="IO52" t="n">
+      <c r="IO52" s="1" t="n">
         <v>28</v>
+      </c>
+      <c r="IP52" t="n">
+        <v>43</v>
       </c>
     </row>
     <row r="53" ht="13.8" customHeight="1" s="2">
@@ -40255,8 +40411,11 @@
       <c r="IN53" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="IO53" t="n">
+      <c r="IO53" s="1" t="n">
         <v>36</v>
+      </c>
+      <c r="IP53" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="54" ht="13.8" customHeight="1" s="2">
@@ -41006,8 +41165,11 @@
       <c r="IN54" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="IO54" t="n">
+      <c r="IO54" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="IP54" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="55" ht="13.8" customHeight="1" s="2">
@@ -41757,8 +41919,11 @@
       <c r="IN55" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="IO55" t="n">
+      <c r="IO55" s="1" t="n">
         <v>9</v>
+      </c>
+      <c r="IP55" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="56" ht="13.8" customHeight="1" s="2">
@@ -42508,8 +42673,11 @@
       <c r="IN56" s="1" t="n">
         <v>66.7</v>
       </c>
-      <c r="IO56" t="n">
+      <c r="IO56" s="1" t="n">
         <v>69.2</v>
+      </c>
+      <c r="IP56" t="n">
+        <v>58.3</v>
       </c>
     </row>
     <row r="57" ht="13.8" customHeight="1" s="2">
@@ -43259,7 +43427,10 @@
       <c r="IN57" s="1" t="n">
         <v>215</v>
       </c>
-      <c r="IO57" t="n">
+      <c r="IO57" s="1" t="n">
+        <v>175</v>
+      </c>
+      <c r="IP57" t="n">
         <v>175</v>
       </c>
     </row>
@@ -44010,8 +44181,11 @@
       <c r="IN58" s="1" t="n">
         <v>137</v>
       </c>
-      <c r="IO58" t="n">
+      <c r="IO58" s="1" t="n">
         <v>140</v>
+      </c>
+      <c r="IP58" t="n">
+        <v>138</v>
       </c>
     </row>
     <row r="59" ht="13.8" customHeight="1" s="2">
@@ -44761,8 +44935,11 @@
       <c r="IN59" s="1" t="n">
         <v>352</v>
       </c>
-      <c r="IO59" t="n">
+      <c r="IO59" s="1" t="n">
         <v>315</v>
+      </c>
+      <c r="IP59" t="n">
+        <v>313</v>
       </c>
     </row>
     <row r="60" ht="13.8" customHeight="1" s="2">
@@ -45512,8 +45689,11 @@
       <c r="IN60" s="1" t="n">
         <v>1.57</v>
       </c>
-      <c r="IO60" t="n">
+      <c r="IO60" s="1" t="n">
         <v>1.25</v>
+      </c>
+      <c r="IP60" t="n">
+        <v>1.27</v>
       </c>
     </row>
     <row r="61" ht="13.8" customHeight="1" s="2">
@@ -46263,8 +46443,11 @@
       <c r="IN61" s="1" t="n">
         <v>92</v>
       </c>
-      <c r="IO61" t="n">
+      <c r="IO61" s="1" t="n">
         <v>69</v>
+      </c>
+      <c r="IP61" t="n">
+        <v>73</v>
       </c>
     </row>
     <row r="62" ht="13.8" customHeight="1" s="2">
@@ -47014,8 +47197,11 @@
       <c r="IN62" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="IO62" t="n">
+      <c r="IO62" s="1" t="n">
         <v>67</v>
+      </c>
+      <c r="IP62" t="n">
+        <v>58</v>
       </c>
     </row>
     <row r="63" ht="13.8" customHeight="1" s="2">
@@ -47765,8 +47951,11 @@
       <c r="IN63" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="IO63" t="n">
+      <c r="IO63" s="1" t="n">
         <v>45</v>
+      </c>
+      <c r="IP63" t="n">
+        <v>41</v>
       </c>
     </row>
     <row r="64" ht="13.8" customHeight="1" s="2">
@@ -48516,8 +48705,11 @@
       <c r="IN64" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="IO64" t="n">
+      <c r="IO64" s="1" t="n">
         <v>19</v>
+      </c>
+      <c r="IP64" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="65" ht="13.8" customHeight="1" s="2">
@@ -49267,8 +49459,11 @@
       <c r="IN65" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="IO65" t="n">
+      <c r="IO65" s="1" t="n">
         <v>14</v>
+      </c>
+      <c r="IP65" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="66" ht="13.8" customHeight="1" s="2">
@@ -50018,8 +50213,11 @@
       <c r="IN66" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="IO66" t="n">
+      <c r="IO66" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="IP66" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="67" ht="13.8" customHeight="1" s="2">
@@ -50769,8 +50967,11 @@
       <c r="IN67" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="IO67" t="n">
+      <c r="IO67" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="IP67" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="68" ht="13.8" customHeight="1" s="2">
@@ -51520,8 +51721,11 @@
       <c r="IN68" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="IO68" t="n">
+      <c r="IO68" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="IP68" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="69" ht="13.8" customHeight="1" s="2">
@@ -52271,8 +52475,11 @@
       <c r="IN69" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="IO69" t="n">
+      <c r="IO69" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="IP69" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="70" ht="13.8" customHeight="1" s="2">
@@ -53022,8 +53229,11 @@
       <c r="IN70" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="IO70" t="n">
+      <c r="IO70" s="1" t="n">
         <v>14</v>
+      </c>
+      <c r="IP70" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="71" ht="13.8" customHeight="1" s="2">
@@ -53773,8 +53983,11 @@
       <c r="IN71" s="1" t="n">
         <v>66.7</v>
       </c>
-      <c r="IO71" t="n">
+      <c r="IO71" s="1" t="n">
         <v>57.1</v>
+      </c>
+      <c r="IP71" t="n">
+        <v>39.3</v>
       </c>
     </row>
     <row r="72" ht="13.8" customHeight="1" s="2">
@@ -54524,8 +54737,11 @@
       <c r="IN72" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="IO72" t="n">
+      <c r="IO72" s="1" t="n">
         <v>39.38</v>
+      </c>
+      <c r="IP72" t="n">
+        <v>28.45</v>
       </c>
     </row>
     <row r="73" ht="13.8" customHeight="1" s="2">
@@ -55275,8 +55491,11 @@
       <c r="IN73" s="1" t="n">
         <v>14.67</v>
       </c>
-      <c r="IO73" t="n">
+      <c r="IO73" s="1" t="n">
         <v>22.5</v>
+      </c>
+      <c r="IP73" t="n">
+        <v>11.18</v>
       </c>
     </row>
     <row r="74" ht="13.8" customHeight="1" s="2">
@@ -56026,8 +56245,11 @@
       <c r="IN74" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="IO74" t="n">
+      <c r="IO74" s="1" t="n">
         <v>26</v>
+      </c>
+      <c r="IP74" t="n">
+        <v>38</v>
       </c>
     </row>
     <row r="75" ht="13.8" customHeight="1" s="2">
@@ -56777,8 +56999,11 @@
       <c r="IN75" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="IO75" t="n">
+      <c r="IO75" s="1" t="n">
         <v>57</v>
+      </c>
+      <c r="IP75" t="n">
+        <v>61</v>
       </c>
     </row>
     <row r="76" ht="13.8" customHeight="1" s="2">
@@ -57528,8 +57753,11 @@
       <c r="IN76" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="IO76" t="n">
+      <c r="IO76" s="1" t="n">
         <v>42</v>
+      </c>
+      <c r="IP76" t="n">
+        <v>36</v>
       </c>
     </row>
     <row r="77" ht="13.8" customHeight="1" s="2">
@@ -58279,8 +58507,11 @@
       <c r="IN77" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="IO77" t="n">
+      <c r="IO77" s="1" t="n">
         <v>37</v>
+      </c>
+      <c r="IP77" t="n">
+        <v>55</v>
       </c>
     </row>
     <row r="78" ht="13.8" customHeight="1" s="2">
@@ -59030,8 +59261,11 @@
       <c r="IN78" s="1" t="n">
         <v>2.46</v>
       </c>
-      <c r="IO78" t="n">
+      <c r="IO78" s="1" t="n">
         <v>2.64</v>
+      </c>
+      <c r="IP78" t="n">
+        <v>1.96</v>
       </c>
     </row>
     <row r="79" ht="13.8" customHeight="1" s="2">
@@ -59781,8 +60015,11 @@
       <c r="IN79" s="1" t="n">
         <v>3.69</v>
       </c>
-      <c r="IO79" t="n">
+      <c r="IO79" s="1" t="n">
         <v>4.62</v>
+      </c>
+      <c r="IP79" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="80" ht="13.8" customHeight="1" s="2">
@@ -60532,8 +60769,11 @@
       <c r="IN80" s="1" t="n">
         <v>40.7</v>
       </c>
-      <c r="IO80" t="n">
+      <c r="IO80" s="1" t="n">
         <v>35.1</v>
+      </c>
+      <c r="IP80" t="n">
+        <v>47.3</v>
       </c>
     </row>
     <row r="81" ht="13.8" customHeight="1" s="2">
@@ -61283,8 +61523,11 @@
       <c r="IN81" s="1" t="n">
         <v>27.1</v>
       </c>
-      <c r="IO81" t="n">
+      <c r="IO81" s="1" t="n">
         <v>21.6</v>
+      </c>
+      <c r="IP81" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="82" ht="13.8" customHeight="1" s="2">
@@ -62034,8 +62277,11 @@
       <c r="IN82" s="1" t="n">
         <v>187.1</v>
       </c>
-      <c r="IO82" t="n">
+      <c r="IO82" s="1" t="n">
         <v>187.6</v>
+      </c>
+      <c r="IP82" t="n">
+        <v>188.7</v>
       </c>
     </row>
     <row r="83" ht="13.8" customHeight="1" s="2">
@@ -62785,8 +63031,11 @@
       <c r="IN83" s="1" t="n">
         <v>84.40000000000001</v>
       </c>
-      <c r="IO83" t="n">
+      <c r="IO83" s="1" t="n">
         <v>83.90000000000001</v>
+      </c>
+      <c r="IP83" t="n">
+        <v>88.3</v>
       </c>
     </row>
     <row r="84" ht="13.8" customHeight="1" s="2">
@@ -63536,7 +63785,10 @@
       <c r="IN84" s="1" t="n">
         <v>24.49</v>
       </c>
-      <c r="IO84" t="n">
+      <c r="IO84" s="1" t="n">
+        <v>24.49</v>
+      </c>
+      <c r="IP84" t="n">
         <v>24.49</v>
       </c>
     </row>
@@ -64287,8 +64539,11 @@
       <c r="IN85" s="1" t="n">
         <v>86.2</v>
       </c>
-      <c r="IO85" t="n">
+      <c r="IO85" s="1" t="n">
         <v>83.2</v>
+      </c>
+      <c r="IP85" t="n">
+        <v>67.3</v>
       </c>
     </row>
     <row r="86" ht="13.8" customHeight="1" s="2">
@@ -65038,8 +65293,11 @@
       <c r="IN86" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="IO86" t="n">
+      <c r="IO86" s="1" t="n">
         <v>9</v>
+      </c>
+      <c r="IP86" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="87" ht="13.8" customHeight="1" s="2">
@@ -65789,8 +66047,11 @@
       <c r="IN87" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="IO87" t="n">
+      <c r="IO87" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="IP87" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="88" ht="13.8" customHeight="1" s="2">
@@ -66540,8 +66801,11 @@
       <c r="IN88" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="IO88" t="n">
+      <c r="IO88" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="IP88" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="89" ht="13.8" customHeight="1" s="2">
@@ -67291,8 +67555,11 @@
       <c r="IN89" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="IO89" t="n">
+      <c r="IO89" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="IP89" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="90" ht="13.8" customHeight="1" s="2">
@@ -68042,8 +68309,11 @@
       <c r="IN90" s="1" t="n">
         <v>139</v>
       </c>
-      <c r="IO90" t="n">
+      <c r="IO90" s="1" t="n">
         <v>111</v>
+      </c>
+      <c r="IP90" t="n">
+        <v>129</v>
       </c>
     </row>
     <row r="91" ht="13.8" customHeight="1" s="2">
@@ -68793,8 +69063,11 @@
       <c r="IN91" s="1" t="n">
         <v>204</v>
       </c>
-      <c r="IO91" t="n">
+      <c r="IO91" s="1" t="n">
         <v>190</v>
+      </c>
+      <c r="IP91" t="n">
+        <v>187</v>
       </c>
     </row>
     <row r="92" ht="13.8" customHeight="1" s="2">
@@ -69544,8 +69817,11 @@
       <c r="IN92" s="1" t="n">
         <v>254</v>
       </c>
-      <c r="IO92" t="n">
+      <c r="IO92" s="1" t="n">
         <v>226</v>
+      </c>
+      <c r="IP92" t="n">
+        <v>237</v>
       </c>
     </row>
     <row r="93" ht="13.8" customHeight="1" s="2">
@@ -70295,8 +70571,11 @@
       <c r="IN93" s="1" t="n">
         <v>72.2</v>
       </c>
-      <c r="IO93" t="n">
+      <c r="IO93" s="1" t="n">
         <v>71.7</v>
+      </c>
+      <c r="IP93" t="n">
+        <v>75.7</v>
       </c>
     </row>
     <row r="94" ht="13.8" customHeight="1" s="2">
@@ -71046,8 +71325,11 @@
       <c r="IN94" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="IO94" t="n">
+      <c r="IO94" s="1" t="n">
         <v>57</v>
+      </c>
+      <c r="IP94" t="n">
+        <v>61</v>
       </c>
     </row>
     <row r="95" ht="13.8" customHeight="1" s="2">
@@ -71797,8 +72079,11 @@
       <c r="IN95" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="IO95" t="n">
+      <c r="IO95" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="IP95" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="96" ht="13.8" customHeight="1" s="2">
@@ -72548,8 +72833,11 @@
       <c r="IN96" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="IO96" t="n">
+      <c r="IO96" s="1" t="n">
         <v>9</v>
+      </c>
+      <c r="IP96" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="97" ht="13.8" customHeight="1" s="2">
@@ -73299,8 +73587,11 @@
       <c r="IN97" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="IO97" t="n">
+      <c r="IO97" s="1" t="n">
         <v>26</v>
+      </c>
+      <c r="IP97" t="n">
+        <v>38</v>
       </c>
     </row>
     <row r="98" ht="13.8" customHeight="1" s="2">
@@ -74050,8 +74341,11 @@
       <c r="IN98" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="IO98" t="n">
+      <c r="IO98" s="1" t="n">
         <v>42</v>
+      </c>
+      <c r="IP98" t="n">
+        <v>36</v>
       </c>
     </row>
     <row r="99" ht="13.8" customHeight="1" s="2">
@@ -74801,8 +75095,11 @@
       <c r="IN99" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="IO99" t="n">
+      <c r="IO99" s="1" t="n">
         <v>44</v>
+      </c>
+      <c r="IP99" t="n">
+        <v>57</v>
       </c>
     </row>
     <row r="100" ht="13.8" customHeight="1" s="2">
@@ -75552,8 +75849,11 @@
       <c r="IN100" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="IO100" t="n">
+      <c r="IO100" s="1" t="n">
         <v>12</v>
+      </c>
+      <c r="IP100" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="101" ht="13.8" customHeight="1" s="2">
@@ -76303,8 +76603,11 @@
       <c r="IN101" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="IO101" t="n">
+      <c r="IO101" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="IP101" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="102" ht="13.8" customHeight="1" s="2">
@@ -77054,8 +77357,11 @@
       <c r="IN102" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="IO102" t="n">
+      <c r="IO102" s="1" t="n">
         <v>37.5</v>
+      </c>
+      <c r="IP102" t="n">
+        <v>72.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Easy round by round update. Round 2 2022 predictions done
</commit_message>
<xml_diff>
--- a/django_AFL_ML/Data/Adelaide_stats.xlsx
+++ b/django_AFL_ML/Data/Adelaide_stats.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:IP102"/>
+  <dimension ref="A1:IQ102"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="GZ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="HA23" activeCellId="0" sqref="HA23"/>
@@ -1206,8 +1206,11 @@
       <c r="IO1" s="1" t="n">
         <v>10524</v>
       </c>
-      <c r="IP1" t="n">
+      <c r="IP1" s="1" t="n">
         <v>10551</v>
+      </c>
+      <c r="IQ1" t="n">
+        <v>10555</v>
       </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="2">
@@ -1960,7 +1963,10 @@
       <c r="IO2" s="1" t="n">
         <v>2021</v>
       </c>
-      <c r="IP2" t="n">
+      <c r="IP2" s="1" t="n">
+        <v>2022</v>
+      </c>
+      <c r="IQ2" t="n">
         <v>2022</v>
       </c>
     </row>
@@ -2714,8 +2720,11 @@
       <c r="IO3" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="IP3" t="n">
+      <c r="IP3" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="IQ3" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="2">
@@ -3468,8 +3477,11 @@
       <c r="IO4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="IP4" t="n">
+      <c r="IP4" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="IQ4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5" ht="13.8" customHeight="1" s="2">
@@ -4222,8 +4234,11 @@
       <c r="IO5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="IP5" t="n">
+      <c r="IP5" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="IQ5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6" ht="13.8" customHeight="1" s="2">
@@ -4976,8 +4991,11 @@
       <c r="IO6" s="1" t="n">
         <v>98</v>
       </c>
-      <c r="IP6" t="n">
+      <c r="IP6" s="1" t="n">
         <v>82</v>
+      </c>
+      <c r="IQ6" t="n">
+        <v>58</v>
       </c>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="2">
@@ -5730,8 +5748,11 @@
       <c r="IO7" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="IP7" t="n">
+      <c r="IP7" s="1" t="n">
         <v>83</v>
+      </c>
+      <c r="IQ7" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="2">
@@ -6484,8 +6505,11 @@
       <c r="IO8" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="IP8" t="n">
+      <c r="IP8" s="1" t="n">
         <v>-1</v>
+      </c>
+      <c r="IQ8" t="n">
+        <v>-42</v>
       </c>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="2">
@@ -7238,7 +7262,10 @@
       <c r="IO9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="IP9" t="n">
+      <c r="IP9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="IQ9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7992,8 +8019,11 @@
       <c r="IO10" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="IP10" t="n">
+      <c r="IP10" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="IQ10" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="11" ht="13.8" customHeight="1" s="2">
@@ -8746,8 +8776,11 @@
       <c r="IO11" s="1" t="n">
         <v>222</v>
       </c>
-      <c r="IP11" t="n">
+      <c r="IP11" s="1" t="n">
         <v>215</v>
+      </c>
+      <c r="IQ11" t="n">
+        <v>220</v>
       </c>
     </row>
     <row r="12" ht="13.8" customHeight="1" s="2">
@@ -9500,8 +9533,11 @@
       <c r="IO12" s="1" t="n">
         <v>196</v>
       </c>
-      <c r="IP12" t="n">
+      <c r="IP12" s="1" t="n">
         <v>144</v>
+      </c>
+      <c r="IQ12" t="n">
+        <v>169</v>
       </c>
     </row>
     <row r="13" ht="13.8" customHeight="1" s="2">
@@ -10254,8 +10290,11 @@
       <c r="IO13" s="1" t="n">
         <v>418</v>
       </c>
-      <c r="IP13" t="n">
+      <c r="IP13" s="1" t="n">
         <v>359</v>
+      </c>
+      <c r="IQ13" t="n">
+        <v>389</v>
       </c>
     </row>
     <row r="14" ht="13.8" customHeight="1" s="2">
@@ -11008,8 +11047,11 @@
       <c r="IO14" s="1" t="n">
         <v>1.13</v>
       </c>
-      <c r="IP14" t="n">
+      <c r="IP14" s="1" t="n">
         <v>1.49</v>
+      </c>
+      <c r="IQ14" t="n">
+        <v>1.3</v>
       </c>
     </row>
     <row r="15" ht="13.8" customHeight="1" s="2">
@@ -11762,8 +11804,11 @@
       <c r="IO15" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="IP15" t="n">
+      <c r="IP15" s="1" t="n">
         <v>92</v>
+      </c>
+      <c r="IQ15" t="n">
+        <v>102</v>
       </c>
     </row>
     <row r="16" ht="13.8" customHeight="1" s="2">
@@ -12516,8 +12561,11 @@
       <c r="IO16" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="IP16" t="n">
+      <c r="IP16" s="1" t="n">
         <v>51</v>
+      </c>
+      <c r="IQ16" t="n">
+        <v>53</v>
       </c>
     </row>
     <row r="17" ht="13.8" customHeight="1" s="2">
@@ -13270,8 +13318,11 @@
       <c r="IO17" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="IP17" t="n">
+      <c r="IP17" s="1" t="n">
         <v>29</v>
+      </c>
+      <c r="IQ17" t="n">
+        <v>33</v>
       </c>
     </row>
     <row r="18" ht="13.8" customHeight="1" s="2">
@@ -14024,8 +14075,11 @@
       <c r="IO18" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="IP18" t="n">
+      <c r="IP18" s="1" t="n">
         <v>32</v>
+      </c>
+      <c r="IQ18" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="19" ht="13.8" customHeight="1" s="2">
@@ -14778,8 +14832,11 @@
       <c r="IO19" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="IP19" t="n">
+      <c r="IP19" s="1" t="n">
         <v>15</v>
+      </c>
+      <c r="IQ19" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="20" ht="13.8" customHeight="1" s="2">
@@ -15532,8 +15589,11 @@
       <c r="IO20" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="IP20" t="n">
+      <c r="IP20" s="1" t="n">
         <v>12</v>
+      </c>
+      <c r="IQ20" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="21" ht="13.8" customHeight="1" s="2">
@@ -16286,8 +16346,11 @@
       <c r="IO21" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="IP21" t="n">
+      <c r="IP21" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="IQ21" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="22" ht="13.8" customHeight="1" s="2">
@@ -17040,8 +17103,11 @@
       <c r="IO22" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="IP22" t="n">
+      <c r="IP22" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="IQ22" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="23" ht="13.8" customHeight="1" s="2">
@@ -17794,8 +17860,11 @@
       <c r="IO23" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="IP23" t="n">
+      <c r="IP23" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="IQ23" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="24" ht="13.8" customHeight="1" s="2">
@@ -18548,8 +18617,11 @@
       <c r="IO24" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="IP24" t="n">
+      <c r="IP24" s="1" t="n">
         <v>22</v>
+      </c>
+      <c r="IQ24" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="25" ht="13.8" customHeight="1" s="2">
@@ -19302,8 +19374,11 @@
       <c r="IO25" s="1" t="n">
         <v>39.4</v>
       </c>
-      <c r="IP25" t="n">
+      <c r="IP25" s="1" t="n">
         <v>54.5</v>
+      </c>
+      <c r="IQ25" t="n">
+        <v>44.4</v>
       </c>
     </row>
     <row r="26" ht="13.8" customHeight="1" s="2">
@@ -20056,8 +20131,11 @@
       <c r="IO26" s="1" t="n">
         <v>32.15</v>
       </c>
-      <c r="IP26" t="n">
+      <c r="IP26" s="1" t="n">
         <v>29.92</v>
+      </c>
+      <c r="IQ26" t="n">
+        <v>48.62</v>
       </c>
     </row>
     <row r="27" ht="13.8" customHeight="1" s="2">
@@ -20810,8 +20888,11 @@
       <c r="IO27" s="1" t="n">
         <v>12.67</v>
       </c>
-      <c r="IP27" t="n">
+      <c r="IP27" s="1" t="n">
         <v>16.32</v>
+      </c>
+      <c r="IQ27" t="n">
+        <v>21.61</v>
       </c>
     </row>
     <row r="28" ht="13.8" customHeight="1" s="2">
@@ -21564,8 +21645,11 @@
       <c r="IO28" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="IP28" t="n">
+      <c r="IP28" s="1" t="n">
         <v>35</v>
+      </c>
+      <c r="IQ28" t="n">
+        <v>36</v>
       </c>
     </row>
     <row r="29" ht="13.8" customHeight="1" s="2">
@@ -22318,8 +22402,11 @@
       <c r="IO29" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="IP29" t="n">
+      <c r="IP29" s="1" t="n">
         <v>55</v>
+      </c>
+      <c r="IQ29" t="n">
+        <v>69</v>
       </c>
     </row>
     <row r="30" ht="13.8" customHeight="1" s="2">
@@ -23072,8 +23159,11 @@
       <c r="IO30" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="IP30" t="n">
+      <c r="IP30" s="1" t="n">
         <v>43</v>
+      </c>
+      <c r="IQ30" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="31" ht="13.8" customHeight="1" s="2">
@@ -23826,8 +23916,11 @@
       <c r="IO31" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="IP31" t="n">
+      <c r="IP31" s="1" t="n">
         <v>48</v>
+      </c>
+      <c r="IQ31" t="n">
+        <v>51</v>
       </c>
     </row>
     <row r="32" ht="13.8" customHeight="1" s="2">
@@ -24580,8 +24673,11 @@
       <c r="IO32" s="1" t="n">
         <v>1.73</v>
       </c>
-      <c r="IP32" t="n">
+      <c r="IP32" s="1" t="n">
         <v>2.18</v>
+      </c>
+      <c r="IQ32" t="n">
+        <v>2.83</v>
       </c>
     </row>
     <row r="33" ht="13.8" customHeight="1" s="2">
@@ -25334,8 +25430,11 @@
       <c r="IO33" s="1" t="n">
         <v>4.38</v>
       </c>
-      <c r="IP33" t="n">
+      <c r="IP33" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="IQ33" t="n">
+        <v>6.38</v>
       </c>
     </row>
     <row r="34" ht="13.8" customHeight="1" s="2">
@@ -26088,8 +26187,11 @@
       <c r="IO34" s="1" t="n">
         <v>52.6</v>
       </c>
-      <c r="IP34" t="n">
+      <c r="IP34" s="1" t="n">
         <v>45.8</v>
+      </c>
+      <c r="IQ34" t="n">
+        <v>31.4</v>
       </c>
     </row>
     <row r="35" ht="13.8" customHeight="1" s="2">
@@ -26842,8 +26944,11 @@
       <c r="IO35" s="1" t="n">
         <v>22.8</v>
       </c>
-      <c r="IP35" t="n">
+      <c r="IP35" s="1" t="n">
         <v>25</v>
+      </c>
+      <c r="IQ35" t="n">
+        <v>15.7</v>
       </c>
     </row>
     <row r="36" ht="13.8" customHeight="1" s="2">
@@ -27596,8 +27701,11 @@
       <c r="IO36" s="1" t="n">
         <v>187.7</v>
       </c>
-      <c r="IP36" t="n">
+      <c r="IP36" s="1" t="n">
         <v>187.2</v>
+      </c>
+      <c r="IQ36" t="n">
+        <v>186.9</v>
       </c>
     </row>
     <row r="37" ht="13.8" customHeight="1" s="2">
@@ -28350,8 +28458,11 @@
       <c r="IO37" s="1" t="n">
         <v>83.7</v>
       </c>
-      <c r="IP37" t="n">
+      <c r="IP37" s="1" t="n">
         <v>87</v>
+      </c>
+      <c r="IQ37" t="n">
+        <v>86</v>
       </c>
     </row>
     <row r="38" ht="13.8" customHeight="1" s="2">
@@ -29104,8 +29215,11 @@
       <c r="IO38" s="1" t="n">
         <v>24.66</v>
       </c>
-      <c r="IP38" t="n">
+      <c r="IP38" s="1" t="n">
         <v>23.8</v>
+      </c>
+      <c r="IQ38" t="n">
+        <v>23.58</v>
       </c>
     </row>
     <row r="39" ht="13.8" customHeight="1" s="2">
@@ -29858,8 +29972,11 @@
       <c r="IO39" s="1" t="n">
         <v>72.5</v>
       </c>
-      <c r="IP39" t="n">
+      <c r="IP39" s="1" t="n">
         <v>58.5</v>
+      </c>
+      <c r="IQ39" t="n">
+        <v>55.2</v>
       </c>
     </row>
     <row r="40" ht="13.8" customHeight="1" s="2">
@@ -30612,8 +30729,11 @@
       <c r="IO40" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="IP40" t="n">
+      <c r="IP40" s="1" t="n">
         <v>14</v>
+      </c>
+      <c r="IQ40" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="41" ht="13.8" customHeight="1" s="2">
@@ -31366,8 +31486,11 @@
       <c r="IO41" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="IP41" t="n">
+      <c r="IP41" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="IQ41" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="42" ht="13.8" customHeight="1" s="2">
@@ -32120,7 +32243,10 @@
       <c r="IO42" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="IP42" t="n">
+      <c r="IP42" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="IQ42" t="n">
         <v>1</v>
       </c>
     </row>
@@ -32874,7 +33000,10 @@
       <c r="IO43" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="IP43" t="n">
+      <c r="IP43" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="IQ43" t="n">
         <v>3</v>
       </c>
     </row>
@@ -33628,8 +33757,11 @@
       <c r="IO44" s="1" t="n">
         <v>152</v>
       </c>
-      <c r="IP44" t="n">
+      <c r="IP44" s="1" t="n">
         <v>143</v>
+      </c>
+      <c r="IQ44" t="n">
+        <v>136</v>
       </c>
     </row>
     <row r="45" ht="13.8" customHeight="1" s="2">
@@ -34382,8 +34514,11 @@
       <c r="IO45" s="1" t="n">
         <v>266</v>
       </c>
-      <c r="IP45" t="n">
+      <c r="IP45" s="1" t="n">
         <v>219</v>
+      </c>
+      <c r="IQ45" t="n">
+        <v>252</v>
       </c>
     </row>
     <row r="46" ht="13.8" customHeight="1" s="2">
@@ -35136,8 +35271,11 @@
       <c r="IO46" s="1" t="n">
         <v>317</v>
       </c>
-      <c r="IP46" t="n">
+      <c r="IP46" s="1" t="n">
         <v>259</v>
+      </c>
+      <c r="IQ46" t="n">
+        <v>281</v>
       </c>
     </row>
     <row r="47" ht="13.8" customHeight="1" s="2">
@@ -35890,8 +36028,11 @@
       <c r="IO47" s="1" t="n">
         <v>75.8</v>
       </c>
-      <c r="IP47" t="n">
+      <c r="IP47" s="1" t="n">
         <v>72.09999999999999</v>
+      </c>
+      <c r="IQ47" t="n">
+        <v>72.2</v>
       </c>
     </row>
     <row r="48" ht="13.8" customHeight="1" s="2">
@@ -36644,8 +36785,11 @@
       <c r="IO48" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="IP48" t="n">
+      <c r="IP48" s="1" t="n">
         <v>55</v>
+      </c>
+      <c r="IQ48" t="n">
+        <v>69</v>
       </c>
     </row>
     <row r="49" ht="13.8" customHeight="1" s="2">
@@ -37398,8 +37542,11 @@
       <c r="IO49" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="IP49" t="n">
+      <c r="IP49" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="IQ49" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="50" ht="13.8" customHeight="1" s="2">
@@ -38152,8 +38299,11 @@
       <c r="IO50" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="IP50" t="n">
+      <c r="IP50" s="1" t="n">
         <v>12</v>
+      </c>
+      <c r="IQ50" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="51" ht="13.8" customHeight="1" s="2">
@@ -38906,8 +39056,11 @@
       <c r="IO51" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="IP51" t="n">
+      <c r="IP51" s="1" t="n">
         <v>35</v>
+      </c>
+      <c r="IQ51" t="n">
+        <v>36</v>
       </c>
     </row>
     <row r="52" ht="13.8" customHeight="1" s="2">
@@ -39660,8 +39813,11 @@
       <c r="IO52" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="IP52" t="n">
+      <c r="IP52" s="1" t="n">
         <v>43</v>
+      </c>
+      <c r="IQ52" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="53" ht="13.8" customHeight="1" s="2">
@@ -40414,8 +40570,11 @@
       <c r="IO53" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="IP53" t="n">
+      <c r="IP53" s="1" t="n">
         <v>45</v>
+      </c>
+      <c r="IQ53" t="n">
+        <v>43</v>
       </c>
     </row>
     <row r="54" ht="13.8" customHeight="1" s="2">
@@ -41168,8 +41327,11 @@
       <c r="IO54" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="IP54" t="n">
+      <c r="IP54" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="IQ54" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="55" ht="13.8" customHeight="1" s="2">
@@ -41922,8 +42084,11 @@
       <c r="IO55" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="IP55" t="n">
+      <c r="IP55" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="IQ55" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="56" ht="13.8" customHeight="1" s="2">
@@ -42676,8 +42841,11 @@
       <c r="IO56" s="1" t="n">
         <v>69.2</v>
       </c>
-      <c r="IP56" t="n">
+      <c r="IP56" s="1" t="n">
         <v>58.3</v>
+      </c>
+      <c r="IQ56" t="n">
+        <v>75</v>
       </c>
     </row>
     <row r="57" ht="13.8" customHeight="1" s="2">
@@ -43430,8 +43598,11 @@
       <c r="IO57" s="1" t="n">
         <v>175</v>
       </c>
-      <c r="IP57" t="n">
+      <c r="IP57" s="1" t="n">
         <v>175</v>
+      </c>
+      <c r="IQ57" t="n">
+        <v>201</v>
       </c>
     </row>
     <row r="58" ht="13.8" customHeight="1" s="2">
@@ -44184,8 +44355,11 @@
       <c r="IO58" s="1" t="n">
         <v>140</v>
       </c>
-      <c r="IP58" t="n">
+      <c r="IP58" s="1" t="n">
         <v>138</v>
+      </c>
+      <c r="IQ58" t="n">
+        <v>183</v>
       </c>
     </row>
     <row r="59" ht="13.8" customHeight="1" s="2">
@@ -44938,8 +45112,11 @@
       <c r="IO59" s="1" t="n">
         <v>315</v>
       </c>
-      <c r="IP59" t="n">
+      <c r="IP59" s="1" t="n">
         <v>313</v>
+      </c>
+      <c r="IQ59" t="n">
+        <v>384</v>
       </c>
     </row>
     <row r="60" ht="13.8" customHeight="1" s="2">
@@ -45692,8 +45869,11 @@
       <c r="IO60" s="1" t="n">
         <v>1.25</v>
       </c>
-      <c r="IP60" t="n">
+      <c r="IP60" s="1" t="n">
         <v>1.27</v>
+      </c>
+      <c r="IQ60" t="n">
+        <v>1.1</v>
       </c>
     </row>
     <row r="61" ht="13.8" customHeight="1" s="2">
@@ -46446,8 +46626,11 @@
       <c r="IO61" s="1" t="n">
         <v>69</v>
       </c>
-      <c r="IP61" t="n">
+      <c r="IP61" s="1" t="n">
         <v>73</v>
+      </c>
+      <c r="IQ61" t="n">
+        <v>72</v>
       </c>
     </row>
     <row r="62" ht="13.8" customHeight="1" s="2">
@@ -47200,8 +47383,11 @@
       <c r="IO62" s="1" t="n">
         <v>67</v>
       </c>
-      <c r="IP62" t="n">
+      <c r="IP62" s="1" t="n">
         <v>58</v>
+      </c>
+      <c r="IQ62" t="n">
+        <v>61</v>
       </c>
     </row>
     <row r="63" ht="13.8" customHeight="1" s="2">
@@ -47954,8 +48140,11 @@
       <c r="IO63" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="IP63" t="n">
+      <c r="IP63" s="1" t="n">
         <v>41</v>
+      </c>
+      <c r="IQ63" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="64" ht="13.8" customHeight="1" s="2">
@@ -48708,8 +48897,11 @@
       <c r="IO64" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="IP64" t="n">
+      <c r="IP64" s="1" t="n">
         <v>16</v>
+      </c>
+      <c r="IQ64" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="65" ht="13.8" customHeight="1" s="2">
@@ -49462,8 +49654,11 @@
       <c r="IO65" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="IP65" t="n">
+      <c r="IP65" s="1" t="n">
         <v>32</v>
+      </c>
+      <c r="IQ65" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="66" ht="13.8" customHeight="1" s="2">
@@ -50216,8 +50411,11 @@
       <c r="IO66" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="IP66" t="n">
+      <c r="IP66" s="1" t="n">
         <v>11</v>
+      </c>
+      <c r="IQ66" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="67" ht="13.8" customHeight="1" s="2">
@@ -50970,8 +51168,11 @@
       <c r="IO67" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="IP67" t="n">
+      <c r="IP67" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="IQ67" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="68" ht="13.8" customHeight="1" s="2">
@@ -51724,8 +51925,11 @@
       <c r="IO68" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="IP68" t="n">
+      <c r="IP68" s="1" t="n">
         <v>15</v>
+      </c>
+      <c r="IQ68" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="69" ht="13.8" customHeight="1" s="2">
@@ -52478,7 +52682,10 @@
       <c r="IO69" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="IP69" t="n">
+      <c r="IP69" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="IQ69" t="n">
         <v>2</v>
       </c>
     </row>
@@ -53232,8 +53439,11 @@
       <c r="IO70" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="IP70" t="n">
+      <c r="IP70" s="1" t="n">
         <v>28</v>
+      </c>
+      <c r="IQ70" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="71" ht="13.8" customHeight="1" s="2">
@@ -53986,8 +54196,11 @@
       <c r="IO71" s="1" t="n">
         <v>57.1</v>
       </c>
-      <c r="IP71" t="n">
+      <c r="IP71" s="1" t="n">
         <v>39.3</v>
+      </c>
+      <c r="IQ71" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="72" ht="13.8" customHeight="1" s="2">
@@ -54740,8 +54953,11 @@
       <c r="IO72" s="1" t="n">
         <v>39.38</v>
       </c>
-      <c r="IP72" t="n">
+      <c r="IP72" s="1" t="n">
         <v>28.45</v>
+      </c>
+      <c r="IQ72" t="n">
+        <v>25.6</v>
       </c>
     </row>
     <row r="73" ht="13.8" customHeight="1" s="2">
@@ -55494,8 +55710,11 @@
       <c r="IO73" s="1" t="n">
         <v>22.5</v>
       </c>
-      <c r="IP73" t="n">
+      <c r="IP73" s="1" t="n">
         <v>11.18</v>
+      </c>
+      <c r="IQ73" t="n">
+        <v>15.36</v>
       </c>
     </row>
     <row r="74" ht="13.8" customHeight="1" s="2">
@@ -56248,8 +56467,11 @@
       <c r="IO74" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="IP74" t="n">
+      <c r="IP74" s="1" t="n">
         <v>38</v>
+      </c>
+      <c r="IQ74" t="n">
+        <v>29</v>
       </c>
     </row>
     <row r="75" ht="13.8" customHeight="1" s="2">
@@ -57002,7 +57224,10 @@
       <c r="IO75" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="IP75" t="n">
+      <c r="IP75" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="IQ75" t="n">
         <v>61</v>
       </c>
     </row>
@@ -57756,8 +57981,11 @@
       <c r="IO76" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="IP76" t="n">
+      <c r="IP76" s="1" t="n">
         <v>36</v>
+      </c>
+      <c r="IQ76" t="n">
+        <v>43</v>
       </c>
     </row>
     <row r="77" ht="13.8" customHeight="1" s="2">
@@ -58510,8 +58738,11 @@
       <c r="IO77" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="IP77" t="n">
+      <c r="IP77" s="1" t="n">
         <v>55</v>
+      </c>
+      <c r="IQ77" t="n">
+        <v>54</v>
       </c>
     </row>
     <row r="78" ht="13.8" customHeight="1" s="2">
@@ -59264,8 +59495,11 @@
       <c r="IO78" s="1" t="n">
         <v>2.64</v>
       </c>
-      <c r="IP78" t="n">
+      <c r="IP78" s="1" t="n">
         <v>1.96</v>
+      </c>
+      <c r="IQ78" t="n">
+        <v>2.16</v>
       </c>
     </row>
     <row r="79" ht="13.8" customHeight="1" s="2">
@@ -60018,8 +60252,11 @@
       <c r="IO79" s="1" t="n">
         <v>4.62</v>
       </c>
-      <c r="IP79" t="n">
+      <c r="IP79" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="IQ79" t="n">
+        <v>3.6</v>
       </c>
     </row>
     <row r="80" ht="13.8" customHeight="1" s="2">
@@ -60772,8 +61009,11 @@
       <c r="IO80" s="1" t="n">
         <v>35.1</v>
       </c>
-      <c r="IP80" t="n">
+      <c r="IP80" s="1" t="n">
         <v>47.3</v>
+      </c>
+      <c r="IQ80" t="n">
+        <v>42.6</v>
       </c>
     </row>
     <row r="81" ht="13.8" customHeight="1" s="2">
@@ -61526,8 +61766,11 @@
       <c r="IO81" s="1" t="n">
         <v>21.6</v>
       </c>
-      <c r="IP81" t="n">
+      <c r="IP81" s="1" t="n">
         <v>20</v>
+      </c>
+      <c r="IQ81" t="n">
+        <v>27.8</v>
       </c>
     </row>
     <row r="82" ht="13.8" customHeight="1" s="2">
@@ -62280,8 +62523,11 @@
       <c r="IO82" s="1" t="n">
         <v>187.6</v>
       </c>
-      <c r="IP82" t="n">
+      <c r="IP82" s="1" t="n">
         <v>188.7</v>
+      </c>
+      <c r="IQ82" t="n">
+        <v>188.5</v>
       </c>
     </row>
     <row r="83" ht="13.8" customHeight="1" s="2">
@@ -63034,8 +63280,11 @@
       <c r="IO83" s="1" t="n">
         <v>83.90000000000001</v>
       </c>
-      <c r="IP83" t="n">
+      <c r="IP83" s="1" t="n">
         <v>88.3</v>
+      </c>
+      <c r="IQ83" t="n">
+        <v>86.59999999999999</v>
       </c>
     </row>
     <row r="84" ht="13.8" customHeight="1" s="2">
@@ -63788,8 +64037,11 @@
       <c r="IO84" s="1" t="n">
         <v>24.49</v>
       </c>
-      <c r="IP84" t="n">
+      <c r="IP84" s="1" t="n">
         <v>24.49</v>
+      </c>
+      <c r="IQ84" t="n">
+        <v>25.91</v>
       </c>
     </row>
     <row r="85" ht="13.8" customHeight="1" s="2">
@@ -64542,8 +64794,11 @@
       <c r="IO85" s="1" t="n">
         <v>83.2</v>
       </c>
-      <c r="IP85" t="n">
+      <c r="IP85" s="1" t="n">
         <v>67.3</v>
+      </c>
+      <c r="IQ85" t="n">
+        <v>97.2</v>
       </c>
     </row>
     <row r="86" ht="13.8" customHeight="1" s="2">
@@ -65296,8 +65551,11 @@
       <c r="IO86" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="IP86" t="n">
+      <c r="IP86" s="1" t="n">
         <v>13</v>
+      </c>
+      <c r="IQ86" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="87" ht="13.8" customHeight="1" s="2">
@@ -66050,8 +66308,11 @@
       <c r="IO87" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="IP87" t="n">
+      <c r="IP87" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="IQ87" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="88" ht="13.8" customHeight="1" s="2">
@@ -66804,8 +67065,11 @@
       <c r="IO88" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="IP88" t="n">
+      <c r="IP88" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="IQ88" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="89" ht="13.8" customHeight="1" s="2">
@@ -67558,8 +67822,11 @@
       <c r="IO89" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="IP89" t="n">
+      <c r="IP89" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="IQ89" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="90" ht="13.8" customHeight="1" s="2">
@@ -68312,8 +68579,11 @@
       <c r="IO90" s="1" t="n">
         <v>111</v>
       </c>
-      <c r="IP90" t="n">
+      <c r="IP90" s="1" t="n">
         <v>129</v>
+      </c>
+      <c r="IQ90" t="n">
+        <v>139</v>
       </c>
     </row>
     <row r="91" ht="13.8" customHeight="1" s="2">
@@ -69066,8 +69336,11 @@
       <c r="IO91" s="1" t="n">
         <v>190</v>
       </c>
-      <c r="IP91" t="n">
+      <c r="IP91" s="1" t="n">
         <v>187</v>
+      </c>
+      <c r="IQ91" t="n">
+        <v>230</v>
       </c>
     </row>
     <row r="92" ht="13.8" customHeight="1" s="2">
@@ -69820,8 +70093,11 @@
       <c r="IO92" s="1" t="n">
         <v>226</v>
       </c>
-      <c r="IP92" t="n">
+      <c r="IP92" s="1" t="n">
         <v>237</v>
+      </c>
+      <c r="IQ92" t="n">
+        <v>282</v>
       </c>
     </row>
     <row r="93" ht="13.8" customHeight="1" s="2">
@@ -70574,8 +70850,11 @@
       <c r="IO93" s="1" t="n">
         <v>71.7</v>
       </c>
-      <c r="IP93" t="n">
+      <c r="IP93" s="1" t="n">
         <v>75.7</v>
+      </c>
+      <c r="IQ93" t="n">
+        <v>73.40000000000001</v>
       </c>
     </row>
     <row r="94" ht="13.8" customHeight="1" s="2">
@@ -71328,7 +71607,10 @@
       <c r="IO94" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="IP94" t="n">
+      <c r="IP94" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="IQ94" t="n">
         <v>61</v>
       </c>
     </row>
@@ -72082,8 +72364,11 @@
       <c r="IO95" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="IP95" t="n">
+      <c r="IP95" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="IQ95" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="96" ht="13.8" customHeight="1" s="2">
@@ -72836,8 +73121,11 @@
       <c r="IO96" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="IP96" t="n">
+      <c r="IP96" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="IQ96" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="97" ht="13.8" customHeight="1" s="2">
@@ -73590,8 +73878,11 @@
       <c r="IO97" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="IP97" t="n">
+      <c r="IP97" s="1" t="n">
         <v>38</v>
+      </c>
+      <c r="IQ97" t="n">
+        <v>29</v>
       </c>
     </row>
     <row r="98" ht="13.8" customHeight="1" s="2">
@@ -74344,8 +74635,11 @@
       <c r="IO98" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="IP98" t="n">
+      <c r="IP98" s="1" t="n">
         <v>36</v>
+      </c>
+      <c r="IQ98" t="n">
+        <v>43</v>
       </c>
     </row>
     <row r="99" ht="13.8" customHeight="1" s="2">
@@ -75098,8 +75392,11 @@
       <c r="IO99" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="IP99" t="n">
+      <c r="IP99" s="1" t="n">
         <v>57</v>
+      </c>
+      <c r="IQ99" t="n">
+        <v>48</v>
       </c>
     </row>
     <row r="100" ht="13.8" customHeight="1" s="2">
@@ -75852,8 +76149,11 @@
       <c r="IO100" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="IP100" t="n">
+      <c r="IP100" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="IQ100" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="101" ht="13.8" customHeight="1" s="2">
@@ -76606,8 +76906,11 @@
       <c r="IO101" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="IP101" t="n">
+      <c r="IP101" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="IQ101" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="102" ht="13.8" customHeight="1" s="2">
@@ -77360,8 +77663,11 @@
       <c r="IO102" s="1" t="n">
         <v>37.5</v>
       </c>
-      <c r="IP102" t="n">
+      <c r="IP102" s="1" t="n">
         <v>72.7</v>
+      </c>
+      <c r="IQ102" t="n">
+        <v>66.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Round 3 2022 Did some feature importance plots. Wasn't enlightening...
</commit_message>
<xml_diff>
--- a/django_AFL_ML/Data/Adelaide_stats.xlsx
+++ b/django_AFL_ML/Data/Adelaide_stats.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:IQ102"/>
+  <dimension ref="A1:IR102"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="GZ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="HA23" activeCellId="0" sqref="HA23"/>
@@ -1209,8 +1209,11 @@
       <c r="IP1" s="1" t="n">
         <v>10551</v>
       </c>
-      <c r="IQ1" t="n">
+      <c r="IQ1" s="1" t="n">
         <v>10555</v>
+      </c>
+      <c r="IR1" t="n">
+        <v>10564</v>
       </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="2">
@@ -1966,7 +1969,10 @@
       <c r="IP2" s="1" t="n">
         <v>2022</v>
       </c>
-      <c r="IQ2" t="n">
+      <c r="IQ2" s="1" t="n">
+        <v>2022</v>
+      </c>
+      <c r="IR2" t="n">
         <v>2022</v>
       </c>
     </row>
@@ -2723,8 +2729,11 @@
       <c r="IP3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="IQ3" t="n">
+      <c r="IQ3" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="IR3" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="2">
@@ -3480,8 +3489,11 @@
       <c r="IP4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="IQ4" t="n">
+      <c r="IQ4" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="IR4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5" ht="13.8" customHeight="1" s="2">
@@ -4237,7 +4249,10 @@
       <c r="IP5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="IQ5" t="n">
+      <c r="IQ5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="IR5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4994,8 +5009,11 @@
       <c r="IP6" s="1" t="n">
         <v>82</v>
       </c>
-      <c r="IQ6" t="n">
+      <c r="IQ6" s="1" t="n">
         <v>58</v>
+      </c>
+      <c r="IR6" t="n">
+        <v>96</v>
       </c>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="2">
@@ -5751,8 +5769,11 @@
       <c r="IP7" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="IQ7" t="n">
+      <c r="IQ7" s="1" t="n">
         <v>100</v>
+      </c>
+      <c r="IR7" t="n">
+        <v>92</v>
       </c>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="2">
@@ -6508,8 +6529,11 @@
       <c r="IP8" s="1" t="n">
         <v>-1</v>
       </c>
-      <c r="IQ8" t="n">
+      <c r="IQ8" s="1" t="n">
         <v>-42</v>
+      </c>
+      <c r="IR8" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="2">
@@ -7265,8 +7289,11 @@
       <c r="IP9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="IQ9" t="n">
+      <c r="IQ9" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="IR9" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10" ht="13.8" customHeight="1" s="2">
@@ -8022,8 +8049,11 @@
       <c r="IP10" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="IQ10" t="n">
+      <c r="IQ10" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="IR10" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="11" ht="13.8" customHeight="1" s="2">
@@ -8779,8 +8809,11 @@
       <c r="IP11" s="1" t="n">
         <v>215</v>
       </c>
-      <c r="IQ11" t="n">
+      <c r="IQ11" s="1" t="n">
         <v>220</v>
+      </c>
+      <c r="IR11" t="n">
+        <v>192</v>
       </c>
     </row>
     <row r="12" ht="13.8" customHeight="1" s="2">
@@ -9536,8 +9569,11 @@
       <c r="IP12" s="1" t="n">
         <v>144</v>
       </c>
-      <c r="IQ12" t="n">
+      <c r="IQ12" s="1" t="n">
         <v>169</v>
+      </c>
+      <c r="IR12" t="n">
+        <v>153</v>
       </c>
     </row>
     <row r="13" ht="13.8" customHeight="1" s="2">
@@ -10293,8 +10329,11 @@
       <c r="IP13" s="1" t="n">
         <v>359</v>
       </c>
-      <c r="IQ13" t="n">
+      <c r="IQ13" s="1" t="n">
         <v>389</v>
+      </c>
+      <c r="IR13" t="n">
+        <v>345</v>
       </c>
     </row>
     <row r="14" ht="13.8" customHeight="1" s="2">
@@ -11050,8 +11089,11 @@
       <c r="IP14" s="1" t="n">
         <v>1.49</v>
       </c>
-      <c r="IQ14" t="n">
+      <c r="IQ14" s="1" t="n">
         <v>1.3</v>
+      </c>
+      <c r="IR14" t="n">
+        <v>1.25</v>
       </c>
     </row>
     <row r="15" ht="13.8" customHeight="1" s="2">
@@ -11807,8 +11849,11 @@
       <c r="IP15" s="1" t="n">
         <v>92</v>
       </c>
-      <c r="IQ15" t="n">
+      <c r="IQ15" s="1" t="n">
         <v>102</v>
+      </c>
+      <c r="IR15" t="n">
+        <v>67</v>
       </c>
     </row>
     <row r="16" ht="13.8" customHeight="1" s="2">
@@ -12564,8 +12609,11 @@
       <c r="IP16" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="IQ16" t="n">
+      <c r="IQ16" s="1" t="n">
         <v>53</v>
+      </c>
+      <c r="IR16" t="n">
+        <v>64</v>
       </c>
     </row>
     <row r="17" ht="13.8" customHeight="1" s="2">
@@ -13321,8 +13369,11 @@
       <c r="IP17" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="IQ17" t="n">
+      <c r="IQ17" s="1" t="n">
         <v>33</v>
+      </c>
+      <c r="IR17" t="n">
+        <v>46</v>
       </c>
     </row>
     <row r="18" ht="13.8" customHeight="1" s="2">
@@ -14078,8 +14129,11 @@
       <c r="IP18" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="IQ18" t="n">
+      <c r="IQ18" s="1" t="n">
         <v>18</v>
+      </c>
+      <c r="IR18" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="19" ht="13.8" customHeight="1" s="2">
@@ -14835,8 +14889,11 @@
       <c r="IP19" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="IQ19" t="n">
+      <c r="IQ19" s="1" t="n">
         <v>30</v>
+      </c>
+      <c r="IR19" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="20" ht="13.8" customHeight="1" s="2">
@@ -15592,8 +15649,11 @@
       <c r="IP20" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="IQ20" t="n">
+      <c r="IQ20" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="IR20" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="21" ht="13.8" customHeight="1" s="2">
@@ -16349,8 +16409,11 @@
       <c r="IP21" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="IQ21" t="n">
+      <c r="IQ21" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="IR21" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="22" ht="13.8" customHeight="1" s="2">
@@ -17106,8 +17169,11 @@
       <c r="IP22" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="IQ22" t="n">
+      <c r="IQ22" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="IR22" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="23" ht="13.8" customHeight="1" s="2">
@@ -17863,8 +17929,11 @@
       <c r="IP23" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="IQ23" t="n">
+      <c r="IQ23" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="IR23" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="24" ht="13.8" customHeight="1" s="2">
@@ -18620,8 +18689,11 @@
       <c r="IP24" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="IQ24" t="n">
+      <c r="IQ24" s="1" t="n">
         <v>18</v>
+      </c>
+      <c r="IR24" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="25" ht="13.8" customHeight="1" s="2">
@@ -19377,8 +19449,11 @@
       <c r="IP25" s="1" t="n">
         <v>54.5</v>
       </c>
-      <c r="IQ25" t="n">
+      <c r="IQ25" s="1" t="n">
         <v>44.4</v>
+      </c>
+      <c r="IR25" t="n">
+        <v>71.40000000000001</v>
       </c>
     </row>
     <row r="26" ht="13.8" customHeight="1" s="2">
@@ -20134,8 +20209,11 @@
       <c r="IP26" s="1" t="n">
         <v>29.92</v>
       </c>
-      <c r="IQ26" t="n">
+      <c r="IQ26" s="1" t="n">
         <v>48.62</v>
+      </c>
+      <c r="IR26" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="27" ht="13.8" customHeight="1" s="2">
@@ -20891,8 +20969,11 @@
       <c r="IP27" s="1" t="n">
         <v>16.32</v>
       </c>
-      <c r="IQ27" t="n">
+      <c r="IQ27" s="1" t="n">
         <v>21.61</v>
+      </c>
+      <c r="IR27" t="n">
+        <v>16.43</v>
       </c>
     </row>
     <row r="28" ht="13.8" customHeight="1" s="2">
@@ -21648,8 +21729,11 @@
       <c r="IP28" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="IQ28" t="n">
+      <c r="IQ28" s="1" t="n">
         <v>36</v>
+      </c>
+      <c r="IR28" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="29" ht="13.8" customHeight="1" s="2">
@@ -22405,8 +22489,11 @@
       <c r="IP29" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="IQ29" t="n">
+      <c r="IQ29" s="1" t="n">
         <v>69</v>
+      </c>
+      <c r="IR29" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="30" ht="13.8" customHeight="1" s="2">
@@ -23162,8 +23249,11 @@
       <c r="IP30" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="IQ30" t="n">
+      <c r="IQ30" s="1" t="n">
         <v>37</v>
+      </c>
+      <c r="IR30" t="n">
+        <v>34</v>
       </c>
     </row>
     <row r="31" ht="13.8" customHeight="1" s="2">
@@ -23919,8 +24009,11 @@
       <c r="IP31" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="IQ31" t="n">
+      <c r="IQ31" s="1" t="n">
         <v>51</v>
+      </c>
+      <c r="IR31" t="n">
+        <v>43</v>
       </c>
     </row>
     <row r="32" ht="13.8" customHeight="1" s="2">
@@ -24676,8 +24769,11 @@
       <c r="IP32" s="1" t="n">
         <v>2.18</v>
       </c>
-      <c r="IQ32" t="n">
+      <c r="IQ32" s="1" t="n">
         <v>2.83</v>
+      </c>
+      <c r="IR32" t="n">
+        <v>2.05</v>
       </c>
     </row>
     <row r="33" ht="13.8" customHeight="1" s="2">
@@ -25433,8 +25529,11 @@
       <c r="IP33" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="IQ33" t="n">
+      <c r="IQ33" s="1" t="n">
         <v>6.38</v>
+      </c>
+      <c r="IR33" t="n">
+        <v>2.87</v>
       </c>
     </row>
     <row r="34" ht="13.8" customHeight="1" s="2">
@@ -26190,8 +26289,11 @@
       <c r="IP34" s="1" t="n">
         <v>45.8</v>
       </c>
-      <c r="IQ34" t="n">
+      <c r="IQ34" s="1" t="n">
         <v>31.4</v>
+      </c>
+      <c r="IR34" t="n">
+        <v>48.8</v>
       </c>
     </row>
     <row r="35" ht="13.8" customHeight="1" s="2">
@@ -26947,8 +27049,11 @@
       <c r="IP35" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="IQ35" t="n">
+      <c r="IQ35" s="1" t="n">
         <v>15.7</v>
+      </c>
+      <c r="IR35" t="n">
+        <v>34.9</v>
       </c>
     </row>
     <row r="36" ht="13.8" customHeight="1" s="2">
@@ -27704,8 +27809,11 @@
       <c r="IP36" s="1" t="n">
         <v>187.2</v>
       </c>
-      <c r="IQ36" t="n">
+      <c r="IQ36" s="1" t="n">
         <v>186.9</v>
+      </c>
+      <c r="IR36" t="n">
+        <v>187</v>
       </c>
     </row>
     <row r="37" ht="13.8" customHeight="1" s="2">
@@ -28461,8 +28569,11 @@
       <c r="IP37" s="1" t="n">
         <v>87</v>
       </c>
-      <c r="IQ37" t="n">
+      <c r="IQ37" s="1" t="n">
         <v>86</v>
+      </c>
+      <c r="IR37" t="n">
+        <v>86.2</v>
       </c>
     </row>
     <row r="38" ht="13.8" customHeight="1" s="2">
@@ -29218,8 +29329,11 @@
       <c r="IP38" s="1" t="n">
         <v>23.8</v>
       </c>
-      <c r="IQ38" t="n">
+      <c r="IQ38" s="1" t="n">
         <v>23.58</v>
+      </c>
+      <c r="IR38" t="n">
+        <v>23.91</v>
       </c>
     </row>
     <row r="39" ht="13.8" customHeight="1" s="2">
@@ -29975,8 +30089,11 @@
       <c r="IP39" s="1" t="n">
         <v>58.5</v>
       </c>
-      <c r="IQ39" t="n">
+      <c r="IQ39" s="1" t="n">
         <v>55.2</v>
+      </c>
+      <c r="IR39" t="n">
+        <v>59.2</v>
       </c>
     </row>
     <row r="40" ht="13.8" customHeight="1" s="2">
@@ -30732,8 +30849,11 @@
       <c r="IP40" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="IQ40" t="n">
+      <c r="IQ40" s="1" t="n">
         <v>15</v>
+      </c>
+      <c r="IR40" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="41" ht="13.8" customHeight="1" s="2">
@@ -31489,8 +31609,11 @@
       <c r="IP41" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="IQ41" t="n">
+      <c r="IQ41" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="IR41" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="42" ht="13.8" customHeight="1" s="2">
@@ -32246,7 +32369,10 @@
       <c r="IP42" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="IQ42" t="n">
+      <c r="IQ42" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="IR42" t="n">
         <v>1</v>
       </c>
     </row>
@@ -33003,7 +33129,10 @@
       <c r="IP43" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="IQ43" t="n">
+      <c r="IQ43" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="IR43" t="n">
         <v>3</v>
       </c>
     </row>
@@ -33760,8 +33889,11 @@
       <c r="IP44" s="1" t="n">
         <v>143</v>
       </c>
-      <c r="IQ44" t="n">
+      <c r="IQ44" s="1" t="n">
         <v>136</v>
+      </c>
+      <c r="IR44" t="n">
+        <v>140</v>
       </c>
     </row>
     <row r="45" ht="13.8" customHeight="1" s="2">
@@ -34517,8 +34649,11 @@
       <c r="IP45" s="1" t="n">
         <v>219</v>
       </c>
-      <c r="IQ45" t="n">
+      <c r="IQ45" s="1" t="n">
         <v>252</v>
+      </c>
+      <c r="IR45" t="n">
+        <v>197</v>
       </c>
     </row>
     <row r="46" ht="13.8" customHeight="1" s="2">
@@ -35274,8 +35409,11 @@
       <c r="IP46" s="1" t="n">
         <v>259</v>
       </c>
-      <c r="IQ46" t="n">
+      <c r="IQ46" s="1" t="n">
         <v>281</v>
+      </c>
+      <c r="IR46" t="n">
+        <v>248</v>
       </c>
     </row>
     <row r="47" ht="13.8" customHeight="1" s="2">
@@ -36031,8 +36169,11 @@
       <c r="IP47" s="1" t="n">
         <v>72.09999999999999</v>
       </c>
-      <c r="IQ47" t="n">
+      <c r="IQ47" s="1" t="n">
         <v>72.2</v>
+      </c>
+      <c r="IR47" t="n">
+        <v>71.90000000000001</v>
       </c>
     </row>
     <row r="48" ht="13.8" customHeight="1" s="2">
@@ -36788,8 +36929,11 @@
       <c r="IP48" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="IQ48" t="n">
+      <c r="IQ48" s="1" t="n">
         <v>69</v>
+      </c>
+      <c r="IR48" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="49" ht="13.8" customHeight="1" s="2">
@@ -37545,8 +37689,11 @@
       <c r="IP49" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="IQ49" t="n">
+      <c r="IQ49" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="IR49" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="50" ht="13.8" customHeight="1" s="2">
@@ -38302,8 +38449,11 @@
       <c r="IP50" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="IQ50" t="n">
+      <c r="IQ50" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="IR50" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="51" ht="13.8" customHeight="1" s="2">
@@ -39059,8 +39209,11 @@
       <c r="IP51" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="IQ51" t="n">
+      <c r="IQ51" s="1" t="n">
         <v>36</v>
+      </c>
+      <c r="IR51" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="52" ht="13.8" customHeight="1" s="2">
@@ -39816,8 +39969,11 @@
       <c r="IP52" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="IQ52" t="n">
+      <c r="IQ52" s="1" t="n">
         <v>37</v>
+      </c>
+      <c r="IR52" t="n">
+        <v>34</v>
       </c>
     </row>
     <row r="53" ht="13.8" customHeight="1" s="2">
@@ -40573,8 +40729,11 @@
       <c r="IP53" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="IQ53" t="n">
+      <c r="IQ53" s="1" t="n">
         <v>43</v>
+      </c>
+      <c r="IR53" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="54" ht="13.8" customHeight="1" s="2">
@@ -41330,8 +41489,11 @@
       <c r="IP54" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="IQ54" t="n">
+      <c r="IQ54" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="IR54" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="55" ht="13.8" customHeight="1" s="2">
@@ -42087,8 +42249,11 @@
       <c r="IP55" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="IQ55" t="n">
+      <c r="IQ55" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="IR55" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="56" ht="13.8" customHeight="1" s="2">
@@ -42844,8 +43009,11 @@
       <c r="IP56" s="1" t="n">
         <v>58.3</v>
       </c>
-      <c r="IQ56" t="n">
+      <c r="IQ56" s="1" t="n">
         <v>75</v>
+      </c>
+      <c r="IR56" t="n">
+        <v>53.3</v>
       </c>
     </row>
     <row r="57" ht="13.8" customHeight="1" s="2">
@@ -43601,8 +43769,11 @@
       <c r="IP57" s="1" t="n">
         <v>175</v>
       </c>
-      <c r="IQ57" t="n">
+      <c r="IQ57" s="1" t="n">
         <v>201</v>
+      </c>
+      <c r="IR57" t="n">
+        <v>192</v>
       </c>
     </row>
     <row r="58" ht="13.8" customHeight="1" s="2">
@@ -44358,8 +44529,11 @@
       <c r="IP58" s="1" t="n">
         <v>138</v>
       </c>
-      <c r="IQ58" t="n">
+      <c r="IQ58" s="1" t="n">
         <v>183</v>
+      </c>
+      <c r="IR58" t="n">
+        <v>151</v>
       </c>
     </row>
     <row r="59" ht="13.8" customHeight="1" s="2">
@@ -45115,8 +45289,11 @@
       <c r="IP59" s="1" t="n">
         <v>313</v>
       </c>
-      <c r="IQ59" t="n">
+      <c r="IQ59" s="1" t="n">
         <v>384</v>
+      </c>
+      <c r="IR59" t="n">
+        <v>343</v>
       </c>
     </row>
     <row r="60" ht="13.8" customHeight="1" s="2">
@@ -45872,8 +46049,11 @@
       <c r="IP60" s="1" t="n">
         <v>1.27</v>
       </c>
-      <c r="IQ60" t="n">
+      <c r="IQ60" s="1" t="n">
         <v>1.1</v>
+      </c>
+      <c r="IR60" t="n">
+        <v>1.27</v>
       </c>
     </row>
     <row r="61" ht="13.8" customHeight="1" s="2">
@@ -46629,8 +46809,11 @@
       <c r="IP61" s="1" t="n">
         <v>73</v>
       </c>
-      <c r="IQ61" t="n">
+      <c r="IQ61" s="1" t="n">
         <v>72</v>
+      </c>
+      <c r="IR61" t="n">
+        <v>67</v>
       </c>
     </row>
     <row r="62" ht="13.8" customHeight="1" s="2">
@@ -47386,8 +47569,11 @@
       <c r="IP62" s="1" t="n">
         <v>58</v>
       </c>
-      <c r="IQ62" t="n">
+      <c r="IQ62" s="1" t="n">
         <v>61</v>
+      </c>
+      <c r="IR62" t="n">
+        <v>80</v>
       </c>
     </row>
     <row r="63" ht="13.8" customHeight="1" s="2">
@@ -48143,8 +48329,11 @@
       <c r="IP63" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="IQ63" t="n">
+      <c r="IQ63" s="1" t="n">
         <v>30</v>
+      </c>
+      <c r="IR63" t="n">
+        <v>33</v>
       </c>
     </row>
     <row r="64" ht="13.8" customHeight="1" s="2">
@@ -48900,8 +49089,11 @@
       <c r="IP64" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="IQ64" t="n">
+      <c r="IQ64" s="1" t="n">
         <v>30</v>
+      </c>
+      <c r="IR64" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="65" ht="13.8" customHeight="1" s="2">
@@ -49657,8 +49849,11 @@
       <c r="IP65" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="IQ65" t="n">
+      <c r="IQ65" s="1" t="n">
         <v>16</v>
+      </c>
+      <c r="IR65" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="66" ht="13.8" customHeight="1" s="2">
@@ -50414,8 +50609,11 @@
       <c r="IP66" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="IQ66" t="n">
+      <c r="IQ66" s="1" t="n">
         <v>15</v>
+      </c>
+      <c r="IR66" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="67" ht="13.8" customHeight="1" s="2">
@@ -51171,8 +51369,11 @@
       <c r="IP67" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="IQ67" t="n">
+      <c r="IQ67" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="IR67" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="68" ht="13.8" customHeight="1" s="2">
@@ -51928,8 +52129,11 @@
       <c r="IP68" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="IQ68" t="n">
+      <c r="IQ68" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="IR68" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="69" ht="13.8" customHeight="1" s="2">
@@ -52685,8 +52889,11 @@
       <c r="IP69" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="IQ69" t="n">
+      <c r="IQ69" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="IR69" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="70" ht="13.8" customHeight="1" s="2">
@@ -53442,8 +53649,11 @@
       <c r="IP70" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="IQ70" t="n">
+      <c r="IQ70" s="1" t="n">
         <v>25</v>
+      </c>
+      <c r="IR70" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="71" ht="13.8" customHeight="1" s="2">
@@ -54199,8 +54409,11 @@
       <c r="IP71" s="1" t="n">
         <v>39.3</v>
       </c>
-      <c r="IQ71" t="n">
+      <c r="IQ71" s="1" t="n">
         <v>60</v>
+      </c>
+      <c r="IR71" t="n">
+        <v>48.1</v>
       </c>
     </row>
     <row r="72" ht="13.8" customHeight="1" s="2">
@@ -54956,8 +55169,11 @@
       <c r="IP72" s="1" t="n">
         <v>28.45</v>
       </c>
-      <c r="IQ72" t="n">
+      <c r="IQ72" s="1" t="n">
         <v>25.6</v>
+      </c>
+      <c r="IR72" t="n">
+        <v>26.38</v>
       </c>
     </row>
     <row r="73" ht="13.8" customHeight="1" s="2">
@@ -55713,8 +55929,11 @@
       <c r="IP73" s="1" t="n">
         <v>11.18</v>
       </c>
-      <c r="IQ73" t="n">
+      <c r="IQ73" s="1" t="n">
         <v>15.36</v>
+      </c>
+      <c r="IR73" t="n">
+        <v>12.7</v>
       </c>
     </row>
     <row r="74" ht="13.8" customHeight="1" s="2">
@@ -56470,8 +56689,11 @@
       <c r="IP74" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="IQ74" t="n">
+      <c r="IQ74" s="1" t="n">
         <v>29</v>
+      </c>
+      <c r="IR74" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="75" ht="13.8" customHeight="1" s="2">
@@ -57227,8 +57449,11 @@
       <c r="IP75" s="1" t="n">
         <v>61</v>
       </c>
-      <c r="IQ75" t="n">
+      <c r="IQ75" s="1" t="n">
         <v>61</v>
+      </c>
+      <c r="IR75" t="n">
+        <v>64</v>
       </c>
     </row>
     <row r="76" ht="13.8" customHeight="1" s="2">
@@ -57984,8 +58209,11 @@
       <c r="IP76" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="IQ76" t="n">
+      <c r="IQ76" s="1" t="n">
         <v>43</v>
+      </c>
+      <c r="IR76" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="77" ht="13.8" customHeight="1" s="2">
@@ -58741,8 +58969,11 @@
       <c r="IP77" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="IQ77" t="n">
+      <c r="IQ77" s="1" t="n">
         <v>54</v>
+      </c>
+      <c r="IR77" t="n">
+        <v>48</v>
       </c>
     </row>
     <row r="78" ht="13.8" customHeight="1" s="2">
@@ -59498,8 +59729,11 @@
       <c r="IP78" s="1" t="n">
         <v>1.96</v>
       </c>
-      <c r="IQ78" t="n">
+      <c r="IQ78" s="1" t="n">
         <v>2.16</v>
+      </c>
+      <c r="IR78" t="n">
+        <v>1.78</v>
       </c>
     </row>
     <row r="79" ht="13.8" customHeight="1" s="2">
@@ -60255,8 +60489,11 @@
       <c r="IP79" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="IQ79" t="n">
+      <c r="IQ79" s="1" t="n">
         <v>3.6</v>
+      </c>
+      <c r="IR79" t="n">
+        <v>3.69</v>
       </c>
     </row>
     <row r="80" ht="13.8" customHeight="1" s="2">
@@ -61012,8 +61249,11 @@
       <c r="IP80" s="1" t="n">
         <v>47.3</v>
       </c>
-      <c r="IQ80" t="n">
+      <c r="IQ80" s="1" t="n">
         <v>42.6</v>
+      </c>
+      <c r="IR80" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="81" ht="13.8" customHeight="1" s="2">
@@ -61769,8 +62009,11 @@
       <c r="IP81" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="IQ81" t="n">
+      <c r="IQ81" s="1" t="n">
         <v>27.8</v>
+      </c>
+      <c r="IR81" t="n">
+        <v>27.1</v>
       </c>
     </row>
     <row r="82" ht="13.8" customHeight="1" s="2">
@@ -62526,8 +62769,11 @@
       <c r="IP82" s="1" t="n">
         <v>188.7</v>
       </c>
-      <c r="IQ82" t="n">
+      <c r="IQ82" s="1" t="n">
         <v>188.5</v>
+      </c>
+      <c r="IR82" t="n">
+        <v>187.1</v>
       </c>
     </row>
     <row r="83" ht="13.8" customHeight="1" s="2">
@@ -63283,8 +63529,11 @@
       <c r="IP83" s="1" t="n">
         <v>88.3</v>
       </c>
-      <c r="IQ83" t="n">
+      <c r="IQ83" s="1" t="n">
         <v>86.59999999999999</v>
+      </c>
+      <c r="IR83" t="n">
+        <v>86.7</v>
       </c>
     </row>
     <row r="84" ht="13.8" customHeight="1" s="2">
@@ -64040,8 +64289,11 @@
       <c r="IP84" s="1" t="n">
         <v>24.49</v>
       </c>
-      <c r="IQ84" t="n">
+      <c r="IQ84" s="1" t="n">
         <v>25.91</v>
+      </c>
+      <c r="IR84" t="n">
+        <v>25.33</v>
       </c>
     </row>
     <row r="85" ht="13.8" customHeight="1" s="2">
@@ -64797,8 +65049,11 @@
       <c r="IP85" s="1" t="n">
         <v>67.3</v>
       </c>
-      <c r="IQ85" t="n">
+      <c r="IQ85" s="1" t="n">
         <v>97.2</v>
+      </c>
+      <c r="IR85" t="n">
+        <v>93.09999999999999</v>
       </c>
     </row>
     <row r="86" ht="13.8" customHeight="1" s="2">
@@ -65554,8 +65809,11 @@
       <c r="IP86" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="IQ86" t="n">
+      <c r="IQ86" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="IR86" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="87" ht="13.8" customHeight="1" s="2">
@@ -66311,8 +66569,11 @@
       <c r="IP87" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="IQ87" t="n">
+      <c r="IQ87" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="IR87" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="88" ht="13.8" customHeight="1" s="2">
@@ -67068,8 +67329,11 @@
       <c r="IP88" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="IQ88" t="n">
+      <c r="IQ88" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="IR88" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="89" ht="13.8" customHeight="1" s="2">
@@ -67825,8 +68089,11 @@
       <c r="IP89" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="IQ89" t="n">
+      <c r="IQ89" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="IR89" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="90" ht="13.8" customHeight="1" s="2">
@@ -68582,8 +68849,11 @@
       <c r="IP90" s="1" t="n">
         <v>129</v>
       </c>
-      <c r="IQ90" t="n">
+      <c r="IQ90" s="1" t="n">
         <v>139</v>
+      </c>
+      <c r="IR90" t="n">
+        <v>134</v>
       </c>
     </row>
     <row r="91" ht="13.8" customHeight="1" s="2">
@@ -69339,8 +69609,11 @@
       <c r="IP91" s="1" t="n">
         <v>187</v>
       </c>
-      <c r="IQ91" t="n">
+      <c r="IQ91" s="1" t="n">
         <v>230</v>
+      </c>
+      <c r="IR91" t="n">
+        <v>194</v>
       </c>
     </row>
     <row r="92" ht="13.8" customHeight="1" s="2">
@@ -70096,8 +70369,11 @@
       <c r="IP92" s="1" t="n">
         <v>237</v>
       </c>
-      <c r="IQ92" t="n">
+      <c r="IQ92" s="1" t="n">
         <v>282</v>
+      </c>
+      <c r="IR92" t="n">
+        <v>249</v>
       </c>
     </row>
     <row r="93" ht="13.8" customHeight="1" s="2">
@@ -70853,8 +71129,11 @@
       <c r="IP93" s="1" t="n">
         <v>75.7</v>
       </c>
-      <c r="IQ93" t="n">
+      <c r="IQ93" s="1" t="n">
         <v>73.40000000000001</v>
+      </c>
+      <c r="IR93" t="n">
+        <v>72.59999999999999</v>
       </c>
     </row>
     <row r="94" ht="13.8" customHeight="1" s="2">
@@ -71610,8 +71889,11 @@
       <c r="IP94" s="1" t="n">
         <v>61</v>
       </c>
-      <c r="IQ94" t="n">
+      <c r="IQ94" s="1" t="n">
         <v>61</v>
+      </c>
+      <c r="IR94" t="n">
+        <v>64</v>
       </c>
     </row>
     <row r="95" ht="13.8" customHeight="1" s="2">
@@ -72367,8 +72649,11 @@
       <c r="IP95" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="IQ95" t="n">
+      <c r="IQ95" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="IR95" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="96" ht="13.8" customHeight="1" s="2">
@@ -73124,8 +73409,11 @@
       <c r="IP96" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="IQ96" t="n">
+      <c r="IQ96" s="1" t="n">
         <v>9</v>
+      </c>
+      <c r="IR96" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="97" ht="13.8" customHeight="1" s="2">
@@ -73881,8 +74169,11 @@
       <c r="IP97" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="IQ97" t="n">
+      <c r="IQ97" s="1" t="n">
         <v>29</v>
+      </c>
+      <c r="IR97" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="98" ht="13.8" customHeight="1" s="2">
@@ -74638,8 +74929,11 @@
       <c r="IP98" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="IQ98" t="n">
+      <c r="IQ98" s="1" t="n">
         <v>43</v>
+      </c>
+      <c r="IR98" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="99" ht="13.8" customHeight="1" s="2">
@@ -75395,8 +75689,11 @@
       <c r="IP99" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="IQ99" t="n">
+      <c r="IQ99" s="1" t="n">
         <v>48</v>
+      </c>
+      <c r="IR99" t="n">
+        <v>49</v>
       </c>
     </row>
     <row r="100" ht="13.8" customHeight="1" s="2">
@@ -76152,8 +76449,11 @@
       <c r="IP100" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="IQ100" t="n">
+      <c r="IQ100" s="1" t="n">
         <v>11</v>
+      </c>
+      <c r="IR100" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="101" ht="13.8" customHeight="1" s="2">
@@ -76909,8 +77209,11 @@
       <c r="IP101" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="IQ101" t="n">
+      <c r="IQ101" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="IR101" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="102" ht="13.8" customHeight="1" s="2">
@@ -77666,8 +77969,11 @@
       <c r="IP102" s="1" t="n">
         <v>72.7</v>
       </c>
-      <c r="IQ102" t="n">
+      <c r="IQ102" s="1" t="n">
         <v>66.7</v>
+      </c>
+      <c r="IR102" t="n">
+        <v>61.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Round 5 2022. Fixed assemble_df bug and tested team specific models. spoiler: not enough data to make good preds
</commit_message>
<xml_diff>
--- a/django_AFL_ML/Data/Adelaide_stats.xlsx
+++ b/django_AFL_ML/Data/Adelaide_stats.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:IR102"/>
+  <dimension ref="A1:IS102"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="GZ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="HA23" activeCellId="0" sqref="HA23"/>
@@ -1212,8 +1212,11 @@
       <c r="IQ1" s="1" t="n">
         <v>10555</v>
       </c>
-      <c r="IR1" t="n">
+      <c r="IR1" s="1" t="n">
         <v>10564</v>
+      </c>
+      <c r="IS1" t="n">
+        <v>10577</v>
       </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="2">
@@ -1972,7 +1975,10 @@
       <c r="IQ2" s="1" t="n">
         <v>2022</v>
       </c>
-      <c r="IR2" t="n">
+      <c r="IR2" s="1" t="n">
+        <v>2022</v>
+      </c>
+      <c r="IS2" t="n">
         <v>2022</v>
       </c>
     </row>
@@ -2732,8 +2738,11 @@
       <c r="IQ3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="IR3" t="n">
+      <c r="IR3" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="IS3" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="2">
@@ -3492,8 +3501,11 @@
       <c r="IQ4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="IR4" t="n">
+      <c r="IR4" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="IS4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5" ht="13.8" customHeight="1" s="2">
@@ -4252,7 +4264,10 @@
       <c r="IQ5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="IR5" t="n">
+      <c r="IR5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="IS5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5012,8 +5027,11 @@
       <c r="IQ6" s="1" t="n">
         <v>58</v>
       </c>
-      <c r="IR6" t="n">
+      <c r="IR6" s="1" t="n">
         <v>96</v>
+      </c>
+      <c r="IS6" t="n">
+        <v>99</v>
       </c>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="2">
@@ -5772,8 +5790,11 @@
       <c r="IQ7" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="IR7" t="n">
+      <c r="IR7" s="1" t="n">
         <v>92</v>
+      </c>
+      <c r="IS7" t="n">
+        <v>103</v>
       </c>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="2">
@@ -6532,8 +6553,11 @@
       <c r="IQ8" s="1" t="n">
         <v>-42</v>
       </c>
-      <c r="IR8" t="n">
+      <c r="IR8" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="IS8" t="n">
+        <v>-4</v>
       </c>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="2">
@@ -7292,8 +7316,11 @@
       <c r="IQ9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="IR9" t="n">
+      <c r="IR9" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="IS9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10" ht="13.8" customHeight="1" s="2">
@@ -8052,8 +8079,11 @@
       <c r="IQ10" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="IR10" t="n">
+      <c r="IR10" s="1" t="n">
         <v>13</v>
+      </c>
+      <c r="IS10" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="11" ht="13.8" customHeight="1" s="2">
@@ -8812,8 +8842,11 @@
       <c r="IQ11" s="1" t="n">
         <v>220</v>
       </c>
-      <c r="IR11" t="n">
+      <c r="IR11" s="1" t="n">
         <v>192</v>
+      </c>
+      <c r="IS11" t="n">
+        <v>211</v>
       </c>
     </row>
     <row r="12" ht="13.8" customHeight="1" s="2">
@@ -9572,8 +9605,11 @@
       <c r="IQ12" s="1" t="n">
         <v>169</v>
       </c>
-      <c r="IR12" t="n">
+      <c r="IR12" s="1" t="n">
         <v>153</v>
+      </c>
+      <c r="IS12" t="n">
+        <v>162</v>
       </c>
     </row>
     <row r="13" ht="13.8" customHeight="1" s="2">
@@ -10332,8 +10368,11 @@
       <c r="IQ13" s="1" t="n">
         <v>389</v>
       </c>
-      <c r="IR13" t="n">
+      <c r="IR13" s="1" t="n">
         <v>345</v>
+      </c>
+      <c r="IS13" t="n">
+        <v>373</v>
       </c>
     </row>
     <row r="14" ht="13.8" customHeight="1" s="2">
@@ -11092,8 +11131,11 @@
       <c r="IQ14" s="1" t="n">
         <v>1.3</v>
       </c>
-      <c r="IR14" t="n">
+      <c r="IR14" s="1" t="n">
         <v>1.25</v>
+      </c>
+      <c r="IS14" t="n">
+        <v>1.3</v>
       </c>
     </row>
     <row r="15" ht="13.8" customHeight="1" s="2">
@@ -11852,8 +11894,11 @@
       <c r="IQ15" s="1" t="n">
         <v>102</v>
       </c>
-      <c r="IR15" t="n">
+      <c r="IR15" s="1" t="n">
         <v>67</v>
+      </c>
+      <c r="IS15" t="n">
+        <v>81</v>
       </c>
     </row>
     <row r="16" ht="13.8" customHeight="1" s="2">
@@ -12612,8 +12657,11 @@
       <c r="IQ16" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="IR16" t="n">
+      <c r="IR16" s="1" t="n">
         <v>64</v>
+      </c>
+      <c r="IS16" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="17" ht="13.8" customHeight="1" s="2">
@@ -13372,8 +13420,11 @@
       <c r="IQ17" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="IR17" t="n">
+      <c r="IR17" s="1" t="n">
         <v>46</v>
+      </c>
+      <c r="IS17" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="18" ht="13.8" customHeight="1" s="2">
@@ -14132,8 +14183,11 @@
       <c r="IQ18" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="IR18" t="n">
+      <c r="IR18" s="1" t="n">
         <v>28</v>
+      </c>
+      <c r="IS18" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="19" ht="13.8" customHeight="1" s="2">
@@ -14892,8 +14946,11 @@
       <c r="IQ19" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="IR19" t="n">
+      <c r="IR19" s="1" t="n">
         <v>23</v>
+      </c>
+      <c r="IS19" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="20" ht="13.8" customHeight="1" s="2">
@@ -15652,7 +15709,10 @@
       <c r="IQ20" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="IR20" t="n">
+      <c r="IR20" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="IS20" t="n">
         <v>15</v>
       </c>
     </row>
@@ -16412,8 +16472,11 @@
       <c r="IQ21" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="IR21" t="n">
+      <c r="IR21" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="IS21" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="22" ht="13.8" customHeight="1" s="2">
@@ -17172,7 +17235,10 @@
       <c r="IQ22" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="IR22" t="n">
+      <c r="IR22" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="IS22" t="n">
         <v>6</v>
       </c>
     </row>
@@ -17932,8 +17998,11 @@
       <c r="IQ23" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="IR23" t="n">
+      <c r="IR23" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="IS23" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="24" ht="13.8" customHeight="1" s="2">
@@ -18692,8 +18761,11 @@
       <c r="IQ24" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="IR24" t="n">
+      <c r="IR24" s="1" t="n">
         <v>21</v>
+      </c>
+      <c r="IS24" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="25" ht="13.8" customHeight="1" s="2">
@@ -19452,8 +19524,11 @@
       <c r="IQ25" s="1" t="n">
         <v>44.4</v>
       </c>
-      <c r="IR25" t="n">
+      <c r="IR25" s="1" t="n">
         <v>71.40000000000001</v>
+      </c>
+      <c r="IS25" t="n">
+        <v>62.5</v>
       </c>
     </row>
     <row r="26" ht="13.8" customHeight="1" s="2">
@@ -20212,8 +20287,11 @@
       <c r="IQ26" s="1" t="n">
         <v>48.62</v>
       </c>
-      <c r="IR26" t="n">
+      <c r="IR26" s="1" t="n">
         <v>23</v>
+      </c>
+      <c r="IS26" t="n">
+        <v>24.87</v>
       </c>
     </row>
     <row r="27" ht="13.8" customHeight="1" s="2">
@@ -20972,8 +21050,11 @@
       <c r="IQ27" s="1" t="n">
         <v>21.61</v>
       </c>
-      <c r="IR27" t="n">
+      <c r="IR27" s="1" t="n">
         <v>16.43</v>
+      </c>
+      <c r="IS27" t="n">
+        <v>15.54</v>
       </c>
     </row>
     <row r="28" ht="13.8" customHeight="1" s="2">
@@ -21732,7 +21813,10 @@
       <c r="IQ28" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="IR28" t="n">
+      <c r="IR28" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="IS28" t="n">
         <v>40</v>
       </c>
     </row>
@@ -22492,8 +22576,11 @@
       <c r="IQ29" s="1" t="n">
         <v>69</v>
       </c>
-      <c r="IR29" t="n">
+      <c r="IR29" s="1" t="n">
         <v>50</v>
+      </c>
+      <c r="IS29" t="n">
+        <v>77</v>
       </c>
     </row>
     <row r="30" ht="13.8" customHeight="1" s="2">
@@ -23252,8 +23339,11 @@
       <c r="IQ30" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="IR30" t="n">
+      <c r="IR30" s="1" t="n">
         <v>34</v>
+      </c>
+      <c r="IS30" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="31" ht="13.8" customHeight="1" s="2">
@@ -24012,8 +24102,11 @@
       <c r="IQ31" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="IR31" t="n">
+      <c r="IR31" s="1" t="n">
         <v>43</v>
+      </c>
+      <c r="IS31" t="n">
+        <v>53</v>
       </c>
     </row>
     <row r="32" ht="13.8" customHeight="1" s="2">
@@ -24772,8 +24865,11 @@
       <c r="IQ32" s="1" t="n">
         <v>2.83</v>
       </c>
-      <c r="IR32" t="n">
+      <c r="IR32" s="1" t="n">
         <v>2.05</v>
+      </c>
+      <c r="IS32" t="n">
+        <v>2.21</v>
       </c>
     </row>
     <row r="33" ht="13.8" customHeight="1" s="2">
@@ -25532,8 +25628,11 @@
       <c r="IQ33" s="1" t="n">
         <v>6.38</v>
       </c>
-      <c r="IR33" t="n">
+      <c r="IR33" s="1" t="n">
         <v>2.87</v>
+      </c>
+      <c r="IS33" t="n">
+        <v>3.53</v>
       </c>
     </row>
     <row r="34" ht="13.8" customHeight="1" s="2">
@@ -26292,8 +26391,11 @@
       <c r="IQ34" s="1" t="n">
         <v>31.4</v>
       </c>
-      <c r="IR34" t="n">
+      <c r="IR34" s="1" t="n">
         <v>48.8</v>
+      </c>
+      <c r="IS34" t="n">
+        <v>39.6</v>
       </c>
     </row>
     <row r="35" ht="13.8" customHeight="1" s="2">
@@ -27052,8 +27154,11 @@
       <c r="IQ35" s="1" t="n">
         <v>15.7</v>
       </c>
-      <c r="IR35" t="n">
+      <c r="IR35" s="1" t="n">
         <v>34.9</v>
+      </c>
+      <c r="IS35" t="n">
+        <v>28.3</v>
       </c>
     </row>
     <row r="36" ht="13.8" customHeight="1" s="2">
@@ -27812,8 +27917,11 @@
       <c r="IQ36" s="1" t="n">
         <v>186.9</v>
       </c>
-      <c r="IR36" t="n">
+      <c r="IR36" s="1" t="n">
         <v>187</v>
+      </c>
+      <c r="IS36" t="n">
+        <v>186.8</v>
       </c>
     </row>
     <row r="37" ht="13.8" customHeight="1" s="2">
@@ -28572,7 +28680,10 @@
       <c r="IQ37" s="1" t="n">
         <v>86</v>
       </c>
-      <c r="IR37" t="n">
+      <c r="IR37" s="1" t="n">
+        <v>86.2</v>
+      </c>
+      <c r="IS37" t="n">
         <v>86.2</v>
       </c>
     </row>
@@ -29332,8 +29443,11 @@
       <c r="IQ38" s="1" t="n">
         <v>23.58</v>
       </c>
-      <c r="IR38" t="n">
+      <c r="IR38" s="1" t="n">
         <v>23.91</v>
+      </c>
+      <c r="IS38" t="n">
+        <v>24.74</v>
       </c>
     </row>
     <row r="39" ht="13.8" customHeight="1" s="2">
@@ -30092,8 +30206,11 @@
       <c r="IQ39" s="1" t="n">
         <v>55.2</v>
       </c>
-      <c r="IR39" t="n">
+      <c r="IR39" s="1" t="n">
         <v>59.2</v>
+      </c>
+      <c r="IS39" t="n">
+        <v>75.40000000000001</v>
       </c>
     </row>
     <row r="40" ht="13.8" customHeight="1" s="2">
@@ -30852,8 +30969,11 @@
       <c r="IQ40" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="IR40" t="n">
+      <c r="IR40" s="1" t="n">
         <v>13</v>
+      </c>
+      <c r="IS40" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="41" ht="13.8" customHeight="1" s="2">
@@ -31612,7 +31732,10 @@
       <c r="IQ41" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="IR41" t="n">
+      <c r="IR41" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="IS41" t="n">
         <v>5</v>
       </c>
     </row>
@@ -32372,7 +32495,10 @@
       <c r="IQ42" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="IR42" t="n">
+      <c r="IR42" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="IS42" t="n">
         <v>1</v>
       </c>
     </row>
@@ -33132,8 +33258,11 @@
       <c r="IQ43" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="IR43" t="n">
+      <c r="IR43" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="IS43" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="44" ht="13.8" customHeight="1" s="2">
@@ -33892,8 +34021,11 @@
       <c r="IQ44" s="1" t="n">
         <v>136</v>
       </c>
-      <c r="IR44" t="n">
+      <c r="IR44" s="1" t="n">
         <v>140</v>
+      </c>
+      <c r="IS44" t="n">
+        <v>157</v>
       </c>
     </row>
     <row r="45" ht="13.8" customHeight="1" s="2">
@@ -34652,8 +34784,11 @@
       <c r="IQ45" s="1" t="n">
         <v>252</v>
       </c>
-      <c r="IR45" t="n">
+      <c r="IR45" s="1" t="n">
         <v>197</v>
+      </c>
+      <c r="IS45" t="n">
+        <v>212</v>
       </c>
     </row>
     <row r="46" ht="13.8" customHeight="1" s="2">
@@ -35412,8 +35547,11 @@
       <c r="IQ46" s="1" t="n">
         <v>281</v>
       </c>
-      <c r="IR46" t="n">
+      <c r="IR46" s="1" t="n">
         <v>248</v>
+      </c>
+      <c r="IS46" t="n">
+        <v>268</v>
       </c>
     </row>
     <row r="47" ht="13.8" customHeight="1" s="2">
@@ -36172,8 +36310,11 @@
       <c r="IQ47" s="1" t="n">
         <v>72.2</v>
       </c>
-      <c r="IR47" t="n">
+      <c r="IR47" s="1" t="n">
         <v>71.90000000000001</v>
+      </c>
+      <c r="IS47" t="n">
+        <v>71.8</v>
       </c>
     </row>
     <row r="48" ht="13.8" customHeight="1" s="2">
@@ -36932,8 +37073,11 @@
       <c r="IQ48" s="1" t="n">
         <v>69</v>
       </c>
-      <c r="IR48" t="n">
+      <c r="IR48" s="1" t="n">
         <v>50</v>
+      </c>
+      <c r="IS48" t="n">
+        <v>77</v>
       </c>
     </row>
     <row r="49" ht="13.8" customHeight="1" s="2">
@@ -37692,8 +37836,11 @@
       <c r="IQ49" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="IR49" t="n">
+      <c r="IR49" s="1" t="n">
         <v>13</v>
+      </c>
+      <c r="IS49" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="50" ht="13.8" customHeight="1" s="2">
@@ -38452,8 +38599,11 @@
       <c r="IQ50" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="IR50" t="n">
+      <c r="IR50" s="1" t="n">
         <v>9</v>
+      </c>
+      <c r="IS50" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="51" ht="13.8" customHeight="1" s="2">
@@ -39212,7 +39362,10 @@
       <c r="IQ51" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="IR51" t="n">
+      <c r="IR51" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="IS51" t="n">
         <v>40</v>
       </c>
     </row>
@@ -39972,8 +40125,11 @@
       <c r="IQ52" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="IR52" t="n">
+      <c r="IR52" s="1" t="n">
         <v>34</v>
+      </c>
+      <c r="IS52" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="53" ht="13.8" customHeight="1" s="2">
@@ -40732,8 +40888,11 @@
       <c r="IQ53" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="IR53" t="n">
+      <c r="IR53" s="1" t="n">
         <v>40</v>
+      </c>
+      <c r="IS53" t="n">
+        <v>53</v>
       </c>
     </row>
     <row r="54" ht="13.8" customHeight="1" s="2">
@@ -41492,8 +41651,11 @@
       <c r="IQ54" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="IR54" t="n">
+      <c r="IR54" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="IS54" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="55" ht="13.8" customHeight="1" s="2">
@@ -42252,8 +42414,11 @@
       <c r="IQ55" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="IR55" t="n">
+      <c r="IR55" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="IS55" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="56" ht="13.8" customHeight="1" s="2">
@@ -43012,8 +43177,11 @@
       <c r="IQ56" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="IR56" t="n">
+      <c r="IR56" s="1" t="n">
         <v>53.3</v>
+      </c>
+      <c r="IS56" t="n">
+        <v>66.7</v>
       </c>
     </row>
     <row r="57" ht="13.8" customHeight="1" s="2">
@@ -43772,8 +43940,11 @@
       <c r="IQ57" s="1" t="n">
         <v>201</v>
       </c>
-      <c r="IR57" t="n">
+      <c r="IR57" s="1" t="n">
         <v>192</v>
+      </c>
+      <c r="IS57" t="n">
+        <v>221</v>
       </c>
     </row>
     <row r="58" ht="13.8" customHeight="1" s="2">
@@ -44532,8 +44703,11 @@
       <c r="IQ58" s="1" t="n">
         <v>183</v>
       </c>
-      <c r="IR58" t="n">
+      <c r="IR58" s="1" t="n">
         <v>151</v>
+      </c>
+      <c r="IS58" t="n">
+        <v>144</v>
       </c>
     </row>
     <row r="59" ht="13.8" customHeight="1" s="2">
@@ -45292,8 +45466,11 @@
       <c r="IQ59" s="1" t="n">
         <v>384</v>
       </c>
-      <c r="IR59" t="n">
+      <c r="IR59" s="1" t="n">
         <v>343</v>
+      </c>
+      <c r="IS59" t="n">
+        <v>365</v>
       </c>
     </row>
     <row r="60" ht="13.8" customHeight="1" s="2">
@@ -46052,8 +46229,11 @@
       <c r="IQ60" s="1" t="n">
         <v>1.1</v>
       </c>
-      <c r="IR60" t="n">
+      <c r="IR60" s="1" t="n">
         <v>1.27</v>
+      </c>
+      <c r="IS60" t="n">
+        <v>1.53</v>
       </c>
     </row>
     <row r="61" ht="13.8" customHeight="1" s="2">
@@ -46812,8 +46992,11 @@
       <c r="IQ61" s="1" t="n">
         <v>72</v>
       </c>
-      <c r="IR61" t="n">
+      <c r="IR61" s="1" t="n">
         <v>67</v>
+      </c>
+      <c r="IS61" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="62" ht="13.8" customHeight="1" s="2">
@@ -47572,8 +47755,11 @@
       <c r="IQ62" s="1" t="n">
         <v>61</v>
       </c>
-      <c r="IR62" t="n">
+      <c r="IR62" s="1" t="n">
         <v>80</v>
+      </c>
+      <c r="IS62" t="n">
+        <v>47</v>
       </c>
     </row>
     <row r="63" ht="13.8" customHeight="1" s="2">
@@ -48332,8 +48518,11 @@
       <c r="IQ63" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="IR63" t="n">
+      <c r="IR63" s="1" t="n">
         <v>33</v>
+      </c>
+      <c r="IS63" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="64" ht="13.8" customHeight="1" s="2">
@@ -49092,8 +49281,11 @@
       <c r="IQ64" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="IR64" t="n">
+      <c r="IR64" s="1" t="n">
         <v>23</v>
+      </c>
+      <c r="IS64" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="65" ht="13.8" customHeight="1" s="2">
@@ -49852,8 +50044,11 @@
       <c r="IQ65" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="IR65" t="n">
+      <c r="IR65" s="1" t="n">
         <v>28</v>
+      </c>
+      <c r="IS65" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="66" ht="13.8" customHeight="1" s="2">
@@ -50612,8 +50807,11 @@
       <c r="IQ66" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="IR66" t="n">
+      <c r="IR66" s="1" t="n">
         <v>13</v>
+      </c>
+      <c r="IS66" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="67" ht="13.8" customHeight="1" s="2">
@@ -51372,8 +51570,11 @@
       <c r="IQ67" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="IR67" t="n">
+      <c r="IR67" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="IS67" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="68" ht="13.8" customHeight="1" s="2">
@@ -52132,8 +52333,11 @@
       <c r="IQ68" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="IR68" t="n">
+      <c r="IR68" s="1" t="n">
         <v>11</v>
+      </c>
+      <c r="IS68" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="69" ht="13.8" customHeight="1" s="2">
@@ -52892,8 +53096,11 @@
       <c r="IQ69" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="IR69" t="n">
+      <c r="IR69" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="IS69" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="70" ht="13.8" customHeight="1" s="2">
@@ -53652,8 +53859,11 @@
       <c r="IQ70" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="IR70" t="n">
+      <c r="IR70" s="1" t="n">
         <v>27</v>
+      </c>
+      <c r="IS70" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="71" ht="13.8" customHeight="1" s="2">
@@ -54412,8 +54622,11 @@
       <c r="IQ71" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="IR71" t="n">
+      <c r="IR71" s="1" t="n">
         <v>48.1</v>
+      </c>
+      <c r="IS71" t="n">
+        <v>53.6</v>
       </c>
     </row>
     <row r="72" ht="13.8" customHeight="1" s="2">
@@ -55172,8 +55385,11 @@
       <c r="IQ72" s="1" t="n">
         <v>25.6</v>
       </c>
-      <c r="IR72" t="n">
+      <c r="IR72" s="1" t="n">
         <v>26.38</v>
+      </c>
+      <c r="IS72" t="n">
+        <v>24.33</v>
       </c>
     </row>
     <row r="73" ht="13.8" customHeight="1" s="2">
@@ -55932,8 +56148,11 @@
       <c r="IQ73" s="1" t="n">
         <v>15.36</v>
       </c>
-      <c r="IR73" t="n">
+      <c r="IR73" s="1" t="n">
         <v>12.7</v>
+      </c>
+      <c r="IS73" t="n">
+        <v>13.04</v>
       </c>
     </row>
     <row r="74" ht="13.8" customHeight="1" s="2">
@@ -56692,8 +56911,11 @@
       <c r="IQ74" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="IR74" t="n">
+      <c r="IR74" s="1" t="n">
         <v>40</v>
+      </c>
+      <c r="IS74" t="n">
+        <v>39</v>
       </c>
     </row>
     <row r="75" ht="13.8" customHeight="1" s="2">
@@ -57452,8 +57674,11 @@
       <c r="IQ75" s="1" t="n">
         <v>61</v>
       </c>
-      <c r="IR75" t="n">
+      <c r="IR75" s="1" t="n">
         <v>64</v>
+      </c>
+      <c r="IS75" t="n">
+        <v>65</v>
       </c>
     </row>
     <row r="76" ht="13.8" customHeight="1" s="2">
@@ -58212,8 +58437,11 @@
       <c r="IQ76" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="IR76" t="n">
+      <c r="IR76" s="1" t="n">
         <v>26</v>
+      </c>
+      <c r="IS76" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="77" ht="13.8" customHeight="1" s="2">
@@ -58972,8 +59200,11 @@
       <c r="IQ77" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="IR77" t="n">
+      <c r="IR77" s="1" t="n">
         <v>48</v>
+      </c>
+      <c r="IS77" t="n">
+        <v>65</v>
       </c>
     </row>
     <row r="78" ht="13.8" customHeight="1" s="2">
@@ -59732,8 +59963,11 @@
       <c r="IQ78" s="1" t="n">
         <v>2.16</v>
       </c>
-      <c r="IR78" t="n">
+      <c r="IR78" s="1" t="n">
         <v>1.78</v>
+      </c>
+      <c r="IS78" t="n">
+        <v>2.32</v>
       </c>
     </row>
     <row r="79" ht="13.8" customHeight="1" s="2">
@@ -60492,8 +60726,11 @@
       <c r="IQ79" s="1" t="n">
         <v>3.6</v>
       </c>
-      <c r="IR79" t="n">
+      <c r="IR79" s="1" t="n">
         <v>3.69</v>
+      </c>
+      <c r="IS79" t="n">
+        <v>4.33</v>
       </c>
     </row>
     <row r="80" ht="13.8" customHeight="1" s="2">
@@ -61252,8 +61489,11 @@
       <c r="IQ80" s="1" t="n">
         <v>42.6</v>
       </c>
-      <c r="IR80" t="n">
+      <c r="IR80" s="1" t="n">
         <v>50</v>
+      </c>
+      <c r="IS80" t="n">
+        <v>36.9</v>
       </c>
     </row>
     <row r="81" ht="13.8" customHeight="1" s="2">
@@ -62012,8 +62252,11 @@
       <c r="IQ81" s="1" t="n">
         <v>27.8</v>
       </c>
-      <c r="IR81" t="n">
+      <c r="IR81" s="1" t="n">
         <v>27.1</v>
+      </c>
+      <c r="IS81" t="n">
+        <v>23.1</v>
       </c>
     </row>
     <row r="82" ht="13.8" customHeight="1" s="2">
@@ -62772,8 +63015,11 @@
       <c r="IQ82" s="1" t="n">
         <v>188.5</v>
       </c>
-      <c r="IR82" t="n">
+      <c r="IR82" s="1" t="n">
         <v>187.1</v>
+      </c>
+      <c r="IS82" t="n">
+        <v>187</v>
       </c>
     </row>
     <row r="83" ht="13.8" customHeight="1" s="2">
@@ -63532,8 +63778,11 @@
       <c r="IQ83" s="1" t="n">
         <v>86.59999999999999</v>
       </c>
-      <c r="IR83" t="n">
+      <c r="IR83" s="1" t="n">
         <v>86.7</v>
+      </c>
+      <c r="IS83" t="n">
+        <v>85.3</v>
       </c>
     </row>
     <row r="84" ht="13.8" customHeight="1" s="2">
@@ -64292,8 +64541,11 @@
       <c r="IQ84" s="1" t="n">
         <v>25.91</v>
       </c>
-      <c r="IR84" t="n">
+      <c r="IR84" s="1" t="n">
         <v>25.33</v>
+      </c>
+      <c r="IS84" t="n">
+        <v>24.74</v>
       </c>
     </row>
     <row r="85" ht="13.8" customHeight="1" s="2">
@@ -65052,8 +65304,11 @@
       <c r="IQ85" s="1" t="n">
         <v>97.2</v>
       </c>
-      <c r="IR85" t="n">
+      <c r="IR85" s="1" t="n">
         <v>93.09999999999999</v>
+      </c>
+      <c r="IS85" t="n">
+        <v>66.3</v>
       </c>
     </row>
     <row r="86" ht="13.8" customHeight="1" s="2">
@@ -65812,8 +66067,11 @@
       <c r="IQ86" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="IR86" t="n">
+      <c r="IR86" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="IS86" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="87" ht="13.8" customHeight="1" s="2">
@@ -66572,8 +66830,11 @@
       <c r="IQ87" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="IR87" t="n">
+      <c r="IR87" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="IS87" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="88" ht="13.8" customHeight="1" s="2">
@@ -67332,8 +67593,11 @@
       <c r="IQ88" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="IR88" t="n">
+      <c r="IR88" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="IS88" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="89" ht="13.8" customHeight="1" s="2">
@@ -68092,8 +68356,11 @@
       <c r="IQ89" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="IR89" t="n">
+      <c r="IR89" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="IS89" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="90" ht="13.8" customHeight="1" s="2">
@@ -68852,8 +69119,11 @@
       <c r="IQ90" s="1" t="n">
         <v>139</v>
       </c>
-      <c r="IR90" t="n">
+      <c r="IR90" s="1" t="n">
         <v>134</v>
+      </c>
+      <c r="IS90" t="n">
+        <v>136</v>
       </c>
     </row>
     <row r="91" ht="13.8" customHeight="1" s="2">
@@ -69612,8 +69882,11 @@
       <c r="IQ91" s="1" t="n">
         <v>230</v>
       </c>
-      <c r="IR91" t="n">
+      <c r="IR91" s="1" t="n">
         <v>194</v>
+      </c>
+      <c r="IS91" t="n">
+        <v>222</v>
       </c>
     </row>
     <row r="92" ht="13.8" customHeight="1" s="2">
@@ -70372,8 +70645,11 @@
       <c r="IQ92" s="1" t="n">
         <v>282</v>
       </c>
-      <c r="IR92" t="n">
+      <c r="IR92" s="1" t="n">
         <v>249</v>
+      </c>
+      <c r="IS92" t="n">
+        <v>278</v>
       </c>
     </row>
     <row r="93" ht="13.8" customHeight="1" s="2">
@@ -71132,8 +71408,11 @@
       <c r="IQ93" s="1" t="n">
         <v>73.40000000000001</v>
       </c>
-      <c r="IR93" t="n">
+      <c r="IR93" s="1" t="n">
         <v>72.59999999999999</v>
+      </c>
+      <c r="IS93" t="n">
+        <v>76.2</v>
       </c>
     </row>
     <row r="94" ht="13.8" customHeight="1" s="2">
@@ -71892,8 +72171,11 @@
       <c r="IQ94" s="1" t="n">
         <v>61</v>
       </c>
-      <c r="IR94" t="n">
+      <c r="IR94" s="1" t="n">
         <v>64</v>
+      </c>
+      <c r="IS94" t="n">
+        <v>65</v>
       </c>
     </row>
     <row r="95" ht="13.8" customHeight="1" s="2">
@@ -72652,8 +72934,11 @@
       <c r="IQ95" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="IR95" t="n">
+      <c r="IR95" s="1" t="n">
         <v>11</v>
+      </c>
+      <c r="IS95" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="96" ht="13.8" customHeight="1" s="2">
@@ -73412,8 +73697,11 @@
       <c r="IQ96" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="IR96" t="n">
+      <c r="IR96" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="IS96" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="97" ht="13.8" customHeight="1" s="2">
@@ -74172,8 +74460,11 @@
       <c r="IQ97" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="IR97" t="n">
+      <c r="IR97" s="1" t="n">
         <v>40</v>
+      </c>
+      <c r="IS97" t="n">
+        <v>39</v>
       </c>
     </row>
     <row r="98" ht="13.8" customHeight="1" s="2">
@@ -74932,8 +75223,11 @@
       <c r="IQ98" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="IR98" t="n">
+      <c r="IR98" s="1" t="n">
         <v>26</v>
+      </c>
+      <c r="IS98" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="99" ht="13.8" customHeight="1" s="2">
@@ -75692,8 +75986,11 @@
       <c r="IQ99" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="IR99" t="n">
+      <c r="IR99" s="1" t="n">
         <v>49</v>
+      </c>
+      <c r="IS99" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="100" ht="13.8" customHeight="1" s="2">
@@ -76452,8 +76749,11 @@
       <c r="IQ100" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="IR100" t="n">
+      <c r="IR100" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="IS100" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="101" ht="13.8" customHeight="1" s="2">
@@ -77212,8 +77512,11 @@
       <c r="IQ101" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="IR101" t="n">
+      <c r="IR101" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="IS101" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="102" ht="13.8" customHeight="1" s="2">
@@ -77972,8 +78275,11 @@
       <c r="IQ102" s="1" t="n">
         <v>66.7</v>
       </c>
-      <c r="IR102" t="n">
+      <c r="IR102" s="1" t="n">
         <v>61.5</v>
+      </c>
+      <c r="IS102" t="n">
+        <v>86.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PAV fix, round 5 PAV updates. round 6 prediction
</commit_message>
<xml_diff>
--- a/django_AFL_ML/Data/Adelaide_stats.xlsx
+++ b/django_AFL_ML/Data/Adelaide_stats.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:IS102"/>
+  <dimension ref="A1:IT102"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="GZ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="HA23" activeCellId="0" sqref="HA23"/>
@@ -1215,8 +1215,11 @@
       <c r="IR1" s="1" t="n">
         <v>10564</v>
       </c>
-      <c r="IS1" t="n">
+      <c r="IS1" s="1" t="n">
         <v>10577</v>
+      </c>
+      <c r="IT1" t="n">
+        <v>10584</v>
       </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="2">
@@ -1978,7 +1981,10 @@
       <c r="IR2" s="1" t="n">
         <v>2022</v>
       </c>
-      <c r="IS2" t="n">
+      <c r="IS2" s="1" t="n">
+        <v>2022</v>
+      </c>
+      <c r="IT2" t="n">
         <v>2022</v>
       </c>
     </row>
@@ -2741,8 +2747,11 @@
       <c r="IR3" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="IS3" t="n">
+      <c r="IS3" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="IT3" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="2">
@@ -3504,8 +3513,11 @@
       <c r="IR4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="IS4" t="n">
+      <c r="IS4" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="IT4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5" ht="13.8" customHeight="1" s="2">
@@ -4267,7 +4279,10 @@
       <c r="IR5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="IS5" t="n">
+      <c r="IS5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="IT5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5030,8 +5045,11 @@
       <c r="IR6" s="1" t="n">
         <v>96</v>
       </c>
-      <c r="IS6" t="n">
+      <c r="IS6" s="1" t="n">
         <v>99</v>
+      </c>
+      <c r="IT6" t="n">
+        <v>101</v>
       </c>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="2">
@@ -5793,8 +5811,11 @@
       <c r="IR7" s="1" t="n">
         <v>92</v>
       </c>
-      <c r="IS7" t="n">
+      <c r="IS7" s="1" t="n">
         <v>103</v>
+      </c>
+      <c r="IT7" t="n">
+        <v>82</v>
       </c>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="2">
@@ -6556,8 +6577,11 @@
       <c r="IR8" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="IS8" t="n">
+      <c r="IS8" s="1" t="n">
         <v>-4</v>
+      </c>
+      <c r="IT8" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="2">
@@ -7319,8 +7343,11 @@
       <c r="IR9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="IS9" t="n">
+      <c r="IS9" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="IT9" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10" ht="13.8" customHeight="1" s="2">
@@ -8082,8 +8109,11 @@
       <c r="IR10" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="IS10" t="n">
+      <c r="IS10" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="IT10" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="11" ht="13.8" customHeight="1" s="2">
@@ -8845,8 +8875,11 @@
       <c r="IR11" s="1" t="n">
         <v>192</v>
       </c>
-      <c r="IS11" t="n">
+      <c r="IS11" s="1" t="n">
         <v>211</v>
+      </c>
+      <c r="IT11" t="n">
+        <v>212</v>
       </c>
     </row>
     <row r="12" ht="13.8" customHeight="1" s="2">
@@ -9608,8 +9641,11 @@
       <c r="IR12" s="1" t="n">
         <v>153</v>
       </c>
-      <c r="IS12" t="n">
+      <c r="IS12" s="1" t="n">
         <v>162</v>
+      </c>
+      <c r="IT12" t="n">
+        <v>161</v>
       </c>
     </row>
     <row r="13" ht="13.8" customHeight="1" s="2">
@@ -10371,7 +10407,10 @@
       <c r="IR13" s="1" t="n">
         <v>345</v>
       </c>
-      <c r="IS13" t="n">
+      <c r="IS13" s="1" t="n">
+        <v>373</v>
+      </c>
+      <c r="IT13" t="n">
         <v>373</v>
       </c>
     </row>
@@ -11134,8 +11173,11 @@
       <c r="IR14" s="1" t="n">
         <v>1.25</v>
       </c>
-      <c r="IS14" t="n">
+      <c r="IS14" s="1" t="n">
         <v>1.3</v>
+      </c>
+      <c r="IT14" t="n">
+        <v>1.32</v>
       </c>
     </row>
     <row r="15" ht="13.8" customHeight="1" s="2">
@@ -11897,7 +11939,10 @@
       <c r="IR15" s="1" t="n">
         <v>67</v>
       </c>
-      <c r="IS15" t="n">
+      <c r="IS15" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="IT15" t="n">
         <v>81</v>
       </c>
     </row>
@@ -12660,8 +12705,11 @@
       <c r="IR16" s="1" t="n">
         <v>64</v>
       </c>
-      <c r="IS16" t="n">
+      <c r="IS16" s="1" t="n">
         <v>45</v>
+      </c>
+      <c r="IT16" t="n">
+        <v>47</v>
       </c>
     </row>
     <row r="17" ht="13.8" customHeight="1" s="2">
@@ -13423,8 +13471,11 @@
       <c r="IR17" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="IS17" t="n">
+      <c r="IS17" s="1" t="n">
         <v>25</v>
+      </c>
+      <c r="IT17" t="n">
+        <v>29</v>
       </c>
     </row>
     <row r="18" ht="13.8" customHeight="1" s="2">
@@ -14186,8 +14237,11 @@
       <c r="IR18" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="IS18" t="n">
+      <c r="IS18" s="1" t="n">
         <v>26</v>
+      </c>
+      <c r="IT18" t="n">
+        <v>33</v>
       </c>
     </row>
     <row r="19" ht="13.8" customHeight="1" s="2">
@@ -14949,8 +15003,11 @@
       <c r="IR19" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="IS19" t="n">
+      <c r="IS19" s="1" t="n">
         <v>24</v>
+      </c>
+      <c r="IT19" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="20" ht="13.8" customHeight="1" s="2">
@@ -15712,7 +15769,10 @@
       <c r="IR20" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="IS20" t="n">
+      <c r="IS20" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="IT20" t="n">
         <v>15</v>
       </c>
     </row>
@@ -16475,8 +16535,11 @@
       <c r="IR21" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="IS21" t="n">
+      <c r="IS21" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="IT21" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="22" ht="13.8" customHeight="1" s="2">
@@ -17238,8 +17301,11 @@
       <c r="IR22" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="IS22" t="n">
+      <c r="IS22" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="IT22" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="23" ht="13.8" customHeight="1" s="2">
@@ -18001,8 +18067,11 @@
       <c r="IR23" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="IS23" t="n">
+      <c r="IS23" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="IT23" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="24" ht="13.8" customHeight="1" s="2">
@@ -18764,8 +18833,11 @@
       <c r="IR24" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="IS24" t="n">
+      <c r="IS24" s="1" t="n">
         <v>24</v>
+      </c>
+      <c r="IT24" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="25" ht="13.8" customHeight="1" s="2">
@@ -19527,8 +19599,11 @@
       <c r="IR25" s="1" t="n">
         <v>71.40000000000001</v>
       </c>
-      <c r="IS25" t="n">
+      <c r="IS25" s="1" t="n">
         <v>62.5</v>
+      </c>
+      <c r="IT25" t="n">
+        <v>57.7</v>
       </c>
     </row>
     <row r="26" ht="13.8" customHeight="1" s="2">
@@ -20290,7 +20365,10 @@
       <c r="IR26" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="IS26" t="n">
+      <c r="IS26" s="1" t="n">
+        <v>24.87</v>
+      </c>
+      <c r="IT26" t="n">
         <v>24.87</v>
       </c>
     </row>
@@ -21053,8 +21131,11 @@
       <c r="IR27" s="1" t="n">
         <v>16.43</v>
       </c>
-      <c r="IS27" t="n">
+      <c r="IS27" s="1" t="n">
         <v>15.54</v>
+      </c>
+      <c r="IT27" t="n">
+        <v>14.35</v>
       </c>
     </row>
     <row r="28" ht="13.8" customHeight="1" s="2">
@@ -21816,8 +21897,11 @@
       <c r="IR28" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="IS28" t="n">
+      <c r="IS28" s="1" t="n">
         <v>40</v>
+      </c>
+      <c r="IT28" t="n">
+        <v>34</v>
       </c>
     </row>
     <row r="29" ht="13.8" customHeight="1" s="2">
@@ -22579,8 +22663,11 @@
       <c r="IR29" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="IS29" t="n">
+      <c r="IS29" s="1" t="n">
         <v>77</v>
+      </c>
+      <c r="IT29" t="n">
+        <v>48</v>
       </c>
     </row>
     <row r="30" ht="13.8" customHeight="1" s="2">
@@ -23342,8 +23429,11 @@
       <c r="IR30" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="IS30" t="n">
+      <c r="IS30" s="1" t="n">
         <v>50</v>
+      </c>
+      <c r="IT30" t="n">
+        <v>49</v>
       </c>
     </row>
     <row r="31" ht="13.8" customHeight="1" s="2">
@@ -24105,8 +24195,11 @@
       <c r="IR31" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="IS31" t="n">
+      <c r="IS31" s="1" t="n">
         <v>53</v>
+      </c>
+      <c r="IT31" t="n">
+        <v>51</v>
       </c>
     </row>
     <row r="32" ht="13.8" customHeight="1" s="2">
@@ -24868,8 +24961,11 @@
       <c r="IR32" s="1" t="n">
         <v>2.05</v>
       </c>
-      <c r="IS32" t="n">
+      <c r="IS32" s="1" t="n">
         <v>2.21</v>
+      </c>
+      <c r="IT32" t="n">
+        <v>1.96</v>
       </c>
     </row>
     <row r="33" ht="13.8" customHeight="1" s="2">
@@ -25631,8 +25727,11 @@
       <c r="IR33" s="1" t="n">
         <v>2.87</v>
       </c>
-      <c r="IS33" t="n">
+      <c r="IS33" s="1" t="n">
         <v>3.53</v>
+      </c>
+      <c r="IT33" t="n">
+        <v>3.4</v>
       </c>
     </row>
     <row r="34" ht="13.8" customHeight="1" s="2">
@@ -26394,8 +26493,11 @@
       <c r="IR34" s="1" t="n">
         <v>48.8</v>
       </c>
-      <c r="IS34" t="n">
+      <c r="IS34" s="1" t="n">
         <v>39.6</v>
+      </c>
+      <c r="IT34" t="n">
+        <v>43.1</v>
       </c>
     </row>
     <row r="35" ht="13.8" customHeight="1" s="2">
@@ -27157,8 +27259,11 @@
       <c r="IR35" s="1" t="n">
         <v>34.9</v>
       </c>
-      <c r="IS35" t="n">
+      <c r="IS35" s="1" t="n">
         <v>28.3</v>
+      </c>
+      <c r="IT35" t="n">
+        <v>29.4</v>
       </c>
     </row>
     <row r="36" ht="13.8" customHeight="1" s="2">
@@ -27920,8 +28025,11 @@
       <c r="IR36" s="1" t="n">
         <v>187</v>
       </c>
-      <c r="IS36" t="n">
+      <c r="IS36" s="1" t="n">
         <v>186.8</v>
+      </c>
+      <c r="IT36" t="n">
+        <v>186.5</v>
       </c>
     </row>
     <row r="37" ht="13.8" customHeight="1" s="2">
@@ -28683,8 +28791,11 @@
       <c r="IR37" s="1" t="n">
         <v>86.2</v>
       </c>
-      <c r="IS37" t="n">
+      <c r="IS37" s="1" t="n">
         <v>86.2</v>
+      </c>
+      <c r="IT37" t="n">
+        <v>85.5</v>
       </c>
     </row>
     <row r="38" ht="13.8" customHeight="1" s="2">
@@ -29446,8 +29557,11 @@
       <c r="IR38" s="1" t="n">
         <v>23.91</v>
       </c>
-      <c r="IS38" t="n">
+      <c r="IS38" s="1" t="n">
         <v>24.74</v>
+      </c>
+      <c r="IT38" t="n">
+        <v>24.8</v>
       </c>
     </row>
     <row r="39" ht="13.8" customHeight="1" s="2">
@@ -30209,8 +30323,11 @@
       <c r="IR39" s="1" t="n">
         <v>59.2</v>
       </c>
-      <c r="IS39" t="n">
+      <c r="IS39" s="1" t="n">
         <v>75.40000000000001</v>
+      </c>
+      <c r="IT39" t="n">
+        <v>76.5</v>
       </c>
     </row>
     <row r="40" ht="13.8" customHeight="1" s="2">
@@ -30972,7 +31089,10 @@
       <c r="IR40" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="IS40" t="n">
+      <c r="IS40" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="IT40" t="n">
         <v>12</v>
       </c>
     </row>
@@ -31735,7 +31855,10 @@
       <c r="IR41" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="IS41" t="n">
+      <c r="IS41" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="IT41" t="n">
         <v>5</v>
       </c>
     </row>
@@ -32498,7 +32621,10 @@
       <c r="IR42" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="IS42" t="n">
+      <c r="IS42" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="IT42" t="n">
         <v>1</v>
       </c>
     </row>
@@ -33261,7 +33387,10 @@
       <c r="IR43" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="IS43" t="n">
+      <c r="IS43" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="IT43" t="n">
         <v>5</v>
       </c>
     </row>
@@ -34024,8 +34153,11 @@
       <c r="IR44" s="1" t="n">
         <v>140</v>
       </c>
-      <c r="IS44" t="n">
+      <c r="IS44" s="1" t="n">
         <v>157</v>
+      </c>
+      <c r="IT44" t="n">
+        <v>146</v>
       </c>
     </row>
     <row r="45" ht="13.8" customHeight="1" s="2">
@@ -34787,8 +34919,11 @@
       <c r="IR45" s="1" t="n">
         <v>197</v>
       </c>
-      <c r="IS45" t="n">
+      <c r="IS45" s="1" t="n">
         <v>212</v>
+      </c>
+      <c r="IT45" t="n">
+        <v>217</v>
       </c>
     </row>
     <row r="46" ht="13.8" customHeight="1" s="2">
@@ -35550,8 +35685,11 @@
       <c r="IR46" s="1" t="n">
         <v>248</v>
       </c>
-      <c r="IS46" t="n">
+      <c r="IS46" s="1" t="n">
         <v>268</v>
+      </c>
+      <c r="IT46" t="n">
+        <v>285</v>
       </c>
     </row>
     <row r="47" ht="13.8" customHeight="1" s="2">
@@ -36313,8 +36451,11 @@
       <c r="IR47" s="1" t="n">
         <v>71.90000000000001</v>
       </c>
-      <c r="IS47" t="n">
+      <c r="IS47" s="1" t="n">
         <v>71.8</v>
+      </c>
+      <c r="IT47" t="n">
+        <v>76.40000000000001</v>
       </c>
     </row>
     <row r="48" ht="13.8" customHeight="1" s="2">
@@ -37076,8 +37217,11 @@
       <c r="IR48" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="IS48" t="n">
+      <c r="IS48" s="1" t="n">
         <v>77</v>
+      </c>
+      <c r="IT48" t="n">
+        <v>48</v>
       </c>
     </row>
     <row r="49" ht="13.8" customHeight="1" s="2">
@@ -37839,8 +37983,11 @@
       <c r="IR49" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="IS49" t="n">
+      <c r="IS49" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="IT49" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="50" ht="13.8" customHeight="1" s="2">
@@ -38602,8 +38749,11 @@
       <c r="IR50" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="IS50" t="n">
+      <c r="IS50" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="IT50" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="51" ht="13.8" customHeight="1" s="2">
@@ -39365,8 +39515,11 @@
       <c r="IR51" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="IS51" t="n">
+      <c r="IS51" s="1" t="n">
         <v>40</v>
+      </c>
+      <c r="IT51" t="n">
+        <v>34</v>
       </c>
     </row>
     <row r="52" ht="13.8" customHeight="1" s="2">
@@ -40128,8 +40281,11 @@
       <c r="IR52" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="IS52" t="n">
+      <c r="IS52" s="1" t="n">
         <v>50</v>
+      </c>
+      <c r="IT52" t="n">
+        <v>49</v>
       </c>
     </row>
     <row r="53" ht="13.8" customHeight="1" s="2">
@@ -40891,8 +41047,11 @@
       <c r="IR53" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="IS53" t="n">
+      <c r="IS53" s="1" t="n">
         <v>53</v>
+      </c>
+      <c r="IT53" t="n">
+        <v>48</v>
       </c>
     </row>
     <row r="54" ht="13.8" customHeight="1" s="2">
@@ -41654,8 +41813,11 @@
       <c r="IR54" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="IS54" t="n">
+      <c r="IS54" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="IT54" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="55" ht="13.8" customHeight="1" s="2">
@@ -42417,8 +42579,11 @@
       <c r="IR55" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="IS55" t="n">
+      <c r="IS55" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="IT55" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="56" ht="13.8" customHeight="1" s="2">
@@ -43180,8 +43345,11 @@
       <c r="IR56" s="1" t="n">
         <v>53.3</v>
       </c>
-      <c r="IS56" t="n">
+      <c r="IS56" s="1" t="n">
         <v>66.7</v>
+      </c>
+      <c r="IT56" t="n">
+        <v>73.3</v>
       </c>
     </row>
     <row r="57" ht="13.8" customHeight="1" s="2">
@@ -43943,8 +44111,11 @@
       <c r="IR57" s="1" t="n">
         <v>192</v>
       </c>
-      <c r="IS57" t="n">
+      <c r="IS57" s="1" t="n">
         <v>221</v>
+      </c>
+      <c r="IT57" t="n">
+        <v>191</v>
       </c>
     </row>
     <row r="58" ht="13.8" customHeight="1" s="2">
@@ -44706,8 +44877,11 @@
       <c r="IR58" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="IS58" t="n">
+      <c r="IS58" s="1" t="n">
         <v>144</v>
+      </c>
+      <c r="IT58" t="n">
+        <v>162</v>
       </c>
     </row>
     <row r="59" ht="13.8" customHeight="1" s="2">
@@ -45469,8 +45643,11 @@
       <c r="IR59" s="1" t="n">
         <v>343</v>
       </c>
-      <c r="IS59" t="n">
+      <c r="IS59" s="1" t="n">
         <v>365</v>
+      </c>
+      <c r="IT59" t="n">
+        <v>353</v>
       </c>
     </row>
     <row r="60" ht="13.8" customHeight="1" s="2">
@@ -46232,8 +46409,11 @@
       <c r="IR60" s="1" t="n">
         <v>1.27</v>
       </c>
-      <c r="IS60" t="n">
+      <c r="IS60" s="1" t="n">
         <v>1.53</v>
+      </c>
+      <c r="IT60" t="n">
+        <v>1.18</v>
       </c>
     </row>
     <row r="61" ht="13.8" customHeight="1" s="2">
@@ -46995,8 +47175,11 @@
       <c r="IR61" s="1" t="n">
         <v>67</v>
       </c>
-      <c r="IS61" t="n">
+      <c r="IS61" s="1" t="n">
         <v>100</v>
+      </c>
+      <c r="IT61" t="n">
+        <v>80</v>
       </c>
     </row>
     <row r="62" ht="13.8" customHeight="1" s="2">
@@ -47758,8 +47941,11 @@
       <c r="IR62" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="IS62" t="n">
+      <c r="IS62" s="1" t="n">
         <v>47</v>
+      </c>
+      <c r="IT62" t="n">
+        <v>42</v>
       </c>
     </row>
     <row r="63" ht="13.8" customHeight="1" s="2">
@@ -48521,8 +48707,11 @@
       <c r="IR63" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="IS63" t="n">
+      <c r="IS63" s="1" t="n">
         <v>44</v>
+      </c>
+      <c r="IT63" t="n">
+        <v>41</v>
       </c>
     </row>
     <row r="64" ht="13.8" customHeight="1" s="2">
@@ -49284,8 +49473,11 @@
       <c r="IR64" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="IS64" t="n">
+      <c r="IS64" s="1" t="n">
         <v>24</v>
+      </c>
+      <c r="IT64" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="65" ht="13.8" customHeight="1" s="2">
@@ -50047,8 +50239,11 @@
       <c r="IR65" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="IS65" t="n">
+      <c r="IS65" s="1" t="n">
         <v>26</v>
+      </c>
+      <c r="IT65" t="n">
+        <v>33</v>
       </c>
     </row>
     <row r="66" ht="13.8" customHeight="1" s="2">
@@ -50810,8 +51005,11 @@
       <c r="IR66" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="IS66" t="n">
+      <c r="IS66" s="1" t="n">
         <v>15</v>
+      </c>
+      <c r="IT66" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="67" ht="13.8" customHeight="1" s="2">
@@ -51573,8 +51771,11 @@
       <c r="IR67" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="IS67" t="n">
+      <c r="IS67" s="1" t="n">
         <v>13</v>
+      </c>
+      <c r="IT67" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="68" ht="13.8" customHeight="1" s="2">
@@ -52336,8 +52537,11 @@
       <c r="IR68" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="IS68" t="n">
+      <c r="IS68" s="1" t="n">
         <v>9</v>
+      </c>
+      <c r="IT68" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="69" ht="13.8" customHeight="1" s="2">
@@ -53099,8 +53303,11 @@
       <c r="IR69" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="IS69" t="n">
+      <c r="IS69" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="IT69" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="70" ht="13.8" customHeight="1" s="2">
@@ -53862,8 +54069,11 @@
       <c r="IR70" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="IS70" t="n">
+      <c r="IS70" s="1" t="n">
         <v>28</v>
+      </c>
+      <c r="IT70" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="71" ht="13.8" customHeight="1" s="2">
@@ -54625,8 +54835,11 @@
       <c r="IR71" s="1" t="n">
         <v>48.1</v>
       </c>
-      <c r="IS71" t="n">
+      <c r="IS71" s="1" t="n">
         <v>53.6</v>
+      </c>
+      <c r="IT71" t="n">
+        <v>54.5</v>
       </c>
     </row>
     <row r="72" ht="13.8" customHeight="1" s="2">
@@ -55388,8 +55601,11 @@
       <c r="IR72" s="1" t="n">
         <v>26.38</v>
       </c>
-      <c r="IS72" t="n">
+      <c r="IS72" s="1" t="n">
         <v>24.33</v>
+      </c>
+      <c r="IT72" t="n">
+        <v>29.42</v>
       </c>
     </row>
     <row r="73" ht="13.8" customHeight="1" s="2">
@@ -56151,8 +56367,11 @@
       <c r="IR73" s="1" t="n">
         <v>12.7</v>
       </c>
-      <c r="IS73" t="n">
+      <c r="IS73" s="1" t="n">
         <v>13.04</v>
+      </c>
+      <c r="IT73" t="n">
+        <v>16.05</v>
       </c>
     </row>
     <row r="74" ht="13.8" customHeight="1" s="2">
@@ -56914,8 +57133,11 @@
       <c r="IR74" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="IS74" t="n">
+      <c r="IS74" s="1" t="n">
         <v>39</v>
+      </c>
+      <c r="IT74" t="n">
+        <v>36</v>
       </c>
     </row>
     <row r="75" ht="13.8" customHeight="1" s="2">
@@ -57677,8 +57899,11 @@
       <c r="IR75" s="1" t="n">
         <v>64</v>
       </c>
-      <c r="IS75" t="n">
+      <c r="IS75" s="1" t="n">
         <v>65</v>
+      </c>
+      <c r="IT75" t="n">
+        <v>66</v>
       </c>
     </row>
     <row r="76" ht="13.8" customHeight="1" s="2">
@@ -58440,8 +58665,11 @@
       <c r="IR76" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="IS76" t="n">
+      <c r="IS76" s="1" t="n">
         <v>37</v>
+      </c>
+      <c r="IT76" t="n">
+        <v>34</v>
       </c>
     </row>
     <row r="77" ht="13.8" customHeight="1" s="2">
@@ -59203,8 +59431,11 @@
       <c r="IR77" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="IS77" t="n">
+      <c r="IS77" s="1" t="n">
         <v>65</v>
+      </c>
+      <c r="IT77" t="n">
+        <v>61</v>
       </c>
     </row>
     <row r="78" ht="13.8" customHeight="1" s="2">
@@ -59966,8 +60197,11 @@
       <c r="IR78" s="1" t="n">
         <v>1.78</v>
       </c>
-      <c r="IS78" t="n">
+      <c r="IS78" s="1" t="n">
         <v>2.32</v>
+      </c>
+      <c r="IT78" t="n">
+        <v>2.77</v>
       </c>
     </row>
     <row r="79" ht="13.8" customHeight="1" s="2">
@@ -60729,8 +60963,11 @@
       <c r="IR79" s="1" t="n">
         <v>3.69</v>
       </c>
-      <c r="IS79" t="n">
+      <c r="IS79" s="1" t="n">
         <v>4.33</v>
+      </c>
+      <c r="IT79" t="n">
+        <v>5.08</v>
       </c>
     </row>
     <row r="80" ht="13.8" customHeight="1" s="2">
@@ -61492,8 +61729,11 @@
       <c r="IR80" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="IS80" t="n">
+      <c r="IS80" s="1" t="n">
         <v>36.9</v>
+      </c>
+      <c r="IT80" t="n">
+        <v>31.1</v>
       </c>
     </row>
     <row r="81" ht="13.8" customHeight="1" s="2">
@@ -62255,8 +62495,11 @@
       <c r="IR81" s="1" t="n">
         <v>27.1</v>
       </c>
-      <c r="IS81" t="n">
+      <c r="IS81" s="1" t="n">
         <v>23.1</v>
+      </c>
+      <c r="IT81" t="n">
+        <v>19.7</v>
       </c>
     </row>
     <row r="82" ht="13.8" customHeight="1" s="2">
@@ -63018,8 +63261,11 @@
       <c r="IR82" s="1" t="n">
         <v>187.1</v>
       </c>
-      <c r="IS82" t="n">
+      <c r="IS82" s="1" t="n">
         <v>187</v>
+      </c>
+      <c r="IT82" t="n">
+        <v>185.9</v>
       </c>
     </row>
     <row r="83" ht="13.8" customHeight="1" s="2">
@@ -63781,8 +64027,11 @@
       <c r="IR83" s="1" t="n">
         <v>86.7</v>
       </c>
-      <c r="IS83" t="n">
+      <c r="IS83" s="1" t="n">
         <v>85.3</v>
+      </c>
+      <c r="IT83" t="n">
+        <v>85.09999999999999</v>
       </c>
     </row>
     <row r="84" ht="13.8" customHeight="1" s="2">
@@ -64544,8 +64793,11 @@
       <c r="IR84" s="1" t="n">
         <v>25.33</v>
       </c>
-      <c r="IS84" t="n">
+      <c r="IS84" s="1" t="n">
         <v>24.74</v>
+      </c>
+      <c r="IT84" t="n">
+        <v>26.74</v>
       </c>
     </row>
     <row r="85" ht="13.8" customHeight="1" s="2">
@@ -65307,8 +65559,11 @@
       <c r="IR85" s="1" t="n">
         <v>93.09999999999999</v>
       </c>
-      <c r="IS85" t="n">
+      <c r="IS85" s="1" t="n">
         <v>66.3</v>
+      </c>
+      <c r="IT85" t="n">
+        <v>112.2</v>
       </c>
     </row>
     <row r="86" ht="13.8" customHeight="1" s="2">
@@ -66070,8 +66325,11 @@
       <c r="IR86" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="IS86" t="n">
+      <c r="IS86" s="1" t="n">
         <v>11</v>
+      </c>
+      <c r="IT86" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="87" ht="13.8" customHeight="1" s="2">
@@ -66833,8 +67091,11 @@
       <c r="IR87" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="IS87" t="n">
+      <c r="IS87" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="IT87" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="88" ht="13.8" customHeight="1" s="2">
@@ -67596,8 +67857,11 @@
       <c r="IR88" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="IS88" t="n">
+      <c r="IS88" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="IT88" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="89" ht="13.8" customHeight="1" s="2">
@@ -68359,8 +68623,11 @@
       <c r="IR89" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="IS89" t="n">
+      <c r="IS89" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="IT89" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="90" ht="13.8" customHeight="1" s="2">
@@ -69122,8 +69389,11 @@
       <c r="IR90" s="1" t="n">
         <v>134</v>
       </c>
-      <c r="IS90" t="n">
+      <c r="IS90" s="1" t="n">
         <v>136</v>
+      </c>
+      <c r="IT90" t="n">
+        <v>131</v>
       </c>
     </row>
     <row r="91" ht="13.8" customHeight="1" s="2">
@@ -69885,8 +70155,11 @@
       <c r="IR91" s="1" t="n">
         <v>194</v>
       </c>
-      <c r="IS91" t="n">
+      <c r="IS91" s="1" t="n">
         <v>222</v>
+      </c>
+      <c r="IT91" t="n">
+        <v>223</v>
       </c>
     </row>
     <row r="92" ht="13.8" customHeight="1" s="2">
@@ -70648,8 +70921,11 @@
       <c r="IR92" s="1" t="n">
         <v>249</v>
       </c>
-      <c r="IS92" t="n">
+      <c r="IS92" s="1" t="n">
         <v>278</v>
+      </c>
+      <c r="IT92" t="n">
+        <v>269</v>
       </c>
     </row>
     <row r="93" ht="13.8" customHeight="1" s="2">
@@ -71411,7 +71687,10 @@
       <c r="IR93" s="1" t="n">
         <v>72.59999999999999</v>
       </c>
-      <c r="IS93" t="n">
+      <c r="IS93" s="1" t="n">
+        <v>76.2</v>
+      </c>
+      <c r="IT93" t="n">
         <v>76.2</v>
       </c>
     </row>
@@ -72174,8 +72453,11 @@
       <c r="IR94" s="1" t="n">
         <v>64</v>
       </c>
-      <c r="IS94" t="n">
+      <c r="IS94" s="1" t="n">
         <v>65</v>
+      </c>
+      <c r="IT94" t="n">
+        <v>66</v>
       </c>
     </row>
     <row r="95" ht="13.8" customHeight="1" s="2">
@@ -72937,7 +73219,10 @@
       <c r="IR95" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="IS95" t="n">
+      <c r="IS95" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="IT95" t="n">
         <v>12</v>
       </c>
     </row>
@@ -73700,8 +73985,11 @@
       <c r="IR96" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="IS96" t="n">
+      <c r="IS96" s="1" t="n">
         <v>14</v>
+      </c>
+      <c r="IT96" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="97" ht="13.8" customHeight="1" s="2">
@@ -74463,8 +74751,11 @@
       <c r="IR97" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="IS97" t="n">
+      <c r="IS97" s="1" t="n">
         <v>39</v>
+      </c>
+      <c r="IT97" t="n">
+        <v>36</v>
       </c>
     </row>
     <row r="98" ht="13.8" customHeight="1" s="2">
@@ -75226,8 +75517,11 @@
       <c r="IR98" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="IS98" t="n">
+      <c r="IS98" s="1" t="n">
         <v>37</v>
+      </c>
+      <c r="IT98" t="n">
+        <v>34</v>
       </c>
     </row>
     <row r="99" ht="13.8" customHeight="1" s="2">
@@ -75989,8 +76283,11 @@
       <c r="IR99" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="IS99" t="n">
+      <c r="IS99" s="1" t="n">
         <v>50</v>
+      </c>
+      <c r="IT99" t="n">
+        <v>55</v>
       </c>
     </row>
     <row r="100" ht="13.8" customHeight="1" s="2">
@@ -76752,8 +77049,11 @@
       <c r="IR100" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="IS100" t="n">
+      <c r="IS100" s="1" t="n">
         <v>11</v>
+      </c>
+      <c r="IT100" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="101" ht="13.8" customHeight="1" s="2">
@@ -77515,8 +77815,11 @@
       <c r="IR101" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="IS101" t="n">
+      <c r="IS101" s="1" t="n">
         <v>13</v>
+      </c>
+      <c r="IT101" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="102" ht="13.8" customHeight="1" s="2">
@@ -78278,8 +78581,11 @@
       <c r="IR102" s="1" t="n">
         <v>61.5</v>
       </c>
-      <c r="IS102" t="n">
+      <c r="IS102" s="1" t="n">
         <v>86.7</v>
+      </c>
+      <c r="IT102" t="n">
+        <v>66.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
round 6 into data, round 7 predictions. removed emergencies from lineups. updated PAV to 2022
</commit_message>
<xml_diff>
--- a/django_AFL_ML/Data/Adelaide_stats.xlsx
+++ b/django_AFL_ML/Data/Adelaide_stats.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:IT102"/>
+  <dimension ref="A1:IU102"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="GZ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="HA23" activeCellId="0" sqref="HA23"/>
@@ -1218,8 +1218,11 @@
       <c r="IS1" s="1" t="n">
         <v>10577</v>
       </c>
-      <c r="IT1" t="n">
+      <c r="IT1" s="1" t="n">
         <v>10584</v>
+      </c>
+      <c r="IU1" t="n">
+        <v>10590</v>
       </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="2">
@@ -1984,7 +1987,10 @@
       <c r="IS2" s="1" t="n">
         <v>2022</v>
       </c>
-      <c r="IT2" t="n">
+      <c r="IT2" s="1" t="n">
+        <v>2022</v>
+      </c>
+      <c r="IU2" t="n">
         <v>2022</v>
       </c>
     </row>
@@ -2750,8 +2756,11 @@
       <c r="IS3" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="IT3" t="n">
+      <c r="IT3" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="IU3" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="2">
@@ -3516,8 +3525,11 @@
       <c r="IS4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="IT4" t="n">
+      <c r="IT4" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="IU4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5" ht="13.8" customHeight="1" s="2">
@@ -4282,8 +4294,11 @@
       <c r="IS5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="IT5" t="n">
+      <c r="IT5" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="IU5" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6" ht="13.8" customHeight="1" s="2">
@@ -5048,8 +5063,11 @@
       <c r="IS6" s="1" t="n">
         <v>99</v>
       </c>
-      <c r="IT6" t="n">
+      <c r="IT6" s="1" t="n">
         <v>101</v>
+      </c>
+      <c r="IU6" t="n">
+        <v>63</v>
       </c>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="2">
@@ -5814,8 +5832,11 @@
       <c r="IS7" s="1" t="n">
         <v>103</v>
       </c>
-      <c r="IT7" t="n">
+      <c r="IT7" s="1" t="n">
         <v>82</v>
+      </c>
+      <c r="IU7" t="n">
+        <v>62</v>
       </c>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="2">
@@ -6580,8 +6601,11 @@
       <c r="IS8" s="1" t="n">
         <v>-4</v>
       </c>
-      <c r="IT8" t="n">
+      <c r="IT8" s="1" t="n">
         <v>19</v>
+      </c>
+      <c r="IU8" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="2">
@@ -7346,7 +7370,10 @@
       <c r="IS9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="IT9" t="n">
+      <c r="IT9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="IU9" t="n">
         <v>1</v>
       </c>
     </row>
@@ -8112,8 +8139,11 @@
       <c r="IS10" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="IT10" t="n">
+      <c r="IT10" s="1" t="n">
         <v>14</v>
+      </c>
+      <c r="IU10" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="11" ht="13.8" customHeight="1" s="2">
@@ -8878,8 +8908,11 @@
       <c r="IS11" s="1" t="n">
         <v>211</v>
       </c>
-      <c r="IT11" t="n">
+      <c r="IT11" s="1" t="n">
         <v>212</v>
+      </c>
+      <c r="IU11" t="n">
+        <v>206</v>
       </c>
     </row>
     <row r="12" ht="13.8" customHeight="1" s="2">
@@ -9644,8 +9677,11 @@
       <c r="IS12" s="1" t="n">
         <v>162</v>
       </c>
-      <c r="IT12" t="n">
+      <c r="IT12" s="1" t="n">
         <v>161</v>
+      </c>
+      <c r="IU12" t="n">
+        <v>158</v>
       </c>
     </row>
     <row r="13" ht="13.8" customHeight="1" s="2">
@@ -10410,8 +10446,11 @@
       <c r="IS13" s="1" t="n">
         <v>373</v>
       </c>
-      <c r="IT13" t="n">
+      <c r="IT13" s="1" t="n">
         <v>373</v>
+      </c>
+      <c r="IU13" t="n">
+        <v>364</v>
       </c>
     </row>
     <row r="14" ht="13.8" customHeight="1" s="2">
@@ -11176,8 +11215,11 @@
       <c r="IS14" s="1" t="n">
         <v>1.3</v>
       </c>
-      <c r="IT14" t="n">
+      <c r="IT14" s="1" t="n">
         <v>1.32</v>
+      </c>
+      <c r="IU14" t="n">
+        <v>1.3</v>
       </c>
     </row>
     <row r="15" ht="13.8" customHeight="1" s="2">
@@ -11942,8 +11984,11 @@
       <c r="IS15" s="1" t="n">
         <v>81</v>
       </c>
-      <c r="IT15" t="n">
+      <c r="IT15" s="1" t="n">
         <v>81</v>
+      </c>
+      <c r="IU15" t="n">
+        <v>91</v>
       </c>
     </row>
     <row r="16" ht="13.8" customHeight="1" s="2">
@@ -12708,8 +12753,11 @@
       <c r="IS16" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="IT16" t="n">
+      <c r="IT16" s="1" t="n">
         <v>47</v>
+      </c>
+      <c r="IU16" t="n">
+        <v>65</v>
       </c>
     </row>
     <row r="17" ht="13.8" customHeight="1" s="2">
@@ -13474,8 +13522,11 @@
       <c r="IS17" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="IT17" t="n">
+      <c r="IT17" s="1" t="n">
         <v>29</v>
+      </c>
+      <c r="IU17" t="n">
+        <v>52</v>
       </c>
     </row>
     <row r="18" ht="13.8" customHeight="1" s="2">
@@ -14240,8 +14291,11 @@
       <c r="IS18" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="IT18" t="n">
+      <c r="IT18" s="1" t="n">
         <v>33</v>
+      </c>
+      <c r="IU18" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="19" ht="13.8" customHeight="1" s="2">
@@ -15006,8 +15060,11 @@
       <c r="IS19" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="IT19" t="n">
+      <c r="IT19" s="1" t="n">
         <v>13</v>
+      </c>
+      <c r="IU19" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="20" ht="13.8" customHeight="1" s="2">
@@ -15772,8 +15829,11 @@
       <c r="IS20" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="IT20" t="n">
+      <c r="IT20" s="1" t="n">
         <v>15</v>
+      </c>
+      <c r="IU20" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="21" ht="13.8" customHeight="1" s="2">
@@ -16538,8 +16598,11 @@
       <c r="IS21" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="IT21" t="n">
+      <c r="IT21" s="1" t="n">
         <v>11</v>
+      </c>
+      <c r="IU21" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="22" ht="13.8" customHeight="1" s="2">
@@ -17304,8 +17367,11 @@
       <c r="IS22" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="IT22" t="n">
+      <c r="IT22" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="IU22" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="23" ht="13.8" customHeight="1" s="2">
@@ -18070,8 +18136,11 @@
       <c r="IS23" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="IT23" t="n">
+      <c r="IT23" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="IU23" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="24" ht="13.8" customHeight="1" s="2">
@@ -18836,8 +18905,11 @@
       <c r="IS24" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="IT24" t="n">
+      <c r="IT24" s="1" t="n">
         <v>26</v>
+      </c>
+      <c r="IU24" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="25" ht="13.8" customHeight="1" s="2">
@@ -19602,8 +19674,11 @@
       <c r="IS25" s="1" t="n">
         <v>62.5</v>
       </c>
-      <c r="IT25" t="n">
+      <c r="IT25" s="1" t="n">
         <v>57.7</v>
+      </c>
+      <c r="IU25" t="n">
+        <v>34.8</v>
       </c>
     </row>
     <row r="26" ht="13.8" customHeight="1" s="2">
@@ -20368,8 +20443,11 @@
       <c r="IS26" s="1" t="n">
         <v>24.87</v>
       </c>
-      <c r="IT26" t="n">
+      <c r="IT26" s="1" t="n">
         <v>24.87</v>
+      </c>
+      <c r="IU26" t="n">
+        <v>45.5</v>
       </c>
     </row>
     <row r="27" ht="13.8" customHeight="1" s="2">
@@ -21134,8 +21212,11 @@
       <c r="IS27" s="1" t="n">
         <v>15.54</v>
       </c>
-      <c r="IT27" t="n">
+      <c r="IT27" s="1" t="n">
         <v>14.35</v>
+      </c>
+      <c r="IU27" t="n">
+        <v>15.83</v>
       </c>
     </row>
     <row r="28" ht="13.8" customHeight="1" s="2">
@@ -21900,8 +21981,11 @@
       <c r="IS28" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="IT28" t="n">
+      <c r="IT28" s="1" t="n">
         <v>34</v>
+      </c>
+      <c r="IU28" t="n">
+        <v>39</v>
       </c>
     </row>
     <row r="29" ht="13.8" customHeight="1" s="2">
@@ -22666,8 +22750,11 @@
       <c r="IS29" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="IT29" t="n">
+      <c r="IT29" s="1" t="n">
         <v>48</v>
+      </c>
+      <c r="IU29" t="n">
+        <v>55</v>
       </c>
     </row>
     <row r="30" ht="13.8" customHeight="1" s="2">
@@ -23432,8 +23519,11 @@
       <c r="IS30" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="IT30" t="n">
+      <c r="IT30" s="1" t="n">
         <v>49</v>
+      </c>
+      <c r="IU30" t="n">
+        <v>33</v>
       </c>
     </row>
     <row r="31" ht="13.8" customHeight="1" s="2">
@@ -24198,8 +24288,11 @@
       <c r="IS31" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="IT31" t="n">
+      <c r="IT31" s="1" t="n">
         <v>51</v>
+      </c>
+      <c r="IU31" t="n">
+        <v>58</v>
       </c>
     </row>
     <row r="32" ht="13.8" customHeight="1" s="2">
@@ -24964,8 +25057,11 @@
       <c r="IS32" s="1" t="n">
         <v>2.21</v>
       </c>
-      <c r="IT32" t="n">
+      <c r="IT32" s="1" t="n">
         <v>1.96</v>
+      </c>
+      <c r="IU32" t="n">
+        <v>2.52</v>
       </c>
     </row>
     <row r="33" ht="13.8" customHeight="1" s="2">
@@ -25730,8 +25826,11 @@
       <c r="IS33" s="1" t="n">
         <v>3.53</v>
       </c>
-      <c r="IT33" t="n">
+      <c r="IT33" s="1" t="n">
         <v>3.4</v>
+      </c>
+      <c r="IU33" t="n">
+        <v>7.25</v>
       </c>
     </row>
     <row r="34" ht="13.8" customHeight="1" s="2">
@@ -26496,8 +26595,11 @@
       <c r="IS34" s="1" t="n">
         <v>39.6</v>
       </c>
-      <c r="IT34" t="n">
+      <c r="IT34" s="1" t="n">
         <v>43.1</v>
+      </c>
+      <c r="IU34" t="n">
+        <v>34.5</v>
       </c>
     </row>
     <row r="35" ht="13.8" customHeight="1" s="2">
@@ -27262,8 +27364,11 @@
       <c r="IS35" s="1" t="n">
         <v>28.3</v>
       </c>
-      <c r="IT35" t="n">
+      <c r="IT35" s="1" t="n">
         <v>29.4</v>
+      </c>
+      <c r="IU35" t="n">
+        <v>13.8</v>
       </c>
     </row>
     <row r="36" ht="13.8" customHeight="1" s="2">
@@ -28028,8 +28133,11 @@
       <c r="IS36" s="1" t="n">
         <v>186.8</v>
       </c>
-      <c r="IT36" t="n">
+      <c r="IT36" s="1" t="n">
         <v>186.5</v>
+      </c>
+      <c r="IU36" t="n">
+        <v>187.5</v>
       </c>
     </row>
     <row r="37" ht="13.8" customHeight="1" s="2">
@@ -28794,8 +28902,11 @@
       <c r="IS37" s="1" t="n">
         <v>86.2</v>
       </c>
-      <c r="IT37" t="n">
+      <c r="IT37" s="1" t="n">
         <v>85.5</v>
+      </c>
+      <c r="IU37" t="n">
+        <v>86.40000000000001</v>
       </c>
     </row>
     <row r="38" ht="13.8" customHeight="1" s="2">
@@ -29560,8 +29671,11 @@
       <c r="IS38" s="1" t="n">
         <v>24.74</v>
       </c>
-      <c r="IT38" t="n">
+      <c r="IT38" s="1" t="n">
         <v>24.8</v>
+      </c>
+      <c r="IU38" t="n">
+        <v>24.49</v>
       </c>
     </row>
     <row r="39" ht="13.8" customHeight="1" s="2">
@@ -30326,8 +30440,11 @@
       <c r="IS39" s="1" t="n">
         <v>75.40000000000001</v>
       </c>
-      <c r="IT39" t="n">
+      <c r="IT39" s="1" t="n">
         <v>76.5</v>
+      </c>
+      <c r="IU39" t="n">
+        <v>70.09999999999999</v>
       </c>
     </row>
     <row r="40" ht="13.8" customHeight="1" s="2">
@@ -31092,7 +31209,10 @@
       <c r="IS40" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="IT40" t="n">
+      <c r="IT40" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="IU40" t="n">
         <v>12</v>
       </c>
     </row>
@@ -31858,7 +31978,10 @@
       <c r="IS41" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="IT41" t="n">
+      <c r="IT41" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="IU41" t="n">
         <v>5</v>
       </c>
     </row>
@@ -32624,7 +32747,10 @@
       <c r="IS42" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="IT42" t="n">
+      <c r="IT42" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="IU42" t="n">
         <v>1</v>
       </c>
     </row>
@@ -33390,8 +33516,11 @@
       <c r="IS43" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="IT43" t="n">
+      <c r="IT43" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="IU43" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="44" ht="13.8" customHeight="1" s="2">
@@ -34156,8 +34285,11 @@
       <c r="IS44" s="1" t="n">
         <v>157</v>
       </c>
-      <c r="IT44" t="n">
+      <c r="IT44" s="1" t="n">
         <v>146</v>
+      </c>
+      <c r="IU44" t="n">
+        <v>149</v>
       </c>
     </row>
     <row r="45" ht="13.8" customHeight="1" s="2">
@@ -34922,8 +35054,11 @@
       <c r="IS45" s="1" t="n">
         <v>212</v>
       </c>
-      <c r="IT45" t="n">
+      <c r="IT45" s="1" t="n">
         <v>217</v>
+      </c>
+      <c r="IU45" t="n">
+        <v>214</v>
       </c>
     </row>
     <row r="46" ht="13.8" customHeight="1" s="2">
@@ -35688,8 +35823,11 @@
       <c r="IS46" s="1" t="n">
         <v>268</v>
       </c>
-      <c r="IT46" t="n">
+      <c r="IT46" s="1" t="n">
         <v>285</v>
+      </c>
+      <c r="IU46" t="n">
+        <v>261</v>
       </c>
     </row>
     <row r="47" ht="13.8" customHeight="1" s="2">
@@ -36454,8 +36592,11 @@
       <c r="IS47" s="1" t="n">
         <v>71.8</v>
       </c>
-      <c r="IT47" t="n">
+      <c r="IT47" s="1" t="n">
         <v>76.40000000000001</v>
+      </c>
+      <c r="IU47" t="n">
+        <v>71.7</v>
       </c>
     </row>
     <row r="48" ht="13.8" customHeight="1" s="2">
@@ -37220,8 +37361,11 @@
       <c r="IS48" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="IT48" t="n">
+      <c r="IT48" s="1" t="n">
         <v>48</v>
+      </c>
+      <c r="IU48" t="n">
+        <v>55</v>
       </c>
     </row>
     <row r="49" ht="13.8" customHeight="1" s="2">
@@ -37986,8 +38130,11 @@
       <c r="IS49" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="IT49" t="n">
+      <c r="IT49" s="1" t="n">
         <v>14</v>
+      </c>
+      <c r="IU49" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="50" ht="13.8" customHeight="1" s="2">
@@ -38752,8 +38899,11 @@
       <c r="IS50" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="IT50" t="n">
+      <c r="IT50" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="IU50" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="51" ht="13.8" customHeight="1" s="2">
@@ -39518,8 +39668,11 @@
       <c r="IS51" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="IT51" t="n">
+      <c r="IT51" s="1" t="n">
         <v>34</v>
+      </c>
+      <c r="IU51" t="n">
+        <v>39</v>
       </c>
     </row>
     <row r="52" ht="13.8" customHeight="1" s="2">
@@ -40284,8 +40437,11 @@
       <c r="IS52" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="IT52" t="n">
+      <c r="IT52" s="1" t="n">
         <v>49</v>
+      </c>
+      <c r="IU52" t="n">
+        <v>33</v>
       </c>
     </row>
     <row r="53" ht="13.8" customHeight="1" s="2">
@@ -41050,7 +41206,10 @@
       <c r="IS53" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="IT53" t="n">
+      <c r="IT53" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="IU53" t="n">
         <v>48</v>
       </c>
     </row>
@@ -41816,8 +41975,11 @@
       <c r="IS54" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="IT54" t="n">
+      <c r="IT54" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="IU54" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="55" ht="13.8" customHeight="1" s="2">
@@ -42582,8 +42744,11 @@
       <c r="IS55" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="IT55" t="n">
+      <c r="IT55" s="1" t="n">
         <v>11</v>
+      </c>
+      <c r="IU55" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="56" ht="13.8" customHeight="1" s="2">
@@ -43348,8 +43513,11 @@
       <c r="IS56" s="1" t="n">
         <v>66.7</v>
       </c>
-      <c r="IT56" t="n">
+      <c r="IT56" s="1" t="n">
         <v>73.3</v>
+      </c>
+      <c r="IU56" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="57" ht="13.8" customHeight="1" s="2">
@@ -44114,8 +44282,11 @@
       <c r="IS57" s="1" t="n">
         <v>221</v>
       </c>
-      <c r="IT57" t="n">
+      <c r="IT57" s="1" t="n">
         <v>191</v>
+      </c>
+      <c r="IU57" t="n">
+        <v>214</v>
       </c>
     </row>
     <row r="58" ht="13.8" customHeight="1" s="2">
@@ -44880,8 +45051,11 @@
       <c r="IS58" s="1" t="n">
         <v>144</v>
       </c>
-      <c r="IT58" t="n">
+      <c r="IT58" s="1" t="n">
         <v>162</v>
+      </c>
+      <c r="IU58" t="n">
+        <v>153</v>
       </c>
     </row>
     <row r="59" ht="13.8" customHeight="1" s="2">
@@ -45646,8 +45820,11 @@
       <c r="IS59" s="1" t="n">
         <v>365</v>
       </c>
-      <c r="IT59" t="n">
+      <c r="IT59" s="1" t="n">
         <v>353</v>
+      </c>
+      <c r="IU59" t="n">
+        <v>367</v>
       </c>
     </row>
     <row r="60" ht="13.8" customHeight="1" s="2">
@@ -46412,8 +46589,11 @@
       <c r="IS60" s="1" t="n">
         <v>1.53</v>
       </c>
-      <c r="IT60" t="n">
+      <c r="IT60" s="1" t="n">
         <v>1.18</v>
+      </c>
+      <c r="IU60" t="n">
+        <v>1.4</v>
       </c>
     </row>
     <row r="61" ht="13.8" customHeight="1" s="2">
@@ -47178,8 +47358,11 @@
       <c r="IS61" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="IT61" t="n">
+      <c r="IT61" s="1" t="n">
         <v>80</v>
+      </c>
+      <c r="IU61" t="n">
+        <v>81</v>
       </c>
     </row>
     <row r="62" ht="13.8" customHeight="1" s="2">
@@ -47944,8 +48127,11 @@
       <c r="IS62" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="IT62" t="n">
+      <c r="IT62" s="1" t="n">
         <v>42</v>
+      </c>
+      <c r="IU62" t="n">
+        <v>78</v>
       </c>
     </row>
     <row r="63" ht="13.8" customHeight="1" s="2">
@@ -48710,8 +48896,11 @@
       <c r="IS63" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="IT63" t="n">
+      <c r="IT63" s="1" t="n">
         <v>41</v>
+      </c>
+      <c r="IU63" t="n">
+        <v>29</v>
       </c>
     </row>
     <row r="64" ht="13.8" customHeight="1" s="2">
@@ -49476,8 +49665,11 @@
       <c r="IS64" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="IT64" t="n">
+      <c r="IT64" s="1" t="n">
         <v>13</v>
+      </c>
+      <c r="IU64" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="65" ht="13.8" customHeight="1" s="2">
@@ -50242,8 +50434,11 @@
       <c r="IS65" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="IT65" t="n">
+      <c r="IT65" s="1" t="n">
         <v>33</v>
+      </c>
+      <c r="IU65" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="66" ht="13.8" customHeight="1" s="2">
@@ -51008,8 +51203,11 @@
       <c r="IS66" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="IT66" t="n">
+      <c r="IT66" s="1" t="n">
         <v>12</v>
+      </c>
+      <c r="IU66" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="67" ht="13.8" customHeight="1" s="2">
@@ -51774,8 +51972,11 @@
       <c r="IS67" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="IT67" t="n">
+      <c r="IT67" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="IU67" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="68" ht="13.8" customHeight="1" s="2">
@@ -52540,8 +52741,11 @@
       <c r="IS68" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="IT68" t="n">
+      <c r="IT68" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="IU68" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="69" ht="13.8" customHeight="1" s="2">
@@ -53306,7 +53510,10 @@
       <c r="IS69" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="IT69" t="n">
+      <c r="IT69" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="IU69" t="n">
         <v>3</v>
       </c>
     </row>
@@ -54072,8 +54279,11 @@
       <c r="IS70" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="IT70" t="n">
+      <c r="IT70" s="1" t="n">
         <v>22</v>
+      </c>
+      <c r="IU70" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="71" ht="13.8" customHeight="1" s="2">
@@ -54838,8 +55048,11 @@
       <c r="IS71" s="1" t="n">
         <v>53.6</v>
       </c>
-      <c r="IT71" t="n">
+      <c r="IT71" s="1" t="n">
         <v>54.5</v>
+      </c>
+      <c r="IU71" t="n">
+        <v>52.9</v>
       </c>
     </row>
     <row r="72" ht="13.8" customHeight="1" s="2">
@@ -55604,8 +55817,11 @@
       <c r="IS72" s="1" t="n">
         <v>24.33</v>
       </c>
-      <c r="IT72" t="n">
+      <c r="IT72" s="1" t="n">
         <v>29.42</v>
+      </c>
+      <c r="IU72" t="n">
+        <v>40.78</v>
       </c>
     </row>
     <row r="73" ht="13.8" customHeight="1" s="2">
@@ -56370,8 +56586,11 @@
       <c r="IS73" s="1" t="n">
         <v>13.04</v>
       </c>
-      <c r="IT73" t="n">
+      <c r="IT73" s="1" t="n">
         <v>16.05</v>
+      </c>
+      <c r="IU73" t="n">
+        <v>21.59</v>
       </c>
     </row>
     <row r="74" ht="13.8" customHeight="1" s="2">
@@ -57136,8 +57355,11 @@
       <c r="IS74" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="IT74" t="n">
+      <c r="IT74" s="1" t="n">
         <v>36</v>
+      </c>
+      <c r="IU74" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="75" ht="13.8" customHeight="1" s="2">
@@ -57902,8 +58124,11 @@
       <c r="IS75" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="IT75" t="n">
+      <c r="IT75" s="1" t="n">
         <v>66</v>
+      </c>
+      <c r="IU75" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="76" ht="13.8" customHeight="1" s="2">
@@ -58668,8 +58893,11 @@
       <c r="IS76" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="IT76" t="n">
+      <c r="IT76" s="1" t="n">
         <v>34</v>
+      </c>
+      <c r="IU76" t="n">
+        <v>49</v>
       </c>
     </row>
     <row r="77" ht="13.8" customHeight="1" s="2">
@@ -59434,8 +59662,11 @@
       <c r="IS77" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="IT77" t="n">
+      <c r="IT77" s="1" t="n">
         <v>61</v>
+      </c>
+      <c r="IU77" t="n">
+        <v>43</v>
       </c>
     </row>
     <row r="78" ht="13.8" customHeight="1" s="2">
@@ -60200,8 +60431,11 @@
       <c r="IS78" s="1" t="n">
         <v>2.32</v>
       </c>
-      <c r="IT78" t="n">
+      <c r="IT78" s="1" t="n">
         <v>2.77</v>
+      </c>
+      <c r="IU78" t="n">
+        <v>2.53</v>
       </c>
     </row>
     <row r="79" ht="13.8" customHeight="1" s="2">
@@ -60966,8 +61200,11 @@
       <c r="IS79" s="1" t="n">
         <v>4.33</v>
       </c>
-      <c r="IT79" t="n">
+      <c r="IT79" s="1" t="n">
         <v>5.08</v>
+      </c>
+      <c r="IU79" t="n">
+        <v>4.78</v>
       </c>
     </row>
     <row r="80" ht="13.8" customHeight="1" s="2">
@@ -61732,8 +61969,11 @@
       <c r="IS80" s="1" t="n">
         <v>36.9</v>
       </c>
-      <c r="IT80" t="n">
+      <c r="IT80" s="1" t="n">
         <v>31.1</v>
+      </c>
+      <c r="IU80" t="n">
+        <v>32.6</v>
       </c>
     </row>
     <row r="81" ht="13.8" customHeight="1" s="2">
@@ -62498,8 +62738,11 @@
       <c r="IS81" s="1" t="n">
         <v>23.1</v>
       </c>
-      <c r="IT81" t="n">
+      <c r="IT81" s="1" t="n">
         <v>19.7</v>
+      </c>
+      <c r="IU81" t="n">
+        <v>20.9</v>
       </c>
     </row>
     <row r="82" ht="13.8" customHeight="1" s="2">
@@ -63264,8 +63507,11 @@
       <c r="IS82" s="1" t="n">
         <v>187</v>
       </c>
-      <c r="IT82" t="n">
+      <c r="IT82" s="1" t="n">
         <v>185.9</v>
+      </c>
+      <c r="IU82" t="n">
+        <v>188.3</v>
       </c>
     </row>
     <row r="83" ht="13.8" customHeight="1" s="2">
@@ -64030,8 +64276,11 @@
       <c r="IS83" s="1" t="n">
         <v>85.3</v>
       </c>
-      <c r="IT83" t="n">
+      <c r="IT83" s="1" t="n">
         <v>85.09999999999999</v>
+      </c>
+      <c r="IU83" t="n">
+        <v>86.5</v>
       </c>
     </row>
     <row r="84" ht="13.8" customHeight="1" s="2">
@@ -64796,8 +65045,11 @@
       <c r="IS84" s="1" t="n">
         <v>24.74</v>
       </c>
-      <c r="IT84" t="n">
+      <c r="IT84" s="1" t="n">
         <v>26.74</v>
+      </c>
+      <c r="IU84" t="n">
+        <v>25.74</v>
       </c>
     </row>
     <row r="85" ht="13.8" customHeight="1" s="2">
@@ -65562,8 +65814,11 @@
       <c r="IS85" s="1" t="n">
         <v>66.3</v>
       </c>
-      <c r="IT85" t="n">
+      <c r="IT85" s="1" t="n">
         <v>112.2</v>
+      </c>
+      <c r="IU85" t="n">
+        <v>96.59999999999999</v>
       </c>
     </row>
     <row r="86" ht="13.8" customHeight="1" s="2">
@@ -66328,8 +66583,11 @@
       <c r="IS86" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="IT86" t="n">
+      <c r="IT86" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="IU86" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="87" ht="13.8" customHeight="1" s="2">
@@ -67094,8 +67352,11 @@
       <c r="IS87" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="IT87" t="n">
+      <c r="IT87" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="IU87" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="88" ht="13.8" customHeight="1" s="2">
@@ -67860,8 +68121,11 @@
       <c r="IS88" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="IT88" t="n">
+      <c r="IT88" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="IU88" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="89" ht="13.8" customHeight="1" s="2">
@@ -68626,8 +68890,11 @@
       <c r="IS89" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="IT89" t="n">
+      <c r="IT89" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="IU89" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="90" ht="13.8" customHeight="1" s="2">
@@ -69392,8 +69659,11 @@
       <c r="IS90" s="1" t="n">
         <v>136</v>
       </c>
-      <c r="IT90" t="n">
+      <c r="IT90" s="1" t="n">
         <v>131</v>
+      </c>
+      <c r="IU90" t="n">
+        <v>145</v>
       </c>
     </row>
     <row r="91" ht="13.8" customHeight="1" s="2">
@@ -70158,8 +70428,11 @@
       <c r="IS91" s="1" t="n">
         <v>222</v>
       </c>
-      <c r="IT91" t="n">
+      <c r="IT91" s="1" t="n">
         <v>223</v>
+      </c>
+      <c r="IU91" t="n">
+        <v>212</v>
       </c>
     </row>
     <row r="92" ht="13.8" customHeight="1" s="2">
@@ -70924,8 +71197,11 @@
       <c r="IS92" s="1" t="n">
         <v>278</v>
       </c>
-      <c r="IT92" t="n">
+      <c r="IT92" s="1" t="n">
         <v>269</v>
+      </c>
+      <c r="IU92" t="n">
+        <v>271</v>
       </c>
     </row>
     <row r="93" ht="13.8" customHeight="1" s="2">
@@ -71690,8 +71966,11 @@
       <c r="IS93" s="1" t="n">
         <v>76.2</v>
       </c>
-      <c r="IT93" t="n">
+      <c r="IT93" s="1" t="n">
         <v>76.2</v>
+      </c>
+      <c r="IU93" t="n">
+        <v>73.8</v>
       </c>
     </row>
     <row r="94" ht="13.8" customHeight="1" s="2">
@@ -72456,8 +72735,11 @@
       <c r="IS94" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="IT94" t="n">
+      <c r="IT94" s="1" t="n">
         <v>66</v>
+      </c>
+      <c r="IU94" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="95" ht="13.8" customHeight="1" s="2">
@@ -73222,7 +73504,10 @@
       <c r="IS95" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="IT95" t="n">
+      <c r="IT95" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="IU95" t="n">
         <v>12</v>
       </c>
     </row>
@@ -73988,8 +74273,11 @@
       <c r="IS96" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="IT96" t="n">
+      <c r="IT96" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="IU96" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="97" ht="13.8" customHeight="1" s="2">
@@ -74754,8 +75042,11 @@
       <c r="IS97" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="IT97" t="n">
+      <c r="IT97" s="1" t="n">
         <v>36</v>
+      </c>
+      <c r="IU97" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="98" ht="13.8" customHeight="1" s="2">
@@ -75520,8 +75811,11 @@
       <c r="IS98" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="IT98" t="n">
+      <c r="IT98" s="1" t="n">
         <v>34</v>
+      </c>
+      <c r="IU98" t="n">
+        <v>49</v>
       </c>
     </row>
     <row r="99" ht="13.8" customHeight="1" s="2">
@@ -76286,8 +76580,11 @@
       <c r="IS99" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="IT99" t="n">
+      <c r="IT99" s="1" t="n">
         <v>55</v>
+      </c>
+      <c r="IU99" t="n">
+        <v>58</v>
       </c>
     </row>
     <row r="100" ht="13.8" customHeight="1" s="2">
@@ -77052,8 +77349,11 @@
       <c r="IS100" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="IT100" t="n">
+      <c r="IT100" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="IU100" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="101" ht="13.8" customHeight="1" s="2">
@@ -77818,8 +78118,11 @@
       <c r="IS101" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="IT101" t="n">
+      <c r="IT101" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="IU101" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="102" ht="13.8" customHeight="1" s="2">
@@ -78584,8 +78887,11 @@
       <c r="IS102" s="1" t="n">
         <v>86.7</v>
       </c>
-      <c r="IT102" t="n">
+      <c r="IT102" s="1" t="n">
         <v>66.7</v>
+      </c>
+      <c r="IU102" t="n">
+        <v>55.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Round 9 and changes
</commit_message>
<xml_diff>
--- a/django_AFL_ML/Data/Adelaide_stats.xlsx
+++ b/django_AFL_ML/Data/Adelaide_stats.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:IU102"/>
+  <dimension ref="A1:IW102"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="GZ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="HA23" activeCellId="0" sqref="HA23"/>
@@ -1221,8 +1221,14 @@
       <c r="IT1" s="1" t="n">
         <v>10584</v>
       </c>
-      <c r="IU1" t="n">
+      <c r="IU1" s="1" t="n">
         <v>10590</v>
+      </c>
+      <c r="IV1" s="1" t="n">
+        <v>10600</v>
+      </c>
+      <c r="IW1" t="n">
+        <v>10615</v>
       </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="2">
@@ -1990,7 +1996,13 @@
       <c r="IT2" s="1" t="n">
         <v>2022</v>
       </c>
-      <c r="IU2" t="n">
+      <c r="IU2" s="1" t="n">
+        <v>2022</v>
+      </c>
+      <c r="IV2" s="1" t="n">
+        <v>2022</v>
+      </c>
+      <c r="IW2" t="n">
         <v>2022</v>
       </c>
     </row>
@@ -2759,8 +2771,14 @@
       <c r="IT3" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="IU3" t="n">
+      <c r="IU3" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="IV3" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="IW3" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="2">
@@ -3528,7 +3546,13 @@
       <c r="IT4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="IU4" t="n">
+      <c r="IU4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="IV4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="IW4" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4297,8 +4321,14 @@
       <c r="IT5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="IU5" t="n">
+      <c r="IU5" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="IV5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="IW5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6" ht="13.8" customHeight="1" s="2">
@@ -5066,8 +5096,14 @@
       <c r="IT6" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="IU6" t="n">
+      <c r="IU6" s="1" t="n">
         <v>63</v>
+      </c>
+      <c r="IV6" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="IW6" t="n">
+        <v>68</v>
       </c>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="2">
@@ -5835,8 +5871,14 @@
       <c r="IT7" s="1" t="n">
         <v>82</v>
       </c>
-      <c r="IU7" t="n">
+      <c r="IU7" s="1" t="n">
         <v>62</v>
+      </c>
+      <c r="IV7" s="1" t="n">
+        <v>113</v>
+      </c>
+      <c r="IW7" t="n">
+        <v>116</v>
       </c>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="2">
@@ -6604,8 +6646,14 @@
       <c r="IT8" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="IU8" t="n">
+      <c r="IU8" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="IV8" s="1" t="n">
+        <v>-59</v>
+      </c>
+      <c r="IW8" t="n">
+        <v>-48</v>
       </c>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="2">
@@ -7373,8 +7421,14 @@
       <c r="IT9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="IU9" t="n">
+      <c r="IU9" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="IV9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="IW9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10" ht="13.8" customHeight="1" s="2">
@@ -8142,8 +8196,14 @@
       <c r="IT10" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="IU10" t="n">
+      <c r="IU10" s="1" t="n">
         <v>18</v>
+      </c>
+      <c r="IV10" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="IW10" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="11" ht="13.8" customHeight="1" s="2">
@@ -8911,8 +8971,14 @@
       <c r="IT11" s="1" t="n">
         <v>212</v>
       </c>
-      <c r="IU11" t="n">
+      <c r="IU11" s="1" t="n">
         <v>206</v>
+      </c>
+      <c r="IV11" s="1" t="n">
+        <v>179</v>
+      </c>
+      <c r="IW11" t="n">
+        <v>218</v>
       </c>
     </row>
     <row r="12" ht="13.8" customHeight="1" s="2">
@@ -9680,8 +9746,14 @@
       <c r="IT12" s="1" t="n">
         <v>161</v>
       </c>
-      <c r="IU12" t="n">
+      <c r="IU12" s="1" t="n">
         <v>158</v>
+      </c>
+      <c r="IV12" s="1" t="n">
+        <v>167</v>
+      </c>
+      <c r="IW12" t="n">
+        <v>145</v>
       </c>
     </row>
     <row r="13" ht="13.8" customHeight="1" s="2">
@@ -10449,8 +10521,14 @@
       <c r="IT13" s="1" t="n">
         <v>373</v>
       </c>
-      <c r="IU13" t="n">
+      <c r="IU13" s="1" t="n">
         <v>364</v>
+      </c>
+      <c r="IV13" s="1" t="n">
+        <v>346</v>
+      </c>
+      <c r="IW13" t="n">
+        <v>363</v>
       </c>
     </row>
     <row r="14" ht="13.8" customHeight="1" s="2">
@@ -11218,8 +11296,14 @@
       <c r="IT14" s="1" t="n">
         <v>1.32</v>
       </c>
-      <c r="IU14" t="n">
+      <c r="IU14" s="1" t="n">
         <v>1.3</v>
+      </c>
+      <c r="IV14" s="1" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="IW14" t="n">
+        <v>1.5</v>
       </c>
     </row>
     <row r="15" ht="13.8" customHeight="1" s="2">
@@ -11987,8 +12071,14 @@
       <c r="IT15" s="1" t="n">
         <v>81</v>
       </c>
-      <c r="IU15" t="n">
+      <c r="IU15" s="1" t="n">
         <v>91</v>
+      </c>
+      <c r="IV15" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="IW15" t="n">
+        <v>93</v>
       </c>
     </row>
     <row r="16" ht="13.8" customHeight="1" s="2">
@@ -12756,8 +12846,14 @@
       <c r="IT16" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="IU16" t="n">
+      <c r="IU16" s="1" t="n">
         <v>65</v>
+      </c>
+      <c r="IV16" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="IW16" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="17" ht="13.8" customHeight="1" s="2">
@@ -13525,8 +13621,14 @@
       <c r="IT17" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="IU17" t="n">
+      <c r="IU17" s="1" t="n">
         <v>52</v>
+      </c>
+      <c r="IV17" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="IW17" t="n">
+        <v>46</v>
       </c>
     </row>
     <row r="18" ht="13.8" customHeight="1" s="2">
@@ -14294,8 +14396,14 @@
       <c r="IT18" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="IU18" t="n">
+      <c r="IU18" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="IV18" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="IW18" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="19" ht="13.8" customHeight="1" s="2">
@@ -15063,8 +15171,14 @@
       <c r="IT19" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="IU19" t="n">
+      <c r="IU19" s="1" t="n">
         <v>24</v>
+      </c>
+      <c r="IV19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="IW19" t="n">
+        <v>29</v>
       </c>
     </row>
     <row r="20" ht="13.8" customHeight="1" s="2">
@@ -15832,8 +15946,14 @@
       <c r="IT20" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="IU20" t="n">
+      <c r="IU20" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="IV20" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="IW20" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="21" ht="13.8" customHeight="1" s="2">
@@ -16601,8 +16721,14 @@
       <c r="IT21" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="IU21" t="n">
+      <c r="IU21" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="IV21" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="IW21" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="22" ht="13.8" customHeight="1" s="2">
@@ -17370,8 +17496,14 @@
       <c r="IT22" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="IU22" t="n">
+      <c r="IU22" s="1" t="n">
         <v>12</v>
+      </c>
+      <c r="IV22" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="IW22" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="23" ht="13.8" customHeight="1" s="2">
@@ -18139,8 +18271,14 @@
       <c r="IT23" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="IU23" t="n">
+      <c r="IU23" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="IV23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="IW23" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="24" ht="13.8" customHeight="1" s="2">
@@ -18908,8 +19046,14 @@
       <c r="IT24" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="IU24" t="n">
+      <c r="IU24" s="1" t="n">
         <v>23</v>
+      </c>
+      <c r="IV24" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="IW24" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="25" ht="13.8" customHeight="1" s="2">
@@ -19677,8 +19821,14 @@
       <c r="IT25" s="1" t="n">
         <v>57.7</v>
       </c>
-      <c r="IU25" t="n">
+      <c r="IU25" s="1" t="n">
         <v>34.8</v>
+      </c>
+      <c r="IV25" s="1" t="n">
+        <v>57.1</v>
+      </c>
+      <c r="IW25" t="n">
+        <v>55.6</v>
       </c>
     </row>
     <row r="26" ht="13.8" customHeight="1" s="2">
@@ -20446,8 +20596,14 @@
       <c r="IT26" s="1" t="n">
         <v>24.87</v>
       </c>
-      <c r="IU26" t="n">
+      <c r="IU26" s="1" t="n">
         <v>45.5</v>
+      </c>
+      <c r="IV26" s="1" t="n">
+        <v>43.25</v>
+      </c>
+      <c r="IW26" t="n">
+        <v>36.3</v>
       </c>
     </row>
     <row r="27" ht="13.8" customHeight="1" s="2">
@@ -21215,8 +21371,14 @@
       <c r="IT27" s="1" t="n">
         <v>14.35</v>
       </c>
-      <c r="IU27" t="n">
+      <c r="IU27" s="1" t="n">
         <v>15.83</v>
+      </c>
+      <c r="IV27" s="1" t="n">
+        <v>24.71</v>
+      </c>
+      <c r="IW27" t="n">
+        <v>20.17</v>
       </c>
     </row>
     <row r="28" ht="13.8" customHeight="1" s="2">
@@ -21984,8 +22146,14 @@
       <c r="IT28" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="IU28" t="n">
+      <c r="IU28" s="1" t="n">
         <v>39</v>
+      </c>
+      <c r="IV28" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="IW28" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="29" ht="13.8" customHeight="1" s="2">
@@ -22753,8 +22921,14 @@
       <c r="IT29" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="IU29" t="n">
+      <c r="IU29" s="1" t="n">
         <v>55</v>
+      </c>
+      <c r="IV29" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="IW29" t="n">
+        <v>72</v>
       </c>
     </row>
     <row r="30" ht="13.8" customHeight="1" s="2">
@@ -23522,8 +23696,14 @@
       <c r="IT30" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="IU30" t="n">
+      <c r="IU30" s="1" t="n">
         <v>33</v>
+      </c>
+      <c r="IV30" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="IW30" t="n">
+        <v>57</v>
       </c>
     </row>
     <row r="31" ht="13.8" customHeight="1" s="2">
@@ -24291,8 +24471,14 @@
       <c r="IT31" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="IU31" t="n">
+      <c r="IU31" s="1" t="n">
         <v>58</v>
+      </c>
+      <c r="IV31" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="IW31" t="n">
+        <v>49</v>
       </c>
     </row>
     <row r="32" ht="13.8" customHeight="1" s="2">
@@ -25060,8 +25246,14 @@
       <c r="IT32" s="1" t="n">
         <v>1.96</v>
       </c>
-      <c r="IU32" t="n">
+      <c r="IU32" s="1" t="n">
         <v>2.52</v>
+      </c>
+      <c r="IV32" s="1" t="n">
+        <v>3.43</v>
+      </c>
+      <c r="IW32" t="n">
+        <v>2.72</v>
       </c>
     </row>
     <row r="33" ht="13.8" customHeight="1" s="2">
@@ -25829,8 +26021,14 @@
       <c r="IT33" s="1" t="n">
         <v>3.4</v>
       </c>
-      <c r="IU33" t="n">
+      <c r="IU33" s="1" t="n">
         <v>7.25</v>
+      </c>
+      <c r="IV33" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="IW33" t="n">
+        <v>4.9</v>
       </c>
     </row>
     <row r="34" ht="13.8" customHeight="1" s="2">
@@ -26598,8 +26796,14 @@
       <c r="IT34" s="1" t="n">
         <v>43.1</v>
       </c>
-      <c r="IU34" t="n">
+      <c r="IU34" s="1" t="n">
         <v>34.5</v>
+      </c>
+      <c r="IV34" s="1" t="n">
+        <v>29.2</v>
+      </c>
+      <c r="IW34" t="n">
+        <v>34.7</v>
       </c>
     </row>
     <row r="35" ht="13.8" customHeight="1" s="2">
@@ -27367,8 +27571,14 @@
       <c r="IT35" s="1" t="n">
         <v>29.4</v>
       </c>
-      <c r="IU35" t="n">
+      <c r="IU35" s="1" t="n">
         <v>13.8</v>
+      </c>
+      <c r="IV35" s="1" t="n">
+        <v>16.7</v>
+      </c>
+      <c r="IW35" t="n">
+        <v>20.4</v>
       </c>
     </row>
     <row r="36" ht="13.8" customHeight="1" s="2">
@@ -28136,8 +28346,14 @@
       <c r="IT36" s="1" t="n">
         <v>186.5</v>
       </c>
-      <c r="IU36" t="n">
+      <c r="IU36" s="1" t="n">
         <v>187.5</v>
+      </c>
+      <c r="IV36" s="1" t="n">
+        <v>187.3</v>
+      </c>
+      <c r="IW36" t="n">
+        <v>187.3</v>
       </c>
     </row>
     <row r="37" ht="13.8" customHeight="1" s="2">
@@ -28905,8 +29121,14 @@
       <c r="IT37" s="1" t="n">
         <v>85.5</v>
       </c>
-      <c r="IU37" t="n">
+      <c r="IU37" s="1" t="n">
         <v>86.40000000000001</v>
+      </c>
+      <c r="IV37" s="1" t="n">
+        <v>86.3</v>
+      </c>
+      <c r="IW37" t="n">
+        <v>86.59999999999999</v>
       </c>
     </row>
     <row r="38" ht="13.8" customHeight="1" s="2">
@@ -29674,8 +29896,14 @@
       <c r="IT38" s="1" t="n">
         <v>24.8</v>
       </c>
-      <c r="IU38" t="n">
+      <c r="IU38" s="1" t="n">
         <v>24.49</v>
+      </c>
+      <c r="IV38" s="1" t="n">
+        <v>24.33</v>
+      </c>
+      <c r="IW38" t="n">
+        <v>23.91</v>
       </c>
     </row>
     <row r="39" ht="13.8" customHeight="1" s="2">
@@ -30443,8 +30671,14 @@
       <c r="IT39" s="1" t="n">
         <v>76.5</v>
       </c>
-      <c r="IU39" t="n">
+      <c r="IU39" s="1" t="n">
         <v>70.09999999999999</v>
+      </c>
+      <c r="IV39" s="1" t="n">
+        <v>69.5</v>
+      </c>
+      <c r="IW39" t="n">
+        <v>56.5</v>
       </c>
     </row>
     <row r="40" ht="13.8" customHeight="1" s="2">
@@ -31212,8 +31446,14 @@
       <c r="IT40" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="IU40" t="n">
+      <c r="IU40" s="1" t="n">
         <v>12</v>
+      </c>
+      <c r="IV40" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="IW40" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="41" ht="13.8" customHeight="1" s="2">
@@ -31981,7 +32221,13 @@
       <c r="IT41" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="IU41" t="n">
+      <c r="IU41" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="IV41" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="IW41" t="n">
         <v>5</v>
       </c>
     </row>
@@ -32750,8 +32996,14 @@
       <c r="IT42" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="IU42" t="n">
+      <c r="IU42" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="IV42" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="IW42" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="43" ht="13.8" customHeight="1" s="2">
@@ -33519,8 +33771,14 @@
       <c r="IT43" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="IU43" t="n">
+      <c r="IU43" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="IV43" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="IW43" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="44" ht="13.8" customHeight="1" s="2">
@@ -34288,8 +34546,14 @@
       <c r="IT44" s="1" t="n">
         <v>146</v>
       </c>
-      <c r="IU44" t="n">
+      <c r="IU44" s="1" t="n">
         <v>149</v>
+      </c>
+      <c r="IV44" s="1" t="n">
+        <v>125</v>
+      </c>
+      <c r="IW44" t="n">
+        <v>128</v>
       </c>
     </row>
     <row r="45" ht="13.8" customHeight="1" s="2">
@@ -35057,8 +35321,14 @@
       <c r="IT45" s="1" t="n">
         <v>217</v>
       </c>
-      <c r="IU45" t="n">
+      <c r="IU45" s="1" t="n">
         <v>214</v>
+      </c>
+      <c r="IV45" s="1" t="n">
+        <v>219</v>
+      </c>
+      <c r="IW45" t="n">
+        <v>232</v>
       </c>
     </row>
     <row r="46" ht="13.8" customHeight="1" s="2">
@@ -35826,8 +36096,14 @@
       <c r="IT46" s="1" t="n">
         <v>285</v>
       </c>
-      <c r="IU46" t="n">
+      <c r="IU46" s="1" t="n">
         <v>261</v>
+      </c>
+      <c r="IV46" s="1" t="n">
+        <v>263</v>
+      </c>
+      <c r="IW46" t="n">
+        <v>280</v>
       </c>
     </row>
     <row r="47" ht="13.8" customHeight="1" s="2">
@@ -36595,8 +36871,14 @@
       <c r="IT47" s="1" t="n">
         <v>76.40000000000001</v>
       </c>
-      <c r="IU47" t="n">
+      <c r="IU47" s="1" t="n">
         <v>71.7</v>
+      </c>
+      <c r="IV47" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="IW47" t="n">
+        <v>77.09999999999999</v>
       </c>
     </row>
     <row r="48" ht="13.8" customHeight="1" s="2">
@@ -37364,8 +37646,14 @@
       <c r="IT48" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="IU48" t="n">
+      <c r="IU48" s="1" t="n">
         <v>55</v>
+      </c>
+      <c r="IV48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="IW48" t="n">
+        <v>72</v>
       </c>
     </row>
     <row r="49" ht="13.8" customHeight="1" s="2">
@@ -38133,8 +38421,14 @@
       <c r="IT49" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="IU49" t="n">
+      <c r="IU49" s="1" t="n">
         <v>16</v>
+      </c>
+      <c r="IV49" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="IW49" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="50" ht="13.8" customHeight="1" s="2">
@@ -38902,8 +39196,14 @@
       <c r="IT50" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="IU50" t="n">
+      <c r="IU50" s="1" t="n">
         <v>16</v>
+      </c>
+      <c r="IV50" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="IW50" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="51" ht="13.8" customHeight="1" s="2">
@@ -39671,8 +39971,14 @@
       <c r="IT51" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="IU51" t="n">
+      <c r="IU51" s="1" t="n">
         <v>39</v>
+      </c>
+      <c r="IV51" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="IW51" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="52" ht="13.8" customHeight="1" s="2">
@@ -40440,8 +40746,14 @@
       <c r="IT52" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="IU52" t="n">
+      <c r="IU52" s="1" t="n">
         <v>33</v>
+      </c>
+      <c r="IV52" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="IW52" t="n">
+        <v>57</v>
       </c>
     </row>
     <row r="53" ht="13.8" customHeight="1" s="2">
@@ -41209,8 +41521,14 @@
       <c r="IT53" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="IU53" t="n">
+      <c r="IU53" s="1" t="n">
         <v>48</v>
+      </c>
+      <c r="IV53" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="IW53" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="54" ht="13.8" customHeight="1" s="2">
@@ -41978,7 +42296,13 @@
       <c r="IT54" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="IU54" t="n">
+      <c r="IU54" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="IV54" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="IW54" t="n">
         <v>3</v>
       </c>
     </row>
@@ -42747,8 +43071,14 @@
       <c r="IT55" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="IU55" t="n">
+      <c r="IU55" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="IV55" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="IW55" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="56" ht="13.8" customHeight="1" s="2">
@@ -43516,8 +43846,14 @@
       <c r="IT56" s="1" t="n">
         <v>73.3</v>
       </c>
-      <c r="IU56" t="n">
+      <c r="IU56" s="1" t="n">
         <v>50</v>
+      </c>
+      <c r="IV56" s="1" t="n">
+        <v>87.5</v>
+      </c>
+      <c r="IW56" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="57" ht="13.8" customHeight="1" s="2">
@@ -44285,8 +44621,14 @@
       <c r="IT57" s="1" t="n">
         <v>191</v>
       </c>
-      <c r="IU57" t="n">
+      <c r="IU57" s="1" t="n">
         <v>214</v>
+      </c>
+      <c r="IV57" s="1" t="n">
+        <v>206</v>
+      </c>
+      <c r="IW57" t="n">
+        <v>243</v>
       </c>
     </row>
     <row r="58" ht="13.8" customHeight="1" s="2">
@@ -45054,8 +45396,14 @@
       <c r="IT58" s="1" t="n">
         <v>162</v>
       </c>
-      <c r="IU58" t="n">
+      <c r="IU58" s="1" t="n">
         <v>153</v>
+      </c>
+      <c r="IV58" s="1" t="n">
+        <v>198</v>
+      </c>
+      <c r="IW58" t="n">
+        <v>145</v>
       </c>
     </row>
     <row r="59" ht="13.8" customHeight="1" s="2">
@@ -45823,8 +46171,14 @@
       <c r="IT59" s="1" t="n">
         <v>353</v>
       </c>
-      <c r="IU59" t="n">
+      <c r="IU59" s="1" t="n">
         <v>367</v>
+      </c>
+      <c r="IV59" s="1" t="n">
+        <v>404</v>
+      </c>
+      <c r="IW59" t="n">
+        <v>388</v>
       </c>
     </row>
     <row r="60" ht="13.8" customHeight="1" s="2">
@@ -46592,8 +46946,14 @@
       <c r="IT60" s="1" t="n">
         <v>1.18</v>
       </c>
-      <c r="IU60" t="n">
+      <c r="IU60" s="1" t="n">
         <v>1.4</v>
+      </c>
+      <c r="IV60" s="1" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="IW60" t="n">
+        <v>1.68</v>
       </c>
     </row>
     <row r="61" ht="13.8" customHeight="1" s="2">
@@ -47361,8 +47721,14 @@
       <c r="IT61" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="IU61" t="n">
+      <c r="IU61" s="1" t="n">
         <v>81</v>
+      </c>
+      <c r="IV61" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="IW61" t="n">
+        <v>114</v>
       </c>
     </row>
     <row r="62" ht="13.8" customHeight="1" s="2">
@@ -48130,8 +48496,14 @@
       <c r="IT62" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="IU62" t="n">
+      <c r="IU62" s="1" t="n">
         <v>78</v>
+      </c>
+      <c r="IV62" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="IW62" t="n">
+        <v>49</v>
       </c>
     </row>
     <row r="63" ht="13.8" customHeight="1" s="2">
@@ -48899,8 +49271,14 @@
       <c r="IT63" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="IU63" t="n">
+      <c r="IU63" s="1" t="n">
         <v>29</v>
+      </c>
+      <c r="IV63" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="IW63" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="64" ht="13.8" customHeight="1" s="2">
@@ -49668,8 +50046,14 @@
       <c r="IT64" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="IU64" t="n">
+      <c r="IU64" s="1" t="n">
         <v>24</v>
+      </c>
+      <c r="IV64" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="IW64" t="n">
+        <v>29</v>
       </c>
     </row>
     <row r="65" ht="13.8" customHeight="1" s="2">
@@ -50437,8 +50821,14 @@
       <c r="IT65" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="IU65" t="n">
+      <c r="IU65" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="IV65" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="IW65" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="66" ht="13.8" customHeight="1" s="2">
@@ -51206,8 +51596,14 @@
       <c r="IT66" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="IU66" t="n">
+      <c r="IU66" s="1" t="n">
         <v>9</v>
+      </c>
+      <c r="IV66" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="IW66" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="67" ht="13.8" customHeight="1" s="2">
@@ -51975,8 +52371,14 @@
       <c r="IT67" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="IU67" t="n">
+      <c r="IU67" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="IV67" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="IW67" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="68" ht="13.8" customHeight="1" s="2">
@@ -52744,8 +53146,14 @@
       <c r="IT68" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="IU68" t="n">
+      <c r="IU68" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="IV68" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="IW68" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="69" ht="13.8" customHeight="1" s="2">
@@ -53513,8 +53921,14 @@
       <c r="IT69" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="IU69" t="n">
+      <c r="IU69" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="IV69" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="IW69" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="70" ht="13.8" customHeight="1" s="2">
@@ -54282,8 +54696,14 @@
       <c r="IT70" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="IU70" t="n">
+      <c r="IU70" s="1" t="n">
         <v>17</v>
+      </c>
+      <c r="IV70" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="IW70" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="71" ht="13.8" customHeight="1" s="2">
@@ -55051,8 +55471,14 @@
       <c r="IT71" s="1" t="n">
         <v>54.5</v>
       </c>
-      <c r="IU71" t="n">
+      <c r="IU71" s="1" t="n">
         <v>52.9</v>
+      </c>
+      <c r="IV71" s="1" t="n">
+        <v>60.7</v>
+      </c>
+      <c r="IW71" t="n">
+        <v>54.8</v>
       </c>
     </row>
     <row r="72" ht="13.8" customHeight="1" s="2">
@@ -55820,8 +56246,14 @@
       <c r="IT72" s="1" t="n">
         <v>29.42</v>
       </c>
-      <c r="IU72" t="n">
+      <c r="IU72" s="1" t="n">
         <v>40.78</v>
+      </c>
+      <c r="IV72" s="1" t="n">
+        <v>23.76</v>
+      </c>
+      <c r="IW72" t="n">
+        <v>22.82</v>
       </c>
     </row>
     <row r="73" ht="13.8" customHeight="1" s="2">
@@ -56589,8 +57021,14 @@
       <c r="IT73" s="1" t="n">
         <v>16.05</v>
       </c>
-      <c r="IU73" t="n">
+      <c r="IU73" s="1" t="n">
         <v>21.59</v>
+      </c>
+      <c r="IV73" s="1" t="n">
+        <v>14.43</v>
+      </c>
+      <c r="IW73" t="n">
+        <v>12.52</v>
       </c>
     </row>
     <row r="74" ht="13.8" customHeight="1" s="2">
@@ -57358,8 +57796,14 @@
       <c r="IT74" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="IU74" t="n">
+      <c r="IU74" s="1" t="n">
         <v>44</v>
+      </c>
+      <c r="IV74" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="IW74" t="n">
+        <v>42</v>
       </c>
     </row>
     <row r="75" ht="13.8" customHeight="1" s="2">
@@ -58127,8 +58571,14 @@
       <c r="IT75" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="IU75" t="n">
+      <c r="IU75" s="1" t="n">
         <v>56</v>
+      </c>
+      <c r="IV75" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="IW75" t="n">
+        <v>59</v>
       </c>
     </row>
     <row r="76" ht="13.8" customHeight="1" s="2">
@@ -58896,8 +59346,14 @@
       <c r="IT76" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="IU76" t="n">
+      <c r="IU76" s="1" t="n">
         <v>49</v>
+      </c>
+      <c r="IV76" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="IW76" t="n">
+        <v>36</v>
       </c>
     </row>
     <row r="77" ht="13.8" customHeight="1" s="2">
@@ -59665,8 +60121,14 @@
       <c r="IT77" s="1" t="n">
         <v>61</v>
       </c>
-      <c r="IU77" t="n">
+      <c r="IU77" s="1" t="n">
         <v>43</v>
+      </c>
+      <c r="IV77" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="IW77" t="n">
+        <v>74</v>
       </c>
     </row>
     <row r="78" ht="13.8" customHeight="1" s="2">
@@ -60434,8 +60896,14 @@
       <c r="IT78" s="1" t="n">
         <v>2.77</v>
       </c>
-      <c r="IU78" t="n">
+      <c r="IU78" s="1" t="n">
         <v>2.53</v>
+      </c>
+      <c r="IV78" s="1" t="n">
+        <v>1.96</v>
+      </c>
+      <c r="IW78" t="n">
+        <v>2.39</v>
       </c>
     </row>
     <row r="79" ht="13.8" customHeight="1" s="2">
@@ -61203,8 +61671,14 @@
       <c r="IT79" s="1" t="n">
         <v>5.08</v>
       </c>
-      <c r="IU79" t="n">
+      <c r="IU79" s="1" t="n">
         <v>4.78</v>
+      </c>
+      <c r="IV79" s="1" t="n">
+        <v>3.24</v>
+      </c>
+      <c r="IW79" t="n">
+        <v>4.35</v>
       </c>
     </row>
     <row r="80" ht="13.8" customHeight="1" s="2">
@@ -61972,8 +62446,14 @@
       <c r="IT80" s="1" t="n">
         <v>31.1</v>
       </c>
-      <c r="IU80" t="n">
+      <c r="IU80" s="1" t="n">
         <v>32.6</v>
+      </c>
+      <c r="IV80" s="1" t="n">
+        <v>45.5</v>
+      </c>
+      <c r="IW80" t="n">
+        <v>40.5</v>
       </c>
     </row>
     <row r="81" ht="13.8" customHeight="1" s="2">
@@ -62741,8 +63221,14 @@
       <c r="IT81" s="1" t="n">
         <v>19.7</v>
       </c>
-      <c r="IU81" t="n">
+      <c r="IU81" s="1" t="n">
         <v>20.9</v>
+      </c>
+      <c r="IV81" s="1" t="n">
+        <v>30.9</v>
+      </c>
+      <c r="IW81" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="82" ht="13.8" customHeight="1" s="2">
@@ -63510,8 +63996,14 @@
       <c r="IT82" s="1" t="n">
         <v>185.9</v>
       </c>
-      <c r="IU82" t="n">
+      <c r="IU82" s="1" t="n">
         <v>188.3</v>
+      </c>
+      <c r="IV82" s="1" t="n">
+        <v>189.5</v>
+      </c>
+      <c r="IW82" t="n">
+        <v>188</v>
       </c>
     </row>
     <row r="83" ht="13.8" customHeight="1" s="2">
@@ -64279,8 +64771,14 @@
       <c r="IT83" s="1" t="n">
         <v>85.09999999999999</v>
       </c>
-      <c r="IU83" t="n">
+      <c r="IU83" s="1" t="n">
         <v>86.5</v>
+      </c>
+      <c r="IV83" s="1" t="n">
+        <v>89.09999999999999</v>
+      </c>
+      <c r="IW83" t="n">
+        <v>86.90000000000001</v>
       </c>
     </row>
     <row r="84" ht="13.8" customHeight="1" s="2">
@@ -65048,8 +65546,14 @@
       <c r="IT84" s="1" t="n">
         <v>26.74</v>
       </c>
-      <c r="IU84" t="n">
+      <c r="IU84" s="1" t="n">
         <v>25.74</v>
+      </c>
+      <c r="IV84" s="1" t="n">
+        <v>25.41</v>
+      </c>
+      <c r="IW84" t="n">
+        <v>24.66</v>
       </c>
     </row>
     <row r="85" ht="13.8" customHeight="1" s="2">
@@ -65817,8 +66321,14 @@
       <c r="IT85" s="1" t="n">
         <v>112.2</v>
       </c>
-      <c r="IU85" t="n">
+      <c r="IU85" s="1" t="n">
         <v>96.59999999999999</v>
+      </c>
+      <c r="IV85" s="1" t="n">
+        <v>91.09999999999999</v>
+      </c>
+      <c r="IW85" t="n">
+        <v>76.7</v>
       </c>
     </row>
     <row r="86" ht="13.8" customHeight="1" s="2">
@@ -66586,8 +67096,14 @@
       <c r="IT86" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="IU86" t="n">
+      <c r="IU86" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="IV86" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="IW86" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="87" ht="13.8" customHeight="1" s="2">
@@ -67355,7 +67871,13 @@
       <c r="IT87" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="IU87" t="n">
+      <c r="IU87" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="IV87" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="IW87" t="n">
         <v>8</v>
       </c>
     </row>
@@ -68124,8 +68646,14 @@
       <c r="IT88" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="IU88" t="n">
+      <c r="IU88" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="IV88" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="IW88" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="89" ht="13.8" customHeight="1" s="2">
@@ -68893,8 +69421,14 @@
       <c r="IT89" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="IU89" t="n">
+      <c r="IU89" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="IV89" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="IW89" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="90" ht="13.8" customHeight="1" s="2">
@@ -69662,8 +70196,14 @@
       <c r="IT90" s="1" t="n">
         <v>131</v>
       </c>
-      <c r="IU90" t="n">
+      <c r="IU90" s="1" t="n">
         <v>145</v>
+      </c>
+      <c r="IV90" s="1" t="n">
+        <v>152</v>
+      </c>
+      <c r="IW90" t="n">
+        <v>142</v>
       </c>
     </row>
     <row r="91" ht="13.8" customHeight="1" s="2">
@@ -70431,8 +70971,14 @@
       <c r="IT91" s="1" t="n">
         <v>223</v>
       </c>
-      <c r="IU91" t="n">
+      <c r="IU91" s="1" t="n">
         <v>212</v>
+      </c>
+      <c r="IV91" s="1" t="n">
+        <v>253</v>
+      </c>
+      <c r="IW91" t="n">
+        <v>243</v>
       </c>
     </row>
     <row r="92" ht="13.8" customHeight="1" s="2">
@@ -71200,8 +71746,14 @@
       <c r="IT92" s="1" t="n">
         <v>269</v>
       </c>
-      <c r="IU92" t="n">
+      <c r="IU92" s="1" t="n">
         <v>271</v>
+      </c>
+      <c r="IV92" s="1" t="n">
+        <v>306</v>
+      </c>
+      <c r="IW92" t="n">
+        <v>294</v>
       </c>
     </row>
     <row r="93" ht="13.8" customHeight="1" s="2">
@@ -71969,8 +72521,14 @@
       <c r="IT93" s="1" t="n">
         <v>76.2</v>
       </c>
-      <c r="IU93" t="n">
+      <c r="IU93" s="1" t="n">
         <v>73.8</v>
+      </c>
+      <c r="IV93" s="1" t="n">
+        <v>75.7</v>
+      </c>
+      <c r="IW93" t="n">
+        <v>75.8</v>
       </c>
     </row>
     <row r="94" ht="13.8" customHeight="1" s="2">
@@ -72738,8 +73296,14 @@
       <c r="IT94" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="IU94" t="n">
+      <c r="IU94" s="1" t="n">
         <v>56</v>
+      </c>
+      <c r="IV94" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="IW94" t="n">
+        <v>59</v>
       </c>
     </row>
     <row r="95" ht="13.8" customHeight="1" s="2">
@@ -73507,7 +74071,13 @@
       <c r="IT95" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="IU95" t="n">
+      <c r="IU95" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="IV95" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="IW95" t="n">
         <v>12</v>
       </c>
     </row>
@@ -74276,8 +74846,14 @@
       <c r="IT96" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="IU96" t="n">
+      <c r="IU96" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="IV96" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="IW96" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="97" ht="13.8" customHeight="1" s="2">
@@ -75045,8 +75621,14 @@
       <c r="IT97" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="IU97" t="n">
+      <c r="IU97" s="1" t="n">
         <v>44</v>
+      </c>
+      <c r="IV97" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="IW97" t="n">
+        <v>42</v>
       </c>
     </row>
     <row r="98" ht="13.8" customHeight="1" s="2">
@@ -75814,8 +76396,14 @@
       <c r="IT98" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="IU98" t="n">
+      <c r="IU98" s="1" t="n">
         <v>49</v>
+      </c>
+      <c r="IV98" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="IW98" t="n">
+        <v>36</v>
       </c>
     </row>
     <row r="99" ht="13.8" customHeight="1" s="2">
@@ -76583,8 +77171,14 @@
       <c r="IT99" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="IU99" t="n">
+      <c r="IU99" s="1" t="n">
         <v>58</v>
+      </c>
+      <c r="IV99" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="IW99" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="100" ht="13.8" customHeight="1" s="2">
@@ -77352,8 +77946,14 @@
       <c r="IT100" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="IU100" t="n">
+      <c r="IU100" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="IV100" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="IW100" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="101" ht="13.8" customHeight="1" s="2">
@@ -78121,8 +78721,14 @@
       <c r="IT101" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="IU101" t="n">
+      <c r="IU101" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="IV101" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="IW101" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="102" ht="13.8" customHeight="1" s="2">
@@ -78890,8 +79496,14 @@
       <c r="IT102" s="1" t="n">
         <v>66.7</v>
       </c>
-      <c r="IU102" t="n">
+      <c r="IU102" s="1" t="n">
         <v>55.6</v>
+      </c>
+      <c r="IV102" s="1" t="n">
+        <v>88.2</v>
+      </c>
+      <c r="IW102" t="n">
+        <v>64.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PAV updates and round 11 preds
</commit_message>
<xml_diff>
--- a/django_AFL_ML/Data/Adelaide_stats.xlsx
+++ b/django_AFL_ML/Data/Adelaide_stats.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:IW102"/>
+  <dimension ref="A1:IY102"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="GZ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="HA23" activeCellId="0" sqref="HA23"/>
@@ -1227,8 +1227,14 @@
       <c r="IV1" s="1" t="n">
         <v>10600</v>
       </c>
-      <c r="IW1" t="n">
+      <c r="IW1" s="1" t="n">
         <v>10615</v>
+      </c>
+      <c r="IX1" s="1" t="n">
+        <v>10621</v>
+      </c>
+      <c r="IY1" t="n">
+        <v>10632</v>
       </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="2">
@@ -2002,7 +2008,13 @@
       <c r="IV2" s="1" t="n">
         <v>2022</v>
       </c>
-      <c r="IW2" t="n">
+      <c r="IW2" s="1" t="n">
+        <v>2022</v>
+      </c>
+      <c r="IX2" s="1" t="n">
+        <v>2022</v>
+      </c>
+      <c r="IY2" t="n">
         <v>2022</v>
       </c>
     </row>
@@ -2777,8 +2789,14 @@
       <c r="IV3" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="IW3" t="n">
+      <c r="IW3" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="IX3" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="IY3" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="2">
@@ -3552,8 +3570,14 @@
       <c r="IV4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="IW4" t="n">
+      <c r="IW4" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="IX4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="IY4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5" ht="13.8" customHeight="1" s="2">
@@ -4327,8 +4351,14 @@
       <c r="IV5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="IW5" t="n">
+      <c r="IW5" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="IX5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="IY5" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6" ht="13.8" customHeight="1" s="2">
@@ -5102,8 +5132,14 @@
       <c r="IV6" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="IW6" t="n">
+      <c r="IW6" s="1" t="n">
         <v>68</v>
+      </c>
+      <c r="IX6" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="IY6" t="n">
+        <v>69</v>
       </c>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="2">
@@ -5877,8 +5913,14 @@
       <c r="IV7" s="1" t="n">
         <v>113</v>
       </c>
-      <c r="IW7" t="n">
+      <c r="IW7" s="1" t="n">
         <v>116</v>
+      </c>
+      <c r="IX7" s="1" t="n">
+        <v>102</v>
+      </c>
+      <c r="IY7" t="n">
+        <v>90</v>
       </c>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="2">
@@ -6652,8 +6694,14 @@
       <c r="IV8" s="1" t="n">
         <v>-59</v>
       </c>
-      <c r="IW8" t="n">
+      <c r="IW8" s="1" t="n">
         <v>-48</v>
+      </c>
+      <c r="IX8" s="1" t="n">
+        <v>-36</v>
+      </c>
+      <c r="IY8" t="n">
+        <v>-21</v>
       </c>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="2">
@@ -7427,7 +7475,13 @@
       <c r="IV9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="IW9" t="n">
+      <c r="IW9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="IX9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="IY9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8202,8 +8256,14 @@
       <c r="IV10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="IW10" t="n">
+      <c r="IW10" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="IX10" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="IY10" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="11" ht="13.8" customHeight="1" s="2">
@@ -8977,8 +9037,14 @@
       <c r="IV11" s="1" t="n">
         <v>179</v>
       </c>
-      <c r="IW11" t="n">
+      <c r="IW11" s="1" t="n">
         <v>218</v>
+      </c>
+      <c r="IX11" s="1" t="n">
+        <v>206</v>
+      </c>
+      <c r="IY11" t="n">
+        <v>211</v>
       </c>
     </row>
     <row r="12" ht="13.8" customHeight="1" s="2">
@@ -9752,8 +9818,14 @@
       <c r="IV12" s="1" t="n">
         <v>167</v>
       </c>
-      <c r="IW12" t="n">
+      <c r="IW12" s="1" t="n">
         <v>145</v>
+      </c>
+      <c r="IX12" s="1" t="n">
+        <v>147</v>
+      </c>
+      <c r="IY12" t="n">
+        <v>125</v>
       </c>
     </row>
     <row r="13" ht="13.8" customHeight="1" s="2">
@@ -10527,8 +10599,14 @@
       <c r="IV13" s="1" t="n">
         <v>346</v>
       </c>
-      <c r="IW13" t="n">
+      <c r="IW13" s="1" t="n">
         <v>363</v>
+      </c>
+      <c r="IX13" s="1" t="n">
+        <v>353</v>
+      </c>
+      <c r="IY13" t="n">
+        <v>336</v>
       </c>
     </row>
     <row r="14" ht="13.8" customHeight="1" s="2">
@@ -11302,8 +11380,14 @@
       <c r="IV14" s="1" t="n">
         <v>1.07</v>
       </c>
-      <c r="IW14" t="n">
+      <c r="IW14" s="1" t="n">
         <v>1.5</v>
+      </c>
+      <c r="IX14" s="1" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="IY14" t="n">
+        <v>1.69</v>
       </c>
     </row>
     <row r="15" ht="13.8" customHeight="1" s="2">
@@ -12077,8 +12161,14 @@
       <c r="IV15" s="1" t="n">
         <v>64</v>
       </c>
-      <c r="IW15" t="n">
+      <c r="IW15" s="1" t="n">
         <v>93</v>
+      </c>
+      <c r="IX15" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="IY15" t="n">
+        <v>89</v>
       </c>
     </row>
     <row r="16" ht="13.8" customHeight="1" s="2">
@@ -12852,8 +12942,14 @@
       <c r="IV16" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="IW16" t="n">
+      <c r="IW16" s="1" t="n">
         <v>56</v>
+      </c>
+      <c r="IX16" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="IY16" t="n">
+        <v>55</v>
       </c>
     </row>
     <row r="17" ht="13.8" customHeight="1" s="2">
@@ -13627,8 +13723,14 @@
       <c r="IV17" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="IW17" t="n">
+      <c r="IW17" s="1" t="n">
         <v>46</v>
+      </c>
+      <c r="IX17" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="IY17" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="18" ht="13.8" customHeight="1" s="2">
@@ -14402,8 +14504,14 @@
       <c r="IV18" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="IW18" t="n">
+      <c r="IW18" s="1" t="n">
         <v>24</v>
+      </c>
+      <c r="IX18" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="IY18" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="19" ht="13.8" customHeight="1" s="2">
@@ -15177,8 +15285,14 @@
       <c r="IV19" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="IW19" t="n">
+      <c r="IW19" s="1" t="n">
         <v>29</v>
+      </c>
+      <c r="IX19" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="IY19" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="20" ht="13.8" customHeight="1" s="2">
@@ -15952,8 +16066,14 @@
       <c r="IV20" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="IW20" t="n">
+      <c r="IW20" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="IX20" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="IY20" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="21" ht="13.8" customHeight="1" s="2">
@@ -16727,8 +16847,14 @@
       <c r="IV21" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="IW21" t="n">
+      <c r="IW21" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="IX21" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="IY21" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="22" ht="13.8" customHeight="1" s="2">
@@ -17502,8 +17628,14 @@
       <c r="IV22" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="IW22" t="n">
+      <c r="IW22" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="IX22" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="IY22" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="23" ht="13.8" customHeight="1" s="2">
@@ -18277,8 +18409,14 @@
       <c r="IV23" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="IW23" t="n">
+      <c r="IW23" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="IX23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="IY23" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="24" ht="13.8" customHeight="1" s="2">
@@ -19052,8 +19190,14 @@
       <c r="IV24" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="IW24" t="n">
+      <c r="IW24" s="1" t="n">
         <v>18</v>
+      </c>
+      <c r="IX24" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="IY24" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="25" ht="13.8" customHeight="1" s="2">
@@ -19827,8 +19971,14 @@
       <c r="IV25" s="1" t="n">
         <v>57.1</v>
       </c>
-      <c r="IW25" t="n">
+      <c r="IW25" s="1" t="n">
         <v>55.6</v>
+      </c>
+      <c r="IX25" s="1" t="n">
+        <v>42.9</v>
+      </c>
+      <c r="IY25" t="n">
+        <v>37.5</v>
       </c>
     </row>
     <row r="26" ht="13.8" customHeight="1" s="2">
@@ -20602,8 +20752,14 @@
       <c r="IV26" s="1" t="n">
         <v>43.25</v>
       </c>
-      <c r="IW26" t="n">
+      <c r="IW26" s="1" t="n">
         <v>36.3</v>
+      </c>
+      <c r="IX26" s="1" t="n">
+        <v>39.22</v>
+      </c>
+      <c r="IY26" t="n">
+        <v>37.33</v>
       </c>
     </row>
     <row r="27" ht="13.8" customHeight="1" s="2">
@@ -21377,8 +21533,14 @@
       <c r="IV27" s="1" t="n">
         <v>24.71</v>
       </c>
-      <c r="IW27" t="n">
+      <c r="IW27" s="1" t="n">
         <v>20.17</v>
+      </c>
+      <c r="IX27" s="1" t="n">
+        <v>16.81</v>
+      </c>
+      <c r="IY27" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="28" ht="13.8" customHeight="1" s="2">
@@ -22152,8 +22314,14 @@
       <c r="IV28" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="IW28" t="n">
+      <c r="IW28" s="1" t="n">
         <v>31</v>
+      </c>
+      <c r="IX28" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="IY28" t="n">
+        <v>36</v>
       </c>
     </row>
     <row r="29" ht="13.8" customHeight="1" s="2">
@@ -22927,8 +23095,14 @@
       <c r="IV29" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="IW29" t="n">
+      <c r="IW29" s="1" t="n">
         <v>72</v>
+      </c>
+      <c r="IX29" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="IY29" t="n">
+        <v>51</v>
       </c>
     </row>
     <row r="30" ht="13.8" customHeight="1" s="2">
@@ -23702,8 +23876,14 @@
       <c r="IV30" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="IW30" t="n">
+      <c r="IW30" s="1" t="n">
         <v>57</v>
+      </c>
+      <c r="IX30" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="IY30" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="31" ht="13.8" customHeight="1" s="2">
@@ -24477,8 +24657,14 @@
       <c r="IV31" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="IW31" t="n">
+      <c r="IW31" s="1" t="n">
         <v>49</v>
+      </c>
+      <c r="IX31" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="IY31" t="n">
+        <v>47</v>
       </c>
     </row>
     <row r="32" ht="13.8" customHeight="1" s="2">
@@ -25252,8 +25438,14 @@
       <c r="IV32" s="1" t="n">
         <v>3.43</v>
       </c>
-      <c r="IW32" t="n">
+      <c r="IW32" s="1" t="n">
         <v>2.72</v>
+      </c>
+      <c r="IX32" s="1" t="n">
+        <v>2.52</v>
+      </c>
+      <c r="IY32" t="n">
+        <v>1.96</v>
       </c>
     </row>
     <row r="33" ht="13.8" customHeight="1" s="2">
@@ -26027,8 +26219,14 @@
       <c r="IV33" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="IW33" t="n">
+      <c r="IW33" s="1" t="n">
         <v>4.9</v>
+      </c>
+      <c r="IX33" s="1" t="n">
+        <v>5.89</v>
+      </c>
+      <c r="IY33" t="n">
+        <v>5.22</v>
       </c>
     </row>
     <row r="34" ht="13.8" customHeight="1" s="2">
@@ -26802,8 +27000,14 @@
       <c r="IV34" s="1" t="n">
         <v>29.2</v>
       </c>
-      <c r="IW34" t="n">
+      <c r="IW34" s="1" t="n">
         <v>34.7</v>
+      </c>
+      <c r="IX34" s="1" t="n">
+        <v>37.7</v>
+      </c>
+      <c r="IY34" t="n">
+        <v>46.8</v>
       </c>
     </row>
     <row r="35" ht="13.8" customHeight="1" s="2">
@@ -27577,8 +27781,14 @@
       <c r="IV35" s="1" t="n">
         <v>16.7</v>
       </c>
-      <c r="IW35" t="n">
+      <c r="IW35" s="1" t="n">
         <v>20.4</v>
+      </c>
+      <c r="IX35" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="IY35" t="n">
+        <v>19.1</v>
       </c>
     </row>
     <row r="36" ht="13.8" customHeight="1" s="2">
@@ -28352,8 +28562,14 @@
       <c r="IV36" s="1" t="n">
         <v>187.3</v>
       </c>
-      <c r="IW36" t="n">
+      <c r="IW36" s="1" t="n">
         <v>187.3</v>
+      </c>
+      <c r="IX36" s="1" t="n">
+        <v>186.7</v>
+      </c>
+      <c r="IY36" t="n">
+        <v>186.2</v>
       </c>
     </row>
     <row r="37" ht="13.8" customHeight="1" s="2">
@@ -29127,8 +29343,14 @@
       <c r="IV37" s="1" t="n">
         <v>86.3</v>
       </c>
-      <c r="IW37" t="n">
+      <c r="IW37" s="1" t="n">
         <v>86.59999999999999</v>
+      </c>
+      <c r="IX37" s="1" t="n">
+        <v>86.2</v>
+      </c>
+      <c r="IY37" t="n">
+        <v>86</v>
       </c>
     </row>
     <row r="38" ht="13.8" customHeight="1" s="2">
@@ -29902,8 +30124,14 @@
       <c r="IV38" s="1" t="n">
         <v>24.33</v>
       </c>
-      <c r="IW38" t="n">
+      <c r="IW38" s="1" t="n">
         <v>23.91</v>
+      </c>
+      <c r="IX38" s="1" t="n">
+        <v>24.16</v>
+      </c>
+      <c r="IY38" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="39" ht="13.8" customHeight="1" s="2">
@@ -30677,8 +30905,14 @@
       <c r="IV39" s="1" t="n">
         <v>69.5</v>
       </c>
-      <c r="IW39" t="n">
+      <c r="IW39" s="1" t="n">
         <v>56.5</v>
+      </c>
+      <c r="IX39" s="1" t="n">
+        <v>63.1</v>
+      </c>
+      <c r="IY39" t="n">
+        <v>63.3</v>
       </c>
     </row>
     <row r="40" ht="13.8" customHeight="1" s="2">
@@ -31452,7 +31686,13 @@
       <c r="IV40" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="IW40" t="n">
+      <c r="IW40" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="IX40" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="IY40" t="n">
         <v>15</v>
       </c>
     </row>
@@ -32227,8 +32467,14 @@
       <c r="IV41" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="IW41" t="n">
+      <c r="IW41" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="IX41" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="IY41" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="42" ht="13.8" customHeight="1" s="2">
@@ -33002,7 +33248,13 @@
       <c r="IV42" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="IW42" t="n">
+      <c r="IW42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="IX42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="IY42" t="n">
         <v>0</v>
       </c>
     </row>
@@ -33777,8 +34029,14 @@
       <c r="IV43" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="IW43" t="n">
+      <c r="IW43" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="IX43" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="IY43" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="44" ht="13.8" customHeight="1" s="2">
@@ -34552,7 +34810,13 @@
       <c r="IV44" s="1" t="n">
         <v>125</v>
       </c>
-      <c r="IW44" t="n">
+      <c r="IW44" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="IX44" s="1" t="n">
+        <v>149</v>
+      </c>
+      <c r="IY44" t="n">
         <v>128</v>
       </c>
     </row>
@@ -35327,8 +35591,14 @@
       <c r="IV45" s="1" t="n">
         <v>219</v>
       </c>
-      <c r="IW45" t="n">
+      <c r="IW45" s="1" t="n">
         <v>232</v>
+      </c>
+      <c r="IX45" s="1" t="n">
+        <v>195</v>
+      </c>
+      <c r="IY45" t="n">
+        <v>202</v>
       </c>
     </row>
     <row r="46" ht="13.8" customHeight="1" s="2">
@@ -36102,8 +36372,14 @@
       <c r="IV46" s="1" t="n">
         <v>263</v>
       </c>
-      <c r="IW46" t="n">
+      <c r="IW46" s="1" t="n">
         <v>280</v>
+      </c>
+      <c r="IX46" s="1" t="n">
+        <v>256</v>
+      </c>
+      <c r="IY46" t="n">
+        <v>248</v>
       </c>
     </row>
     <row r="47" ht="13.8" customHeight="1" s="2">
@@ -36877,8 +37153,14 @@
       <c r="IV47" s="1" t="n">
         <v>76</v>
       </c>
-      <c r="IW47" t="n">
+      <c r="IW47" s="1" t="n">
         <v>77.09999999999999</v>
+      </c>
+      <c r="IX47" s="1" t="n">
+        <v>72.5</v>
+      </c>
+      <c r="IY47" t="n">
+        <v>73.8</v>
       </c>
     </row>
     <row r="48" ht="13.8" customHeight="1" s="2">
@@ -37652,8 +37934,14 @@
       <c r="IV48" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="IW48" t="n">
+      <c r="IW48" s="1" t="n">
         <v>72</v>
+      </c>
+      <c r="IX48" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="IY48" t="n">
+        <v>51</v>
       </c>
     </row>
     <row r="49" ht="13.8" customHeight="1" s="2">
@@ -38427,8 +38715,14 @@
       <c r="IV49" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="IW49" t="n">
+      <c r="IW49" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="IX49" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="IY49" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="50" ht="13.8" customHeight="1" s="2">
@@ -39202,8 +39496,14 @@
       <c r="IV50" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="IW50" t="n">
+      <c r="IW50" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="IX50" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="IY50" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="51" ht="13.8" customHeight="1" s="2">
@@ -39977,8 +40277,14 @@
       <c r="IV51" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="IW51" t="n">
+      <c r="IW51" s="1" t="n">
         <v>31</v>
+      </c>
+      <c r="IX51" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="IY51" t="n">
+        <v>36</v>
       </c>
     </row>
     <row r="52" ht="13.8" customHeight="1" s="2">
@@ -40752,8 +41058,14 @@
       <c r="IV52" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="IW52" t="n">
+      <c r="IW52" s="1" t="n">
         <v>57</v>
+      </c>
+      <c r="IX52" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="IY52" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="53" ht="13.8" customHeight="1" s="2">
@@ -41527,8 +41839,14 @@
       <c r="IV53" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="IW53" t="n">
+      <c r="IW53" s="1" t="n">
         <v>50</v>
+      </c>
+      <c r="IX53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="IY53" t="n">
+        <v>46</v>
       </c>
     </row>
     <row r="54" ht="13.8" customHeight="1" s="2">
@@ -42302,8 +42620,14 @@
       <c r="IV54" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="IW54" t="n">
+      <c r="IW54" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="IX54" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="IY54" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="55" ht="13.8" customHeight="1" s="2">
@@ -43077,8 +43401,14 @@
       <c r="IV55" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="IW55" t="n">
+      <c r="IW55" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="IX55" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="IY55" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="56" ht="13.8" customHeight="1" s="2">
@@ -43852,8 +44182,14 @@
       <c r="IV56" s="1" t="n">
         <v>87.5</v>
       </c>
-      <c r="IW56" t="n">
+      <c r="IW56" s="1" t="n">
         <v>70</v>
+      </c>
+      <c r="IX56" s="1" t="n">
+        <v>77.8</v>
+      </c>
+      <c r="IY56" t="n">
+        <v>44.4</v>
       </c>
     </row>
     <row r="57" ht="13.8" customHeight="1" s="2">
@@ -44627,8 +44963,14 @@
       <c r="IV57" s="1" t="n">
         <v>206</v>
       </c>
-      <c r="IW57" t="n">
+      <c r="IW57" s="1" t="n">
         <v>243</v>
+      </c>
+      <c r="IX57" s="1" t="n">
+        <v>224</v>
+      </c>
+      <c r="IY57" t="n">
+        <v>208</v>
       </c>
     </row>
     <row r="58" ht="13.8" customHeight="1" s="2">
@@ -45402,8 +45744,14 @@
       <c r="IV58" s="1" t="n">
         <v>198</v>
       </c>
-      <c r="IW58" t="n">
+      <c r="IW58" s="1" t="n">
         <v>145</v>
+      </c>
+      <c r="IX58" s="1" t="n">
+        <v>119</v>
+      </c>
+      <c r="IY58" t="n">
+        <v>142</v>
       </c>
     </row>
     <row r="59" ht="13.8" customHeight="1" s="2">
@@ -46177,8 +46525,14 @@
       <c r="IV59" s="1" t="n">
         <v>404</v>
       </c>
-      <c r="IW59" t="n">
+      <c r="IW59" s="1" t="n">
         <v>388</v>
+      </c>
+      <c r="IX59" s="1" t="n">
+        <v>343</v>
+      </c>
+      <c r="IY59" t="n">
+        <v>350</v>
       </c>
     </row>
     <row r="60" ht="13.8" customHeight="1" s="2">
@@ -46952,8 +47306,14 @@
       <c r="IV60" s="1" t="n">
         <v>1.04</v>
       </c>
-      <c r="IW60" t="n">
+      <c r="IW60" s="1" t="n">
         <v>1.68</v>
+      </c>
+      <c r="IX60" s="1" t="n">
+        <v>1.88</v>
+      </c>
+      <c r="IY60" t="n">
+        <v>1.46</v>
       </c>
     </row>
     <row r="61" ht="13.8" customHeight="1" s="2">
@@ -47727,8 +48087,14 @@
       <c r="IV61" s="1" t="n">
         <v>95</v>
       </c>
-      <c r="IW61" t="n">
+      <c r="IW61" s="1" t="n">
         <v>114</v>
+      </c>
+      <c r="IX61" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="IY61" t="n">
+        <v>93</v>
       </c>
     </row>
     <row r="62" ht="13.8" customHeight="1" s="2">
@@ -48502,8 +48868,14 @@
       <c r="IV62" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="IW62" t="n">
+      <c r="IW62" s="1" t="n">
         <v>49</v>
+      </c>
+      <c r="IX62" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="IY62" t="n">
+        <v>41</v>
       </c>
     </row>
     <row r="63" ht="13.8" customHeight="1" s="2">
@@ -49277,8 +49649,14 @@
       <c r="IV63" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="IW63" t="n">
+      <c r="IW63" s="1" t="n">
         <v>22</v>
+      </c>
+      <c r="IX63" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="IY63" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="64" ht="13.8" customHeight="1" s="2">
@@ -50052,8 +50430,14 @@
       <c r="IV64" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="IW64" t="n">
+      <c r="IW64" s="1" t="n">
         <v>29</v>
+      </c>
+      <c r="IX64" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="IY64" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="65" ht="13.8" customHeight="1" s="2">
@@ -50827,8 +51211,14 @@
       <c r="IV65" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="IW65" t="n">
+      <c r="IW65" s="1" t="n">
         <v>24</v>
+      </c>
+      <c r="IX65" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="IY65" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="66" ht="13.8" customHeight="1" s="2">
@@ -51602,8 +51992,14 @@
       <c r="IV66" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="IW66" t="n">
+      <c r="IW66" s="1" t="n">
         <v>17</v>
+      </c>
+      <c r="IX66" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="IY66" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="67" ht="13.8" customHeight="1" s="2">
@@ -52377,7 +52773,13 @@
       <c r="IV67" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="IW67" t="n">
+      <c r="IW67" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="IX67" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="IY67" t="n">
         <v>11</v>
       </c>
     </row>
@@ -53152,8 +53554,14 @@
       <c r="IV68" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="IW68" t="n">
+      <c r="IW68" s="1" t="n">
         <v>13</v>
+      </c>
+      <c r="IX68" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="IY68" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="69" ht="13.8" customHeight="1" s="2">
@@ -53927,8 +54335,14 @@
       <c r="IV69" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="IW69" t="n">
+      <c r="IW69" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="IX69" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="IY69" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="70" ht="13.8" customHeight="1" s="2">
@@ -54702,8 +55116,14 @@
       <c r="IV70" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="IW70" t="n">
+      <c r="IW70" s="1" t="n">
         <v>31</v>
+      </c>
+      <c r="IX70" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="IY70" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="71" ht="13.8" customHeight="1" s="2">
@@ -55477,8 +55897,14 @@
       <c r="IV71" s="1" t="n">
         <v>60.7</v>
       </c>
-      <c r="IW71" t="n">
+      <c r="IW71" s="1" t="n">
         <v>54.8</v>
+      </c>
+      <c r="IX71" s="1" t="n">
+        <v>72.7</v>
+      </c>
+      <c r="IY71" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="72" ht="13.8" customHeight="1" s="2">
@@ -56252,8 +56678,14 @@
       <c r="IV72" s="1" t="n">
         <v>23.76</v>
       </c>
-      <c r="IW72" t="n">
+      <c r="IW72" s="1" t="n">
         <v>22.82</v>
+      </c>
+      <c r="IX72" s="1" t="n">
+        <v>21.44</v>
+      </c>
+      <c r="IY72" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="73" ht="13.8" customHeight="1" s="2">
@@ -57027,8 +57459,14 @@
       <c r="IV73" s="1" t="n">
         <v>14.43</v>
       </c>
-      <c r="IW73" t="n">
+      <c r="IW73" s="1" t="n">
         <v>12.52</v>
+      </c>
+      <c r="IX73" s="1" t="n">
+        <v>15.59</v>
+      </c>
+      <c r="IY73" t="n">
+        <v>17.5</v>
       </c>
     </row>
     <row r="74" ht="13.8" customHeight="1" s="2">
@@ -57802,8 +58240,14 @@
       <c r="IV74" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="IW74" t="n">
+      <c r="IW74" s="1" t="n">
         <v>42</v>
+      </c>
+      <c r="IX74" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="IY74" t="n">
+        <v>29</v>
       </c>
     </row>
     <row r="75" ht="13.8" customHeight="1" s="2">
@@ -58577,8 +59021,14 @@
       <c r="IV75" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="IW75" t="n">
+      <c r="IW75" s="1" t="n">
         <v>59</v>
+      </c>
+      <c r="IX75" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="IY75" t="n">
+        <v>73</v>
       </c>
     </row>
     <row r="76" ht="13.8" customHeight="1" s="2">
@@ -59352,8 +59802,14 @@
       <c r="IV76" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="IW76" t="n">
+      <c r="IW76" s="1" t="n">
         <v>36</v>
+      </c>
+      <c r="IX76" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="IY76" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="77" ht="13.8" customHeight="1" s="2">
@@ -60127,8 +60583,14 @@
       <c r="IV77" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="IW77" t="n">
+      <c r="IW77" s="1" t="n">
         <v>74</v>
+      </c>
+      <c r="IX77" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="IY77" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="78" ht="13.8" customHeight="1" s="2">
@@ -60902,8 +61364,14 @@
       <c r="IV78" s="1" t="n">
         <v>1.96</v>
       </c>
-      <c r="IW78" t="n">
+      <c r="IW78" s="1" t="n">
         <v>2.39</v>
+      </c>
+      <c r="IX78" s="1" t="n">
+        <v>2.59</v>
+      </c>
+      <c r="IY78" t="n">
+        <v>2.25</v>
       </c>
     </row>
     <row r="79" ht="13.8" customHeight="1" s="2">
@@ -61677,8 +62145,14 @@
       <c r="IV79" s="1" t="n">
         <v>3.24</v>
       </c>
-      <c r="IW79" t="n">
+      <c r="IW79" s="1" t="n">
         <v>4.35</v>
+      </c>
+      <c r="IX79" s="1" t="n">
+        <v>3.56</v>
+      </c>
+      <c r="IY79" t="n">
+        <v>3.21</v>
       </c>
     </row>
     <row r="80" ht="13.8" customHeight="1" s="2">
@@ -62452,8 +62926,14 @@
       <c r="IV80" s="1" t="n">
         <v>45.5</v>
       </c>
-      <c r="IW80" t="n">
+      <c r="IW80" s="1" t="n">
         <v>40.5</v>
+      </c>
+      <c r="IX80" s="1" t="n">
+        <v>38.6</v>
+      </c>
+      <c r="IY80" t="n">
+        <v>37.8</v>
       </c>
     </row>
     <row r="81" ht="13.8" customHeight="1" s="2">
@@ -63227,8 +63707,14 @@
       <c r="IV81" s="1" t="n">
         <v>30.9</v>
       </c>
-      <c r="IW81" t="n">
+      <c r="IW81" s="1" t="n">
         <v>23</v>
+      </c>
+      <c r="IX81" s="1" t="n">
+        <v>28.1</v>
+      </c>
+      <c r="IY81" t="n">
+        <v>31.1</v>
       </c>
     </row>
     <row r="82" ht="13.8" customHeight="1" s="2">
@@ -64002,8 +64488,14 @@
       <c r="IV82" s="1" t="n">
         <v>189.5</v>
       </c>
-      <c r="IW82" t="n">
+      <c r="IW82" s="1" t="n">
         <v>188</v>
+      </c>
+      <c r="IX82" s="1" t="n">
+        <v>188.2</v>
+      </c>
+      <c r="IY82" t="n">
+        <v>188.2</v>
       </c>
     </row>
     <row r="83" ht="13.8" customHeight="1" s="2">
@@ -64777,8 +65269,14 @@
       <c r="IV83" s="1" t="n">
         <v>89.09999999999999</v>
       </c>
-      <c r="IW83" t="n">
+      <c r="IW83" s="1" t="n">
         <v>86.90000000000001</v>
+      </c>
+      <c r="IX83" s="1" t="n">
+        <v>88.5</v>
+      </c>
+      <c r="IY83" t="n">
+        <v>85.8</v>
       </c>
     </row>
     <row r="84" ht="13.8" customHeight="1" s="2">
@@ -65552,8 +66050,14 @@
       <c r="IV84" s="1" t="n">
         <v>25.41</v>
       </c>
-      <c r="IW84" t="n">
+      <c r="IW84" s="1" t="n">
         <v>24.66</v>
+      </c>
+      <c r="IX84" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="IY84" t="n">
+        <v>25.74</v>
       </c>
     </row>
     <row r="85" ht="13.8" customHeight="1" s="2">
@@ -66327,8 +66831,14 @@
       <c r="IV85" s="1" t="n">
         <v>91.09999999999999</v>
       </c>
-      <c r="IW85" t="n">
+      <c r="IW85" s="1" t="n">
         <v>76.7</v>
+      </c>
+      <c r="IX85" s="1" t="n">
+        <v>103.6</v>
+      </c>
+      <c r="IY85" t="n">
+        <v>95.59999999999999</v>
       </c>
     </row>
     <row r="86" ht="13.8" customHeight="1" s="2">
@@ -67102,8 +67612,14 @@
       <c r="IV86" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="IW86" t="n">
+      <c r="IW86" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="IX86" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="IY86" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="87" ht="13.8" customHeight="1" s="2">
@@ -67877,8 +68393,14 @@
       <c r="IV87" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="IW87" t="n">
+      <c r="IW87" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="IX87" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="IY87" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="88" ht="13.8" customHeight="1" s="2">
@@ -68652,8 +69174,14 @@
       <c r="IV88" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="IW88" t="n">
+      <c r="IW88" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="IX88" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="IY88" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="89" ht="13.8" customHeight="1" s="2">
@@ -69427,8 +69955,14 @@
       <c r="IV89" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="IW89" t="n">
+      <c r="IW89" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="IX89" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="IY89" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="90" ht="13.8" customHeight="1" s="2">
@@ -70202,8 +70736,14 @@
       <c r="IV90" s="1" t="n">
         <v>152</v>
       </c>
-      <c r="IW90" t="n">
+      <c r="IW90" s="1" t="n">
         <v>142</v>
+      </c>
+      <c r="IX90" s="1" t="n">
+        <v>162</v>
+      </c>
+      <c r="IY90" t="n">
+        <v>127</v>
       </c>
     </row>
     <row r="91" ht="13.8" customHeight="1" s="2">
@@ -70977,8 +71517,14 @@
       <c r="IV91" s="1" t="n">
         <v>253</v>
       </c>
-      <c r="IW91" t="n">
+      <c r="IW91" s="1" t="n">
         <v>243</v>
+      </c>
+      <c r="IX91" s="1" t="n">
+        <v>167</v>
+      </c>
+      <c r="IY91" t="n">
+        <v>215</v>
       </c>
     </row>
     <row r="92" ht="13.8" customHeight="1" s="2">
@@ -71752,8 +72298,14 @@
       <c r="IV92" s="1" t="n">
         <v>306</v>
       </c>
-      <c r="IW92" t="n">
+      <c r="IW92" s="1" t="n">
         <v>294</v>
+      </c>
+      <c r="IX92" s="1" t="n">
+        <v>237</v>
+      </c>
+      <c r="IY92" t="n">
+        <v>268</v>
       </c>
     </row>
     <row r="93" ht="13.8" customHeight="1" s="2">
@@ -72527,8 +73079,14 @@
       <c r="IV93" s="1" t="n">
         <v>75.7</v>
       </c>
-      <c r="IW93" t="n">
+      <c r="IW93" s="1" t="n">
         <v>75.8</v>
+      </c>
+      <c r="IX93" s="1" t="n">
+        <v>69.09999999999999</v>
+      </c>
+      <c r="IY93" t="n">
+        <v>76.59999999999999</v>
       </c>
     </row>
     <row r="94" ht="13.8" customHeight="1" s="2">
@@ -73302,8 +73860,14 @@
       <c r="IV94" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="IW94" t="n">
+      <c r="IW94" s="1" t="n">
         <v>59</v>
+      </c>
+      <c r="IX94" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="IY94" t="n">
+        <v>73</v>
       </c>
     </row>
     <row r="95" ht="13.8" customHeight="1" s="2">
@@ -74077,8 +74641,14 @@
       <c r="IV95" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="IW95" t="n">
+      <c r="IW95" s="1" t="n">
         <v>12</v>
+      </c>
+      <c r="IX95" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="IY95" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="96" ht="13.8" customHeight="1" s="2">
@@ -74852,8 +75422,14 @@
       <c r="IV96" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="IW96" t="n">
+      <c r="IW96" s="1" t="n">
         <v>11</v>
+      </c>
+      <c r="IX96" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="IY96" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="97" ht="13.8" customHeight="1" s="2">
@@ -75627,8 +76203,14 @@
       <c r="IV97" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="IW97" t="n">
+      <c r="IW97" s="1" t="n">
         <v>42</v>
+      </c>
+      <c r="IX97" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="IY97" t="n">
+        <v>29</v>
       </c>
     </row>
     <row r="98" ht="13.8" customHeight="1" s="2">
@@ -76402,8 +76984,14 @@
       <c r="IV98" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="IW98" t="n">
+      <c r="IW98" s="1" t="n">
         <v>36</v>
+      </c>
+      <c r="IX98" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="IY98" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="99" ht="13.8" customHeight="1" s="2">
@@ -77177,8 +77765,14 @@
       <c r="IV99" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="IW99" t="n">
+      <c r="IW99" s="1" t="n">
         <v>45</v>
+      </c>
+      <c r="IX99" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="IY99" t="n">
+        <v>61</v>
       </c>
     </row>
     <row r="100" ht="13.8" customHeight="1" s="2">
@@ -77952,8 +78546,14 @@
       <c r="IV100" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="IW100" t="n">
+      <c r="IW100" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="IX100" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="IY100" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="101" ht="13.8" customHeight="1" s="2">
@@ -78727,7 +79327,13 @@
       <c r="IV101" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="IW101" t="n">
+      <c r="IW101" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="IX101" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="IY101" t="n">
         <v>11</v>
       </c>
     </row>
@@ -79502,8 +80108,14 @@
       <c r="IV102" s="1" t="n">
         <v>88.2</v>
       </c>
-      <c r="IW102" t="n">
+      <c r="IW102" s="1" t="n">
         <v>64.7</v>
+      </c>
+      <c r="IX102" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="IY102" t="n">
+        <v>78.59999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
home and away season complete. Predictions for first finals. new model optimised.
</commit_message>
<xml_diff>
--- a/django_AFL_ML/Data/Adelaide_stats.xlsx
+++ b/django_AFL_ML/Data/Adelaide_stats.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:JE102"/>
+  <dimension ref="A1:JP102"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="GZ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="HA23" activeCellId="0" sqref="HA23"/>
@@ -1251,8 +1251,41 @@
       <c r="JD1" s="1" t="n">
         <v>10677</v>
       </c>
-      <c r="JE1" t="n">
+      <c r="JE1" s="1" t="n">
         <v>10683</v>
+      </c>
+      <c r="JF1" s="1" t="n">
+        <v>10694</v>
+      </c>
+      <c r="JG1" s="1" t="n">
+        <v>10694</v>
+      </c>
+      <c r="JH1" s="1" t="n">
+        <v>10694</v>
+      </c>
+      <c r="JI1" s="1" t="n">
+        <v>10694</v>
+      </c>
+      <c r="JJ1" s="1" t="n">
+        <v>10694</v>
+      </c>
+      <c r="JK1" s="1" t="n">
+        <v>10694</v>
+      </c>
+      <c r="JL1" s="1" t="n">
+        <v>10702</v>
+      </c>
+      <c r="JM1" s="1" t="n">
+        <v>10713</v>
+      </c>
+      <c r="JN1" s="1" t="n">
+        <v>10723</v>
+      </c>
+      <c r="JO1" s="1" t="n">
+        <v>10731</v>
+      </c>
+      <c r="JP1" t="n">
+        <v>10741</v>
       </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="2">
@@ -2050,7 +2083,40 @@
       <c r="JD2" s="1" t="n">
         <v>2022</v>
       </c>
-      <c r="JE2" t="n">
+      <c r="JE2" s="1" t="n">
+        <v>2022</v>
+      </c>
+      <c r="JF2" s="1" t="n">
+        <v>2022</v>
+      </c>
+      <c r="JG2" s="1" t="n">
+        <v>2022</v>
+      </c>
+      <c r="JH2" s="1" t="n">
+        <v>2022</v>
+      </c>
+      <c r="JI2" s="1" t="n">
+        <v>2022</v>
+      </c>
+      <c r="JJ2" s="1" t="n">
+        <v>2022</v>
+      </c>
+      <c r="JK2" s="1" t="n">
+        <v>2022</v>
+      </c>
+      <c r="JL2" s="1" t="n">
+        <v>2022</v>
+      </c>
+      <c r="JM2" s="1" t="n">
+        <v>2022</v>
+      </c>
+      <c r="JN2" s="1" t="n">
+        <v>2022</v>
+      </c>
+      <c r="JO2" s="1" t="n">
+        <v>2022</v>
+      </c>
+      <c r="JP2" t="n">
         <v>2022</v>
       </c>
     </row>
@@ -2849,8 +2915,41 @@
       <c r="JD3" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="JE3" t="n">
+      <c r="JE3" s="1" t="n">
         <v>17</v>
+      </c>
+      <c r="JF3" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="JG3" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="JH3" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="JI3" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="JJ3" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="JK3" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="JL3" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="JM3" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="JN3" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="JO3" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="JP3" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="2">
@@ -3648,7 +3747,40 @@
       <c r="JD4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="JE4" t="n">
+      <c r="JE4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JF4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JG4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JH4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JI4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JJ4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JK4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JL4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JM4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JN4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JO4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JP4" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4447,7 +4579,40 @@
       <c r="JD5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="JE5" t="n">
+      <c r="JE5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JF5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JG5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JH5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JI5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JJ5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JK5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JL5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JM5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JN5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JO5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JP5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5246,8 +5411,41 @@
       <c r="JD6" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="JE6" t="n">
+      <c r="JE6" s="1" t="n">
         <v>54</v>
+      </c>
+      <c r="JF6" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="JG6" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="JH6" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="JI6" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="JJ6" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="JK6" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="JL6" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="JM6" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="JN6" s="1" t="n">
+        <v>102</v>
+      </c>
+      <c r="JO6" s="1" t="n">
+        <v>103</v>
+      </c>
+      <c r="JP6" t="n">
+        <v>55</v>
       </c>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="2">
@@ -6045,8 +6243,41 @@
       <c r="JD7" s="1" t="n">
         <v>94</v>
       </c>
-      <c r="JE7" t="n">
+      <c r="JE7" s="1" t="n">
         <v>86</v>
+      </c>
+      <c r="JF7" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="JG7" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="JH7" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="JI7" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="JJ7" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="JK7" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="JL7" s="1" t="n">
+        <v>118</v>
+      </c>
+      <c r="JM7" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="JN7" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="JO7" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="JP7" t="n">
+        <v>111</v>
       </c>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="2">
@@ -6844,8 +7075,41 @@
       <c r="JD8" s="1" t="n">
         <v>-29</v>
       </c>
-      <c r="JE8" t="n">
+      <c r="JE8" s="1" t="n">
         <v>-32</v>
+      </c>
+      <c r="JF8" s="1" t="n">
+        <v>-5</v>
+      </c>
+      <c r="JG8" s="1" t="n">
+        <v>-5</v>
+      </c>
+      <c r="JH8" s="1" t="n">
+        <v>-5</v>
+      </c>
+      <c r="JI8" s="1" t="n">
+        <v>-5</v>
+      </c>
+      <c r="JJ8" s="1" t="n">
+        <v>-5</v>
+      </c>
+      <c r="JK8" s="1" t="n">
+        <v>-5</v>
+      </c>
+      <c r="JL8" s="1" t="n">
+        <v>-33</v>
+      </c>
+      <c r="JM8" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="JN8" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="JO8" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="JP8" t="n">
+        <v>-56</v>
       </c>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="2">
@@ -7643,7 +7907,40 @@
       <c r="JD9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="JE9" t="n">
+      <c r="JE9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JF9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JG9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JH9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JI9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JJ9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JK9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JL9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JM9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JN9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JO9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JP9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8442,8 +8739,41 @@
       <c r="JD10" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="JE10" t="n">
+      <c r="JE10" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="JF10" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="JG10" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="JH10" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="JI10" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="JJ10" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="JK10" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="JL10" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="JM10" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="JN10" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="JO10" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="JP10" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="11" ht="13.8" customHeight="1" s="2">
@@ -9241,8 +9571,41 @@
       <c r="JD11" s="1" t="n">
         <v>198</v>
       </c>
-      <c r="JE11" t="n">
+      <c r="JE11" s="1" t="n">
         <v>196</v>
+      </c>
+      <c r="JF11" s="1" t="n">
+        <v>192</v>
+      </c>
+      <c r="JG11" s="1" t="n">
+        <v>192</v>
+      </c>
+      <c r="JH11" s="1" t="n">
+        <v>192</v>
+      </c>
+      <c r="JI11" s="1" t="n">
+        <v>192</v>
+      </c>
+      <c r="JJ11" s="1" t="n">
+        <v>192</v>
+      </c>
+      <c r="JK11" s="1" t="n">
+        <v>192</v>
+      </c>
+      <c r="JL11" s="1" t="n">
+        <v>180</v>
+      </c>
+      <c r="JM11" s="1" t="n">
+        <v>207</v>
+      </c>
+      <c r="JN11" s="1" t="n">
+        <v>165</v>
+      </c>
+      <c r="JO11" s="1" t="n">
+        <v>212</v>
+      </c>
+      <c r="JP11" t="n">
+        <v>166</v>
       </c>
     </row>
     <row r="12" ht="13.8" customHeight="1" s="2">
@@ -10040,8 +10403,41 @@
       <c r="JD12" s="1" t="n">
         <v>144</v>
       </c>
-      <c r="JE12" t="n">
+      <c r="JE12" s="1" t="n">
         <v>179</v>
+      </c>
+      <c r="JF12" s="1" t="n">
+        <v>125</v>
+      </c>
+      <c r="JG12" s="1" t="n">
+        <v>125</v>
+      </c>
+      <c r="JH12" s="1" t="n">
+        <v>125</v>
+      </c>
+      <c r="JI12" s="1" t="n">
+        <v>125</v>
+      </c>
+      <c r="JJ12" s="1" t="n">
+        <v>125</v>
+      </c>
+      <c r="JK12" s="1" t="n">
+        <v>125</v>
+      </c>
+      <c r="JL12" s="1" t="n">
+        <v>130</v>
+      </c>
+      <c r="JM12" s="1" t="n">
+        <v>166</v>
+      </c>
+      <c r="JN12" s="1" t="n">
+        <v>123</v>
+      </c>
+      <c r="JO12" s="1" t="n">
+        <v>137</v>
+      </c>
+      <c r="JP12" t="n">
+        <v>121</v>
       </c>
     </row>
     <row r="13" ht="13.8" customHeight="1" s="2">
@@ -10839,8 +11235,41 @@
       <c r="JD13" s="1" t="n">
         <v>342</v>
       </c>
-      <c r="JE13" t="n">
+      <c r="JE13" s="1" t="n">
         <v>375</v>
+      </c>
+      <c r="JF13" s="1" t="n">
+        <v>317</v>
+      </c>
+      <c r="JG13" s="1" t="n">
+        <v>317</v>
+      </c>
+      <c r="JH13" s="1" t="n">
+        <v>317</v>
+      </c>
+      <c r="JI13" s="1" t="n">
+        <v>317</v>
+      </c>
+      <c r="JJ13" s="1" t="n">
+        <v>317</v>
+      </c>
+      <c r="JK13" s="1" t="n">
+        <v>317</v>
+      </c>
+      <c r="JL13" s="1" t="n">
+        <v>310</v>
+      </c>
+      <c r="JM13" s="1" t="n">
+        <v>373</v>
+      </c>
+      <c r="JN13" s="1" t="n">
+        <v>288</v>
+      </c>
+      <c r="JO13" s="1" t="n">
+        <v>349</v>
+      </c>
+      <c r="JP13" t="n">
+        <v>287</v>
       </c>
     </row>
     <row r="14" ht="13.8" customHeight="1" s="2">
@@ -11638,8 +12067,41 @@
       <c r="JD14" s="1" t="n">
         <v>1.38</v>
       </c>
-      <c r="JE14" t="n">
+      <c r="JE14" s="1" t="n">
         <v>1.09</v>
+      </c>
+      <c r="JF14" s="1" t="n">
+        <v>1.54</v>
+      </c>
+      <c r="JG14" s="1" t="n">
+        <v>1.54</v>
+      </c>
+      <c r="JH14" s="1" t="n">
+        <v>1.54</v>
+      </c>
+      <c r="JI14" s="1" t="n">
+        <v>1.54</v>
+      </c>
+      <c r="JJ14" s="1" t="n">
+        <v>1.54</v>
+      </c>
+      <c r="JK14" s="1" t="n">
+        <v>1.54</v>
+      </c>
+      <c r="JL14" s="1" t="n">
+        <v>1.38</v>
+      </c>
+      <c r="JM14" s="1" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="JN14" s="1" t="n">
+        <v>1.34</v>
+      </c>
+      <c r="JO14" s="1" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="JP14" t="n">
+        <v>1.37</v>
       </c>
     </row>
     <row r="15" ht="13.8" customHeight="1" s="2">
@@ -12437,8 +12899,41 @@
       <c r="JD15" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="JE15" t="n">
+      <c r="JE15" s="1" t="n">
         <v>89</v>
+      </c>
+      <c r="JF15" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="JG15" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="JH15" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="JI15" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="JJ15" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="JK15" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="JL15" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="JM15" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="JN15" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="JO15" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="JP15" t="n">
+        <v>48</v>
       </c>
     </row>
     <row r="16" ht="13.8" customHeight="1" s="2">
@@ -13236,8 +13731,41 @@
       <c r="JD16" s="1" t="n">
         <v>76</v>
       </c>
-      <c r="JE16" t="n">
+      <c r="JE16" s="1" t="n">
         <v>72</v>
+      </c>
+      <c r="JF16" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="JG16" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="JH16" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="JI16" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="JJ16" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="JK16" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="JL16" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="JM16" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="JN16" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="JO16" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="JP16" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="17" ht="13.8" customHeight="1" s="2">
@@ -14035,8 +14563,41 @@
       <c r="JD17" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="JE17" t="n">
+      <c r="JE17" s="1" t="n">
         <v>41</v>
+      </c>
+      <c r="JF17" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="JG17" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="JH17" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="JI17" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="JJ17" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="JK17" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="JL17" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="JM17" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="JN17" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="JO17" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="JP17" t="n">
+        <v>59</v>
       </c>
     </row>
     <row r="18" ht="13.8" customHeight="1" s="2">
@@ -14834,8 +15395,41 @@
       <c r="JD18" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="JE18" t="n">
+      <c r="JE18" s="1" t="n">
         <v>15</v>
+      </c>
+      <c r="JF18" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="JG18" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="JH18" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="JI18" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="JJ18" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="JK18" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="JL18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="JM18" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="JN18" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="JO18" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="JP18" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="19" ht="13.8" customHeight="1" s="2">
@@ -15633,8 +16227,41 @@
       <c r="JD19" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="JE19" t="n">
+      <c r="JE19" s="1" t="n">
         <v>27</v>
+      </c>
+      <c r="JF19" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="JG19" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="JH19" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="JI19" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="JJ19" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="JK19" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="JL19" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="JM19" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="JN19" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="JO19" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="JP19" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="20" ht="13.8" customHeight="1" s="2">
@@ -16432,8 +17059,41 @@
       <c r="JD20" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="JE20" t="n">
+      <c r="JE20" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="JF20" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="JG20" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="JH20" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="JI20" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="JJ20" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="JK20" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="JL20" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="JM20" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="JN20" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="JO20" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="JP20" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="21" ht="13.8" customHeight="1" s="2">
@@ -17231,7 +17891,40 @@
       <c r="JD21" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="JE21" t="n">
+      <c r="JE21" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="JF21" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JG21" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JH21" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JI21" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JJ21" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JK21" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JL21" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JM21" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="JN21" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="JO21" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="JP21" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18030,8 +18723,41 @@
       <c r="JD22" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="JE22" t="n">
+      <c r="JE22" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="JF22" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JG22" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JH22" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JI22" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JJ22" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JK22" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JL22" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="JM22" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="JN22" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="JO22" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="JP22" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="23" ht="13.8" customHeight="1" s="2">
@@ -18829,8 +19555,41 @@
       <c r="JD23" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="JE23" t="n">
+      <c r="JE23" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="JF23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JG23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JH23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JI23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JJ23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JK23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JL23" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="JM23" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="JN23" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="JO23" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="JP23" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="24" ht="13.8" customHeight="1" s="2">
@@ -19628,8 +20387,41 @@
       <c r="JD24" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="JE24" t="n">
+      <c r="JE24" s="1" t="n">
         <v>14</v>
+      </c>
+      <c r="JF24" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="JG24" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="JH24" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="JI24" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="JJ24" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="JK24" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="JL24" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="JM24" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="JN24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="JO24" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="JP24" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="25" ht="13.8" customHeight="1" s="2">
@@ -20427,8 +21219,41 @@
       <c r="JD25" s="1" t="n">
         <v>66.7</v>
       </c>
-      <c r="JE25" t="n">
+      <c r="JE25" s="1" t="n">
         <v>57.1</v>
+      </c>
+      <c r="JF25" s="1" t="n">
+        <v>61.9</v>
+      </c>
+      <c r="JG25" s="1" t="n">
+        <v>61.9</v>
+      </c>
+      <c r="JH25" s="1" t="n">
+        <v>61.9</v>
+      </c>
+      <c r="JI25" s="1" t="n">
+        <v>61.9</v>
+      </c>
+      <c r="JJ25" s="1" t="n">
+        <v>61.9</v>
+      </c>
+      <c r="JK25" s="1" t="n">
+        <v>61.9</v>
+      </c>
+      <c r="JL25" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="JM25" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="JN25" s="1" t="n">
+        <v>72.7</v>
+      </c>
+      <c r="JO25" s="1" t="n">
+        <v>53.6</v>
+      </c>
+      <c r="JP25" t="n">
+        <v>35</v>
       </c>
     </row>
     <row r="26" ht="13.8" customHeight="1" s="2">
@@ -21226,8 +22051,41 @@
       <c r="JD26" s="1" t="n">
         <v>34.2</v>
       </c>
-      <c r="JE26" t="n">
+      <c r="JE26" s="1" t="n">
         <v>46.88</v>
+      </c>
+      <c r="JF26" s="1" t="n">
+        <v>24.38</v>
+      </c>
+      <c r="JG26" s="1" t="n">
+        <v>24.38</v>
+      </c>
+      <c r="JH26" s="1" t="n">
+        <v>24.38</v>
+      </c>
+      <c r="JI26" s="1" t="n">
+        <v>24.38</v>
+      </c>
+      <c r="JJ26" s="1" t="n">
+        <v>24.38</v>
+      </c>
+      <c r="JK26" s="1" t="n">
+        <v>24.38</v>
+      </c>
+      <c r="JL26" s="1" t="n">
+        <v>25.83</v>
+      </c>
+      <c r="JM26" s="1" t="n">
+        <v>31.08</v>
+      </c>
+      <c r="JN26" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="JO26" s="1" t="n">
+        <v>23.27</v>
+      </c>
+      <c r="JP26" t="n">
+        <v>41</v>
       </c>
     </row>
     <row r="27" ht="13.8" customHeight="1" s="2">
@@ -22025,8 +22883,41 @@
       <c r="JD27" s="1" t="n">
         <v>22.8</v>
       </c>
-      <c r="JE27" t="n">
+      <c r="JE27" s="1" t="n">
         <v>26.79</v>
+      </c>
+      <c r="JF27" s="1" t="n">
+        <v>15.1</v>
+      </c>
+      <c r="JG27" s="1" t="n">
+        <v>15.1</v>
+      </c>
+      <c r="JH27" s="1" t="n">
+        <v>15.1</v>
+      </c>
+      <c r="JI27" s="1" t="n">
+        <v>15.1</v>
+      </c>
+      <c r="JJ27" s="1" t="n">
+        <v>15.1</v>
+      </c>
+      <c r="JK27" s="1" t="n">
+        <v>15.1</v>
+      </c>
+      <c r="JL27" s="1" t="n">
+        <v>12.4</v>
+      </c>
+      <c r="JM27" s="1" t="n">
+        <v>15.54</v>
+      </c>
+      <c r="JN27" s="1" t="n">
+        <v>13.09</v>
+      </c>
+      <c r="JO27" s="1" t="n">
+        <v>12.46</v>
+      </c>
+      <c r="JP27" t="n">
+        <v>14.35</v>
       </c>
     </row>
     <row r="28" ht="13.8" customHeight="1" s="2">
@@ -22824,8 +23715,41 @@
       <c r="JD28" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="JE28" t="n">
+      <c r="JE28" s="1" t="n">
         <v>43</v>
+      </c>
+      <c r="JF28" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="JG28" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="JH28" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="JI28" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="JJ28" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="JK28" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="JL28" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="JM28" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="JN28" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="JO28" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="JP28" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="29" ht="13.8" customHeight="1" s="2">
@@ -23623,8 +24547,41 @@
       <c r="JD29" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="JE29" t="n">
+      <c r="JE29" s="1" t="n">
         <v>71</v>
+      </c>
+      <c r="JF29" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="JG29" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="JH29" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="JI29" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="JJ29" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="JK29" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="JL29" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="JM29" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="JN29" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="JO29" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="JP29" t="n">
+        <v>65</v>
       </c>
     </row>
     <row r="30" ht="13.8" customHeight="1" s="2">
@@ -24422,8 +25379,41 @@
       <c r="JD30" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="JE30" t="n">
+      <c r="JE30" s="1" t="n">
         <v>40</v>
+      </c>
+      <c r="JF30" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="JG30" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="JH30" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="JI30" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="JJ30" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="JK30" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="JL30" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="JM30" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="JN30" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="JO30" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="JP30" t="n">
+        <v>42</v>
       </c>
     </row>
     <row r="31" ht="13.8" customHeight="1" s="2">
@@ -25221,8 +26211,41 @@
       <c r="JD31" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="JE31" t="n">
+      <c r="JE31" s="1" t="n">
         <v>44</v>
+      </c>
+      <c r="JF31" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="JG31" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="JH31" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="JI31" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="JJ31" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="JK31" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="JL31" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="JM31" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="JN31" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="JO31" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="JP31" t="n">
+        <v>48</v>
       </c>
     </row>
     <row r="32" ht="13.8" customHeight="1" s="2">
@@ -26020,8 +27043,41 @@
       <c r="JD32" s="1" t="n">
         <v>3.07</v>
       </c>
-      <c r="JE32" t="n">
+      <c r="JE32" s="1" t="n">
         <v>3.14</v>
+      </c>
+      <c r="JF32" s="1" t="n">
+        <v>2.33</v>
+      </c>
+      <c r="JG32" s="1" t="n">
+        <v>2.33</v>
+      </c>
+      <c r="JH32" s="1" t="n">
+        <v>2.33</v>
+      </c>
+      <c r="JI32" s="1" t="n">
+        <v>2.33</v>
+      </c>
+      <c r="JJ32" s="1" t="n">
+        <v>2.33</v>
+      </c>
+      <c r="JK32" s="1" t="n">
+        <v>2.33</v>
+      </c>
+      <c r="JL32" s="1" t="n">
+        <v>2.32</v>
+      </c>
+      <c r="JM32" s="1" t="n">
+        <v>2.71</v>
+      </c>
+      <c r="JN32" s="1" t="n">
+        <v>2.18</v>
+      </c>
+      <c r="JO32" s="1" t="n">
+        <v>1.86</v>
+      </c>
+      <c r="JP32" t="n">
+        <v>2.4</v>
       </c>
     </row>
     <row r="33" ht="13.8" customHeight="1" s="2">
@@ -26819,8 +27875,41 @@
       <c r="JD33" s="1" t="n">
         <v>4.6</v>
       </c>
-      <c r="JE33" t="n">
+      <c r="JE33" s="1" t="n">
         <v>5.5</v>
+      </c>
+      <c r="JF33" s="1" t="n">
+        <v>3.77</v>
+      </c>
+      <c r="JG33" s="1" t="n">
+        <v>3.77</v>
+      </c>
+      <c r="JH33" s="1" t="n">
+        <v>3.77</v>
+      </c>
+      <c r="JI33" s="1" t="n">
+        <v>3.77</v>
+      </c>
+      <c r="JJ33" s="1" t="n">
+        <v>3.77</v>
+      </c>
+      <c r="JK33" s="1" t="n">
+        <v>3.77</v>
+      </c>
+      <c r="JL33" s="1" t="n">
+        <v>4.83</v>
+      </c>
+      <c r="JM33" s="1" t="n">
+        <v>5.42</v>
+      </c>
+      <c r="JN33" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="JO33" s="1" t="n">
+        <v>3.47</v>
+      </c>
+      <c r="JP33" t="n">
+        <v>6.86</v>
       </c>
     </row>
     <row r="34" ht="13.8" customHeight="1" s="2">
@@ -27618,8 +28707,41 @@
       <c r="JD34" s="1" t="n">
         <v>30.4</v>
       </c>
-      <c r="JE34" t="n">
+      <c r="JE34" s="1" t="n">
         <v>25</v>
+      </c>
+      <c r="JF34" s="1" t="n">
+        <v>40.8</v>
+      </c>
+      <c r="JG34" s="1" t="n">
+        <v>40.8</v>
+      </c>
+      <c r="JH34" s="1" t="n">
+        <v>40.8</v>
+      </c>
+      <c r="JI34" s="1" t="n">
+        <v>40.8</v>
+      </c>
+      <c r="JJ34" s="1" t="n">
+        <v>40.8</v>
+      </c>
+      <c r="JK34" s="1" t="n">
+        <v>40.8</v>
+      </c>
+      <c r="JL34" s="1" t="n">
+        <v>39.7</v>
+      </c>
+      <c r="JM34" s="1" t="n">
+        <v>33.8</v>
+      </c>
+      <c r="JN34" s="1" t="n">
+        <v>41.7</v>
+      </c>
+      <c r="JO34" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="JP34" t="n">
+        <v>31.2</v>
       </c>
     </row>
     <row r="35" ht="13.8" customHeight="1" s="2">
@@ -28417,8 +29539,41 @@
       <c r="JD35" s="1" t="n">
         <v>21.7</v>
       </c>
-      <c r="JE35" t="n">
+      <c r="JE35" s="1" t="n">
         <v>18.2</v>
+      </c>
+      <c r="JF35" s="1" t="n">
+        <v>26.5</v>
+      </c>
+      <c r="JG35" s="1" t="n">
+        <v>26.5</v>
+      </c>
+      <c r="JH35" s="1" t="n">
+        <v>26.5</v>
+      </c>
+      <c r="JI35" s="1" t="n">
+        <v>26.5</v>
+      </c>
+      <c r="JJ35" s="1" t="n">
+        <v>26.5</v>
+      </c>
+      <c r="JK35" s="1" t="n">
+        <v>26.5</v>
+      </c>
+      <c r="JL35" s="1" t="n">
+        <v>20.7</v>
+      </c>
+      <c r="JM35" s="1" t="n">
+        <v>18.5</v>
+      </c>
+      <c r="JN35" s="1" t="n">
+        <v>33.3</v>
+      </c>
+      <c r="JO35" s="1" t="n">
+        <v>28.8</v>
+      </c>
+      <c r="JP35" t="n">
+        <v>14.6</v>
       </c>
     </row>
     <row r="36" ht="13.8" customHeight="1" s="2">
@@ -29216,7 +30371,40 @@
       <c r="JD36" s="1" t="n">
         <v>186.7</v>
       </c>
-      <c r="JE36" t="n">
+      <c r="JE36" s="1" t="n">
+        <v>186.9</v>
+      </c>
+      <c r="JF36" s="1" t="n">
+        <v>186.3</v>
+      </c>
+      <c r="JG36" s="1" t="n">
+        <v>186.3</v>
+      </c>
+      <c r="JH36" s="1" t="n">
+        <v>186.3</v>
+      </c>
+      <c r="JI36" s="1" t="n">
+        <v>186.3</v>
+      </c>
+      <c r="JJ36" s="1" t="n">
+        <v>186.3</v>
+      </c>
+      <c r="JK36" s="1" t="n">
+        <v>186.3</v>
+      </c>
+      <c r="JL36" s="1" t="n">
+        <v>187.1</v>
+      </c>
+      <c r="JM36" s="1" t="n">
+        <v>187.3</v>
+      </c>
+      <c r="JN36" s="1" t="n">
+        <v>187.3</v>
+      </c>
+      <c r="JO36" s="1" t="n">
+        <v>186.8</v>
+      </c>
+      <c r="JP36" t="n">
         <v>186.9</v>
       </c>
     </row>
@@ -30015,8 +31203,41 @@
       <c r="JD37" s="1" t="n">
         <v>87</v>
       </c>
-      <c r="JE37" t="n">
+      <c r="JE37" s="1" t="n">
         <v>86.90000000000001</v>
+      </c>
+      <c r="JF37" s="1" t="n">
+        <v>86.3</v>
+      </c>
+      <c r="JG37" s="1" t="n">
+        <v>86.3</v>
+      </c>
+      <c r="JH37" s="1" t="n">
+        <v>86.3</v>
+      </c>
+      <c r="JI37" s="1" t="n">
+        <v>86.3</v>
+      </c>
+      <c r="JJ37" s="1" t="n">
+        <v>86.3</v>
+      </c>
+      <c r="JK37" s="1" t="n">
+        <v>86.3</v>
+      </c>
+      <c r="JL37" s="1" t="n">
+        <v>86.7</v>
+      </c>
+      <c r="JM37" s="1" t="n">
+        <v>86.90000000000001</v>
+      </c>
+      <c r="JN37" s="1" t="n">
+        <v>86.90000000000001</v>
+      </c>
+      <c r="JO37" s="1" t="n">
+        <v>87.09999999999999</v>
+      </c>
+      <c r="JP37" t="n">
+        <v>87.3</v>
       </c>
     </row>
     <row r="38" ht="13.8" customHeight="1" s="2">
@@ -30814,8 +32035,41 @@
       <c r="JD38" s="1" t="n">
         <v>23.58</v>
       </c>
-      <c r="JE38" t="n">
+      <c r="JE38" s="1" t="n">
         <v>23.91</v>
+      </c>
+      <c r="JF38" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="JG38" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="JH38" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="JI38" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="JJ38" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="JK38" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="JL38" s="1" t="n">
+        <v>23.8</v>
+      </c>
+      <c r="JM38" s="1" t="n">
+        <v>24.8</v>
+      </c>
+      <c r="JN38" s="1" t="n">
+        <v>24.16</v>
+      </c>
+      <c r="JO38" s="1" t="n">
+        <v>24.8</v>
+      </c>
+      <c r="JP38" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="39" ht="13.8" customHeight="1" s="2">
@@ -31613,8 +32867,41 @@
       <c r="JD39" s="1" t="n">
         <v>63.7</v>
       </c>
-      <c r="JE39" t="n">
+      <c r="JE39" s="1" t="n">
         <v>68.09999999999999</v>
+      </c>
+      <c r="JF39" s="1" t="n">
+        <v>67.09999999999999</v>
+      </c>
+      <c r="JG39" s="1" t="n">
+        <v>67.09999999999999</v>
+      </c>
+      <c r="JH39" s="1" t="n">
+        <v>67.09999999999999</v>
+      </c>
+      <c r="JI39" s="1" t="n">
+        <v>67.09999999999999</v>
+      </c>
+      <c r="JJ39" s="1" t="n">
+        <v>67.09999999999999</v>
+      </c>
+      <c r="JK39" s="1" t="n">
+        <v>67.09999999999999</v>
+      </c>
+      <c r="JL39" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="JM39" s="1" t="n">
+        <v>65.5</v>
+      </c>
+      <c r="JN39" s="1" t="n">
+        <v>66.5</v>
+      </c>
+      <c r="JO39" s="1" t="n">
+        <v>66.5</v>
+      </c>
+      <c r="JP39" t="n">
+        <v>68.8</v>
       </c>
     </row>
     <row r="40" ht="13.8" customHeight="1" s="2">
@@ -32412,7 +33699,40 @@
       <c r="JD40" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="JE40" t="n">
+      <c r="JE40" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="JF40" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="JG40" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="JH40" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="JI40" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="JJ40" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="JK40" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="JL40" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="JM40" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="JN40" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="JO40" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="JP40" t="n">
         <v>12</v>
       </c>
     </row>
@@ -33211,8 +34531,41 @@
       <c r="JD41" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="JE41" t="n">
+      <c r="JE41" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="JF41" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="JG41" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="JH41" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="JI41" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="JJ41" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="JK41" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="JL41" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="JM41" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JN41" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JO41" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JP41" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="42" ht="13.8" customHeight="1" s="2">
@@ -34010,8 +35363,41 @@
       <c r="JD42" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="JE42" t="n">
+      <c r="JE42" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="JF42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JG42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JH42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JI42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JJ42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JK42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JL42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JM42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JN42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JO42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="JP42" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="43" ht="13.8" customHeight="1" s="2">
@@ -34809,7 +36195,40 @@
       <c r="JD43" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="JE43" t="n">
+      <c r="JE43" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="JF43" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="JG43" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="JH43" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="JI43" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="JJ43" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="JK43" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="JL43" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="JM43" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="JN43" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="JO43" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="JP43" t="n">
         <v>3</v>
       </c>
     </row>
@@ -35608,8 +37027,41 @@
       <c r="JD44" s="1" t="n">
         <v>141</v>
       </c>
-      <c r="JE44" t="n">
+      <c r="JE44" s="1" t="n">
         <v>133</v>
+      </c>
+      <c r="JF44" s="1" t="n">
+        <v>159</v>
+      </c>
+      <c r="JG44" s="1" t="n">
+        <v>159</v>
+      </c>
+      <c r="JH44" s="1" t="n">
+        <v>159</v>
+      </c>
+      <c r="JI44" s="1" t="n">
+        <v>159</v>
+      </c>
+      <c r="JJ44" s="1" t="n">
+        <v>159</v>
+      </c>
+      <c r="JK44" s="1" t="n">
+        <v>159</v>
+      </c>
+      <c r="JL44" s="1" t="n">
+        <v>158</v>
+      </c>
+      <c r="JM44" s="1" t="n">
+        <v>155</v>
+      </c>
+      <c r="JN44" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="JO44" s="1" t="n">
+        <v>127</v>
+      </c>
+      <c r="JP44" t="n">
+        <v>146</v>
       </c>
     </row>
     <row r="45" ht="13.8" customHeight="1" s="2">
@@ -36407,8 +37859,41 @@
       <c r="JD45" s="1" t="n">
         <v>191</v>
       </c>
-      <c r="JE45" t="n">
+      <c r="JE45" s="1" t="n">
         <v>242</v>
+      </c>
+      <c r="JF45" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="JG45" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="JH45" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="JI45" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="JJ45" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="JK45" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="JL45" s="1" t="n">
+        <v>142</v>
+      </c>
+      <c r="JM45" s="1" t="n">
+        <v>205</v>
+      </c>
+      <c r="JN45" s="1" t="n">
+        <v>159</v>
+      </c>
+      <c r="JO45" s="1" t="n">
+        <v>213</v>
+      </c>
+      <c r="JP45" t="n">
+        <v>129</v>
       </c>
     </row>
     <row r="46" ht="13.8" customHeight="1" s="2">
@@ -37206,8 +38691,41 @@
       <c r="JD46" s="1" t="n">
         <v>245</v>
       </c>
-      <c r="JE46" t="n">
+      <c r="JE46" s="1" t="n">
         <v>290</v>
+      </c>
+      <c r="JF46" s="1" t="n">
+        <v>201</v>
+      </c>
+      <c r="JG46" s="1" t="n">
+        <v>201</v>
+      </c>
+      <c r="JH46" s="1" t="n">
+        <v>201</v>
+      </c>
+      <c r="JI46" s="1" t="n">
+        <v>201</v>
+      </c>
+      <c r="JJ46" s="1" t="n">
+        <v>201</v>
+      </c>
+      <c r="JK46" s="1" t="n">
+        <v>201</v>
+      </c>
+      <c r="JL46" s="1" t="n">
+        <v>207</v>
+      </c>
+      <c r="JM46" s="1" t="n">
+        <v>273</v>
+      </c>
+      <c r="JN46" s="1" t="n">
+        <v>196</v>
+      </c>
+      <c r="JO46" s="1" t="n">
+        <v>272</v>
+      </c>
+      <c r="JP46" t="n">
+        <v>181</v>
       </c>
     </row>
     <row r="47" ht="13.8" customHeight="1" s="2">
@@ -38005,8 +39523,41 @@
       <c r="JD47" s="1" t="n">
         <v>71.59999999999999</v>
       </c>
-      <c r="JE47" t="n">
+      <c r="JE47" s="1" t="n">
         <v>77.3</v>
+      </c>
+      <c r="JF47" s="1" t="n">
+        <v>63.4</v>
+      </c>
+      <c r="JG47" s="1" t="n">
+        <v>63.4</v>
+      </c>
+      <c r="JH47" s="1" t="n">
+        <v>63.4</v>
+      </c>
+      <c r="JI47" s="1" t="n">
+        <v>63.4</v>
+      </c>
+      <c r="JJ47" s="1" t="n">
+        <v>63.4</v>
+      </c>
+      <c r="JK47" s="1" t="n">
+        <v>63.4</v>
+      </c>
+      <c r="JL47" s="1" t="n">
+        <v>66.8</v>
+      </c>
+      <c r="JM47" s="1" t="n">
+        <v>73.2</v>
+      </c>
+      <c r="JN47" s="1" t="n">
+        <v>68.09999999999999</v>
+      </c>
+      <c r="JO47" s="1" t="n">
+        <v>77.90000000000001</v>
+      </c>
+      <c r="JP47" t="n">
+        <v>63.1</v>
       </c>
     </row>
     <row r="48" ht="13.8" customHeight="1" s="2">
@@ -38804,8 +40355,41 @@
       <c r="JD48" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="JE48" t="n">
+      <c r="JE48" s="1" t="n">
         <v>71</v>
+      </c>
+      <c r="JF48" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="JG48" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="JH48" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="JI48" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="JJ48" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="JK48" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="JL48" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="JM48" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="JN48" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="JO48" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="JP48" t="n">
+        <v>65</v>
       </c>
     </row>
     <row r="49" ht="13.8" customHeight="1" s="2">
@@ -39603,8 +41187,41 @@
       <c r="JD49" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="JE49" t="n">
+      <c r="JE49" s="1" t="n">
         <v>12</v>
+      </c>
+      <c r="JF49" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="JG49" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="JH49" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="JI49" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="JJ49" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="JK49" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="JL49" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="JM49" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="JN49" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="JO49" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="JP49" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="50" ht="13.8" customHeight="1" s="2">
@@ -40402,8 +42019,41 @@
       <c r="JD50" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="JE50" t="n">
+      <c r="JE50" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="JF50" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="JG50" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="JH50" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="JI50" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="JJ50" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="JK50" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="JL50" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="JM50" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="JN50" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="JO50" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="JP50" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="51" ht="13.8" customHeight="1" s="2">
@@ -41201,8 +42851,41 @@
       <c r="JD51" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="JE51" t="n">
+      <c r="JE51" s="1" t="n">
         <v>43</v>
+      </c>
+      <c r="JF51" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="JG51" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="JH51" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="JI51" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="JJ51" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="JK51" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="JL51" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="JM51" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="JN51" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="JO51" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="JP51" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="52" ht="13.8" customHeight="1" s="2">
@@ -42000,8 +43683,41 @@
       <c r="JD52" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="JE52" t="n">
+      <c r="JE52" s="1" t="n">
         <v>40</v>
+      </c>
+      <c r="JF52" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="JG52" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="JH52" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="JI52" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="JJ52" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="JK52" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="JL52" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="JM52" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="JN52" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="JO52" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="JP52" t="n">
+        <v>42</v>
       </c>
     </row>
     <row r="53" ht="13.8" customHeight="1" s="2">
@@ -42799,8 +44515,41 @@
       <c r="JD53" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="JE53" t="n">
+      <c r="JE53" s="1" t="n">
         <v>40</v>
+      </c>
+      <c r="JF53" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="JG53" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="JH53" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="JI53" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="JJ53" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="JK53" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="JL53" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="JM53" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="JN53" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="JO53" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="JP53" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="54" ht="13.8" customHeight="1" s="2">
@@ -43598,8 +45347,41 @@
       <c r="JD54" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="JE54" t="n">
+      <c r="JE54" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="JF54" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="JG54" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="JH54" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="JI54" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="JJ54" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="JK54" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="JL54" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JM54" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="JN54" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="JO54" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="JP54" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="55" ht="13.8" customHeight="1" s="2">
@@ -44397,7 +46179,40 @@
       <c r="JD55" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="JE55" t="n">
+      <c r="JE55" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="JF55" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JG55" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JH55" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JI55" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JJ55" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JK55" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JL55" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JM55" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="JN55" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="JO55" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="JP55" t="n">
         <v>5</v>
       </c>
     </row>
@@ -45196,8 +47011,41 @@
       <c r="JD56" s="1" t="n">
         <v>70</v>
       </c>
-      <c r="JE56" t="n">
+      <c r="JE56" s="1" t="n">
         <v>62.5</v>
+      </c>
+      <c r="JF56" s="1" t="n">
+        <v>53.8</v>
+      </c>
+      <c r="JG56" s="1" t="n">
+        <v>53.8</v>
+      </c>
+      <c r="JH56" s="1" t="n">
+        <v>53.8</v>
+      </c>
+      <c r="JI56" s="1" t="n">
+        <v>53.8</v>
+      </c>
+      <c r="JJ56" s="1" t="n">
+        <v>53.8</v>
+      </c>
+      <c r="JK56" s="1" t="n">
+        <v>53.8</v>
+      </c>
+      <c r="JL56" s="1" t="n">
+        <v>58.3</v>
+      </c>
+      <c r="JM56" s="1" t="n">
+        <v>83.3</v>
+      </c>
+      <c r="JN56" s="1" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="JO56" s="1" t="n">
+        <v>86.7</v>
+      </c>
+      <c r="JP56" t="n">
+        <v>71.40000000000001</v>
       </c>
     </row>
     <row r="57" ht="13.8" customHeight="1" s="2">
@@ -45995,8 +47843,41 @@
       <c r="JD57" s="1" t="n">
         <v>214</v>
       </c>
-      <c r="JE57" t="n">
+      <c r="JE57" s="1" t="n">
         <v>224</v>
+      </c>
+      <c r="JF57" s="1" t="n">
+        <v>228</v>
+      </c>
+      <c r="JG57" s="1" t="n">
+        <v>228</v>
+      </c>
+      <c r="JH57" s="1" t="n">
+        <v>228</v>
+      </c>
+      <c r="JI57" s="1" t="n">
+        <v>228</v>
+      </c>
+      <c r="JJ57" s="1" t="n">
+        <v>228</v>
+      </c>
+      <c r="JK57" s="1" t="n">
+        <v>228</v>
+      </c>
+      <c r="JL57" s="1" t="n">
+        <v>249</v>
+      </c>
+      <c r="JM57" s="1" t="n">
+        <v>227</v>
+      </c>
+      <c r="JN57" s="1" t="n">
+        <v>206</v>
+      </c>
+      <c r="JO57" s="1" t="n">
+        <v>203</v>
+      </c>
+      <c r="JP57" t="n">
+        <v>237</v>
       </c>
     </row>
     <row r="58" ht="13.8" customHeight="1" s="2">
@@ -46794,8 +48675,41 @@
       <c r="JD58" s="1" t="n">
         <v>155</v>
       </c>
-      <c r="JE58" t="n">
+      <c r="JE58" s="1" t="n">
         <v>155</v>
+      </c>
+      <c r="JF58" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="JG58" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="JH58" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="JI58" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="JJ58" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="JK58" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="JL58" s="1" t="n">
+        <v>157</v>
+      </c>
+      <c r="JM58" s="1" t="n">
+        <v>149</v>
+      </c>
+      <c r="JN58" s="1" t="n">
+        <v>136</v>
+      </c>
+      <c r="JO58" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="JP58" t="n">
+        <v>164</v>
       </c>
     </row>
     <row r="59" ht="13.8" customHeight="1" s="2">
@@ -47593,8 +49507,41 @@
       <c r="JD59" s="1" t="n">
         <v>369</v>
       </c>
-      <c r="JE59" t="n">
+      <c r="JE59" s="1" t="n">
         <v>379</v>
+      </c>
+      <c r="JF59" s="1" t="n">
+        <v>374</v>
+      </c>
+      <c r="JG59" s="1" t="n">
+        <v>374</v>
+      </c>
+      <c r="JH59" s="1" t="n">
+        <v>374</v>
+      </c>
+      <c r="JI59" s="1" t="n">
+        <v>374</v>
+      </c>
+      <c r="JJ59" s="1" t="n">
+        <v>374</v>
+      </c>
+      <c r="JK59" s="1" t="n">
+        <v>374</v>
+      </c>
+      <c r="JL59" s="1" t="n">
+        <v>406</v>
+      </c>
+      <c r="JM59" s="1" t="n">
+        <v>376</v>
+      </c>
+      <c r="JN59" s="1" t="n">
+        <v>342</v>
+      </c>
+      <c r="JO59" s="1" t="n">
+        <v>353</v>
+      </c>
+      <c r="JP59" t="n">
+        <v>401</v>
       </c>
     </row>
     <row r="60" ht="13.8" customHeight="1" s="2">
@@ -48392,7 +50339,40 @@
       <c r="JD60" s="1" t="n">
         <v>1.38</v>
       </c>
-      <c r="JE60" t="n">
+      <c r="JE60" s="1" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="JF60" s="1" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="JG60" s="1" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="JH60" s="1" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="JI60" s="1" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="JJ60" s="1" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="JK60" s="1" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="JL60" s="1" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="JM60" s="1" t="n">
+        <v>1.52</v>
+      </c>
+      <c r="JN60" s="1" t="n">
+        <v>1.51</v>
+      </c>
+      <c r="JO60" s="1" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="JP60" t="n">
         <v>1.45</v>
       </c>
     </row>
@@ -49191,8 +51171,41 @@
       <c r="JD61" s="1" t="n">
         <v>99</v>
       </c>
-      <c r="JE61" t="n">
+      <c r="JE61" s="1" t="n">
         <v>96</v>
+      </c>
+      <c r="JF61" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="JG61" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="JH61" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="JI61" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="JJ61" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="JK61" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="JL61" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="JM61" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="JN61" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="JO61" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="JP61" t="n">
+        <v>97</v>
       </c>
     </row>
     <row r="62" ht="13.8" customHeight="1" s="2">
@@ -49990,8 +52003,41 @@
       <c r="JD62" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="JE62" t="n">
+      <c r="JE62" s="1" t="n">
         <v>66</v>
+      </c>
+      <c r="JF62" s="1" t="n">
+        <v>126</v>
+      </c>
+      <c r="JG62" s="1" t="n">
+        <v>126</v>
+      </c>
+      <c r="JH62" s="1" t="n">
+        <v>126</v>
+      </c>
+      <c r="JI62" s="1" t="n">
+        <v>126</v>
+      </c>
+      <c r="JJ62" s="1" t="n">
+        <v>126</v>
+      </c>
+      <c r="JK62" s="1" t="n">
+        <v>126</v>
+      </c>
+      <c r="JL62" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="JM62" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="JN62" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="JO62" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="JP62" t="n">
+        <v>68</v>
       </c>
     </row>
     <row r="63" ht="13.8" customHeight="1" s="2">
@@ -50789,8 +52835,41 @@
       <c r="JD63" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="JE63" t="n">
+      <c r="JE63" s="1" t="n">
         <v>46</v>
+      </c>
+      <c r="JF63" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="JG63" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="JH63" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="JI63" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="JJ63" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="JK63" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="JL63" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="JM63" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="JN63" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="JO63" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="JP63" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="64" ht="13.8" customHeight="1" s="2">
@@ -51588,8 +53667,41 @@
       <c r="JD64" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="JE64" t="n">
+      <c r="JE64" s="1" t="n">
         <v>27</v>
+      </c>
+      <c r="JF64" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="JG64" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="JH64" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="JI64" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="JJ64" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="JK64" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="JL64" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="JM64" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="JN64" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="JO64" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="JP64" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="65" ht="13.8" customHeight="1" s="2">
@@ -52387,8 +54499,41 @@
       <c r="JD65" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="JE65" t="n">
+      <c r="JE65" s="1" t="n">
         <v>15</v>
+      </c>
+      <c r="JF65" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="JG65" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="JH65" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="JI65" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="JJ65" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="JK65" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="JL65" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="JM65" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="JN65" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="JO65" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="JP65" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="66" ht="13.8" customHeight="1" s="2">
@@ -53186,8 +55331,41 @@
       <c r="JD66" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="JE66" t="n">
+      <c r="JE66" s="1" t="n">
         <v>13</v>
+      </c>
+      <c r="JF66" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="JG66" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="JH66" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="JI66" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="JJ66" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="JK66" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="JL66" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="JM66" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="JN66" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="JO66" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="JP66" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="67" ht="13.8" customHeight="1" s="2">
@@ -53985,8 +56163,41 @@
       <c r="JD67" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="JE67" t="n">
+      <c r="JE67" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="JF67" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="JG67" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="JH67" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="JI67" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="JJ67" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="JK67" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="JL67" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="JM67" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JN67" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="JO67" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="JP67" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="68" ht="13.8" customHeight="1" s="2">
@@ -54784,8 +56995,41 @@
       <c r="JD68" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="JE68" t="n">
+      <c r="JE68" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="JF68" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="JG68" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="JH68" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="JI68" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="JJ68" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="JK68" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="JL68" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="JM68" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="JN68" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JO68" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="JP68" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="69" ht="13.8" customHeight="1" s="2">
@@ -55583,8 +57827,41 @@
       <c r="JD69" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="JE69" t="n">
+      <c r="JE69" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="JF69" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="JG69" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="JH69" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="JI69" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="JJ69" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="JK69" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="JL69" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="JM69" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JN69" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JO69" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JP69" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="70" ht="13.8" customHeight="1" s="2">
@@ -56382,8 +58659,41 @@
       <c r="JD70" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="JE70" t="n">
+      <c r="JE70" s="1" t="n">
         <v>21</v>
+      </c>
+      <c r="JF70" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="JG70" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="JH70" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="JI70" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="JJ70" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="JK70" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="JL70" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="JM70" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="JN70" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="JO70" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="JP70" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="71" ht="13.8" customHeight="1" s="2">
@@ -57181,8 +59491,41 @@
       <c r="JD71" s="1" t="n">
         <v>58.3</v>
       </c>
-      <c r="JE71" t="n">
+      <c r="JE71" s="1" t="n">
         <v>61.9</v>
+      </c>
+      <c r="JF71" s="1" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="JG71" s="1" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="JH71" s="1" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="JI71" s="1" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="JJ71" s="1" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="JK71" s="1" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="JL71" s="1" t="n">
+        <v>51.5</v>
+      </c>
+      <c r="JM71" s="1" t="n">
+        <v>53.3</v>
+      </c>
+      <c r="JN71" s="1" t="n">
+        <v>61.9</v>
+      </c>
+      <c r="JO71" s="1" t="n">
+        <v>41.7</v>
+      </c>
+      <c r="JP71" t="n">
+        <v>51.6</v>
       </c>
     </row>
     <row r="72" ht="13.8" customHeight="1" s="2">
@@ -57980,8 +60323,41 @@
       <c r="JD72" s="1" t="n">
         <v>26.36</v>
       </c>
-      <c r="JE72" t="n">
+      <c r="JE72" s="1" t="n">
         <v>29.15</v>
+      </c>
+      <c r="JF72" s="1" t="n">
+        <v>26.71</v>
+      </c>
+      <c r="JG72" s="1" t="n">
+        <v>26.71</v>
+      </c>
+      <c r="JH72" s="1" t="n">
+        <v>26.71</v>
+      </c>
+      <c r="JI72" s="1" t="n">
+        <v>26.71</v>
+      </c>
+      <c r="JJ72" s="1" t="n">
+        <v>26.71</v>
+      </c>
+      <c r="JK72" s="1" t="n">
+        <v>26.71</v>
+      </c>
+      <c r="JL72" s="1" t="n">
+        <v>23.88</v>
+      </c>
+      <c r="JM72" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="JN72" s="1" t="n">
+        <v>26.31</v>
+      </c>
+      <c r="JO72" s="1" t="n">
+        <v>35.3</v>
+      </c>
+      <c r="JP72" t="n">
+        <v>25.06</v>
       </c>
     </row>
     <row r="73" ht="13.8" customHeight="1" s="2">
@@ -58779,8 +61155,41 @@
       <c r="JD73" s="1" t="n">
         <v>15.38</v>
       </c>
-      <c r="JE73" t="n">
+      <c r="JE73" s="1" t="n">
         <v>18.05</v>
+      </c>
+      <c r="JF73" s="1" t="n">
+        <v>17.81</v>
+      </c>
+      <c r="JG73" s="1" t="n">
+        <v>17.81</v>
+      </c>
+      <c r="JH73" s="1" t="n">
+        <v>17.81</v>
+      </c>
+      <c r="JI73" s="1" t="n">
+        <v>17.81</v>
+      </c>
+      <c r="JJ73" s="1" t="n">
+        <v>17.81</v>
+      </c>
+      <c r="JK73" s="1" t="n">
+        <v>17.81</v>
+      </c>
+      <c r="JL73" s="1" t="n">
+        <v>12.3</v>
+      </c>
+      <c r="JM73" s="1" t="n">
+        <v>25.07</v>
+      </c>
+      <c r="JN73" s="1" t="n">
+        <v>16.29</v>
+      </c>
+      <c r="JO73" s="1" t="n">
+        <v>14.71</v>
+      </c>
+      <c r="JP73" t="n">
+        <v>12.94</v>
       </c>
     </row>
     <row r="74" ht="13.8" customHeight="1" s="2">
@@ -59578,8 +61987,41 @@
       <c r="JD74" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="JE74" t="n">
+      <c r="JE74" s="1" t="n">
         <v>35</v>
+      </c>
+      <c r="JF74" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="JG74" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="JH74" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="JI74" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="JJ74" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="JK74" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="JL74" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="JM74" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="JN74" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="JO74" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="JP74" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="75" ht="13.8" customHeight="1" s="2">
@@ -60377,8 +62819,41 @@
       <c r="JD75" s="1" t="n">
         <v>62</v>
       </c>
-      <c r="JE75" t="n">
+      <c r="JE75" s="1" t="n">
         <v>57</v>
+      </c>
+      <c r="JF75" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="JG75" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="JH75" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="JI75" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="JJ75" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="JK75" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="JL75" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="JM75" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="JN75" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="JO75" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="JP75" t="n">
+        <v>54</v>
       </c>
     </row>
     <row r="76" ht="13.8" customHeight="1" s="2">
@@ -61176,8 +63651,41 @@
       <c r="JD76" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="JE76" t="n">
+      <c r="JE76" s="1" t="n">
         <v>35</v>
+      </c>
+      <c r="JF76" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="JG76" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="JH76" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="JI76" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="JJ76" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="JK76" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="JL76" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="JM76" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="JN76" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="JO76" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="JP76" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="77" ht="13.8" customHeight="1" s="2">
@@ -61975,8 +64483,41 @@
       <c r="JD77" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="JE77" t="n">
+      <c r="JE77" s="1" t="n">
         <v>54</v>
+      </c>
+      <c r="JF77" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="JG77" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="JH77" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="JI77" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="JJ77" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="JK77" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="JL77" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="JM77" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="JN77" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="JO77" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="JP77" t="n">
+        <v>61</v>
       </c>
     </row>
     <row r="78" ht="13.8" customHeight="1" s="2">
@@ -62774,8 +65315,41 @@
       <c r="JD78" s="1" t="n">
         <v>2.17</v>
       </c>
-      <c r="JE78" t="n">
+      <c r="JE78" s="1" t="n">
         <v>2.57</v>
+      </c>
+      <c r="JF78" s="1" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="JG78" s="1" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="JH78" s="1" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="JI78" s="1" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="JJ78" s="1" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="JK78" s="1" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="JL78" s="1" t="n">
+        <v>1.82</v>
+      </c>
+      <c r="JM78" s="1" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="JN78" s="1" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="JO78" s="1" t="n">
+        <v>2.46</v>
+      </c>
+      <c r="JP78" t="n">
+        <v>1.97</v>
       </c>
     </row>
     <row r="79" ht="13.8" customHeight="1" s="2">
@@ -63573,8 +66147,41 @@
       <c r="JD79" s="1" t="n">
         <v>3.71</v>
       </c>
-      <c r="JE79" t="n">
+      <c r="JE79" s="1" t="n">
         <v>4.15</v>
+      </c>
+      <c r="JF79" s="1" t="n">
+        <v>4.36</v>
+      </c>
+      <c r="JG79" s="1" t="n">
+        <v>4.36</v>
+      </c>
+      <c r="JH79" s="1" t="n">
+        <v>4.36</v>
+      </c>
+      <c r="JI79" s="1" t="n">
+        <v>4.36</v>
+      </c>
+      <c r="JJ79" s="1" t="n">
+        <v>4.36</v>
+      </c>
+      <c r="JK79" s="1" t="n">
+        <v>4.36</v>
+      </c>
+      <c r="JL79" s="1" t="n">
+        <v>3.53</v>
+      </c>
+      <c r="JM79" s="1" t="n">
+        <v>5.88</v>
+      </c>
+      <c r="JN79" s="1" t="n">
+        <v>3.62</v>
+      </c>
+      <c r="JO79" s="1" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="JP79" t="n">
+        <v>3.81</v>
       </c>
     </row>
     <row r="80" ht="13.8" customHeight="1" s="2">
@@ -64372,8 +66979,41 @@
       <c r="JD80" s="1" t="n">
         <v>40.4</v>
       </c>
-      <c r="JE80" t="n">
+      <c r="JE80" s="1" t="n">
         <v>37</v>
+      </c>
+      <c r="JF80" s="1" t="n">
+        <v>31.1</v>
+      </c>
+      <c r="JG80" s="1" t="n">
+        <v>31.1</v>
+      </c>
+      <c r="JH80" s="1" t="n">
+        <v>31.1</v>
+      </c>
+      <c r="JI80" s="1" t="n">
+        <v>31.1</v>
+      </c>
+      <c r="JJ80" s="1" t="n">
+        <v>31.1</v>
+      </c>
+      <c r="JK80" s="1" t="n">
+        <v>31.1</v>
+      </c>
+      <c r="JL80" s="1" t="n">
+        <v>46.7</v>
+      </c>
+      <c r="JM80" s="1" t="n">
+        <v>29.8</v>
+      </c>
+      <c r="JN80" s="1" t="n">
+        <v>42.6</v>
+      </c>
+      <c r="JO80" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="JP80" t="n">
+        <v>42.6</v>
       </c>
     </row>
     <row r="81" ht="13.8" customHeight="1" s="2">
@@ -65171,8 +67811,41 @@
       <c r="JD81" s="1" t="n">
         <v>26.9</v>
       </c>
-      <c r="JE81" t="n">
+      <c r="JE81" s="1" t="n">
         <v>24.1</v>
+      </c>
+      <c r="JF81" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="JG81" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="JH81" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="JI81" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="JJ81" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="JK81" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="JL81" s="1" t="n">
+        <v>28.3</v>
+      </c>
+      <c r="JM81" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="JN81" s="1" t="n">
+        <v>27.7</v>
+      </c>
+      <c r="JO81" s="1" t="n">
+        <v>16.9</v>
+      </c>
+      <c r="JP81" t="n">
+        <v>26.2</v>
       </c>
     </row>
     <row r="82" ht="13.8" customHeight="1" s="2">
@@ -65970,8 +68643,41 @@
       <c r="JD82" s="1" t="n">
         <v>186.3</v>
       </c>
-      <c r="JE82" t="n">
+      <c r="JE82" s="1" t="n">
         <v>188.1</v>
+      </c>
+      <c r="JF82" s="1" t="n">
+        <v>189.5</v>
+      </c>
+      <c r="JG82" s="1" t="n">
+        <v>189.5</v>
+      </c>
+      <c r="JH82" s="1" t="n">
+        <v>189.5</v>
+      </c>
+      <c r="JI82" s="1" t="n">
+        <v>189.5</v>
+      </c>
+      <c r="JJ82" s="1" t="n">
+        <v>189.5</v>
+      </c>
+      <c r="JK82" s="1" t="n">
+        <v>189.5</v>
+      </c>
+      <c r="JL82" s="1" t="n">
+        <v>187.5</v>
+      </c>
+      <c r="JM82" s="1" t="n">
+        <v>189.3</v>
+      </c>
+      <c r="JN82" s="1" t="n">
+        <v>187.6</v>
+      </c>
+      <c r="JO82" s="1" t="n">
+        <v>189</v>
+      </c>
+      <c r="JP82" t="n">
+        <v>187.4</v>
       </c>
     </row>
     <row r="83" ht="13.8" customHeight="1" s="2">
@@ -66769,8 +69475,41 @@
       <c r="JD83" s="1" t="n">
         <v>86</v>
       </c>
-      <c r="JE83" t="n">
+      <c r="JE83" s="1" t="n">
         <v>85.59999999999999</v>
+      </c>
+      <c r="JF83" s="1" t="n">
+        <v>86.3</v>
+      </c>
+      <c r="JG83" s="1" t="n">
+        <v>86.3</v>
+      </c>
+      <c r="JH83" s="1" t="n">
+        <v>86.3</v>
+      </c>
+      <c r="JI83" s="1" t="n">
+        <v>86.3</v>
+      </c>
+      <c r="JJ83" s="1" t="n">
+        <v>86.3</v>
+      </c>
+      <c r="JK83" s="1" t="n">
+        <v>86.3</v>
+      </c>
+      <c r="JL83" s="1" t="n">
+        <v>86.5</v>
+      </c>
+      <c r="JM83" s="1" t="n">
+        <v>88.2</v>
+      </c>
+      <c r="JN83" s="1" t="n">
+        <v>85.90000000000001</v>
+      </c>
+      <c r="JO83" s="1" t="n">
+        <v>85.2</v>
+      </c>
+      <c r="JP83" t="n">
+        <v>85.40000000000001</v>
       </c>
     </row>
     <row r="84" ht="13.8" customHeight="1" s="2">
@@ -67568,8 +70307,41 @@
       <c r="JD84" s="1" t="n">
         <v>25.8</v>
       </c>
-      <c r="JE84" t="n">
+      <c r="JE84" s="1" t="n">
         <v>24.49</v>
+      </c>
+      <c r="JF84" s="1" t="n">
+        <v>25.66</v>
+      </c>
+      <c r="JG84" s="1" t="n">
+        <v>25.66</v>
+      </c>
+      <c r="JH84" s="1" t="n">
+        <v>25.66</v>
+      </c>
+      <c r="JI84" s="1" t="n">
+        <v>25.66</v>
+      </c>
+      <c r="JJ84" s="1" t="n">
+        <v>25.66</v>
+      </c>
+      <c r="JK84" s="1" t="n">
+        <v>25.66</v>
+      </c>
+      <c r="JL84" s="1" t="n">
+        <v>25.74</v>
+      </c>
+      <c r="JM84" s="1" t="n">
+        <v>24.74</v>
+      </c>
+      <c r="JN84" s="1" t="n">
+        <v>26.8</v>
+      </c>
+      <c r="JO84" s="1" t="n">
+        <v>25.24</v>
+      </c>
+      <c r="JP84" t="n">
+        <v>25.58</v>
       </c>
     </row>
     <row r="85" ht="13.8" customHeight="1" s="2">
@@ -68367,8 +71139,41 @@
       <c r="JD85" s="1" t="n">
         <v>105.3</v>
       </c>
-      <c r="JE85" t="n">
+      <c r="JE85" s="1" t="n">
         <v>81.3</v>
+      </c>
+      <c r="JF85" s="1" t="n">
+        <v>95.8</v>
+      </c>
+      <c r="JG85" s="1" t="n">
+        <v>95.8</v>
+      </c>
+      <c r="JH85" s="1" t="n">
+        <v>95.8</v>
+      </c>
+      <c r="JI85" s="1" t="n">
+        <v>95.8</v>
+      </c>
+      <c r="JJ85" s="1" t="n">
+        <v>95.8</v>
+      </c>
+      <c r="JK85" s="1" t="n">
+        <v>95.8</v>
+      </c>
+      <c r="JL85" s="1" t="n">
+        <v>109.3</v>
+      </c>
+      <c r="JM85" s="1" t="n">
+        <v>78.8</v>
+      </c>
+      <c r="JN85" s="1" t="n">
+        <v>126.6</v>
+      </c>
+      <c r="JO85" s="1" t="n">
+        <v>92.7</v>
+      </c>
+      <c r="JP85" t="n">
+        <v>112.1</v>
       </c>
     </row>
     <row r="86" ht="13.8" customHeight="1" s="2">
@@ -69166,8 +71971,41 @@
       <c r="JD86" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="JE86" t="n">
+      <c r="JE86" s="1" t="n">
         <v>13</v>
+      </c>
+      <c r="JF86" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="JG86" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="JH86" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="JI86" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="JJ86" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="JK86" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="JL86" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="JM86" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JN86" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JO86" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JP86" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="87" ht="13.8" customHeight="1" s="2">
@@ -69965,8 +72803,41 @@
       <c r="JD87" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="JE87" t="n">
+      <c r="JE87" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="JF87" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="JG87" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="JH87" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="JI87" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="JJ87" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="JK87" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="JL87" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="JM87" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="JN87" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="JO87" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="JP87" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="88" ht="13.8" customHeight="1" s="2">
@@ -70764,8 +73635,41 @@
       <c r="JD88" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="JE88" t="n">
+      <c r="JE88" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="JF88" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="JG88" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="JH88" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="JI88" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="JJ88" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="JK88" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="JL88" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="JM88" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="JN88" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="JO88" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="JP88" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="89" ht="13.8" customHeight="1" s="2">
@@ -71563,8 +74467,41 @@
       <c r="JD89" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="JE89" t="n">
+      <c r="JE89" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="JF89" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="JG89" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="JH89" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="JI89" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="JJ89" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="JK89" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="JL89" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="JM89" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JN89" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="JO89" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="JP89" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="90" ht="13.8" customHeight="1" s="2">
@@ -72362,8 +75299,41 @@
       <c r="JD90" s="1" t="n">
         <v>145</v>
       </c>
-      <c r="JE90" t="n">
+      <c r="JE90" s="1" t="n">
         <v>148</v>
+      </c>
+      <c r="JF90" s="1" t="n">
+        <v>149</v>
+      </c>
+      <c r="JG90" s="1" t="n">
+        <v>149</v>
+      </c>
+      <c r="JH90" s="1" t="n">
+        <v>149</v>
+      </c>
+      <c r="JI90" s="1" t="n">
+        <v>149</v>
+      </c>
+      <c r="JJ90" s="1" t="n">
+        <v>149</v>
+      </c>
+      <c r="JK90" s="1" t="n">
+        <v>149</v>
+      </c>
+      <c r="JL90" s="1" t="n">
+        <v>179</v>
+      </c>
+      <c r="JM90" s="1" t="n">
+        <v>141</v>
+      </c>
+      <c r="JN90" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="JO90" s="1" t="n">
+        <v>125</v>
+      </c>
+      <c r="JP90" t="n">
+        <v>146</v>
       </c>
     </row>
     <row r="91" ht="13.8" customHeight="1" s="2">
@@ -73161,8 +76131,41 @@
       <c r="JD91" s="1" t="n">
         <v>219</v>
       </c>
-      <c r="JE91" t="n">
+      <c r="JE91" s="1" t="n">
         <v>230</v>
+      </c>
+      <c r="JF91" s="1" t="n">
+        <v>181</v>
+      </c>
+      <c r="JG91" s="1" t="n">
+        <v>181</v>
+      </c>
+      <c r="JH91" s="1" t="n">
+        <v>181</v>
+      </c>
+      <c r="JI91" s="1" t="n">
+        <v>181</v>
+      </c>
+      <c r="JJ91" s="1" t="n">
+        <v>181</v>
+      </c>
+      <c r="JK91" s="1" t="n">
+        <v>181</v>
+      </c>
+      <c r="JL91" s="1" t="n">
+        <v>216</v>
+      </c>
+      <c r="JM91" s="1" t="n">
+        <v>224</v>
+      </c>
+      <c r="JN91" s="1" t="n">
+        <v>201</v>
+      </c>
+      <c r="JO91" s="1" t="n">
+        <v>221</v>
+      </c>
+      <c r="JP91" t="n">
+        <v>236</v>
       </c>
     </row>
     <row r="92" ht="13.8" customHeight="1" s="2">
@@ -73960,8 +76963,41 @@
       <c r="JD92" s="1" t="n">
         <v>262</v>
       </c>
-      <c r="JE92" t="n">
+      <c r="JE92" s="1" t="n">
         <v>277</v>
+      </c>
+      <c r="JF92" s="1" t="n">
+        <v>239</v>
+      </c>
+      <c r="JG92" s="1" t="n">
+        <v>239</v>
+      </c>
+      <c r="JH92" s="1" t="n">
+        <v>239</v>
+      </c>
+      <c r="JI92" s="1" t="n">
+        <v>239</v>
+      </c>
+      <c r="JJ92" s="1" t="n">
+        <v>239</v>
+      </c>
+      <c r="JK92" s="1" t="n">
+        <v>239</v>
+      </c>
+      <c r="JL92" s="1" t="n">
+        <v>278</v>
+      </c>
+      <c r="JM92" s="1" t="n">
+        <v>267</v>
+      </c>
+      <c r="JN92" s="1" t="n">
+        <v>246</v>
+      </c>
+      <c r="JO92" s="1" t="n">
+        <v>267</v>
+      </c>
+      <c r="JP92" t="n">
+        <v>287</v>
       </c>
     </row>
     <row r="93" ht="13.8" customHeight="1" s="2">
@@ -74759,8 +77795,41 @@
       <c r="JD93" s="1" t="n">
         <v>71</v>
       </c>
-      <c r="JE93" t="n">
+      <c r="JE93" s="1" t="n">
         <v>73.09999999999999</v>
+      </c>
+      <c r="JF93" s="1" t="n">
+        <v>63.9</v>
+      </c>
+      <c r="JG93" s="1" t="n">
+        <v>63.9</v>
+      </c>
+      <c r="JH93" s="1" t="n">
+        <v>63.9</v>
+      </c>
+      <c r="JI93" s="1" t="n">
+        <v>63.9</v>
+      </c>
+      <c r="JJ93" s="1" t="n">
+        <v>63.9</v>
+      </c>
+      <c r="JK93" s="1" t="n">
+        <v>63.9</v>
+      </c>
+      <c r="JL93" s="1" t="n">
+        <v>68.5</v>
+      </c>
+      <c r="JM93" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="JN93" s="1" t="n">
+        <v>71.90000000000001</v>
+      </c>
+      <c r="JO93" s="1" t="n">
+        <v>75.59999999999999</v>
+      </c>
+      <c r="JP93" t="n">
+        <v>71.59999999999999</v>
       </c>
     </row>
     <row r="94" ht="13.8" customHeight="1" s="2">
@@ -75558,8 +78627,41 @@
       <c r="JD94" s="1" t="n">
         <v>62</v>
       </c>
-      <c r="JE94" t="n">
+      <c r="JE94" s="1" t="n">
         <v>57</v>
+      </c>
+      <c r="JF94" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="JG94" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="JH94" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="JI94" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="JJ94" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="JK94" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="JL94" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="JM94" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="JN94" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="JO94" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="JP94" t="n">
+        <v>54</v>
       </c>
     </row>
     <row r="95" ht="13.8" customHeight="1" s="2">
@@ -76357,8 +79459,41 @@
       <c r="JD95" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="JE95" t="n">
+      <c r="JE95" s="1" t="n">
         <v>11</v>
+      </c>
+      <c r="JF95" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JG95" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JH95" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JI95" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JJ95" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JK95" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="JL95" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="JM95" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="JN95" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="JO95" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="JP95" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="96" ht="13.8" customHeight="1" s="2">
@@ -77156,8 +80291,41 @@
       <c r="JD96" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="JE96" t="n">
+      <c r="JE96" s="1" t="n">
         <v>9</v>
+      </c>
+      <c r="JF96" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="JG96" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="JH96" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="JI96" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="JJ96" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="JK96" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="JL96" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="JM96" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JN96" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="JO96" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="JP96" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="97" ht="13.8" customHeight="1" s="2">
@@ -77955,8 +81123,41 @@
       <c r="JD97" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="JE97" t="n">
+      <c r="JE97" s="1" t="n">
         <v>35</v>
+      </c>
+      <c r="JF97" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="JG97" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="JH97" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="JI97" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="JJ97" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="JK97" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="JL97" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="JM97" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="JN97" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="JO97" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="JP97" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="98" ht="13.8" customHeight="1" s="2">
@@ -78754,8 +81955,41 @@
       <c r="JD98" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="JE98" t="n">
+      <c r="JE98" s="1" t="n">
         <v>35</v>
+      </c>
+      <c r="JF98" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="JG98" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="JH98" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="JI98" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="JJ98" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="JK98" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="JL98" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="JM98" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="JN98" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="JO98" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="JP98" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="99" ht="13.8" customHeight="1" s="2">
@@ -79553,8 +82787,41 @@
       <c r="JD99" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="JE99" t="n">
+      <c r="JE99" s="1" t="n">
         <v>46</v>
+      </c>
+      <c r="JF99" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="JG99" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="JH99" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="JI99" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="JJ99" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="JK99" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="JL99" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="JM99" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="JN99" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="JO99" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="JP99" t="n">
+        <v>54</v>
       </c>
     </row>
     <row r="100" ht="13.8" customHeight="1" s="2">
@@ -80352,8 +83619,41 @@
       <c r="JD100" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="JE100" t="n">
+      <c r="JE100" s="1" t="n">
         <v>12</v>
+      </c>
+      <c r="JF100" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="JG100" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="JH100" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="JI100" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="JJ100" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="JK100" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="JL100" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="JM100" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="JN100" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="JO100" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="JP100" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="101" ht="13.8" customHeight="1" s="2">
@@ -81151,8 +84451,41 @@
       <c r="JD101" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="JE101" t="n">
+      <c r="JE101" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="JF101" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="JG101" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="JH101" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="JI101" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="JJ101" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="JK101" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="JL101" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="JM101" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="JN101" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="JO101" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="JP101" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="102" ht="13.8" customHeight="1" s="2">
@@ -81950,8 +85283,41 @@
       <c r="JD102" s="1" t="n">
         <v>64.3</v>
       </c>
-      <c r="JE102" t="n">
+      <c r="JE102" s="1" t="n">
         <v>53.8</v>
+      </c>
+      <c r="JF102" s="1" t="n">
+        <v>64.3</v>
+      </c>
+      <c r="JG102" s="1" t="n">
+        <v>64.3</v>
+      </c>
+      <c r="JH102" s="1" t="n">
+        <v>64.3</v>
+      </c>
+      <c r="JI102" s="1" t="n">
+        <v>64.3</v>
+      </c>
+      <c r="JJ102" s="1" t="n">
+        <v>64.3</v>
+      </c>
+      <c r="JK102" s="1" t="n">
+        <v>64.3</v>
+      </c>
+      <c r="JL102" s="1" t="n">
+        <v>64.7</v>
+      </c>
+      <c r="JM102" s="1" t="n">
+        <v>87.5</v>
+      </c>
+      <c r="JN102" s="1" t="n">
+        <v>84.59999999999999</v>
+      </c>
+      <c r="JO102" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="JP102" t="n">
+        <v>68.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>